<commit_message>
correctOCR.py deletes hyphens and that-symbol
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -2,12 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22040" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
+    <sheet name="exploratory charts" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -2286,10 +2287,10 @@
   <dimension ref="A1:FD211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="M173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G180" sqref="G180"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2299,7 +2300,7 @@
     <col min="3" max="3" width="4.5" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="22" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" style="7" customWidth="1"/>
@@ -25504,4 +25505,40 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
settings up to 65
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="0" windowWidth="20280" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="4040" yWindow="0" windowWidth="20280" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="600">
   <si>
     <t>f</t>
   </si>
@@ -1751,6 +1751,9 @@
     <t>14th century</t>
   </si>
   <si>
+    <t>Spain</t>
+  </si>
+  <si>
     <t>mentions Castile and Lisbon</t>
   </si>
   <si>
@@ -1803,6 +1806,24 @@
   </si>
   <si>
     <t>France and Switzerland</t>
+  </si>
+  <si>
+    <t>six stories, featuring desert, Sicily, Patagonia, Russia, Cornwall, Circassia, and desert again</t>
+  </si>
+  <si>
+    <t>Italy, Patagonia, Russia, England, desert</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>also somewhere other than Spain?</t>
+  </si>
+  <si>
+    <t>Henry II, 1133 – 1189</t>
+  </si>
+  <si>
+    <t>Germany and England</t>
   </si>
 </sst>
 </file>
@@ -1974,8 +1995,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2037,11 +2060,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6146,10 +6171,10 @@
   <dimension ref="A1:FD209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="M38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomRight" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9318,13 +9343,13 @@
     </row>
     <row r="29" spans="2:160">
       <c r="B29" s="3" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>574</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>536</v>
@@ -9761,7 +9786,7 @@
         <v>327</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>535</v>
@@ -10086,10 +10111,10 @@
         <v>327</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="D33" s="27" t="s">
         <v>579</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>578</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>545</v>
@@ -10163,7 +10188,7 @@
     </row>
     <row r="34" spans="1:160">
       <c r="B34" s="3" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>574</v>
@@ -10385,7 +10410,7 @@
     </row>
     <row r="35" spans="1:160">
       <c r="B35" s="3" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>349</v>
@@ -10597,7 +10622,7 @@
     </row>
     <row r="37" spans="1:160">
       <c r="B37" s="3" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>327</v>
@@ -10725,7 +10750,7 @@
         <v>327</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>538</v>
@@ -10808,7 +10833,7 @@
         <v>565</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>535</v>
@@ -11099,7 +11124,7 @@
     </row>
     <row r="42" spans="1:160">
       <c r="B42" s="3" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>327</v>
@@ -11230,7 +11255,7 @@
     </row>
     <row r="43" spans="1:160">
       <c r="B43" s="3" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>327</v>
@@ -11355,7 +11380,7 @@
         <v>327</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>535</v>
@@ -11481,7 +11506,7 @@
         <v>327</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>535</v>
@@ -11935,13 +11960,13 @@
     </row>
     <row r="49" spans="2:160">
       <c r="B49" s="3" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>363</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>535</v>
@@ -12054,7 +12079,7 @@
     </row>
     <row r="50" spans="2:160">
       <c r="B50" s="3" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>327</v>
@@ -12209,7 +12234,7 @@
     </row>
     <row r="51" spans="2:160">
       <c r="B51" s="3" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>349</v>
@@ -12392,6 +12417,15 @@
       </c>
     </row>
     <row r="53" spans="2:160">
+      <c r="B53" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>352</v>
+      </c>
       <c r="E53" s="3" t="s">
         <v>535</v>
       </c>
@@ -12475,6 +12509,12 @@
       </c>
     </row>
     <row r="54" spans="2:160">
+      <c r="B54" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E54" s="3" t="s">
         <v>537</v>
       </c>
@@ -12577,6 +12617,15 @@
       </c>
     </row>
     <row r="55" spans="2:160">
+      <c r="B55" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>569</v>
+      </c>
       <c r="E55" s="3" t="s">
         <v>535</v>
       </c>
@@ -12687,6 +12736,15 @@
       </c>
     </row>
     <row r="56" spans="2:160">
+      <c r="B56" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>594</v>
+      </c>
       <c r="E56" s="3" t="s">
         <v>538</v>
       </c>
@@ -12773,6 +12831,12 @@
       </c>
     </row>
     <row r="57" spans="2:160">
+      <c r="B57" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E57" s="3" t="s">
         <v>536</v>
       </c>
@@ -12889,6 +12953,15 @@
       </c>
     </row>
     <row r="58" spans="2:160">
+      <c r="B58" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>352</v>
+      </c>
       <c r="E58" s="3" t="s">
         <v>536</v>
       </c>
@@ -12996,6 +13069,12 @@
       </c>
     </row>
     <row r="59" spans="2:160">
+      <c r="B59" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E59" s="3" t="s">
         <v>536</v>
       </c>
@@ -13061,6 +13140,12 @@
       </c>
     </row>
     <row r="60" spans="2:160">
+      <c r="B60" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E60" s="3" t="s">
         <v>538</v>
       </c>
@@ -13198,6 +13283,12 @@
       </c>
     </row>
     <row r="61" spans="2:160">
+      <c r="B61" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E61" s="3" t="s">
         <v>538</v>
       </c>
@@ -13311,6 +13402,12 @@
       </c>
     </row>
     <row r="62" spans="2:160">
+      <c r="B62" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>597</v>
+      </c>
       <c r="E62" s="3" t="s">
         <v>537</v>
       </c>
@@ -13436,6 +13533,15 @@
       </c>
     </row>
     <row r="63" spans="2:160">
+      <c r="B63" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>598</v>
+      </c>
       <c r="E63" s="3" t="s">
         <v>537</v>
       </c>
@@ -13597,6 +13703,12 @@
       </c>
     </row>
     <row r="64" spans="2:160">
+      <c r="B64" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E64" s="3" t="s">
         <v>537</v>
       </c>
@@ -13658,7 +13770,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="5:160">
+    <row r="65" spans="2:160">
+      <c r="B65" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>327</v>
+      </c>
       <c r="E65" s="3" t="s">
         <v>538</v>
       </c>
@@ -13837,7 +13955,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="5:160">
+    <row r="66" spans="2:160">
+      <c r="B66" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>349</v>
+      </c>
       <c r="E66" s="3" t="s">
         <v>538</v>
       </c>
@@ -13974,7 +14098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="5:160">
+    <row r="67" spans="2:160">
       <c r="E67" s="3" t="s">
         <v>536</v>
       </c>
@@ -14096,7 +14220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="5:160">
+    <row r="68" spans="2:160">
       <c r="E68" s="3" t="s">
         <v>535</v>
       </c>
@@ -14161,7 +14285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="5:160">
+    <row r="69" spans="2:160">
       <c r="E69" s="3" t="s">
         <v>547</v>
       </c>
@@ -14253,7 +14377,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="5:160">
+    <row r="70" spans="2:160">
       <c r="E70" s="3" t="s">
         <v>535</v>
       </c>
@@ -14375,7 +14499,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="5:160">
+    <row r="71" spans="2:160">
       <c r="E71" s="3" t="s">
         <v>537</v>
       </c>
@@ -14554,7 +14678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="5:160">
+    <row r="72" spans="2:160">
       <c r="E72" s="3" t="s">
         <v>537</v>
       </c>
@@ -14718,7 +14842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="5:160">
+    <row r="73" spans="2:160">
       <c r="E73" s="3" t="s">
         <v>536</v>
       </c>
@@ -14762,7 +14886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="5:160">
+    <row r="74" spans="2:160">
       <c r="E74" s="3" t="s">
         <v>537</v>
       </c>
@@ -14836,7 +14960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="5:160">
+    <row r="75" spans="2:160">
       <c r="E75" s="3" t="s">
         <v>538</v>
       </c>
@@ -15000,7 +15124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="5:160">
+    <row r="76" spans="2:160">
       <c r="E76" s="3" t="s">
         <v>538</v>
       </c>
@@ -15188,7 +15312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="5:160">
+    <row r="77" spans="2:160">
       <c r="E77" s="3" t="s">
         <v>538</v>
       </c>
@@ -15367,7 +15491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="5:160">
+    <row r="78" spans="2:160">
       <c r="E78" s="3" t="s">
         <v>538</v>
       </c>
@@ -15469,7 +15593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="5:160">
+    <row r="79" spans="2:160">
       <c r="E79" s="3" t="s">
         <v>538</v>
       </c>
@@ -15588,7 +15712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="5:160">
+    <row r="80" spans="2:160">
       <c r="E80" s="3" t="s">
         <v>537</v>
       </c>

</xml_diff>

<commit_message>
jotted down ideas found on sticky notes
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="80" windowWidth="20800" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="2180" yWindow="1320" windowWidth="20800" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="618">
   <si>
     <t>f</t>
   </si>
@@ -1875,6 +1875,9 @@
   </si>
   <si>
     <t>http://books.google.ca/books?id=gLwNAAAAQAAJ&amp;printsec=frontcover&amp;dq=SIR+RALPH+WILLOUGHBY&amp;hl=en&amp;sa=X&amp;ei=S7rUU_HCM-GejALasYDYAw&amp;redir_esc=y#v=onepage&amp;q&amp;f=false</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWGHZMQ556013712</t>
   </si>
 </sst>
 </file>
@@ -6279,7 +6282,7 @@
       <pane xSplit="13" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8413,6 +8416,12 @@
       <c r="F16" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="G16" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>605</v>
+      </c>
       <c r="I16" s="3" t="s">
         <v>346</v>
       </c>

</xml_diff>

<commit_message>
settings to 104 - halfway!
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="657">
   <si>
     <t>f</t>
   </si>
@@ -1947,6 +1947,54 @@
   </si>
   <si>
     <t>mentions Lady Jane Gray and Henry VIII; Edward VI is an active character</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>girls are daughters of Mary Queen of Scots; QEI is a character</t>
+  </si>
+  <si>
+    <t>historical'</t>
+  </si>
+  <si>
+    <t>historical'; Earl of Salisbury is a character; Salisbury is son of Henry II</t>
+  </si>
+  <si>
+    <t>Henry II</t>
+  </si>
+  <si>
+    <t>Venice; there is a Doge</t>
+  </si>
+  <si>
+    <t>mentions Emperor- of France? what time?</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>four stories</t>
+  </si>
+  <si>
+    <t>twenty verse tales</t>
+  </si>
+  <si>
+    <t>Verse! Verse! Not a novel at all!!</t>
+  </si>
+  <si>
+    <t>Lewis, Matthew (apparently false)</t>
+  </si>
+  <si>
+    <t>mentions Godwin</t>
+  </si>
+  <si>
+    <t>Wales AND NEWGATE?</t>
+  </si>
+  <si>
+    <t>character born in Newgate; mentions Frankenstein; might involve more locations, since it mentions 'travels'</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2219,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2227,6 +2275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6380,7 +6429,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I92" sqref="I92"/>
+      <selection pane="bottomRight" activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17809,8 +17858,12 @@
       <c r="F92" s="18">
         <v>91</v>
       </c>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
+      <c r="G92" s="27" t="s">
+        <v>641</v>
+      </c>
+      <c r="H92" s="27" t="s">
+        <v>327</v>
+      </c>
       <c r="I92" s="27"/>
       <c r="J92" s="27" t="s">
         <v>537</v>
@@ -17897,9 +17950,15 @@
       <c r="F93" s="18">
         <v>92</v>
       </c>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
+      <c r="G93" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H93" s="27" t="s">
+        <v>639</v>
+      </c>
+      <c r="I93" s="27" t="s">
+        <v>642</v>
+      </c>
       <c r="J93" s="27" t="s">
         <v>534</v>
       </c>
@@ -18045,8 +18104,12 @@
       <c r="F94" s="18">
         <v>93</v>
       </c>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
+      <c r="G94" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H94" s="27" t="s">
+        <v>327</v>
+      </c>
       <c r="I94" s="27"/>
       <c r="J94" s="27" t="s">
         <v>539</v>
@@ -18121,9 +18184,15 @@
       <c r="F95" s="18">
         <v>94</v>
       </c>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
+      <c r="G95" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H95" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I95" s="27" t="s">
+        <v>352</v>
+      </c>
       <c r="J95" s="27" t="s">
         <v>534</v>
       </c>
@@ -18185,9 +18254,15 @@
       <c r="F96" s="18">
         <v>95</v>
       </c>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
+      <c r="G96" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H96" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="I96" s="29" t="s">
+        <v>644</v>
+      </c>
       <c r="J96" s="27" t="s">
         <v>536</v>
       </c>
@@ -18342,9 +18417,15 @@
       <c r="F97" s="18">
         <v>96</v>
       </c>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
+      <c r="G97" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="H97" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I97" s="27" t="s">
+        <v>646</v>
+      </c>
       <c r="J97" s="27" t="s">
         <v>535</v>
       </c>
@@ -18397,9 +18478,15 @@
       <c r="F98" s="18">
         <v>97</v>
       </c>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
+      <c r="G98" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H98" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I98" s="27" t="s">
+        <v>647</v>
+      </c>
       <c r="J98" s="27" t="s">
         <v>537</v>
       </c>
@@ -18584,9 +18671,15 @@
       <c r="F99" s="18">
         <v>98</v>
       </c>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
+      <c r="G99" s="27" t="s">
+        <v>648</v>
+      </c>
+      <c r="H99" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I99" s="29" t="s">
+        <v>643</v>
+      </c>
       <c r="J99" s="27" t="s">
         <v>547</v>
       </c>
@@ -18663,9 +18756,15 @@
       <c r="F100" s="18">
         <v>99</v>
       </c>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
+      <c r="G100" s="27" t="s">
+        <v>574</v>
+      </c>
+      <c r="H100" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I100" s="27" t="s">
+        <v>649</v>
+      </c>
       <c r="J100" s="27" t="s">
         <v>534</v>
       </c>
@@ -18913,9 +19012,15 @@
       <c r="F101" s="18">
         <v>100</v>
       </c>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
+      <c r="G101" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H101" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I101" s="27" t="s">
+        <v>650</v>
+      </c>
       <c r="J101" s="27" t="s">
         <v>537</v>
       </c>
@@ -19046,8 +19151,11 @@
       </c>
     </row>
     <row r="102" spans="1:161">
+      <c r="A102" s="3" t="s">
+        <v>652</v>
+      </c>
       <c r="B102" s="3" t="s">
-        <v>209</v>
+        <v>653</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>9</v>
@@ -19061,9 +19169,15 @@
       <c r="F102" s="18">
         <v>101</v>
       </c>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
+      <c r="G102" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H102" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I102" s="27" t="s">
+        <v>651</v>
+      </c>
       <c r="J102" s="27" t="s">
         <v>548</v>
       </c>
@@ -19164,8 +19278,12 @@
       <c r="F103" s="18">
         <v>102</v>
       </c>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
+      <c r="G103" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="H103" s="27" t="s">
+        <v>327</v>
+      </c>
       <c r="I103" s="27"/>
       <c r="J103" s="27" t="s">
         <v>549</v>
@@ -19231,9 +19349,15 @@
       <c r="F104" s="18">
         <v>103</v>
       </c>
-      <c r="G104" s="27"/>
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
+      <c r="G104" s="27" t="s">
+        <v>655</v>
+      </c>
+      <c r="H104" s="27" t="s">
+        <v>624</v>
+      </c>
+      <c r="I104" s="27" t="s">
+        <v>656</v>
+      </c>
       <c r="J104" s="27" t="s">
         <v>534</v>
       </c>
@@ -19274,9 +19398,15 @@
       <c r="F105" s="18">
         <v>104</v>
       </c>
-      <c r="G105" s="27"/>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
+      <c r="G105" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H105" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="I105" s="27" t="s">
+        <v>654</v>
+      </c>
       <c r="J105" s="27" t="s">
         <v>537</v>
       </c>

</xml_diff>

<commit_message>
full text of 19
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="675">
   <si>
     <t>f</t>
   </si>
@@ -2043,6 +2043,12 @@
   </si>
   <si>
     <t>Uvic</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CNQEWFD661209029</t>
+  </si>
+  <si>
+    <t>http://books.google.ca/books?id=BWEmAAAAMAAJ&amp;printsec=frontcover&amp;dq=SALATHIEL.+A+STORY+OF+THE+PAST,+THE+PRESENT,+AND+THE+FUTURE&amp;hl=en&amp;sa=X&amp;ei=OcHhU8v5DdDdoATYiIHwCQ&amp;ved=0CBsQ6AEwAA#v=onepage&amp;q=SALATHIEL.%20A%20STORY%20OF%20THE%20PAST%2C%20THE%20PRESENT%2C%20AND%20THE%20FUTURE&amp;f=false</t>
   </si>
 </sst>
 </file>
@@ -2214,8 +2220,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2339,7 +2349,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2372,6 +2382,8 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2404,6 +2416,8 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5933,7 +5947,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6059,112 +6179,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -6505,7 +6519,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9012,9 +9026,15 @@
       <c r="K20" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
+      <c r="L20" s="27" t="s">
+        <v>674</v>
+      </c>
+      <c r="M20" s="27" t="s">
+        <v>673</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>602</v>
+      </c>
       <c r="AF20" s="21">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
failed to find texts 20-27
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="800" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="1580" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="676">
   <si>
     <t>f</t>
   </si>
@@ -1034,12 +1034,6 @@
     <t>THE MYSTERIOUS MURDER, OR, THE USURPER OF NAPLES. AN ORIGINAL ROMANCE. TO WHICH IS PREFIXED THE NOCTURNAL ASSASSIN, OR, SPANISH JEALOUSY</t>
   </si>
   <si>
-    <t>THE ITALIAN BANDITTI, OR, THE SECRET HISTORY OF HENRY AND MATILDA. A ROMANCE. With HORRIBLE REVENGE is bound HOPELESS LOVE. AN INTERESTING TALE</t>
-  </si>
-  <si>
-    <t>HORRIBLE REVENGE, OR, THE MONSTER OF ITALY!!</t>
-  </si>
-  <si>
     <t>FATAL SECRETS, OR, ETHERLINDA DE SALMONI. A SICILIAN STORY</t>
   </si>
   <si>
@@ -2049,6 +2043,15 @@
   </si>
   <si>
     <t>http://books.google.ca/books?id=BWEmAAAAMAAJ&amp;printsec=frontcover&amp;dq=SALATHIEL.+A+STORY+OF+THE+PAST,+THE+PRESENT,+AND+THE+FUTURE&amp;hl=en&amp;sa=X&amp;ei=OcHhU8v5DdDdoATYiIHwCQ&amp;ved=0CBsQ6AEwAA#v=onepage&amp;q=SALATHIEL.%20A%20STORY%20OF%20THE%20PAST%2C%20THE%20PRESENT%2C%20AND%20THE%20FUTURE&amp;f=false</t>
+  </si>
+  <si>
+    <t>none!</t>
+  </si>
+  <si>
+    <t>THE ITALIAN BANDITTI, OR, THE SECRET HISTORY OF HENRY AND MATILDA. A ROMANCE.</t>
+  </si>
+  <si>
+    <t>HORRIBLE REVENGE, OR, THE MONSTER OF ITALY!! With HORRIBLE REVENGE is bound HOPELESS LOVE. AN INTERESTING TALE</t>
   </si>
 </sst>
 </file>
@@ -2220,8 +2223,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2349,7 +2380,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2384,6 +2415,20 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2418,6 +2463,20 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5947,113 +6006,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6179,6 +6132,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -6519,7 +6578,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6687,82 +6746,82 @@
   <sheetData>
     <row r="1" spans="1:162" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>526</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>525</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>524</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>531</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>530</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>529</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>532</v>
-      </c>
       <c r="K1" s="9" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>670</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>672</v>
-      </c>
       <c r="N1" s="9" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="W1" s="16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="Z1" s="14" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="AA1" s="8" t="s">
         <v>36</v>
@@ -6771,112 +6830,112 @@
         <v>212</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="AG1" s="16" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="AI1" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AK1" s="15" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AL1" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="AN1" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="AO1" s="15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="AP1" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AQ1" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AR1" s="8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AS1" s="15" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AT1" s="16" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AU1" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="AV1" s="8" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AW1" s="8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="AX1" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AY1" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="AZ1" s="8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="BA1" s="8" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="BB1" s="8" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="BC1" s="15" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="BD1" s="8" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="BE1" s="8" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="BF1" s="8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="BG1" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="BH1" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="BI1" s="16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="BJ1" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="BK1" s="16" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="BL1" s="8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="BM1" s="8" t="s">
         <v>11</v>
@@ -6888,181 +6947,181 @@
         <v>200</v>
       </c>
       <c r="BP1" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="BQ1" s="16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="BR1" s="16" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="BS1" s="8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="BT1" s="8" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="BU1" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="BV1" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="BW1" s="17" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="BX1" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="BY1" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="BZ1" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="CA1" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="CB1" s="17" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="CC1" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="CD1" s="16" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="CE1" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="CF1" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="CG1" s="17" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="CH1" s="16" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="CI1" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="CJ1" s="17" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="CK1" s="8" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="CL1" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="CM1" s="8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="CN1" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="CO1" s="17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="CP1" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="CQ1" s="8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="CR1" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="CS1" s="8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="CT1" s="8" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="CU1" s="17" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="CV1" s="8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="CW1" s="17" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="CX1" s="8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="CY1" s="14" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="CZ1" s="8" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="DA1" s="8" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="DB1" s="8" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="DC1" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="DD1" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="DE1" s="8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="DF1" s="8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="DG1" s="8" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="DH1" s="8" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="DI1" s="8" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="DJ1" s="16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="DK1" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="DL1" s="8" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="DM1" s="8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="DN1" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="DO1" s="8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="DP1" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="DQ1" s="16" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="DR1" s="8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="DS1" s="16" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="DT1" s="16" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="DU1" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="DV1" s="8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="DW1" s="8" t="s">
         <v>8</v>
@@ -7071,117 +7130,117 @@
         <v>38</v>
       </c>
       <c r="DY1" s="8" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="DZ1" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="EA1" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="EB1" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="EC1" s="17" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="ED1" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="EE1" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="EF1" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="EG1" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="EH1" s="17" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="EI1" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="EJ1" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="EK1" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="EL1" s="15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="EM1" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="EN1" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="EO1" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="EP1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="EQ1" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="ER1" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="ES1" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="ET1" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="EU1" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="EV1" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="EW1" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="EX1" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="EY1" s="16" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="EZ1" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="FA1" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="FB1" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="FC1" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="FD1" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="FE1" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="FF1" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:162">
       <c r="B2" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E2" s="4">
         <v>1819</v>
@@ -7197,19 +7256,19 @@
       </c>
       <c r="I2" s="27"/>
       <c r="J2" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="S2" s="19">
         <v>2</v>
@@ -7386,18 +7445,18 @@
         <v>1</v>
       </c>
       <c r="FF2" s="20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:162">
       <c r="B3" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E3" s="4">
         <v>1792</v>
@@ -7413,17 +7472,17 @@
       </c>
       <c r="I3" s="27"/>
       <c r="J3" s="27" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L3" s="27"/>
       <c r="M3" s="27" t="s">
+        <v>598</v>
+      </c>
+      <c r="N3" s="27" t="s">
         <v>600</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>602</v>
       </c>
       <c r="CC3" s="3">
         <v>1</v>
@@ -7434,13 +7493,13 @@
     </row>
     <row r="4" spans="1:162">
       <c r="B4" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E4" s="4">
         <v>1786</v>
@@ -7449,24 +7508,24 @@
         <v>3</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H4" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K4" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="27"/>
       <c r="M4" s="27" t="s">
+        <v>599</v>
+      </c>
+      <c r="N4" s="27" t="s">
         <v>601</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>603</v>
       </c>
       <c r="AG4" s="21">
         <v>1</v>
@@ -7525,7 +7584,7 @@
     </row>
     <row r="5" spans="1:162">
       <c r="A5" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>65</v>
@@ -7534,7 +7593,7 @@
         <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>32</v>
@@ -7543,23 +7602,25 @@
         <v>4</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K5" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
+      <c r="N5" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="Y5" s="19">
         <v>1</v>
       </c>
@@ -7623,13 +7684,13 @@
     </row>
     <row r="6" spans="1:162">
       <c r="B6" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E6" s="4">
         <v>1826</v>
@@ -7638,26 +7699,26 @@
         <v>5</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="27" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="S6" s="19">
         <v>1</v>
@@ -7761,13 +7822,13 @@
     </row>
     <row r="7" spans="1:162">
       <c r="B7" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E7" s="4">
         <v>1796</v>
@@ -7783,17 +7844,17 @@
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K7" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="27"/>
       <c r="M7" s="27" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="Z7" s="19">
         <v>1</v>
@@ -7880,18 +7941,18 @@
         <v>1</v>
       </c>
       <c r="FF7" s="20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:162">
       <c r="B8" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E8" s="4">
         <v>1790</v>
@@ -7900,26 +7961,26 @@
         <v>7</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K8" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="27" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="N8" s="27" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="BD8" s="3">
         <v>1</v>
@@ -7987,13 +8048,13 @@
     </row>
     <row r="9" spans="1:162">
       <c r="B9" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E9" s="4">
         <v>1773</v>
@@ -8009,17 +8070,17 @@
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K9" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="27"/>
       <c r="M9" s="27" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="BQ9" s="21">
         <v>1</v>
@@ -8051,13 +8112,13 @@
     </row>
     <row r="10" spans="1:162">
       <c r="B10" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E10" s="4">
         <v>1799</v>
@@ -8066,26 +8127,26 @@
         <v>9</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H10" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K10" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L10" s="27"/>
       <c r="M10" s="27" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="Y10" s="19">
         <v>1</v>
@@ -8237,13 +8298,13 @@
     </row>
     <row r="11" spans="1:162">
       <c r="B11" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E11" s="4">
         <v>1808</v>
@@ -8259,17 +8320,17 @@
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K11" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="27" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="N11" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="W11" s="21">
         <v>1</v>
@@ -8352,13 +8413,13 @@
     </row>
     <row r="12" spans="1:162">
       <c r="B12" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E12" s="4">
         <v>1819</v>
@@ -8367,24 +8428,24 @@
         <v>11</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H12" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K12" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L12" s="27"/>
       <c r="M12" s="27" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="N12" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AH12" s="3">
         <v>1</v>
@@ -8461,13 +8522,13 @@
     </row>
     <row r="13" spans="1:162">
       <c r="B13" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E13" s="4">
         <v>1802</v>
@@ -8476,24 +8537,24 @@
         <v>12</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K13" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="27"/>
       <c r="M13" s="27" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="N13" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="S13" s="19">
         <v>1</v>
@@ -8546,13 +8607,13 @@
     </row>
     <row r="14" spans="1:162">
       <c r="B14" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E14" s="4">
         <v>1792</v>
@@ -8567,20 +8628,20 @@
         <v>327</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="27" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="N14" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AH14" s="23"/>
       <c r="AY14" s="3">
@@ -8620,13 +8681,13 @@
     </row>
     <row r="15" spans="1:162">
       <c r="B15" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E15" s="4">
         <v>1820</v>
@@ -8635,21 +8696,21 @@
         <v>14</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I15" s="27"/>
       <c r="J15" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K15" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="27" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="N15" s="27" t="s">
         <v>125</v>
@@ -8669,13 +8730,13 @@
     </row>
     <row r="16" spans="1:162">
       <c r="B16" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E16" s="4">
         <v>1796</v>
@@ -8690,20 +8751,20 @@
         <v>327</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K16" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="N16" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AY16" s="3">
         <v>1</v>
@@ -8735,13 +8796,13 @@
     </row>
     <row r="17" spans="2:162">
       <c r="B17" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E17" s="4">
         <v>1797</v>
@@ -8750,26 +8811,26 @@
         <v>16</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H17" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K17" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="27"/>
       <c r="M17" s="27" t="s">
+        <v>664</v>
+      </c>
+      <c r="N17" s="27" t="s">
         <v>666</v>
-      </c>
-      <c r="N17" s="27" t="s">
-        <v>668</v>
       </c>
       <c r="AE17" s="21">
         <v>1</v>
@@ -8867,7 +8928,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E18" s="4">
         <v>1802</v>
@@ -8876,26 +8937,26 @@
         <v>17</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K18" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L18" s="27"/>
       <c r="M18" s="27" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="S18" s="19">
         <v>1</v>
@@ -8927,7 +8988,7 @@
         <v>64</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E19" s="4">
         <v>1794</v>
@@ -8943,17 +9004,17 @@
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K19" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L19" s="27"/>
       <c r="M19" s="27" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="N19" s="27" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="W19" s="21">
         <v>1</v>
@@ -8997,13 +9058,13 @@
     </row>
     <row r="20" spans="2:162">
       <c r="B20" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E20" s="4">
         <v>1828</v>
@@ -9012,28 +9073,28 @@
         <v>19</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K20" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M20" s="27" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="N20" s="27" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AF20" s="21">
         <v>1</v>
@@ -9095,7 +9156,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E21" s="4">
         <v>1806</v>
@@ -9104,23 +9165,25 @@
         <v>20</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H21" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K21" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
+      <c r="N21" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="S21" s="19">
         <v>1</v>
       </c>
@@ -9226,7 +9289,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>337</v>
+        <v>675</v>
       </c>
       <c r="E22" s="4">
         <v>1808</v>
@@ -9235,21 +9298,23 @@
         <v>21</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H22" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K22" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
+      <c r="N22" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="BR22" s="21">
         <v>1</v>
       </c>
@@ -9298,7 +9363,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>336</v>
+        <v>674</v>
       </c>
       <c r="E23" s="4">
         <v>1811</v>
@@ -9307,21 +9372,23 @@
         <v>22</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H23" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I23" s="27"/>
       <c r="J23" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K23" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
+      <c r="N23" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="S23" s="19">
         <v>1</v>
       </c>
@@ -9370,23 +9437,25 @@
         <v>23</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H24" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K24" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
+      <c r="N24" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="AL24" s="3">
         <v>1</v>
       </c>
@@ -9441,23 +9510,25 @@
         <v>24</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H25" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="K25" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
+      <c r="N25" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="O25" s="19">
         <v>1</v>
       </c>
@@ -9669,14 +9740,16 @@
       </c>
       <c r="I26" s="27"/>
       <c r="J26" s="27" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="K26" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
+      <c r="N26" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="S26" s="19">
         <v>1</v>
       </c>
@@ -9747,14 +9820,16 @@
       </c>
       <c r="I27" s="27"/>
       <c r="J27" s="27" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K27" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
+      <c r="N27" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="S27" s="19">
         <v>1</v>
       </c>
@@ -9834,14 +9909,16 @@
       </c>
       <c r="I28" s="27"/>
       <c r="J28" s="27" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K28" s="27" t="s">
         <v>35</v>
       </c>
       <c r="L28" s="27"/>
       <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
+      <c r="N28" s="27" t="s">
+        <v>673</v>
+      </c>
       <c r="S28" s="19">
         <v>1</v>
       </c>
@@ -9882,16 +9959,16 @@
         <v>28</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H29" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="I29" s="27" t="s">
         <v>572</v>
       </c>
-      <c r="I29" s="27" t="s">
-        <v>574</v>
-      </c>
       <c r="J29" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K29" s="27" t="s">
         <v>2</v>
@@ -10062,7 +10139,7 @@
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K30" s="27" t="s">
         <v>2</v>
@@ -10332,10 +10409,10 @@
         <v>327</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K31" s="27" t="s">
         <v>2</v>
@@ -10473,7 +10550,7 @@
       </c>
       <c r="I32" s="27"/>
       <c r="J32" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K32" s="27" t="s">
         <v>2</v>
@@ -10664,13 +10741,13 @@
         <v>327</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I33" s="27" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K33" s="27" t="s">
         <v>2</v>
@@ -10744,14 +10821,14 @@
         <v>33</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I34" s="27"/>
       <c r="J34" s="27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K34" s="27" t="s">
         <v>2</v>
@@ -10970,16 +11047,16 @@
         <v>34</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I35" s="27">
         <v>1516</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K35" s="27" t="s">
         <v>2</v>
@@ -11072,7 +11149,7 @@
       </c>
       <c r="I36" s="27"/>
       <c r="J36" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K36" s="27" t="s">
         <v>2</v>
@@ -11189,14 +11266,14 @@
         <v>36</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H37" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I37" s="27"/>
       <c r="J37" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K37" s="27" t="s">
         <v>2</v>
@@ -11315,16 +11392,16 @@
         <v>37</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H38" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K38" s="27" t="s">
         <v>2</v>
@@ -11404,14 +11481,14 @@
         <v>38</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K39" s="27" t="s">
         <v>2</v>
@@ -11551,10 +11628,10 @@
         <v>327</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K40" s="27" t="s">
         <v>2</v>
@@ -11595,14 +11672,14 @@
         <v>40</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H41" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I41" s="27"/>
       <c r="J41" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K41" s="27" t="s">
         <v>2</v>
@@ -11709,14 +11786,14 @@
         <v>41</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H42" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I42" s="27"/>
       <c r="J42" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K42" s="27" t="s">
         <v>2</v>
@@ -11844,14 +11921,14 @@
         <v>42</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H43" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I43" s="27"/>
       <c r="J43" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K43" s="27" t="s">
         <v>2</v>
@@ -11973,10 +12050,10 @@
         <v>327</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K44" s="27" t="s">
         <v>2</v>
@@ -12102,10 +12179,10 @@
         <v>327</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J45" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K45" s="27" t="s">
         <v>2</v>
@@ -12189,7 +12266,7 @@
       </c>
       <c r="I46" s="27"/>
       <c r="J46" s="27" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="K46" s="27" t="s">
         <v>35</v>
@@ -12322,7 +12399,7 @@
       </c>
       <c r="I47" s="27"/>
       <c r="J47" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K47" s="27" t="s">
         <v>2</v>
@@ -12410,7 +12487,7 @@
       </c>
       <c r="I48" s="27"/>
       <c r="J48" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K48" s="27" t="s">
         <v>2</v>
@@ -12571,16 +12648,16 @@
         <v>48</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K49" s="27" t="s">
         <v>2</v>
@@ -12693,14 +12770,14 @@
         <v>49</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="H50" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K50" s="27" t="s">
         <v>2</v>
@@ -12852,14 +12929,14 @@
         <v>50</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K51" s="27" t="s">
         <v>2</v>
@@ -12954,14 +13031,14 @@
         <v>51</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I52" s="27"/>
       <c r="J52" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K52" s="27" t="s">
         <v>2</v>
@@ -13044,16 +13121,16 @@
         <v>52</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H53" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I53" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J53" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K53" s="27" t="s">
         <v>2</v>
@@ -13146,7 +13223,7 @@
       </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K54" s="27" t="s">
         <v>2</v>
@@ -13251,16 +13328,16 @@
         <v>54</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H55" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J55" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K55" s="27" t="s">
         <v>2</v>
@@ -13373,16 +13450,16 @@
         <v>55</v>
       </c>
       <c r="G56" s="27" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H56" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="J56" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K56" s="27" t="s">
         <v>2</v>
@@ -13471,14 +13548,14 @@
         <v>56</v>
       </c>
       <c r="G57" s="27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H57" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I57" s="27"/>
       <c r="J57" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K57" s="27" t="s">
         <v>2</v>
@@ -13603,10 +13680,10 @@
         <v>327</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J58" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K58" s="27" t="s">
         <v>2</v>
@@ -13723,7 +13800,7 @@
       </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K59" s="27" t="s">
         <v>2</v>
@@ -13798,7 +13875,7 @@
       </c>
       <c r="I60" s="27"/>
       <c r="J60" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K60" s="27" t="s">
         <v>2</v>
@@ -13938,14 +14015,14 @@
         <v>60</v>
       </c>
       <c r="G61" s="27" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H61" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I61" s="27"/>
       <c r="J61" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K61" s="27" t="s">
         <v>2</v>
@@ -14061,14 +14138,14 @@
         <v>61</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H62" s="27"/>
       <c r="I62" s="27" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J62" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K62" s="27" t="s">
         <v>2</v>
@@ -14196,16 +14273,16 @@
         <v>62</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H63" s="27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I63" s="27" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J63" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K63" s="27" t="s">
         <v>2</v>
@@ -14369,14 +14446,14 @@
         <v>63</v>
       </c>
       <c r="G64" s="27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H64" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I64" s="27"/>
       <c r="J64" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K64" s="27" t="s">
         <v>2</v>
@@ -14441,14 +14518,14 @@
         <v>64</v>
       </c>
       <c r="G65" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H65" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I65" s="27"/>
       <c r="J65" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K65" s="27" t="s">
         <v>2</v>
@@ -14630,14 +14707,14 @@
         <v>65</v>
       </c>
       <c r="G66" s="27" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I66" s="27"/>
       <c r="J66" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K66" s="27" t="s">
         <v>2</v>
@@ -14777,14 +14854,14 @@
         <v>66</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H67" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I67" s="27"/>
       <c r="J67" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K67" s="27" t="s">
         <v>2</v>
@@ -14909,16 +14986,16 @@
         <v>67</v>
       </c>
       <c r="G68" s="27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H68" s="27" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J68" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K68" s="27" t="s">
         <v>2</v>
@@ -14986,16 +15063,16 @@
         <v>68</v>
       </c>
       <c r="G69" s="27" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H69" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I69" s="27" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="J69" s="27" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="K69" s="27" t="s">
         <v>2</v>
@@ -15090,16 +15167,16 @@
         <v>69</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H70" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="J70" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K70" s="27" t="s">
         <v>2</v>
@@ -15224,16 +15301,16 @@
         <v>70</v>
       </c>
       <c r="G71" s="27" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H71" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="J71" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K71" s="27" t="s">
         <v>2</v>
@@ -15421,10 +15498,10 @@
         <v>327</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="J72" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K72" s="27" t="s">
         <v>2</v>
@@ -15591,16 +15668,16 @@
         <v>72</v>
       </c>
       <c r="G73" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H73" s="27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I73" s="27" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J73" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K73" s="27" t="s">
         <v>2</v>
@@ -15653,7 +15730,7 @@
         <v>327</v>
       </c>
       <c r="J74" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K74" s="27" t="s">
         <v>2</v>
@@ -15730,16 +15807,16 @@
         <v>74</v>
       </c>
       <c r="G75" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H75" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I75" s="27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="J75" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K75" s="27" t="s">
         <v>2</v>
@@ -15906,16 +15983,16 @@
         <v>75</v>
       </c>
       <c r="G76" s="27" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H76" s="27" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="I76" s="27" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J76" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K76" s="27" t="s">
         <v>2</v>
@@ -16113,7 +16190,7 @@
       </c>
       <c r="I77" s="27"/>
       <c r="J77" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K77" s="27" t="s">
         <v>2</v>
@@ -16302,7 +16379,7 @@
       </c>
       <c r="I78" s="27"/>
       <c r="J78" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K78" s="27" t="s">
         <v>2</v>
@@ -16407,16 +16484,16 @@
         <v>78</v>
       </c>
       <c r="G79" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="J79" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K79" s="27" t="s">
         <v>2</v>
@@ -16545,7 +16622,7 @@
       </c>
       <c r="I80" s="27"/>
       <c r="J80" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K80" s="27" t="s">
         <v>2</v>
@@ -16626,7 +16703,7 @@
       </c>
       <c r="I81" s="27"/>
       <c r="J81" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K81" s="27" t="s">
         <v>2</v>
@@ -16754,10 +16831,10 @@
         <v>327</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J82" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K82" s="27" t="s">
         <v>2</v>
@@ -16837,16 +16914,16 @@
         <v>82</v>
       </c>
       <c r="G83" s="27" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H83" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="J83" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K83" s="27" t="s">
         <v>2</v>
@@ -16962,14 +17039,14 @@
         <v>83</v>
       </c>
       <c r="G84" s="27" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H84" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I84" s="27"/>
       <c r="J84" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K84" s="27" t="s">
         <v>2</v>
@@ -17149,16 +17226,16 @@
         <v>84</v>
       </c>
       <c r="G85" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H85" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I85" s="27" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="J85" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K85" s="27" t="s">
         <v>2</v>
@@ -17227,7 +17304,7 @@
       </c>
       <c r="I86" s="27"/>
       <c r="J86" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K86" s="27" t="s">
         <v>2</v>
@@ -17376,16 +17453,16 @@
         <v>86</v>
       </c>
       <c r="G87" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H87" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I87" s="27" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J87" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K87" s="27" t="s">
         <v>2</v>
@@ -17552,16 +17629,16 @@
         <v>87</v>
       </c>
       <c r="G88" s="27" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H88" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I88" s="27" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J88" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K88" s="27" t="s">
         <v>2</v>
@@ -17695,16 +17772,16 @@
         <v>88</v>
       </c>
       <c r="G89" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H89" s="27" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="I89" s="27" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J89" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K89" s="27" t="s">
         <v>2</v>
@@ -17829,14 +17906,14 @@
         <v>89</v>
       </c>
       <c r="G90" s="27" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H90" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I90" s="27"/>
       <c r="J90" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K90" s="27" t="s">
         <v>2</v>
@@ -17910,16 +17987,16 @@
         <v>90</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H91" s="27" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="I91" s="27" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J91" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K91" s="27" t="s">
         <v>2</v>
@@ -18062,14 +18139,14 @@
         <v>91</v>
       </c>
       <c r="G92" s="27" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H92" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I92" s="27"/>
       <c r="J92" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K92" s="27" t="s">
         <v>2</v>
@@ -18155,16 +18232,16 @@
         <v>92</v>
       </c>
       <c r="G93" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H93" s="27" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="I93" s="27" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J93" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K93" s="27" t="s">
         <v>2</v>
@@ -18317,7 +18394,7 @@
       </c>
       <c r="I94" s="27"/>
       <c r="J94" s="27" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K94" s="27" t="s">
         <v>35</v>
@@ -18397,10 +18474,10 @@
         <v>327</v>
       </c>
       <c r="I95" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J95" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K95" s="27" t="s">
         <v>2</v>
@@ -18462,16 +18539,16 @@
         <v>95</v>
       </c>
       <c r="G96" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="I96" s="29" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J96" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K96" s="27" t="s">
         <v>2</v>
@@ -18626,16 +18703,16 @@
         <v>96</v>
       </c>
       <c r="G97" s="27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H97" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I97" s="27" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J97" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K97" s="27" t="s">
         <v>2</v>
@@ -18694,10 +18771,10 @@
         <v>327</v>
       </c>
       <c r="I98" s="27" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J98" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K98" s="27" t="s">
         <v>2</v>
@@ -18882,16 +18959,16 @@
         <v>98</v>
       </c>
       <c r="G99" s="27" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H99" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I99" s="29" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J99" s="27" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K99" s="27" t="s">
         <v>35</v>
@@ -18968,16 +19045,16 @@
         <v>99</v>
       </c>
       <c r="G100" s="27" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H100" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I100" s="27" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J100" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K100" s="27" t="s">
         <v>2</v>
@@ -19231,10 +19308,10 @@
         <v>327</v>
       </c>
       <c r="I101" s="27" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J101" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K101" s="27" t="s">
         <v>2</v>
@@ -19365,10 +19442,10 @@
     </row>
     <row r="102" spans="1:162">
       <c r="A102" s="3" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>9</v>
@@ -19389,10 +19466,10 @@
         <v>327</v>
       </c>
       <c r="I102" s="27" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J102" s="27" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="K102" s="27" t="s">
         <v>35</v>
@@ -19500,7 +19577,7 @@
       </c>
       <c r="I103" s="27"/>
       <c r="J103" s="27" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="K103" s="27" t="s">
         <v>35</v>
@@ -19565,16 +19642,16 @@
         <v>103</v>
       </c>
       <c r="G104" s="27" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H104" s="27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I104" s="27" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J104" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K104" s="27" t="s">
         <v>2</v>
@@ -19615,16 +19692,16 @@
         <v>104</v>
       </c>
       <c r="G105" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H105" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I105" s="27" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J105" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K105" s="27" t="s">
         <v>2</v>
@@ -19716,16 +19793,16 @@
         <v>105</v>
       </c>
       <c r="G106" s="27" t="s">
+        <v>652</v>
+      </c>
+      <c r="H106" s="27" t="s">
         <v>654</v>
       </c>
-      <c r="H106" s="27" t="s">
-        <v>656</v>
-      </c>
       <c r="I106" s="29" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J106" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K106" s="27" t="s">
         <v>2</v>
@@ -19787,14 +19864,14 @@
         <v>106</v>
       </c>
       <c r="G107" s="27" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="H107" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I107" s="27"/>
       <c r="J107" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K107" s="27" t="s">
         <v>2</v>
@@ -19889,10 +19966,10 @@
         <v>327</v>
       </c>
       <c r="I108" s="27" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J108" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K108" s="27" t="s">
         <v>2</v>
@@ -20055,7 +20132,7 @@
       </c>
       <c r="I109" s="27"/>
       <c r="J109" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K109" s="27" t="s">
         <v>2</v>
@@ -20228,16 +20305,16 @@
         <v>109</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H110" s="27" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="I110" s="27" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J110" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K110" s="27" t="s">
         <v>2</v>
@@ -20428,14 +20505,14 @@
         <v>110</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H111" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I111" s="27"/>
       <c r="J111" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K111" s="27" t="s">
         <v>2</v>
@@ -20492,16 +20569,16 @@
         <v>111</v>
       </c>
       <c r="G112" s="27" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H112" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I112" s="27" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J112" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K112" s="27" t="s">
         <v>2</v>
@@ -20614,7 +20691,7 @@
       <c r="H113" s="27"/>
       <c r="I113" s="27"/>
       <c r="J113" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K113" s="27" t="s">
         <v>2</v>
@@ -20754,7 +20831,7 @@
       <c r="H114" s="27"/>
       <c r="I114" s="27"/>
       <c r="J114" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K114" s="27" t="s">
         <v>2</v>
@@ -20834,7 +20911,7 @@
       <c r="H115" s="27"/>
       <c r="I115" s="27"/>
       <c r="J115" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K115" s="27" t="s">
         <v>2</v>
@@ -20962,7 +21039,7 @@
       <c r="H116" s="27"/>
       <c r="I116" s="27"/>
       <c r="J116" s="27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K116" s="27" t="s">
         <v>2</v>
@@ -21024,7 +21101,7 @@
       <c r="H117" s="27"/>
       <c r="I117" s="27"/>
       <c r="J117" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K117" s="27" t="s">
         <v>35</v>
@@ -21143,7 +21220,7 @@
       <c r="H118" s="27"/>
       <c r="I118" s="27"/>
       <c r="J118" s="27" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K118" s="27" t="s">
         <v>35</v>
@@ -21238,7 +21315,7 @@
       <c r="H119" s="27"/>
       <c r="I119" s="27"/>
       <c r="J119" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K119" s="27" t="s">
         <v>2</v>
@@ -21345,7 +21422,7 @@
       <c r="H120" s="27"/>
       <c r="I120" s="27"/>
       <c r="J120" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K120" s="27" t="s">
         <v>2</v>
@@ -21602,7 +21679,7 @@
       <c r="H121" s="27"/>
       <c r="I121" s="27"/>
       <c r="J121" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K121" s="27" t="s">
         <v>2</v>
@@ -21745,7 +21822,7 @@
       <c r="H122" s="27"/>
       <c r="I122" s="27"/>
       <c r="J122" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K122" s="27" t="s">
         <v>2</v>
@@ -21805,7 +21882,7 @@
       <c r="H123" s="27"/>
       <c r="I123" s="27"/>
       <c r="J123" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K123" s="27" t="s">
         <v>2</v>
@@ -21942,7 +22019,7 @@
       <c r="H124" s="27"/>
       <c r="I124" s="27"/>
       <c r="J124" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K124" s="27" t="s">
         <v>2</v>
@@ -22058,7 +22135,7 @@
       <c r="H125" s="27"/>
       <c r="I125" s="27"/>
       <c r="J125" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K125" s="27" t="s">
         <v>2</v>
@@ -22105,7 +22182,7 @@
       <c r="H126" s="27"/>
       <c r="I126" s="27"/>
       <c r="J126" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K126" s="27" t="s">
         <v>2</v>
@@ -22221,7 +22298,7 @@
       <c r="H127" s="27"/>
       <c r="I127" s="27"/>
       <c r="J127" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K127" s="27" t="s">
         <v>2</v>
@@ -22301,7 +22378,7 @@
       <c r="H128" s="27"/>
       <c r="I128" s="27"/>
       <c r="J128" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K128" s="27" t="s">
         <v>2</v>
@@ -22474,7 +22551,7 @@
       <c r="H129" s="27"/>
       <c r="I129" s="27"/>
       <c r="J129" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K129" s="27" t="s">
         <v>2</v>
@@ -22623,7 +22700,7 @@
       <c r="H130" s="27"/>
       <c r="I130" s="27"/>
       <c r="J130" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K130" s="27" t="s">
         <v>2</v>
@@ -22874,7 +22951,7 @@
       <c r="H131" s="27"/>
       <c r="I131" s="27"/>
       <c r="J131" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K131" s="27" t="s">
         <v>2</v>
@@ -23062,7 +23139,7 @@
       <c r="H132" s="27"/>
       <c r="I132" s="27"/>
       <c r="J132" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K132" s="27" t="s">
         <v>2</v>
@@ -23118,7 +23195,7 @@
       <c r="H133" s="27"/>
       <c r="I133" s="27"/>
       <c r="J133" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K133" s="27" t="s">
         <v>2</v>
@@ -23192,7 +23269,7 @@
       <c r="H134" s="27"/>
       <c r="I134" s="27"/>
       <c r="J134" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K134" s="27" t="s">
         <v>2</v>
@@ -23299,7 +23376,7 @@
       <c r="H135" s="27"/>
       <c r="I135" s="27"/>
       <c r="J135" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K135" s="27" t="s">
         <v>2</v>
@@ -23400,7 +23477,7 @@
       <c r="H136" s="27"/>
       <c r="I136" s="27"/>
       <c r="J136" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K136" s="27" t="s">
         <v>2</v>
@@ -23597,7 +23674,7 @@
       <c r="H137" s="27"/>
       <c r="I137" s="27"/>
       <c r="J137" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K137" s="27" t="s">
         <v>2</v>
@@ -23779,7 +23856,7 @@
       <c r="H138" s="27"/>
       <c r="I138" s="27"/>
       <c r="J138" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K138" s="27" t="s">
         <v>2</v>
@@ -23961,7 +24038,7 @@
       <c r="H139" s="27"/>
       <c r="I139" s="27"/>
       <c r="J139" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K139" s="27" t="s">
         <v>2</v>
@@ -24143,7 +24220,7 @@
       <c r="H140" s="27"/>
       <c r="I140" s="27"/>
       <c r="J140" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K140" s="27" t="s">
         <v>2</v>
@@ -24280,7 +24357,7 @@
       <c r="H141" s="27"/>
       <c r="I141" s="27"/>
       <c r="J141" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K141" s="27" t="s">
         <v>2</v>
@@ -24378,7 +24455,7 @@
       <c r="H142" s="27"/>
       <c r="I142" s="27"/>
       <c r="J142" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K142" s="27" t="s">
         <v>2</v>
@@ -24413,7 +24490,7 @@
       <c r="H143" s="27"/>
       <c r="I143" s="27"/>
       <c r="J143" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K143" s="27" t="s">
         <v>2</v>
@@ -24487,7 +24564,7 @@
       <c r="H144" s="27"/>
       <c r="I144" s="27"/>
       <c r="J144" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K144" s="27" t="s">
         <v>2</v>
@@ -24558,7 +24635,7 @@
       <c r="H145" s="27"/>
       <c r="I145" s="27"/>
       <c r="J145" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K145" s="27" t="s">
         <v>2</v>
@@ -24671,7 +24748,7 @@
       <c r="H146" s="27"/>
       <c r="I146" s="27"/>
       <c r="J146" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K146" s="27" t="s">
         <v>2</v>
@@ -24787,7 +24864,7 @@
       <c r="H147" s="27"/>
       <c r="I147" s="27"/>
       <c r="J147" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K147" s="27" t="s">
         <v>2</v>
@@ -24870,7 +24947,7 @@
       <c r="H148" s="27"/>
       <c r="I148" s="27"/>
       <c r="J148" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K148" s="27" t="s">
         <v>2</v>
@@ -24947,7 +25024,7 @@
       <c r="H149" s="27"/>
       <c r="I149" s="27"/>
       <c r="J149" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K149" s="27" t="s">
         <v>2</v>
@@ -25027,7 +25104,7 @@
       <c r="H150" s="27"/>
       <c r="I150" s="27"/>
       <c r="J150" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K150" s="27" t="s">
         <v>2</v>
@@ -25215,7 +25292,7 @@
       <c r="H151" s="27"/>
       <c r="I151" s="27"/>
       <c r="J151" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K151" s="27" t="s">
         <v>2</v>
@@ -25349,7 +25426,7 @@
       <c r="H152" s="27"/>
       <c r="I152" s="27"/>
       <c r="J152" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K152" s="27" t="s">
         <v>2</v>
@@ -25462,7 +25539,7 @@
       <c r="H153" s="27"/>
       <c r="I153" s="27"/>
       <c r="J153" s="27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K153" s="27" t="s">
         <v>2</v>
@@ -25578,7 +25655,7 @@
       <c r="H154" s="27"/>
       <c r="I154" s="27"/>
       <c r="J154" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K154" s="27" t="s">
         <v>2</v>
@@ -25625,7 +25702,7 @@
       <c r="H155" s="27"/>
       <c r="I155" s="27"/>
       <c r="J155" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K155" s="27" t="s">
         <v>2</v>
@@ -25813,7 +25890,7 @@
       <c r="H156" s="27"/>
       <c r="I156" s="27"/>
       <c r="J156" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K156" s="27" t="s">
         <v>2</v>
@@ -25935,7 +26012,7 @@
       <c r="H157" s="27"/>
       <c r="I157" s="27"/>
       <c r="J157" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K157" s="27" t="s">
         <v>2</v>
@@ -25964,7 +26041,7 @@
       <c r="H158" s="27"/>
       <c r="I158" s="27"/>
       <c r="J158" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K158" s="27" t="s">
         <v>2</v>
@@ -26011,7 +26088,7 @@
       <c r="H159" s="27"/>
       <c r="I159" s="27"/>
       <c r="J159" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K159" s="27" t="s">
         <v>2</v>
@@ -26073,7 +26150,7 @@
       <c r="H160" s="27"/>
       <c r="I160" s="27"/>
       <c r="J160" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K160" s="27" t="s">
         <v>2</v>
@@ -26141,7 +26218,7 @@
       <c r="H161" s="27"/>
       <c r="I161" s="27"/>
       <c r="J161" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K161" s="27" t="s">
         <v>2</v>
@@ -26218,7 +26295,7 @@
       <c r="H162" s="27"/>
       <c r="I162" s="27"/>
       <c r="J162" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K162" s="27" t="s">
         <v>2</v>
@@ -26286,7 +26363,7 @@
       <c r="H163" s="27"/>
       <c r="I163" s="27"/>
       <c r="J163" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K163" s="27" t="s">
         <v>2</v>
@@ -26433,7 +26510,7 @@
       <c r="H164" s="27"/>
       <c r="I164" s="27"/>
       <c r="J164" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K164" s="27" t="s">
         <v>2</v>
@@ -26486,7 +26563,7 @@
       <c r="H165" s="27"/>
       <c r="I165" s="27"/>
       <c r="J165" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K165" s="27" t="s">
         <v>2</v>
@@ -26536,7 +26613,7 @@
       <c r="H166" s="27"/>
       <c r="I166" s="27"/>
       <c r="J166" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K166" s="27" t="s">
         <v>2</v>
@@ -26655,7 +26732,7 @@
       <c r="H167" s="27"/>
       <c r="I167" s="27"/>
       <c r="J167" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K167" s="27" t="s">
         <v>2</v>
@@ -26762,7 +26839,7 @@
       <c r="H168" s="27"/>
       <c r="I168" s="27"/>
       <c r="J168" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K168" s="27" t="s">
         <v>2</v>
@@ -26857,7 +26934,7 @@
       <c r="H169" s="27"/>
       <c r="I169" s="27"/>
       <c r="J169" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K169" s="27" t="s">
         <v>2</v>
@@ -27003,7 +27080,7 @@
       <c r="H170" s="27"/>
       <c r="I170" s="27"/>
       <c r="J170" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K170" s="27" t="s">
         <v>2</v>
@@ -27068,7 +27145,7 @@
       <c r="H171" s="27"/>
       <c r="I171" s="27"/>
       <c r="J171" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K171" s="27" t="s">
         <v>2</v>
@@ -27167,7 +27244,7 @@
       <c r="H172" s="27"/>
       <c r="I172" s="27"/>
       <c r="J172" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K172" s="27" t="s">
         <v>2</v>
@@ -27289,7 +27366,7 @@
       <c r="H173" s="27"/>
       <c r="I173" s="27"/>
       <c r="J173" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K173" s="27" t="s">
         <v>2</v>
@@ -27403,7 +27480,7 @@
       <c r="H174" s="27"/>
       <c r="I174" s="27"/>
       <c r="J174" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K174" s="27" t="s">
         <v>2</v>
@@ -27477,7 +27554,7 @@
       <c r="H175" s="27"/>
       <c r="I175" s="27"/>
       <c r="J175" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K175" s="27" t="s">
         <v>2</v>
@@ -27662,7 +27739,7 @@
       <c r="H176" s="27"/>
       <c r="I176" s="27"/>
       <c r="J176" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K176" s="27" t="s">
         <v>2</v>
@@ -27751,7 +27828,7 @@
       <c r="H177" s="27"/>
       <c r="I177" s="27"/>
       <c r="J177" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K177" s="27" t="s">
         <v>2</v>
@@ -27813,7 +27890,7 @@
       <c r="H178" s="27"/>
       <c r="I178" s="27"/>
       <c r="J178" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K178" s="27" t="s">
         <v>2</v>
@@ -27978,7 +28055,7 @@
       <c r="H179" s="27"/>
       <c r="I179" s="27"/>
       <c r="J179" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K179" s="27" t="s">
         <v>2</v>
@@ -28085,7 +28162,7 @@
       <c r="H180" s="27"/>
       <c r="I180" s="27"/>
       <c r="J180" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K180" s="27" t="s">
         <v>2</v>
@@ -28156,7 +28233,7 @@
       <c r="H181" s="27"/>
       <c r="I181" s="27"/>
       <c r="J181" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K181" s="27" t="s">
         <v>2</v>
@@ -28314,7 +28391,7 @@
       <c r="H182" s="27"/>
       <c r="I182" s="27"/>
       <c r="J182" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K182" s="27" t="s">
         <v>2</v>
@@ -28379,7 +28456,7 @@
       <c r="H183" s="27"/>
       <c r="I183" s="27"/>
       <c r="J183" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K183" s="27" t="s">
         <v>2</v>
@@ -28477,7 +28554,7 @@
       <c r="H184" s="27"/>
       <c r="I184" s="27"/>
       <c r="J184" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K184" s="27" t="s">
         <v>2</v>
@@ -28584,7 +28661,7 @@
       <c r="H185" s="27"/>
       <c r="I185" s="27"/>
       <c r="J185" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K185" s="27" t="s">
         <v>2</v>
@@ -28655,7 +28732,7 @@
       <c r="H186" s="27"/>
       <c r="I186" s="27"/>
       <c r="J186" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K186" s="27" t="s">
         <v>2</v>
@@ -28777,7 +28854,7 @@
       <c r="H187" s="27"/>
       <c r="I187" s="27"/>
       <c r="J187" s="27" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K187" s="27" t="s">
         <v>2</v>
@@ -28866,7 +28943,7 @@
     </row>
     <row r="188" spans="1:162">
       <c r="A188" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>68</v>
@@ -28887,7 +28964,7 @@
       <c r="H188" s="27"/>
       <c r="I188" s="27"/>
       <c r="J188" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K188" s="27" t="s">
         <v>2</v>
@@ -29030,7 +29107,7 @@
       <c r="H189" s="27"/>
       <c r="I189" s="27"/>
       <c r="J189" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K189" s="27" t="s">
         <v>35</v>
@@ -29125,7 +29202,7 @@
       <c r="H190" s="27"/>
       <c r="I190" s="27"/>
       <c r="J190" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K190" s="27" t="s">
         <v>2</v>
@@ -29214,7 +29291,7 @@
       <c r="H191" s="27"/>
       <c r="I191" s="27"/>
       <c r="J191" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K191" s="27" t="s">
         <v>2</v>
@@ -29330,7 +29407,7 @@
       <c r="H192" s="27"/>
       <c r="I192" s="27"/>
       <c r="J192" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K192" s="27" t="s">
         <v>2</v>
@@ -29470,7 +29547,7 @@
       <c r="H193" s="27"/>
       <c r="I193" s="27"/>
       <c r="J193" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K193" s="27" t="s">
         <v>2</v>
@@ -29572,7 +29649,7 @@
       <c r="H194" s="27"/>
       <c r="I194" s="27"/>
       <c r="J194" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K194" s="27" t="s">
         <v>2</v>
@@ -29721,7 +29798,7 @@
       <c r="H195" s="27"/>
       <c r="I195" s="27"/>
       <c r="J195" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K195" s="27" t="s">
         <v>2</v>
@@ -29801,7 +29878,7 @@
       <c r="H196" s="27"/>
       <c r="I196" s="27"/>
       <c r="J196" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K196" s="27" t="s">
         <v>2</v>
@@ -29860,7 +29937,7 @@
       <c r="H197" s="27"/>
       <c r="I197" s="27"/>
       <c r="J197" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K197" s="27" t="s">
         <v>2</v>
@@ -29898,7 +29975,7 @@
       <c r="H198" s="27"/>
       <c r="I198" s="27"/>
       <c r="J198" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K198" s="27" t="s">
         <v>2</v>
@@ -29930,7 +30007,7 @@
       <c r="H199" s="27"/>
       <c r="I199" s="27"/>
       <c r="J199" s="27" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="K199" s="27" t="s">
         <v>35</v>
@@ -29971,7 +30048,7 @@
       <c r="H200" s="27"/>
       <c r="I200" s="27"/>
       <c r="J200" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K200" s="27" t="s">
         <v>2</v>
@@ -30117,7 +30194,7 @@
       <c r="H201" s="27"/>
       <c r="I201" s="27"/>
       <c r="J201" s="27" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="K201" s="27" t="s">
         <v>35</v>
@@ -30215,7 +30292,7 @@
       <c r="H202" s="27"/>
       <c r="I202" s="27"/>
       <c r="J202" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K202" s="27" t="s">
         <v>35</v>
@@ -30310,7 +30387,7 @@
       <c r="H203" s="27"/>
       <c r="I203" s="27"/>
       <c r="J203" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K203" s="27" t="s">
         <v>35</v>
@@ -30381,7 +30458,7 @@
       <c r="H204" s="27"/>
       <c r="I204" s="27"/>
       <c r="J204" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K204" s="27" t="s">
         <v>2</v>
@@ -30448,7 +30525,7 @@
       <c r="H205" s="27"/>
       <c r="I205" s="27"/>
       <c r="J205" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K205" s="27" t="s">
         <v>2</v>
@@ -30603,7 +30680,7 @@
       <c r="H206" s="27"/>
       <c r="I206" s="27"/>
       <c r="J206" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K206" s="27" t="s">
         <v>2</v>
@@ -30680,7 +30757,7 @@
       <c r="H207" s="27"/>
       <c r="I207" s="27"/>
       <c r="J207" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K207" s="27" t="s">
         <v>2</v>
@@ -30834,7 +30911,7 @@
       <c r="H208" s="27"/>
       <c r="I208" s="27"/>
       <c r="J208" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K208" s="27" t="s">
         <v>2</v>
@@ -31043,7 +31120,7 @@
       <c r="H209" s="27"/>
       <c r="I209" s="27"/>
       <c r="J209" s="27" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K209" s="27" t="s">
         <v>2</v>
@@ -31113,7 +31190,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="F1" s="10" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -31121,21 +31198,21 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -31144,10 +31221,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -31156,12 +31233,12 @@
         <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B5" s="12">
         <v>6</v>
@@ -31173,7 +31250,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="G5" s="12">
         <v>6</v>
@@ -31187,7 +31264,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12">
@@ -31197,7 +31274,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G6" s="12">
         <v>23</v>
@@ -31211,7 +31288,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12">
@@ -31221,7 +31298,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G7" s="12">
         <v>41</v>
@@ -31235,7 +31312,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B8" s="12">
         <v>23</v>
@@ -31247,7 +31324,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="G8" s="12">
         <v>25</v>
@@ -31261,7 +31338,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12">
@@ -31271,7 +31348,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G9" s="12">
         <v>3</v>
@@ -31285,7 +31362,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12">
@@ -31295,7 +31372,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12">
@@ -31307,7 +31384,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B11" s="12">
         <v>41</v>
@@ -31319,7 +31396,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G11" s="12">
         <v>98</v>
@@ -31333,7 +31410,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B12" s="12">
         <v>1</v>
@@ -31345,7 +31422,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12">
@@ -31357,7 +31434,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12">
@@ -31369,7 +31446,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B15" s="12">
         <v>1</v>
@@ -31381,7 +31458,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
@@ -31395,7 +31472,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12">
@@ -31407,7 +31484,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B18" s="12">
         <v>25</v>
@@ -31421,7 +31498,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12">
@@ -31433,7 +31510,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12">
@@ -31445,7 +31522,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B21" s="12">
         <v>3</v>
@@ -31459,7 +31536,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12">
@@ -31471,7 +31548,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B23" s="12">
         <v>102</v>

</xml_diff>

<commit_message>
full text of 28
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="677">
   <si>
     <t>f</t>
   </si>
@@ -2052,6 +2052,9 @@
   </si>
   <si>
     <t>HORRIBLE REVENGE, OR, THE MONSTER OF ITALY!! With HORRIBLE REVENGE is bound HOPELESS LOVE. AN INTERESTING TALE</t>
+  </si>
+  <si>
+    <t>http://find.galegroup.com.ezproxy.library.uvic.ca/ecco/retrieve.do?inPS=true&amp;prodId=ECCO&amp;userGroupName=uvictoria&amp;tabID=T001&amp;bookId=0036800600&amp;resultListType=RESULT_LIST&amp;contentSet=ECCOArticles&amp;showLOI=&amp;docId=CW3309159972&amp;docLevel=FASCIMILE&amp;workId=CW109159972&amp;relevancePageBatch=CW109159972&amp;retrieveFormat=MULTIPAGE_DOCUMENT&amp;callistoContentSet=ECLL&amp;docPage=article&amp;hilite=y</t>
   </si>
 </sst>
 </file>
@@ -2223,8 +2226,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2380,7 +2385,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2429,6 +2434,7 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2477,6 +2483,7 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6575,10 +6582,10 @@
   <dimension ref="A1:FF209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9974,8 +9981,12 @@
         <v>2</v>
       </c>
       <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
+      <c r="M29" s="27" t="s">
+        <v>676</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>666</v>
+      </c>
       <c r="S29" s="19">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
google books to 28
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="683">
   <si>
     <t>f</t>
   </si>
@@ -1829,9 +1829,6 @@
     <t>horrid</t>
   </si>
   <si>
-    <t>great</t>
-  </si>
-  <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGOJRZI394238419</t>
   </si>
   <si>
@@ -2055,6 +2052,27 @@
   </si>
   <si>
     <t>http://find.galegroup.com.ezproxy.library.uvic.ca/ecco/retrieve.do?inPS=true&amp;prodId=ECCO&amp;userGroupName=uvictoria&amp;tabID=T001&amp;bookId=0036800600&amp;resultListType=RESULT_LIST&amp;contentSet=ECCOArticles&amp;showLOI=&amp;docId=CW3309159972&amp;docLevel=FASCIMILE&amp;workId=CW109159972&amp;relevancePageBatch=CW109159972&amp;retrieveFormat=MULTIPAGE_DOCUMENT&amp;callistoContentSet=ECLL&amp;docPage=article&amp;hilite=y</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>too many; not needed</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=vZglAAAAMAAJ and books.google.com/books?id=gLwNAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.ca/books?id=xKgBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=a6cBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=-VQHAAAAQAAJ</t>
   </si>
 </sst>
 </file>
@@ -2226,8 +2244,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2385,7 +2479,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2435,6 +2529,44 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2484,6 +2616,44 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6582,10 +6752,10 @@
   <dimension ref="A1:FF209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6601,8 +6771,7 @@
     <col min="9" max="9" width="6.5" style="23" customWidth="1"/>
     <col min="10" max="10" width="8.5" style="23" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" style="23" customWidth="1"/>
-    <col min="12" max="12" width="8" style="23" customWidth="1"/>
-    <col min="13" max="14" width="8.33203125" style="23" customWidth="1"/>
+    <col min="12" max="14" width="8.33203125" style="23" customWidth="1"/>
     <col min="15" max="15" width="6.5" style="19" customWidth="1"/>
     <col min="16" max="16" width="3.83203125" style="3" customWidth="1"/>
     <col min="17" max="17" width="4.83203125" style="3" customWidth="1"/>
@@ -6753,7 +6922,7 @@
   <sheetData>
     <row r="1" spans="1:162" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>526</v>
@@ -6786,13 +6955,13 @@
         <v>551</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>521</v>
@@ -7269,7 +7438,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M2" s="27" t="s">
         <v>596</v>
@@ -7484,7 +7653,9 @@
       <c r="K3" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="L3" s="27"/>
+      <c r="L3" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M3" s="27" t="s">
         <v>598</v>
       </c>
@@ -7527,12 +7698,14 @@
       <c r="K4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="27"/>
+      <c r="L4" s="27" t="s">
+        <v>678</v>
+      </c>
       <c r="M4" s="27" t="s">
         <v>599</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>601</v>
+        <v>676</v>
       </c>
       <c r="AG4" s="21">
         <v>1</v>
@@ -7623,10 +7796,12 @@
       <c r="K5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="27"/>
+      <c r="L5" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M5" s="27"/>
       <c r="N5" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="Y5" s="19">
         <v>1</v>
@@ -7720,9 +7895,11 @@
       <c r="K6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="27"/>
+      <c r="L6" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M6" s="27" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N6" s="27" t="s">
         <v>600</v>
@@ -7856,9 +8033,11 @@
       <c r="K7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="27"/>
+      <c r="L7" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M7" s="27" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N7" s="27" t="s">
         <v>600</v>
@@ -7982,12 +8161,14 @@
       <c r="K8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="27"/>
+      <c r="L8" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M8" s="27" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N8" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="BD8" s="3">
         <v>1</v>
@@ -8082,12 +8263,14 @@
       <c r="K9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="27"/>
+      <c r="L9" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M9" s="27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="BQ9" s="21">
         <v>1</v>
@@ -8148,9 +8331,11 @@
       <c r="K10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="27"/>
+      <c r="L10" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M10" s="27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="N10" s="27" t="s">
         <v>600</v>
@@ -8332,7 +8517,9 @@
       <c r="K11" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="27"/>
+      <c r="L11" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M11" s="27" t="s">
         <v>597</v>
       </c>
@@ -8447,9 +8634,11 @@
       <c r="K12" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L12" s="27"/>
+      <c r="L12" s="27" t="s">
+        <v>680</v>
+      </c>
       <c r="M12" s="27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="N12" s="27" t="s">
         <v>600</v>
@@ -8556,9 +8745,11 @@
       <c r="K13" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="27"/>
+      <c r="L13" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M13" s="27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="N13" s="27" t="s">
         <v>600</v>
@@ -8643,9 +8834,11 @@
       <c r="K14" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="27"/>
+      <c r="L14" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M14" s="27" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N14" s="27" t="s">
         <v>600</v>
@@ -8715,9 +8908,11 @@
       <c r="K15" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="27"/>
+      <c r="L15" s="27" t="s">
+        <v>679</v>
+      </c>
       <c r="M15" s="27" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="N15" s="27" t="s">
         <v>125</v>
@@ -8766,9 +8961,11 @@
       <c r="K16" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="27"/>
+      <c r="L16" s="27" t="s">
+        <v>681</v>
+      </c>
       <c r="M16" s="27" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="N16" s="27" t="s">
         <v>600</v>
@@ -8832,12 +9029,14 @@
       <c r="K17" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="27"/>
+      <c r="L17" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M17" s="27" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AE17" s="21">
         <v>1</v>
@@ -8958,12 +9157,14 @@
       <c r="K18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="27"/>
+      <c r="L18" s="27" t="s">
+        <v>682</v>
+      </c>
       <c r="M18" s="27" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="S18" s="19">
         <v>1</v>
@@ -9016,12 +9217,14 @@
       <c r="K19" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="27"/>
+      <c r="L19" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M19" s="27" t="s">
+        <v>664</v>
+      </c>
+      <c r="N19" s="27" t="s">
         <v>665</v>
-      </c>
-      <c r="N19" s="27" t="s">
-        <v>666</v>
       </c>
       <c r="W19" s="21">
         <v>1</v>
@@ -9095,10 +9298,10 @@
         <v>2</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M20" s="27" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N20" s="27" t="s">
         <v>600</v>
@@ -9186,10 +9389,12 @@
       <c r="K21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="27"/>
+      <c r="L21" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M21" s="27"/>
       <c r="N21" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="S21" s="19">
         <v>1</v>
@@ -9296,7 +9501,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E22" s="4">
         <v>1808</v>
@@ -9317,10 +9522,12 @@
       <c r="K22" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="27"/>
+      <c r="L22" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M22" s="27"/>
       <c r="N22" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="BR22" s="21">
         <v>1</v>
@@ -9370,7 +9577,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E23" s="4">
         <v>1811</v>
@@ -9391,10 +9598,12 @@
       <c r="K23" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L23" s="27"/>
+      <c r="L23" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M23" s="27"/>
       <c r="N23" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="S23" s="19">
         <v>1</v>
@@ -9458,10 +9667,12 @@
       <c r="K24" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L24" s="27"/>
+      <c r="L24" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M24" s="27"/>
       <c r="N24" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AL24" s="3">
         <v>1</v>
@@ -9531,10 +9742,12 @@
       <c r="K25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L25" s="27"/>
+      <c r="L25" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M25" s="27"/>
       <c r="N25" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O25" s="19">
         <v>1</v>
@@ -9752,10 +9965,12 @@
       <c r="K26" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L26" s="27"/>
+      <c r="L26" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M26" s="27"/>
       <c r="N26" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="S26" s="19">
         <v>1</v>
@@ -9832,10 +10047,12 @@
       <c r="K27" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L27" s="27"/>
+      <c r="L27" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M27" s="27"/>
       <c r="N27" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="S27" s="19">
         <v>1</v>
@@ -9921,10 +10138,12 @@
       <c r="K28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L28" s="27"/>
+      <c r="L28" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M28" s="27"/>
       <c r="N28" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="S28" s="19">
         <v>1</v>
@@ -9980,12 +10199,14 @@
       <c r="K29" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="27"/>
+      <c r="L29" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M29" s="27" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="N29" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="S29" s="19">
         <v>1</v>
@@ -15003,7 +15224,7 @@
         <v>570</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J68" s="27" t="s">
         <v>531</v>
@@ -15080,7 +15301,7 @@
         <v>327</v>
       </c>
       <c r="I69" s="27" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J69" s="27" t="s">
         <v>543</v>
@@ -15178,13 +15399,13 @@
         <v>69</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H70" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J70" s="27" t="s">
         <v>531</v>
@@ -15318,7 +15539,7 @@
         <v>327</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J71" s="27" t="s">
         <v>533</v>
@@ -15509,7 +15730,7 @@
         <v>327</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J72" s="27" t="s">
         <v>533</v>
@@ -15682,10 +15903,10 @@
         <v>348</v>
       </c>
       <c r="H73" s="27" t="s">
+        <v>618</v>
+      </c>
+      <c r="I73" s="27" t="s">
         <v>619</v>
-      </c>
-      <c r="I73" s="27" t="s">
-        <v>620</v>
       </c>
       <c r="J73" s="27" t="s">
         <v>532</v>
@@ -15824,7 +16045,7 @@
         <v>327</v>
       </c>
       <c r="I75" s="27" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J75" s="27" t="s">
         <v>534</v>
@@ -15994,13 +16215,13 @@
         <v>75</v>
       </c>
       <c r="G76" s="27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H76" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="I76" s="27" t="s">
         <v>622</v>
-      </c>
-      <c r="I76" s="27" t="s">
-        <v>623</v>
       </c>
       <c r="J76" s="27" t="s">
         <v>534</v>
@@ -16501,7 +16722,7 @@
         <v>570</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J79" s="27" t="s">
         <v>534</v>
@@ -16842,7 +17063,7 @@
         <v>327</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J82" s="27" t="s">
         <v>531</v>
@@ -16925,13 +17146,13 @@
         <v>82</v>
       </c>
       <c r="G83" s="27" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H83" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J83" s="27" t="s">
         <v>531</v>
@@ -17050,7 +17271,7 @@
         <v>83</v>
       </c>
       <c r="G84" s="27" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H84" s="27" t="s">
         <v>327</v>
@@ -17243,7 +17464,7 @@
         <v>361</v>
       </c>
       <c r="I85" s="27" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J85" s="27" t="s">
         <v>533</v>
@@ -17470,7 +17691,7 @@
         <v>327</v>
       </c>
       <c r="I87" s="27" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J87" s="27" t="s">
         <v>531</v>
@@ -17646,7 +17867,7 @@
         <v>327</v>
       </c>
       <c r="I88" s="27" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J88" s="27" t="s">
         <v>531</v>
@@ -17786,10 +18007,10 @@
         <v>348</v>
       </c>
       <c r="H89" s="27" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I89" s="27" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J89" s="27" t="s">
         <v>534</v>
@@ -18001,10 +18222,10 @@
         <v>348</v>
       </c>
       <c r="H91" s="27" t="s">
+        <v>633</v>
+      </c>
+      <c r="I91" s="27" t="s">
         <v>634</v>
-      </c>
-      <c r="I91" s="27" t="s">
-        <v>635</v>
       </c>
       <c r="J91" s="27" t="s">
         <v>531</v>
@@ -18150,7 +18371,7 @@
         <v>91</v>
       </c>
       <c r="G92" s="27" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="H92" s="27" t="s">
         <v>327</v>
@@ -18246,10 +18467,10 @@
         <v>348</v>
       </c>
       <c r="H93" s="27" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I93" s="27" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J93" s="27" t="s">
         <v>531</v>
@@ -18553,10 +18774,10 @@
         <v>348</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I96" s="29" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J96" s="27" t="s">
         <v>533</v>
@@ -18720,7 +18941,7 @@
         <v>327</v>
       </c>
       <c r="I97" s="27" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J97" s="27" t="s">
         <v>532</v>
@@ -18782,7 +19003,7 @@
         <v>327</v>
       </c>
       <c r="I98" s="27" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J98" s="27" t="s">
         <v>534</v>
@@ -18970,13 +19191,13 @@
         <v>98</v>
       </c>
       <c r="G99" s="27" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H99" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I99" s="29" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J99" s="27" t="s">
         <v>544</v>
@@ -19062,7 +19283,7 @@
         <v>327</v>
       </c>
       <c r="I100" s="27" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J100" s="27" t="s">
         <v>531</v>
@@ -19319,7 +19540,7 @@
         <v>327</v>
       </c>
       <c r="I101" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J101" s="27" t="s">
         <v>534</v>
@@ -19453,10 +19674,10 @@
     </row>
     <row r="102" spans="1:162">
       <c r="A102" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>647</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>648</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>9</v>
@@ -19477,7 +19698,7 @@
         <v>327</v>
       </c>
       <c r="I102" s="27" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J102" s="27" t="s">
         <v>545</v>
@@ -19653,13 +19874,13 @@
         <v>103</v>
       </c>
       <c r="G104" s="27" t="s">
+        <v>649</v>
+      </c>
+      <c r="H104" s="27" t="s">
+        <v>618</v>
+      </c>
+      <c r="I104" s="27" t="s">
         <v>650</v>
-      </c>
-      <c r="H104" s="27" t="s">
-        <v>619</v>
-      </c>
-      <c r="I104" s="27" t="s">
-        <v>651</v>
       </c>
       <c r="J104" s="27" t="s">
         <v>531</v>
@@ -19709,7 +19930,7 @@
         <v>361</v>
       </c>
       <c r="I105" s="27" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J105" s="27" t="s">
         <v>534</v>
@@ -19804,13 +20025,13 @@
         <v>105</v>
       </c>
       <c r="G106" s="27" t="s">
+        <v>651</v>
+      </c>
+      <c r="H106" s="27" t="s">
+        <v>653</v>
+      </c>
+      <c r="I106" s="29" t="s">
         <v>652</v>
-      </c>
-      <c r="H106" s="27" t="s">
-        <v>654</v>
-      </c>
-      <c r="I106" s="29" t="s">
-        <v>653</v>
       </c>
       <c r="J106" s="27" t="s">
         <v>533</v>
@@ -19875,7 +20096,7 @@
         <v>106</v>
       </c>
       <c r="G107" s="27" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H107" s="27" t="s">
         <v>327</v>
@@ -19977,7 +20198,7 @@
         <v>327</v>
       </c>
       <c r="I108" s="27" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J108" s="27" t="s">
         <v>534</v>
@@ -20316,13 +20537,13 @@
         <v>109</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H110" s="27" t="s">
+        <v>657</v>
+      </c>
+      <c r="I110" s="27" t="s">
         <v>658</v>
-      </c>
-      <c r="I110" s="27" t="s">
-        <v>659</v>
       </c>
       <c r="J110" s="27" t="s">
         <v>534</v>
@@ -20516,7 +20737,7 @@
         <v>110</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H111" s="27" t="s">
         <v>327</v>
@@ -20580,13 +20801,13 @@
         <v>111</v>
       </c>
       <c r="G112" s="27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H112" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I112" s="27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J112" s="27" t="s">
         <v>531</v>

</xml_diff>

<commit_message>
sought in vain for full texts 31 to 33
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1580" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="1480" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="687">
   <si>
     <t>f</t>
   </si>
@@ -2073,6 +2073,18 @@
   </si>
   <si>
     <t>books.google.com/books?id=-VQHAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDYDQDI691770196</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CMKPRWY596071328</t>
+  </si>
+  <si>
+    <t>http://books.google.ca/books?id=5LQBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWBJGAJ868344290</t>
   </si>
 </sst>
 </file>
@@ -2244,8 +2256,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2479,7 +2529,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2567,6 +2617,25 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2654,6 +2723,25 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6183,7 +6271,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6309,112 +6503,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -6752,10 +6840,10 @@
   <dimension ref="A1:FF209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10376,9 +10464,15 @@
       <c r="K30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
+      <c r="L30" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>683</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="O30" s="19">
         <v>2</v>
       </c>
@@ -10649,9 +10743,15 @@
       <c r="K31" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
+      <c r="L31" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>684</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="S31" s="19">
         <v>2</v>
       </c>
@@ -10787,9 +10887,13 @@
       <c r="K32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="27"/>
+      <c r="L32" s="27" t="s">
+        <v>685</v>
+      </c>
       <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
+      <c r="N32" s="27" t="s">
+        <v>672</v>
+      </c>
       <c r="S32" s="19">
         <v>1</v>
       </c>
@@ -10984,9 +11088,13 @@
       <c r="K33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L33" s="27"/>
+      <c r="L33" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
+      <c r="N33" s="27" t="s">
+        <v>672</v>
+      </c>
       <c r="W33" s="21">
         <v>1</v>
       </c>
@@ -11065,9 +11173,13 @@
       <c r="K34" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L34" s="27"/>
+      <c r="L34" s="27" t="s">
+        <v>677</v>
+      </c>
       <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
+      <c r="N34" s="27" t="s">
+        <v>672</v>
+      </c>
       <c r="O34" s="19">
         <v>1</v>
       </c>
@@ -11293,9 +11405,15 @@
       <c r="K35" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
+      <c r="L35" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="M35" s="27" t="s">
+        <v>686</v>
+      </c>
+      <c r="N35" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="S35" s="19">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
full texts of 35 and 36
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="1480" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="2160" yWindow="1580" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="691">
   <si>
     <t>f</t>
   </si>
@@ -2085,6 +2085,18 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWBJGAJ868344290</t>
+  </si>
+  <si>
+    <t>could scan my own physical copy</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CBCOLNN022408250</t>
+  </si>
+  <si>
+    <t>http://books.google.ca/books?id=Sr1LAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=KE+LIBERTINE+charlotte+dacre&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=NCCO-2%2CNCCO-1%2CNCCO-3%2CNCCO-10%2CNCCO-5%2CNCCO-4%2CNCCO-11%2CNCCO-6%2CNCCO-12%2CNCCO-7%2CNCCO-9%2CNCCO-8&amp;display-query=KE+THE+LIBERTINE+charlotte+dacre&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=&amp;limiter=&amp;u=uvictoria&amp;currPage=1&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=BasicSearch&amp;scanId=&amp;documentId=GALE%7CVCTZDI504410513</t>
   </si>
 </sst>
 </file>
@@ -2256,8 +2268,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2529,7 +2547,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2636,6 +2654,9 @@
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2742,6 +2763,9 @@
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6840,10 +6864,10 @@
   <dimension ref="A1:FF209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11504,9 +11528,15 @@
       <c r="K36" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
+      <c r="L36" s="27" t="s">
+        <v>687</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>688</v>
+      </c>
+      <c r="N36" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="W36" s="21">
         <v>1</v>
       </c>
@@ -11628,9 +11658,15 @@
       <c r="K37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
+      <c r="L37" s="27" t="s">
+        <v>689</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>690</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AP37" s="3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
full texts to 38
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1580" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="2000" yWindow="1580" windowWidth="24880" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="695">
   <si>
     <t>f</t>
   </si>
@@ -2097,6 +2097,18 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=KE+LIBERTINE+charlotte+dacre&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=NCCO-2%2CNCCO-1%2CNCCO-3%2CNCCO-10%2CNCCO-5%2CNCCO-4%2CNCCO-11%2CNCCO-6%2CNCCO-12%2CNCCO-7%2CNCCO-9%2CNCCO-8&amp;display-query=KE+THE+LIBERTINE+charlotte+dacre&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=&amp;limiter=&amp;u=uvictoria&amp;currPage=1&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=BasicSearch&amp;scanId=&amp;documentId=GALE%7CVCTZDI504410513</t>
+  </si>
+  <si>
+    <t>http://voyager.library.uvic.ca/vwebv/holdingsInfo?bibId=239345</t>
+  </si>
+  <si>
+    <t>PRINT ONLY (?!)</t>
+  </si>
+  <si>
+    <t>http://books.google.ca/books?id=faZBAQAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://literature.proquest.com.ezproxy.library.uvic.ca/searchFulltext.do?id=Z000031929&amp;divLevel=0&amp;area=Prose&amp;DurUrl=Yes&amp;forward=textsFT&amp;queryType=findWork</t>
   </si>
 </sst>
 </file>
@@ -2268,8 +2280,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="219">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2547,7 +2563,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="219">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2657,6 +2673,8 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2766,6 +2784,8 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6864,10 +6884,10 @@
   <dimension ref="A1:FF209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
+      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11792,9 +11812,15 @@
       <c r="K38" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
+      <c r="L38" s="27" t="s">
+        <v>677</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>691</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>692</v>
+      </c>
       <c r="AY38" s="3">
         <v>1</v>
       </c>
@@ -11879,9 +11905,15 @@
       <c r="K39" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
+      <c r="L39" s="27" t="s">
+        <v>693</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>694</v>
+      </c>
+      <c r="N39" s="27" t="s">
+        <v>676</v>
+      </c>
       <c r="W39" s="21">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
☂ add full text 80 thru 100
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8560" yWindow="0" windowWidth="24880" windowHeight="13020" tabRatio="500"/>
+    <workbookView xWindow="9400" yWindow="0" windowWidth="24880" windowHeight="13020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2912" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="844">
   <si>
     <t>f</t>
   </si>
@@ -2449,12 +2449,150 @@
   <si>
     <t>http://search.proquest.com.ezproxy.library.uvic.ca/docview/4666843?pq-origsite=summon</t>
   </si>
+  <si>
+    <t>none ;A;</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=z8sjAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t9571xn09;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101066591759;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=a_pLAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDXDAES958231608</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Cv0yAQAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CACKWDM496797608</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t8sb4332n;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>none ;~;</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGOVJNN133700940</t>
+  </si>
+  <si>
+    <t>none ;n;</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=9H4jT25HBhUC</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJROTDD314259271</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.32044010442572;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CRCUJJF450012249</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=tTY4AQAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Yx8GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CYGLSXB264288900</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=gR4GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CRROBDA995697122</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=wakBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=LQQ1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=MJ5WAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CAMCNSC439866904</t>
+  </si>
+  <si>
+    <t>none ;_;</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDXSDQD695706418</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=tAY1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://www.jstor.org.ezproxy.library.uvic.ca/stable/40099721</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=vKASAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CRFUYIT033653098</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=AqwBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWSLQTX314633710</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101032329086;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://search.proquest.com.ezproxy.library.uvic.ca/docview/4682971?pq-origsite=summon</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=lVoCAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc1.b4105463;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=RvEOAAAAIAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Ht4NAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074874755;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hn4el8;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hn4ekf;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=BFEhAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CFBCTLJ316755750</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074877691;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074874276;view=1up;seq=11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2505,6 +2643,12 @@
       <color rgb="FF006621"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7242,10 +7386,10 @@
   <dimension ref="A1:FL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q83" sqref="Q83"/>
+      <selection pane="bottomRight" activeCell="T101" sqref="T101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18412,7 +18556,9 @@
       <c r="K82" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L82" s="27"/>
+      <c r="L82" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M82" s="27"/>
       <c r="N82" s="27"/>
       <c r="O82" s="27"/>
@@ -18420,7 +18566,9 @@
       <c r="Q82" s="27"/>
       <c r="R82" s="27"/>
       <c r="S82" s="27"/>
-      <c r="T82" s="27"/>
+      <c r="T82" s="27" t="s">
+        <v>798</v>
+      </c>
       <c r="AM82" s="21">
         <v>1</v>
       </c>
@@ -18476,7 +18624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:168">
+    <row r="83" spans="1:168" ht="16">
       <c r="B83" s="3" t="s">
         <v>240</v>
       </c>
@@ -18507,15 +18655,23 @@
       <c r="K83" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L83" s="27"/>
+      <c r="L83" s="30" t="s">
+        <v>799</v>
+      </c>
       <c r="M83" s="27"/>
       <c r="N83" s="27"/>
-      <c r="O83" s="27"/>
-      <c r="P83" s="27"/>
+      <c r="O83" s="27" t="s">
+        <v>800</v>
+      </c>
+      <c r="P83" s="27" t="s">
+        <v>801</v>
+      </c>
       <c r="Q83" s="27"/>
       <c r="R83" s="27"/>
       <c r="S83" s="27"/>
-      <c r="T83" s="27"/>
+      <c r="T83" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y83" s="19">
         <v>2</v>
       </c>
@@ -18607,7 +18763,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:168">
+    <row r="84" spans="1:168" ht="16">
       <c r="B84" s="3" t="s">
         <v>240</v>
       </c>
@@ -18636,15 +18792,21 @@
       <c r="K84" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L84" s="27"/>
+      <c r="L84" s="30" t="s">
+        <v>802</v>
+      </c>
       <c r="M84" s="27"/>
       <c r="N84" s="27"/>
-      <c r="O84" s="27"/>
+      <c r="O84" s="27" t="s">
+        <v>803</v>
+      </c>
       <c r="P84" s="27"/>
       <c r="Q84" s="27"/>
       <c r="R84" s="27"/>
       <c r="S84" s="27"/>
-      <c r="T84" s="27"/>
+      <c r="T84" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y84" s="19">
         <v>1</v>
       </c>
@@ -18800,7 +18962,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:168">
+    <row r="85" spans="1:168" ht="16">
       <c r="B85" s="3" t="s">
         <v>240</v>
       </c>
@@ -18831,15 +18993,23 @@
       <c r="K85" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L85" s="27"/>
+      <c r="L85" s="30" t="s">
+        <v>804</v>
+      </c>
       <c r="M85" s="27"/>
       <c r="N85" s="27"/>
-      <c r="O85" s="27"/>
-      <c r="P85" s="27"/>
+      <c r="O85" s="27" t="s">
+        <v>805</v>
+      </c>
+      <c r="P85" s="27" t="s">
+        <v>806</v>
+      </c>
       <c r="Q85" s="27"/>
       <c r="R85" s="27"/>
       <c r="S85" s="27"/>
-      <c r="T85" s="27"/>
+      <c r="T85" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AR85" s="3">
         <v>1</v>
       </c>
@@ -18906,7 +19076,9 @@
       <c r="K86" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L86" s="27"/>
+      <c r="L86" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M86" s="27"/>
       <c r="N86" s="27"/>
       <c r="O86" s="27"/>
@@ -18914,7 +19086,9 @@
       <c r="Q86" s="27"/>
       <c r="R86" s="27"/>
       <c r="S86" s="27"/>
-      <c r="T86" s="27"/>
+      <c r="T86" s="27" t="s">
+        <v>807</v>
+      </c>
       <c r="Y86" s="19">
         <v>1</v>
       </c>
@@ -19070,15 +19244,21 @@
       <c r="K87" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L87" s="27"/>
+      <c r="L87" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M87" s="27"/>
       <c r="N87" s="27"/>
-      <c r="O87" s="27"/>
+      <c r="O87" s="27" t="s">
+        <v>808</v>
+      </c>
       <c r="P87" s="27"/>
       <c r="Q87" s="27"/>
       <c r="R87" s="27"/>
       <c r="S87" s="27"/>
-      <c r="T87" s="27"/>
+      <c r="T87" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y87" s="19">
         <v>2</v>
       </c>
@@ -19252,7 +19432,9 @@
       <c r="K88" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L88" s="27"/>
+      <c r="L88" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M88" s="27"/>
       <c r="N88" s="27"/>
       <c r="O88" s="27"/>
@@ -19260,7 +19442,9 @@
       <c r="Q88" s="27"/>
       <c r="R88" s="27"/>
       <c r="S88" s="27"/>
-      <c r="T88" s="27"/>
+      <c r="T88" s="27" t="s">
+        <v>809</v>
+      </c>
       <c r="Y88" s="19">
         <v>1</v>
       </c>
@@ -19370,7 +19554,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:168">
+    <row r="89" spans="1:168" ht="16">
       <c r="B89" s="3" t="s">
         <v>233</v>
       </c>
@@ -19401,15 +19585,23 @@
       <c r="K89" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L89" s="27"/>
+      <c r="L89" s="30" t="s">
+        <v>810</v>
+      </c>
       <c r="M89" s="27"/>
       <c r="N89" s="27"/>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
+      <c r="O89" s="27" t="s">
+        <v>811</v>
+      </c>
+      <c r="P89" s="27" t="s">
+        <v>812</v>
+      </c>
       <c r="Q89" s="27"/>
       <c r="R89" s="27"/>
       <c r="S89" s="27"/>
-      <c r="T89" s="27"/>
+      <c r="T89" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y89" s="19">
         <v>1</v>
       </c>
@@ -19539,15 +19731,21 @@
       <c r="K90" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L90" s="27"/>
+      <c r="L90" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M90" s="27"/>
       <c r="N90" s="27"/>
-      <c r="O90" s="27"/>
+      <c r="O90" s="27" t="s">
+        <v>813</v>
+      </c>
       <c r="P90" s="27"/>
       <c r="Q90" s="27"/>
       <c r="R90" s="27"/>
       <c r="S90" s="27"/>
-      <c r="T90" s="27"/>
+      <c r="T90" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="BA90" s="3">
         <v>1</v>
       </c>
@@ -19597,7 +19795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:168">
+    <row r="91" spans="1:168" ht="16">
       <c r="B91" s="3" t="s">
         <v>233</v>
       </c>
@@ -19628,15 +19826,23 @@
       <c r="K91" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L91" s="27"/>
-      <c r="M91" s="27"/>
+      <c r="L91" s="30" t="s">
+        <v>814</v>
+      </c>
+      <c r="M91" s="30" t="s">
+        <v>815</v>
+      </c>
       <c r="N91" s="27"/>
-      <c r="O91" s="27"/>
+      <c r="O91" s="27" t="s">
+        <v>816</v>
+      </c>
       <c r="P91" s="27"/>
       <c r="Q91" s="27"/>
       <c r="R91" s="27"/>
       <c r="S91" s="27"/>
-      <c r="T91" s="27"/>
+      <c r="T91" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y91" s="19">
         <v>1</v>
       </c>
@@ -19755,7 +19961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:168">
+    <row r="92" spans="1:168" ht="16">
       <c r="B92" s="3" t="s">
         <v>231</v>
       </c>
@@ -19784,15 +19990,21 @@
       <c r="K92" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L92" s="27"/>
+      <c r="L92" s="30" t="s">
+        <v>817</v>
+      </c>
       <c r="M92" s="27"/>
       <c r="N92" s="27"/>
-      <c r="O92" s="27"/>
+      <c r="O92" s="27" t="s">
+        <v>818</v>
+      </c>
       <c r="P92" s="27"/>
       <c r="Q92" s="27"/>
       <c r="R92" s="27"/>
       <c r="S92" s="27"/>
-      <c r="T92" s="27"/>
+      <c r="T92" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y92" s="19">
         <v>2</v>
       </c>
@@ -19851,7 +20063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:168">
+    <row r="93" spans="1:168" ht="16">
       <c r="A93" s="3" t="s">
         <v>229</v>
       </c>
@@ -19885,15 +20097,25 @@
       <c r="K93" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="N93" s="27"/>
-      <c r="O93" s="27"/>
+      <c r="L93" s="30" t="s">
+        <v>819</v>
+      </c>
+      <c r="M93" s="30" t="s">
+        <v>820</v>
+      </c>
+      <c r="N93" s="30" t="s">
+        <v>821</v>
+      </c>
+      <c r="O93" s="27" t="s">
+        <v>822</v>
+      </c>
       <c r="P93" s="27"/>
       <c r="Q93" s="27"/>
       <c r="R93" s="27"/>
       <c r="S93" s="27"/>
-      <c r="T93" s="27"/>
+      <c r="T93" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AN93" s="3">
         <v>1</v>
       </c>
@@ -20044,7 +20266,9 @@
       <c r="K94" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L94" s="27"/>
+      <c r="L94" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M94" s="27"/>
       <c r="N94" s="27"/>
       <c r="O94" s="27"/>
@@ -20052,7 +20276,9 @@
       <c r="Q94" s="27"/>
       <c r="R94" s="27"/>
       <c r="S94" s="27"/>
-      <c r="T94" s="27"/>
+      <c r="T94" s="27" t="s">
+        <v>823</v>
+      </c>
       <c r="Y94" s="19">
         <v>1</v>
       </c>
@@ -20133,15 +20359,21 @@
       <c r="K95" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L95" s="27"/>
+      <c r="L95" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M95" s="27"/>
       <c r="N95" s="27"/>
-      <c r="O95" s="27"/>
+      <c r="O95" s="27" t="s">
+        <v>824</v>
+      </c>
       <c r="P95" s="27"/>
       <c r="Q95" s="27"/>
       <c r="R95" s="27"/>
       <c r="S95" s="27"/>
-      <c r="T95" s="27"/>
+      <c r="T95" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AK95" s="21">
         <v>1</v>
       </c>
@@ -20179,7 +20411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:168">
+    <row r="96" spans="1:168" ht="16">
       <c r="B96" s="3" t="s">
         <v>221</v>
       </c>
@@ -20210,15 +20442,21 @@
       <c r="K96" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L96" s="27"/>
+      <c r="L96" s="30" t="s">
+        <v>825</v>
+      </c>
       <c r="M96" s="27"/>
       <c r="N96" s="27"/>
-      <c r="O96" s="27"/>
+      <c r="O96" s="27" t="s">
+        <v>826</v>
+      </c>
       <c r="P96" s="27"/>
       <c r="Q96" s="27"/>
       <c r="R96" s="27"/>
       <c r="S96" s="27"/>
-      <c r="T96" s="27"/>
+      <c r="T96" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y96" s="19">
         <v>1</v>
       </c>
@@ -20349,7 +20587,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:168">
+    <row r="97" spans="1:168" ht="16">
       <c r="B97" s="3" t="s">
         <v>209</v>
       </c>
@@ -20380,15 +20618,21 @@
       <c r="K97" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L97" s="27"/>
+      <c r="L97" s="30" t="s">
+        <v>827</v>
+      </c>
       <c r="M97" s="27"/>
       <c r="N97" s="27"/>
-      <c r="O97" s="27"/>
+      <c r="O97" s="27" t="s">
+        <v>828</v>
+      </c>
       <c r="P97" s="27"/>
       <c r="Q97" s="27"/>
       <c r="R97" s="27"/>
       <c r="S97" s="27"/>
-      <c r="T97" s="27"/>
+      <c r="T97" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AD97" s="3">
         <v>1</v>
       </c>
@@ -20417,7 +20661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:168">
+    <row r="98" spans="1:168" ht="16">
       <c r="B98" s="3" t="s">
         <v>209</v>
       </c>
@@ -20448,15 +20692,25 @@
       <c r="K98" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L98" s="27"/>
+      <c r="L98" s="30" t="s">
+        <v>829</v>
+      </c>
       <c r="M98" s="27"/>
       <c r="N98" s="27"/>
-      <c r="O98" s="27"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="27"/>
+      <c r="O98" s="27" t="s">
+        <v>830</v>
+      </c>
+      <c r="P98" s="27" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q98" s="27" t="s">
+        <v>832</v>
+      </c>
       <c r="R98" s="27"/>
       <c r="S98" s="27"/>
-      <c r="T98" s="27"/>
+      <c r="T98" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="U98" s="19">
         <v>2</v>
       </c>
@@ -20617,7 +20871,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:168">
+    <row r="99" spans="1:168" ht="16">
       <c r="B99" s="3" t="s">
         <v>209</v>
       </c>
@@ -20648,15 +20902,21 @@
       <c r="K99" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L99" s="27"/>
+      <c r="L99" s="30" t="s">
+        <v>833</v>
+      </c>
       <c r="M99" s="27"/>
       <c r="N99" s="27"/>
-      <c r="O99" s="27"/>
+      <c r="O99" s="27" t="s">
+        <v>834</v>
+      </c>
       <c r="P99" s="27"/>
       <c r="Q99" s="27"/>
       <c r="R99" s="27"/>
       <c r="S99" s="27"/>
-      <c r="T99" s="27"/>
+      <c r="T99" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AJ99" s="3">
         <v>1</v>
       </c>
@@ -20709,7 +20969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:168">
+    <row r="100" spans="1:168" ht="16">
       <c r="B100" s="3" t="s">
         <v>209</v>
       </c>
@@ -20740,15 +21000,27 @@
       <c r="K100" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L100" s="27"/>
-      <c r="M100" s="27"/>
+      <c r="L100" s="30" t="s">
+        <v>835</v>
+      </c>
+      <c r="M100" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="N100" s="27"/>
-      <c r="O100" s="27"/>
-      <c r="P100" s="27"/>
-      <c r="Q100" s="27"/>
+      <c r="O100" s="27" t="s">
+        <v>837</v>
+      </c>
+      <c r="P100" s="27" t="s">
+        <v>838</v>
+      </c>
+      <c r="Q100" s="27" t="s">
+        <v>839</v>
+      </c>
       <c r="R100" s="27"/>
       <c r="S100" s="27"/>
-      <c r="T100" s="27"/>
+      <c r="T100" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AD100" s="3">
         <v>1</v>
       </c>
@@ -20972,7 +21244,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:168">
+    <row r="101" spans="1:168" ht="16">
       <c r="B101" s="3" t="s">
         <v>209</v>
       </c>
@@ -21003,15 +21275,25 @@
       <c r="K101" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L101" s="27"/>
+      <c r="L101" s="30" t="s">
+        <v>840</v>
+      </c>
       <c r="M101" s="27"/>
       <c r="N101" s="27"/>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="27"/>
+      <c r="O101" s="27" t="s">
+        <v>841</v>
+      </c>
+      <c r="P101" s="27" t="s">
+        <v>842</v>
+      </c>
+      <c r="Q101" s="27" t="s">
+        <v>843</v>
+      </c>
       <c r="R101" s="27"/>
       <c r="S101" s="27"/>
-      <c r="T101" s="27"/>
+      <c r="T101" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AF101" s="19">
         <v>1</v>
       </c>
@@ -33572,6 +33854,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
added full text of 39
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="0" windowWidth="24880" windowHeight="13020" tabRatio="500"/>
+    <workbookView xWindow="6520" yWindow="820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="846">
   <si>
     <t>f</t>
   </si>
@@ -2586,6 +2586,12 @@
   </si>
   <si>
     <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074874276;view=1up;seq=11</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=mrgBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CMRXHLR953938931</t>
   </si>
 </sst>
 </file>
@@ -2776,8 +2782,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3063,7 +3071,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="227">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3176,6 +3184,7 @@
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3288,6 +3297,7 @@
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6817,6 +6827,112 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -6943,112 +7059,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7386,10 +7396,10 @@
   <dimension ref="A1:FL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T101" sqref="T101"/>
+      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12809,10 +12819,14 @@
       <c r="K40" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L40" s="27"/>
+      <c r="L40" s="27" t="s">
+        <v>844</v>
+      </c>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
+      <c r="O40" s="27" t="s">
+        <v>845</v>
+      </c>
       <c r="P40" s="27"/>
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>

</xml_diff>

<commit_message>
notes on MSc dissertation
discovered the Oxford Text Archive!!
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -2782,8 +2782,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="227">
+  <cellStyleXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3071,7 +3085,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="227">
+  <cellStyles count="241">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3185,6 +3199,13 @@
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3298,6 +3319,13 @@
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6827,113 +6855,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7059,6 +6981,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7396,10 +7424,10 @@
   <dimension ref="A1:FL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
☂ updated spreadsheet 101 thru 125
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="19220" windowHeight="13500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3064" uniqueCount="887">
   <si>
     <t>f</t>
   </si>
@@ -2592,6 +2592,129 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CMRXHLR953938931</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=1120785898</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=jE_KnQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://search.proquest.com.ezproxy.library.uvic.ca/docview/6101620?pq-origsite=summon</t>
+  </si>
+  <si>
+    <t>http://literature.proquest.com.ezproxy.library.uvic.ca/toc.do?sourceId=Z000415796&amp;action=new&amp;area=poetry-toc&amp;divLevel=0&amp;queryId=&amp;mapping=toc#scroll&amp;DurUrl=Yes</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=cFg8qAAACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CQAFHNQ976858902</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=bgU1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Zr4NAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJRRZUB024809038</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015027528697;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Q8IjAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWEVAVX487647602</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t6k073h5r;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074893037;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CPWRONY984169496</t>
+  </si>
+  <si>
+    <t>http://literature.proquest.com.ezproxy.library.uvic.ca/searchFulltext.do?id=Z000034404&amp;divLevel=0&amp;area=Prose&amp;DurUrl=Yes&amp;forward=textsFT&amp;queryType=findWork</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=jag_AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nnc1.0315131394;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CYYKIWY600421040</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=WPU7AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CINYPIR812344132</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CCJMYEF264449673</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CBMVOGQ485912935</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CYSQUBT472639316</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=-qkBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CCUCQHB853419200</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t63496n5k;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJIEOCY729182639</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=YCQJAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=3rUNAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CXLCTXW459217013</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015012371368;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t85h7q10h;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t7fq9s098;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=YEM1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=1KRbAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDUUQRB605059981</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101065844480;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015029497743;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015063949815;view=1up;seq=6</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=oEFWAAAAcAAJ</t>
   </si>
 </sst>
 </file>
@@ -6855,7 +6978,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6981,112 +7210,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7424,10 +7547,10 @@
   <dimension ref="A1:FL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="Q126" sqref="Q126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21491,15 +21614,25 @@
       <c r="K102" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L102" s="27"/>
-      <c r="M102" s="27"/>
+      <c r="L102" s="27" t="s">
+        <v>846</v>
+      </c>
+      <c r="M102" s="27" t="s">
+        <v>847</v>
+      </c>
       <c r="N102" s="27"/>
-      <c r="O102" s="27"/>
-      <c r="P102" s="27"/>
+      <c r="O102" s="27" t="s">
+        <v>848</v>
+      </c>
+      <c r="P102" s="27" t="s">
+        <v>849</v>
+      </c>
       <c r="Q102" s="27"/>
       <c r="R102" s="27"/>
       <c r="S102" s="27"/>
-      <c r="T102" s="27"/>
+      <c r="T102" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y102" s="19">
         <v>1</v>
       </c>
@@ -21605,7 +21738,9 @@
       <c r="K103" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L103" s="27"/>
+      <c r="L103" s="27" t="s">
+        <v>850</v>
+      </c>
       <c r="M103" s="27"/>
       <c r="N103" s="27"/>
       <c r="O103" s="27"/>
@@ -21613,7 +21748,9 @@
       <c r="Q103" s="27"/>
       <c r="R103" s="27"/>
       <c r="S103" s="27"/>
-      <c r="T103" s="27"/>
+      <c r="T103" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AF103" s="19">
         <v>1</v>
       </c>
@@ -21685,15 +21822,21 @@
       <c r="K104" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L104" s="27"/>
+      <c r="L104" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M104" s="27"/>
       <c r="N104" s="27"/>
-      <c r="O104" s="27"/>
+      <c r="O104" s="27" t="s">
+        <v>851</v>
+      </c>
       <c r="P104" s="27"/>
       <c r="Q104" s="27"/>
       <c r="R104" s="27"/>
       <c r="S104" s="27"/>
-      <c r="T104" s="27"/>
+      <c r="T104" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="BA104" s="3">
         <v>1</v>
       </c>
@@ -21710,7 +21853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:168">
+    <row r="105" spans="1:168" ht="16">
       <c r="B105" s="3" t="s">
         <v>206</v>
       </c>
@@ -21741,15 +21884,25 @@
       <c r="K105" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L105" s="27"/>
-      <c r="M105" s="27"/>
+      <c r="L105" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="M105" s="30" t="s">
+        <v>853</v>
+      </c>
       <c r="N105" s="27"/>
-      <c r="O105" s="27"/>
-      <c r="P105" s="27"/>
+      <c r="O105" s="27" t="s">
+        <v>854</v>
+      </c>
+      <c r="P105" s="27" t="s">
+        <v>855</v>
+      </c>
       <c r="Q105" s="27"/>
       <c r="R105" s="27"/>
       <c r="S105" s="27"/>
-      <c r="T105" s="27"/>
+      <c r="T105" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y105" s="19">
         <v>1</v>
       </c>
@@ -21848,7 +22001,9 @@
       <c r="K106" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L106" s="27"/>
+      <c r="L106" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M106" s="27"/>
       <c r="N106" s="27"/>
       <c r="O106" s="27"/>
@@ -21856,7 +22011,9 @@
       <c r="Q106" s="27"/>
       <c r="R106" s="27"/>
       <c r="S106" s="27"/>
-      <c r="T106" s="27"/>
+      <c r="T106" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U106" s="19">
         <v>1</v>
       </c>
@@ -21923,7 +22080,9 @@
       <c r="K107" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L107" s="27"/>
+      <c r="L107" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M107" s="27"/>
       <c r="N107" s="27"/>
       <c r="O107" s="27"/>
@@ -21931,7 +22090,9 @@
       <c r="Q107" s="27"/>
       <c r="R107" s="27"/>
       <c r="S107" s="27"/>
-      <c r="T107" s="27"/>
+      <c r="T107" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AR107" s="3">
         <v>1</v>
       </c>
@@ -21996,7 +22157,7 @@
       </c>
       <c r="FF107" s="23"/>
     </row>
-    <row r="108" spans="1:168">
+    <row r="108" spans="1:168" ht="16">
       <c r="B108" s="3" t="s">
         <v>196</v>
       </c>
@@ -22027,15 +22188,25 @@
       <c r="K108" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L108" s="27"/>
+      <c r="L108" s="30" t="s">
+        <v>856</v>
+      </c>
       <c r="M108" s="27"/>
       <c r="N108" s="27"/>
-      <c r="O108" s="27"/>
-      <c r="P108" s="27"/>
-      <c r="Q108" s="27"/>
+      <c r="O108" s="27" t="s">
+        <v>857</v>
+      </c>
+      <c r="P108" s="27" t="s">
+        <v>858</v>
+      </c>
+      <c r="Q108" s="27" t="s">
+        <v>859</v>
+      </c>
       <c r="R108" s="27"/>
       <c r="S108" s="27"/>
-      <c r="T108" s="27"/>
+      <c r="T108" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y108" s="19">
         <v>1</v>
       </c>
@@ -22196,15 +22367,21 @@
       <c r="K109" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L109" s="27"/>
+      <c r="L109" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M109" s="27"/>
       <c r="N109" s="27"/>
-      <c r="O109" s="27"/>
+      <c r="O109" s="27" t="s">
+        <v>860</v>
+      </c>
       <c r="P109" s="27"/>
       <c r="Q109" s="27"/>
       <c r="R109" s="27"/>
       <c r="S109" s="27"/>
-      <c r="T109" s="27"/>
+      <c r="T109" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="U109" s="19">
         <v>1</v>
       </c>
@@ -22384,15 +22561,21 @@
       <c r="K110" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L110" s="27"/>
+      <c r="L110" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M110" s="27"/>
       <c r="N110" s="27"/>
-      <c r="O110" s="27"/>
+      <c r="O110" s="27" t="s">
+        <v>861</v>
+      </c>
       <c r="P110" s="27"/>
       <c r="Q110" s="27"/>
       <c r="R110" s="27"/>
       <c r="S110" s="27"/>
-      <c r="T110" s="27"/>
+      <c r="T110" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AD110" s="3">
         <v>1</v>
       </c>
@@ -22559,7 +22742,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:168">
+    <row r="111" spans="1:168" ht="16">
       <c r="B111" s="3" t="s">
         <v>196</v>
       </c>
@@ -22588,15 +22771,23 @@
       <c r="K111" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L111" s="27"/>
+      <c r="L111" s="30" t="s">
+        <v>862</v>
+      </c>
       <c r="M111" s="27"/>
       <c r="N111" s="27"/>
-      <c r="O111" s="27"/>
-      <c r="P111" s="27"/>
+      <c r="O111" s="27" t="s">
+        <v>864</v>
+      </c>
+      <c r="P111" s="27" t="s">
+        <v>863</v>
+      </c>
       <c r="Q111" s="27"/>
       <c r="R111" s="27"/>
       <c r="S111" s="27"/>
-      <c r="T111" s="27"/>
+      <c r="T111" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AN111" s="22">
         <v>1</v>
       </c>
@@ -22629,7 +22820,7 @@
       </c>
       <c r="FF111" s="23"/>
     </row>
-    <row r="112" spans="1:168">
+    <row r="112" spans="1:168" ht="16">
       <c r="B112" s="3" t="s">
         <v>196</v>
       </c>
@@ -22660,15 +22851,21 @@
       <c r="K112" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L112" s="27"/>
+      <c r="L112" s="30" t="s">
+        <v>865</v>
+      </c>
       <c r="M112" s="27"/>
       <c r="N112" s="27"/>
-      <c r="O112" s="27"/>
+      <c r="O112" s="27" t="s">
+        <v>866</v>
+      </c>
       <c r="P112" s="27"/>
       <c r="Q112" s="27"/>
       <c r="R112" s="27"/>
       <c r="S112" s="27"/>
-      <c r="T112" s="27"/>
+      <c r="T112" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AE112" s="19">
         <v>1</v>
       </c>
@@ -22785,7 +22982,9 @@
       <c r="K113" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L113" s="27"/>
+      <c r="L113" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M113" s="27"/>
       <c r="N113" s="27"/>
       <c r="O113" s="27"/>
@@ -22793,7 +22992,9 @@
       <c r="Q113" s="27"/>
       <c r="R113" s="27"/>
       <c r="S113" s="27"/>
-      <c r="T113" s="27"/>
+      <c r="T113" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U113" s="19">
         <v>1</v>
       </c>
@@ -22937,15 +23138,21 @@
       <c r="K114" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L114" s="27"/>
+      <c r="L114" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M114" s="27"/>
       <c r="N114" s="27"/>
-      <c r="O114" s="27"/>
+      <c r="O114" s="27" t="s">
+        <v>867</v>
+      </c>
       <c r="P114" s="27"/>
       <c r="Q114" s="27"/>
       <c r="R114" s="27"/>
       <c r="S114" s="27"/>
-      <c r="T114" s="27"/>
+      <c r="T114" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y114" s="19">
         <v>1</v>
       </c>
@@ -23029,15 +23236,21 @@
       <c r="K115" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L115" s="27"/>
+      <c r="L115" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M115" s="27"/>
       <c r="N115" s="27"/>
-      <c r="O115" s="27"/>
+      <c r="O115" s="27" t="s">
+        <v>868</v>
+      </c>
       <c r="P115" s="27"/>
       <c r="Q115" s="27"/>
       <c r="R115" s="27"/>
       <c r="S115" s="27"/>
-      <c r="T115" s="27"/>
+      <c r="T115" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AC115" s="21">
         <v>1</v>
       </c>
@@ -23169,15 +23382,21 @@
       <c r="K116" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L116" s="27"/>
+      <c r="L116" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M116" s="27"/>
       <c r="N116" s="27"/>
-      <c r="O116" s="27"/>
+      <c r="O116" s="27" t="s">
+        <v>869</v>
+      </c>
       <c r="P116" s="27"/>
       <c r="Q116" s="27"/>
       <c r="R116" s="27"/>
       <c r="S116" s="27"/>
-      <c r="T116" s="27"/>
+      <c r="T116" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="BR116" s="3">
         <v>1</v>
       </c>
@@ -23241,7 +23460,9 @@
       <c r="K117" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L117" s="27"/>
+      <c r="L117" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M117" s="27"/>
       <c r="N117" s="27"/>
       <c r="O117" s="27"/>
@@ -23249,7 +23470,9 @@
       <c r="Q117" s="27"/>
       <c r="R117" s="27"/>
       <c r="S117" s="27"/>
-      <c r="T117" s="27"/>
+      <c r="T117" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y117" s="19">
         <v>1</v>
       </c>
@@ -23341,7 +23564,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="118" spans="2:168">
+    <row r="118" spans="2:168" ht="16">
       <c r="B118" s="3" t="s">
         <v>186</v>
       </c>
@@ -23372,7 +23595,9 @@
       <c r="K118" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L118" s="27"/>
+      <c r="L118" s="30" t="s">
+        <v>870</v>
+      </c>
       <c r="M118" s="27"/>
       <c r="N118" s="27"/>
       <c r="O118" s="27"/>
@@ -23380,7 +23605,9 @@
       <c r="Q118" s="27"/>
       <c r="R118" s="27"/>
       <c r="S118" s="27"/>
-      <c r="T118" s="27"/>
+      <c r="T118" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y118" s="19">
         <v>1</v>
       </c>
@@ -23479,15 +23706,23 @@
       <c r="K119" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L119" s="27"/>
+      <c r="L119" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M119" s="27"/>
       <c r="N119" s="27"/>
-      <c r="O119" s="27"/>
-      <c r="P119" s="27"/>
+      <c r="O119" s="27" t="s">
+        <v>871</v>
+      </c>
+      <c r="P119" s="27" t="s">
+        <v>872</v>
+      </c>
       <c r="Q119" s="27"/>
       <c r="R119" s="27"/>
       <c r="S119" s="27"/>
-      <c r="T119" s="27"/>
+      <c r="T119" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AD119" s="3">
         <v>1</v>
       </c>
@@ -23596,15 +23831,21 @@
       <c r="K120" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L120" s="27"/>
+      <c r="L120" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M120" s="27"/>
       <c r="N120" s="27"/>
-      <c r="O120" s="27"/>
+      <c r="O120" s="27" t="s">
+        <v>873</v>
+      </c>
       <c r="P120" s="27"/>
       <c r="Q120" s="27"/>
       <c r="R120" s="27"/>
       <c r="S120" s="27"/>
-      <c r="T120" s="27"/>
+      <c r="T120" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="U120" s="19">
         <v>2</v>
       </c>
@@ -23834,7 +24075,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="121" spans="2:168">
+    <row r="121" spans="2:168" ht="16">
       <c r="B121" s="3" t="s">
         <v>181</v>
       </c>
@@ -23863,15 +24104,29 @@
       <c r="K121" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L121" s="27"/>
-      <c r="M121" s="27"/>
+      <c r="L121" s="30" t="s">
+        <v>874</v>
+      </c>
+      <c r="M121" s="30" t="s">
+        <v>875</v>
+      </c>
       <c r="N121" s="27"/>
-      <c r="O121" s="27"/>
-      <c r="P121" s="27"/>
-      <c r="Q121" s="27"/>
-      <c r="R121" s="27"/>
+      <c r="O121" s="27" t="s">
+        <v>876</v>
+      </c>
+      <c r="P121" s="27" t="s">
+        <v>877</v>
+      </c>
+      <c r="Q121" s="27" t="s">
+        <v>878</v>
+      </c>
+      <c r="R121" s="27" t="s">
+        <v>879</v>
+      </c>
       <c r="S121" s="27"/>
-      <c r="T121" s="27"/>
+      <c r="T121" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AC121" s="21">
         <v>1</v>
       </c>
@@ -23987,7 +24242,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="2:168">
+    <row r="122" spans="2:168" ht="16">
       <c r="B122" s="3" t="s">
         <v>179</v>
       </c>
@@ -24018,15 +24273,29 @@
       <c r="K122" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L122" s="27"/>
-      <c r="M122" s="27"/>
+      <c r="L122" s="30" t="s">
+        <v>880</v>
+      </c>
+      <c r="M122" s="30" t="s">
+        <v>881</v>
+      </c>
       <c r="N122" s="27"/>
-      <c r="O122" s="27"/>
-      <c r="P122" s="27"/>
-      <c r="Q122" s="27"/>
-      <c r="R122" s="27"/>
+      <c r="O122" s="27" t="s">
+        <v>882</v>
+      </c>
+      <c r="P122" s="27" t="s">
+        <v>883</v>
+      </c>
+      <c r="Q122" s="27" t="s">
+        <v>884</v>
+      </c>
+      <c r="R122" s="27" t="s">
+        <v>885</v>
+      </c>
       <c r="S122" s="27"/>
-      <c r="T122" s="27"/>
+      <c r="T122" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AR122" s="3">
         <v>1</v>
       </c>
@@ -24090,7 +24359,9 @@
       <c r="K123" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L123" s="27"/>
+      <c r="L123" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M123" s="27"/>
       <c r="N123" s="27"/>
       <c r="O123" s="27"/>
@@ -24098,7 +24369,9 @@
       <c r="Q123" s="27"/>
       <c r="R123" s="27"/>
       <c r="S123" s="27"/>
-      <c r="T123" s="27"/>
+      <c r="T123" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U123" s="19">
         <v>1</v>
       </c>
@@ -24237,7 +24510,9 @@
       <c r="K124" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L124" s="27"/>
+      <c r="L124" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M124" s="27"/>
       <c r="N124" s="27"/>
       <c r="O124" s="27"/>
@@ -24245,7 +24520,9 @@
       <c r="Q124" s="27"/>
       <c r="R124" s="27"/>
       <c r="S124" s="27"/>
-      <c r="T124" s="27"/>
+      <c r="T124" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y124" s="19">
         <v>2</v>
       </c>
@@ -24363,7 +24640,9 @@
       <c r="K125" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L125" s="27"/>
+      <c r="L125" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M125" s="27"/>
       <c r="N125" s="27"/>
       <c r="O125" s="27"/>
@@ -24371,7 +24650,9 @@
       <c r="Q125" s="27"/>
       <c r="R125" s="27"/>
       <c r="S125" s="27"/>
-      <c r="T125" s="27"/>
+      <c r="T125" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="BO125" s="21">
         <v>1</v>
       </c>
@@ -24422,7 +24703,9 @@
       <c r="K126" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L126" s="27"/>
+      <c r="L126" s="27" t="s">
+        <v>886</v>
+      </c>
       <c r="M126" s="27"/>
       <c r="N126" s="27"/>
       <c r="O126" s="27"/>
@@ -24430,7 +24713,9 @@
       <c r="Q126" s="27"/>
       <c r="R126" s="27"/>
       <c r="S126" s="27"/>
-      <c r="T126" s="27"/>
+      <c r="T126" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y126" s="19">
         <v>1</v>
       </c>
@@ -33898,7 +34183,6 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
☂ add full text 126 thru 150
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="19220" windowHeight="13500" tabRatio="500"/>
+    <workbookView xWindow="8000" yWindow="0" windowWidth="25600" windowHeight="12780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3064" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3161" uniqueCount="948">
   <si>
     <t>f</t>
   </si>
@@ -2715,6 +2715,249 @@
   </si>
   <si>
     <t>books.google.com/books?id=oEFWAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CAOBYFS557419000</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=v6oBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLPBZMC111870068</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CIXCSSU125807932</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=ZMsBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CNHGLPF453616603</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=dul1.ark:/13960/t76t1w51q;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Xi41AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://books.google.com/books?id=Lh0GAAAAQAAJ&amp;printsec=frontcover&amp;dq=ROCHE-BLANCHE,+OR,+THE+HUNTERS+OF+THE+PYRENEES.+A+ROMANCE&amp;hl=en&amp;sa=X&amp;ei=dqPvU_3ICZWAygT1vYHoAQ&amp;ved=0CCIQ6AEwAQ#v=onepage&amp;q=ROCHE-BLANCHE%2C%20OR%2C%20THE%20HUNTERS%20OF%20THE%20PYRENEES.%20A%20ROMANCE&amp;f=false</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CHCSXEQ349552668</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t1pg28w38;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hwe3lz;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=-15NAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=3T1WAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CQVQSGU814063448</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=dzA3AAAAIAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CTDNAWV734800945</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Les9AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=5RkGAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hwnnx2;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=wu.89016100521;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hwnnx6;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=CXvUWr9RDU4C</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=ko8VAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=XDA1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015063950110;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015021305142;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015013472025;view=1up;seq=3</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=e_W0eXirZ3oC</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=VCY1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=zQxHAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJBSTAD774871921#</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=KlsmAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=y1omAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=lgwGAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://literature.proquest.com.ezproxy.library.uvic.ca/searchFulltext.do?id=Z000042501&amp;divLevel=0&amp;area=Prose&amp;DurUrl=Yes&amp;forward=textsFT&amp;queryType=findWork</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CBPDOUY440978194</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=X-U8AQAAIAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=q1kmAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=vksJAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGFDZMU204246389</t>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=7xw5AAAAMAAJ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=Rw0UAAAAQAAJ</t>
+    </r>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015033367650;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=F1smAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=_gwUAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CEMGYCB036187635</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=dul1.ark:/13960/t3708t937;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=ucm.5325889951;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CUDQKZA306700773</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t76t1924s;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t86h4h94q;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Id8GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CISCFGW667105458</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=PSU7AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101065709832;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=hvd.hn3q3c;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101065710756;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc2.ark:/13960/t3rv0g31p;view=1up;seq=11</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101062743727;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGDCZDK029671388</t>
   </si>
 </sst>
 </file>
@@ -6978,113 +7221,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7210,6 +7347,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7547,10 +7790,10 @@
   <dimension ref="A1:FL209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L116" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q126" sqref="Q126"/>
+      <selection pane="bottomRight" activeCell="M151" sqref="M151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24829,7 +25072,9 @@
       <c r="K127" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L127" s="27"/>
+      <c r="L127" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M127" s="27"/>
       <c r="N127" s="27"/>
       <c r="O127" s="27"/>
@@ -24837,7 +25082,9 @@
       <c r="Q127" s="27"/>
       <c r="R127" s="27"/>
       <c r="S127" s="27"/>
-      <c r="T127" s="27"/>
+      <c r="T127" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="BE127" s="3">
         <v>1</v>
       </c>
@@ -24915,7 +25162,9 @@
       <c r="K128" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L128" s="27"/>
+      <c r="L128" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M128" s="27"/>
       <c r="N128" s="27"/>
       <c r="O128" s="27"/>
@@ -24923,7 +25172,9 @@
       <c r="Q128" s="27"/>
       <c r="R128" s="27"/>
       <c r="S128" s="27"/>
-      <c r="T128" s="27"/>
+      <c r="T128" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y128" s="19">
         <v>1</v>
       </c>
@@ -25094,15 +25345,21 @@
       <c r="K129" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L129" s="27"/>
+      <c r="L129" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M129" s="27"/>
       <c r="N129" s="27"/>
-      <c r="O129" s="27"/>
+      <c r="O129" s="27" t="s">
+        <v>887</v>
+      </c>
       <c r="P129" s="27"/>
       <c r="Q129" s="27"/>
       <c r="R129" s="27"/>
       <c r="S129" s="27"/>
-      <c r="T129" s="27"/>
+      <c r="T129" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="U129" s="19">
         <v>1</v>
       </c>
@@ -25224,7 +25481,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="2:168">
+    <row r="130" spans="2:168" ht="16">
       <c r="B130" s="3" t="s">
         <v>165</v>
       </c>
@@ -25249,15 +25506,21 @@
       <c r="K130" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L130" s="27"/>
+      <c r="L130" s="30" t="s">
+        <v>888</v>
+      </c>
       <c r="M130" s="27"/>
       <c r="N130" s="27"/>
-      <c r="O130" s="27"/>
+      <c r="O130" s="27" t="s">
+        <v>889</v>
+      </c>
       <c r="P130" s="27"/>
       <c r="Q130" s="27"/>
       <c r="R130" s="27"/>
       <c r="S130" s="27"/>
-      <c r="T130" s="27"/>
+      <c r="T130" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y130" s="19">
         <v>2</v>
       </c>
@@ -25506,15 +25769,21 @@
       <c r="K131" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L131" s="27"/>
+      <c r="L131" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M131" s="27"/>
       <c r="N131" s="27"/>
-      <c r="O131" s="27"/>
+      <c r="O131" s="27" t="s">
+        <v>890</v>
+      </c>
       <c r="P131" s="27"/>
       <c r="Q131" s="27"/>
       <c r="R131" s="27"/>
       <c r="S131" s="27"/>
-      <c r="T131" s="27"/>
+      <c r="T131" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AD131" s="3">
         <v>1</v>
       </c>
@@ -25675,7 +25944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:168">
+    <row r="132" spans="2:168" ht="16">
       <c r="B132" s="3" t="s">
         <v>161</v>
       </c>
@@ -25700,15 +25969,23 @@
       <c r="K132" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L132" s="27"/>
+      <c r="L132" s="30" t="s">
+        <v>891</v>
+      </c>
       <c r="M132" s="27"/>
       <c r="N132" s="27"/>
-      <c r="O132" s="27"/>
-      <c r="P132" s="27"/>
+      <c r="O132" s="27" t="s">
+        <v>892</v>
+      </c>
+      <c r="P132" s="27" t="s">
+        <v>893</v>
+      </c>
       <c r="Q132" s="27"/>
       <c r="R132" s="27"/>
       <c r="S132" s="27"/>
-      <c r="T132" s="27"/>
+      <c r="T132" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="BR132" s="3">
         <v>1</v>
       </c>
@@ -25737,7 +26014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:168">
+    <row r="133" spans="2:168" ht="16">
       <c r="B133" s="3" t="s">
         <v>159</v>
       </c>
@@ -25762,15 +26039,27 @@
       <c r="K133" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L133" s="27"/>
-      <c r="M133" s="27"/>
+      <c r="L133" s="30" t="s">
+        <v>894</v>
+      </c>
+      <c r="M133" s="27" t="s">
+        <v>895</v>
+      </c>
       <c r="N133" s="27"/>
-      <c r="O133" s="27"/>
-      <c r="P133" s="27"/>
-      <c r="Q133" s="27"/>
+      <c r="O133" s="27" t="s">
+        <v>896</v>
+      </c>
+      <c r="P133" s="27" t="s">
+        <v>897</v>
+      </c>
+      <c r="Q133" s="27" t="s">
+        <v>898</v>
+      </c>
       <c r="R133" s="27"/>
       <c r="S133" s="27"/>
-      <c r="T133" s="27"/>
+      <c r="T133" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AR133" s="3">
         <v>1</v>
       </c>
@@ -25817,7 +26106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:168">
+    <row r="134" spans="2:168" ht="16">
       <c r="B134" s="3" t="s">
         <v>150</v>
       </c>
@@ -25842,15 +26131,23 @@
       <c r="K134" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L134" s="27"/>
-      <c r="M134" s="27"/>
+      <c r="L134" s="30" t="s">
+        <v>899</v>
+      </c>
+      <c r="M134" s="30" t="s">
+        <v>900</v>
+      </c>
       <c r="N134" s="27"/>
-      <c r="O134" s="27"/>
+      <c r="O134" s="27" t="s">
+        <v>901</v>
+      </c>
       <c r="P134" s="27"/>
       <c r="Q134" s="27"/>
       <c r="R134" s="27"/>
       <c r="S134" s="27"/>
-      <c r="T134" s="27"/>
+      <c r="T134" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y134" s="19">
         <v>1</v>
       </c>
@@ -25930,7 +26227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:168">
+    <row r="135" spans="2:168" ht="16">
       <c r="B135" s="3" t="s">
         <v>150</v>
       </c>
@@ -25955,15 +26252,21 @@
       <c r="K135" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L135" s="27"/>
+      <c r="L135" s="30" t="s">
+        <v>902</v>
+      </c>
       <c r="M135" s="27"/>
       <c r="N135" s="27"/>
-      <c r="O135" s="27"/>
+      <c r="O135" s="27" t="s">
+        <v>903</v>
+      </c>
       <c r="P135" s="27"/>
       <c r="Q135" s="27"/>
       <c r="R135" s="27"/>
       <c r="S135" s="27"/>
-      <c r="T135" s="27"/>
+      <c r="T135" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AD135" s="3">
         <v>1</v>
       </c>
@@ -26037,7 +26340,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="2:168">
+    <row r="136" spans="2:168" ht="16">
       <c r="B136" s="3" t="s">
         <v>150</v>
       </c>
@@ -26062,15 +26365,27 @@
       <c r="K136" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L136" s="27"/>
-      <c r="M136" s="27"/>
+      <c r="L136" s="30" t="s">
+        <v>904</v>
+      </c>
+      <c r="M136" s="30" t="s">
+        <v>905</v>
+      </c>
       <c r="N136" s="27"/>
-      <c r="O136" s="27"/>
-      <c r="P136" s="27"/>
-      <c r="Q136" s="27"/>
+      <c r="O136" s="27" t="s">
+        <v>906</v>
+      </c>
+      <c r="P136" s="27" t="s">
+        <v>907</v>
+      </c>
+      <c r="Q136" s="27" t="s">
+        <v>908</v>
+      </c>
       <c r="R136" s="27"/>
       <c r="S136" s="27"/>
-      <c r="T136" s="27"/>
+      <c r="T136" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U136" s="19">
         <v>2</v>
       </c>
@@ -26240,7 +26555,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="137" spans="2:168">
+    <row r="137" spans="2:168" ht="16">
       <c r="B137" s="3" t="s">
         <v>150</v>
       </c>
@@ -26265,15 +26580,29 @@
       <c r="K137" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L137" s="27"/>
-      <c r="M137" s="27"/>
-      <c r="N137" s="27"/>
-      <c r="O137" s="27"/>
-      <c r="P137" s="27"/>
-      <c r="Q137" s="27"/>
+      <c r="L137" s="30" t="s">
+        <v>909</v>
+      </c>
+      <c r="M137" s="30" t="s">
+        <v>910</v>
+      </c>
+      <c r="N137" s="30" t="s">
+        <v>911</v>
+      </c>
+      <c r="O137" s="27" t="s">
+        <v>912</v>
+      </c>
+      <c r="P137" s="27" t="s">
+        <v>913</v>
+      </c>
+      <c r="Q137" s="27" t="s">
+        <v>914</v>
+      </c>
       <c r="R137" s="27"/>
       <c r="S137" s="27"/>
-      <c r="T137" s="27"/>
+      <c r="T137" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U137" s="19">
         <v>1</v>
       </c>
@@ -26428,7 +26757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:168">
+    <row r="138" spans="2:168" ht="16">
       <c r="B138" s="3" t="s">
         <v>150</v>
       </c>
@@ -26453,15 +26782,25 @@
       <c r="K138" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L138" s="27"/>
-      <c r="M138" s="27"/>
-      <c r="N138" s="27"/>
-      <c r="O138" s="27"/>
+      <c r="L138" s="30" t="s">
+        <v>915</v>
+      </c>
+      <c r="M138" s="30" t="s">
+        <v>916</v>
+      </c>
+      <c r="N138" s="30" t="s">
+        <v>917</v>
+      </c>
+      <c r="O138" s="27" t="s">
+        <v>918</v>
+      </c>
       <c r="P138" s="27"/>
       <c r="Q138" s="27"/>
       <c r="R138" s="27"/>
       <c r="S138" s="27"/>
-      <c r="T138" s="27"/>
+      <c r="T138" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="U138" s="19">
         <v>1</v>
       </c>
@@ -26616,7 +26955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:168">
+    <row r="139" spans="2:168" ht="16">
       <c r="B139" s="3" t="s">
         <v>150</v>
       </c>
@@ -26641,15 +26980,25 @@
       <c r="K139" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L139" s="27"/>
-      <c r="M139" s="27"/>
-      <c r="N139" s="27"/>
-      <c r="O139" s="27"/>
+      <c r="L139" s="30" t="s">
+        <v>919</v>
+      </c>
+      <c r="M139" s="30" t="s">
+        <v>920</v>
+      </c>
+      <c r="N139" s="30" t="s">
+        <v>921</v>
+      </c>
+      <c r="O139" s="27" t="s">
+        <v>922</v>
+      </c>
       <c r="P139" s="27"/>
       <c r="Q139" s="27"/>
       <c r="R139" s="27"/>
       <c r="S139" s="27"/>
-      <c r="T139" s="27"/>
+      <c r="T139" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="Y139" s="19">
         <v>2</v>
       </c>
@@ -26829,15 +27178,21 @@
       <c r="K140" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L140" s="27"/>
+      <c r="L140" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M140" s="27"/>
       <c r="N140" s="27"/>
-      <c r="O140" s="27"/>
+      <c r="O140" s="27" t="s">
+        <v>923</v>
+      </c>
       <c r="P140" s="27"/>
       <c r="Q140" s="27"/>
       <c r="R140" s="27"/>
       <c r="S140" s="27"/>
-      <c r="T140" s="27"/>
+      <c r="T140" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y140" s="19">
         <v>1</v>
       </c>
@@ -26972,7 +27327,9 @@
       <c r="K141" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L141" s="27"/>
+      <c r="L141" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M141" s="27"/>
       <c r="N141" s="27"/>
       <c r="O141" s="27"/>
@@ -26980,7 +27337,9 @@
       <c r="Q141" s="27"/>
       <c r="R141" s="27"/>
       <c r="S141" s="27"/>
-      <c r="T141" s="27"/>
+      <c r="T141" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AE141" s="19">
         <v>1</v>
       </c>
@@ -27051,7 +27410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="142" spans="2:168">
+    <row r="142" spans="2:168" ht="16">
       <c r="B142" s="3" t="s">
         <v>144</v>
       </c>
@@ -27076,15 +27435,25 @@
       <c r="K142" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L142" s="27"/>
-      <c r="M142" s="27"/>
-      <c r="N142" s="27"/>
-      <c r="O142" s="27"/>
+      <c r="L142" s="30" t="s">
+        <v>924</v>
+      </c>
+      <c r="M142" s="30" t="s">
+        <v>925</v>
+      </c>
+      <c r="N142" s="30" t="s">
+        <v>926</v>
+      </c>
+      <c r="O142" s="27" t="s">
+        <v>927</v>
+      </c>
       <c r="P142" s="27"/>
       <c r="Q142" s="27"/>
       <c r="R142" s="27"/>
       <c r="S142" s="27"/>
-      <c r="T142" s="27"/>
+      <c r="T142" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="DV142" s="21">
         <v>1</v>
       </c>
@@ -27092,7 +27461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:168">
+    <row r="143" spans="2:168" ht="16">
       <c r="B143" s="3" t="s">
         <v>144</v>
       </c>
@@ -27117,15 +27486,23 @@
       <c r="K143" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L143" s="27"/>
-      <c r="M143" s="27"/>
+      <c r="L143" s="31" t="s">
+        <v>928</v>
+      </c>
+      <c r="M143" s="31" t="s">
+        <v>929</v>
+      </c>
       <c r="N143" s="27"/>
-      <c r="O143" s="27"/>
+      <c r="O143" s="27" t="s">
+        <v>930</v>
+      </c>
       <c r="P143" s="27"/>
       <c r="Q143" s="27"/>
       <c r="R143" s="27"/>
       <c r="S143" s="27"/>
-      <c r="T143" s="27"/>
+      <c r="T143" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AJ143" s="3">
         <v>1</v>
       </c>
@@ -27172,7 +27549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="144" spans="2:168">
+    <row r="144" spans="2:168" ht="16">
       <c r="B144" s="3" t="s">
         <v>144</v>
       </c>
@@ -27197,15 +27574,27 @@
       <c r="K144" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L144" s="27"/>
-      <c r="M144" s="27"/>
+      <c r="L144" s="30" t="s">
+        <v>931</v>
+      </c>
+      <c r="M144" s="30" t="s">
+        <v>932</v>
+      </c>
       <c r="N144" s="27"/>
-      <c r="O144" s="27"/>
-      <c r="P144" s="27"/>
-      <c r="Q144" s="27"/>
+      <c r="O144" s="27" t="s">
+        <v>933</v>
+      </c>
+      <c r="P144" s="27" t="s">
+        <v>934</v>
+      </c>
+      <c r="Q144" s="27" t="s">
+        <v>935</v>
+      </c>
       <c r="R144" s="27"/>
       <c r="S144" s="27"/>
-      <c r="T144" s="27"/>
+      <c r="T144" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y144" s="19">
         <v>1</v>
       </c>
@@ -27274,7 +27663,9 @@
       <c r="K145" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L145" s="27"/>
+      <c r="L145" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M145" s="27"/>
       <c r="N145" s="27"/>
       <c r="O145" s="27"/>
@@ -27282,7 +27673,9 @@
       <c r="Q145" s="27"/>
       <c r="R145" s="27"/>
       <c r="S145" s="27"/>
-      <c r="T145" s="27"/>
+      <c r="T145" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y145" s="19">
         <v>1</v>
       </c>
@@ -27393,7 +27786,9 @@
       <c r="K146" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L146" s="27"/>
+      <c r="L146" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M146" s="27"/>
       <c r="N146" s="27"/>
       <c r="O146" s="27"/>
@@ -27401,7 +27796,9 @@
       <c r="Q146" s="27"/>
       <c r="R146" s="27"/>
       <c r="S146" s="27"/>
-      <c r="T146" s="27"/>
+      <c r="T146" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="AE146" s="19">
         <v>1</v>
       </c>
@@ -27515,15 +27912,25 @@
       <c r="K147" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L147" s="27"/>
+      <c r="L147" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M147" s="27"/>
       <c r="N147" s="27"/>
-      <c r="O147" s="27"/>
-      <c r="P147" s="27"/>
-      <c r="Q147" s="27"/>
+      <c r="O147" s="27" t="s">
+        <v>936</v>
+      </c>
+      <c r="P147" s="27" t="s">
+        <v>937</v>
+      </c>
+      <c r="Q147" s="27" t="s">
+        <v>938</v>
+      </c>
       <c r="R147" s="27"/>
       <c r="S147" s="27"/>
-      <c r="T147" s="27"/>
+      <c r="T147" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AR147" s="3">
         <v>1</v>
       </c>
@@ -27604,7 +28011,9 @@
       <c r="K148" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L148" s="27"/>
+      <c r="L148" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M148" s="27"/>
       <c r="N148" s="27"/>
       <c r="O148" s="27"/>
@@ -27612,7 +28021,9 @@
       <c r="Q148" s="27"/>
       <c r="R148" s="27"/>
       <c r="S148" s="27"/>
-      <c r="T148" s="27"/>
+      <c r="T148" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="Y148" s="19">
         <v>2</v>
       </c>
@@ -27662,7 +28073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="149" spans="2:168">
+    <row r="149" spans="2:168" ht="16">
       <c r="B149" s="3" t="s">
         <v>127</v>
       </c>
@@ -27687,15 +28098,21 @@
       <c r="K149" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L149" s="27"/>
+      <c r="L149" s="30" t="s">
+        <v>939</v>
+      </c>
       <c r="M149" s="27"/>
       <c r="N149" s="27"/>
-      <c r="O149" s="27"/>
+      <c r="O149" s="27" t="s">
+        <v>940</v>
+      </c>
       <c r="P149" s="27"/>
       <c r="Q149" s="27"/>
       <c r="R149" s="27"/>
       <c r="S149" s="27"/>
-      <c r="T149" s="27"/>
+      <c r="T149" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="AZ149" s="21">
         <v>1</v>
       </c>
@@ -27748,7 +28165,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="150" spans="2:168">
+    <row r="150" spans="2:168" ht="16">
       <c r="B150" s="3" t="s">
         <v>127</v>
       </c>
@@ -27773,15 +28190,29 @@
       <c r="K150" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L150" s="27"/>
+      <c r="L150" s="30" t="s">
+        <v>941</v>
+      </c>
       <c r="M150" s="27"/>
       <c r="N150" s="27"/>
-      <c r="O150" s="27"/>
-      <c r="P150" s="27"/>
-      <c r="Q150" s="27"/>
-      <c r="R150" s="27"/>
-      <c r="S150" s="27"/>
-      <c r="T150" s="27"/>
+      <c r="O150" s="27" t="s">
+        <v>942</v>
+      </c>
+      <c r="P150" s="27" t="s">
+        <v>943</v>
+      </c>
+      <c r="Q150" s="27" t="s">
+        <v>944</v>
+      </c>
+      <c r="R150" s="27" t="s">
+        <v>945</v>
+      </c>
+      <c r="S150" s="27" t="s">
+        <v>946</v>
+      </c>
+      <c r="T150" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="U150" s="19">
         <v>1</v>
       </c>
@@ -27967,15 +28398,21 @@
       <c r="K151" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L151" s="27"/>
+      <c r="L151" s="27" t="s">
+        <v>670</v>
+      </c>
       <c r="M151" s="27"/>
       <c r="N151" s="27"/>
-      <c r="O151" s="27"/>
+      <c r="O151" s="27" t="s">
+        <v>947</v>
+      </c>
       <c r="P151" s="27"/>
       <c r="Q151" s="27"/>
       <c r="R151" s="27"/>
       <c r="S151" s="27"/>
-      <c r="T151" s="27"/>
+      <c r="T151" s="27" t="s">
+        <v>600</v>
+      </c>
       <c r="Y151" s="19">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
full texts 151 to 156 (and 147) ❃
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24140" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3140" yWindow="0" windowWidth="23760" windowHeight="11800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="986">
   <si>
     <t>f</t>
   </si>
@@ -2345,39 +2345,6 @@
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CPWKGVG302908236</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=FmZVAAAAcAAJ</t>
-    </r>
-  </si>
-  <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDYSCIO002576125</t>
   </si>
   <si>
@@ -2837,72 +2804,6 @@
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGFDZMU204246389</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=7xw5AAAAMAAJ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=Rw0UAAAAQAAJ</t>
-    </r>
-  </si>
-  <si>
     <t>http://babel.hathitrust.org/cgi/pt?id=mdp.39015033367650;view=1up;seq=9</t>
   </si>
   <si>
@@ -3012,13 +2913,82 @@
   </si>
   <si>
     <t>past - Elizabethan</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=FmZVAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=7xw5AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Rw0UAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://libsysdigi.library.uiuc.edu/OCA/Books2010-04/contrast/contrast01roch/</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CUAQSWB823242206</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=sq0TAAAAIAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t2h711v1w</t>
+  </si>
+  <si>
+    <t>http://infoweb.newsbank.com.ezproxy.library.uvic.ca/iw-search/we/Evans?p_action=doc&amp;p_theme=eai&amp;p_topdoc=1&amp;p_docnum=1&amp;p_sort=YMD_date:D&amp;p_product=SHAW&amp;p_text_direct-0=u433=(%2013512%20)|u433ad=(%2013512%20)&amp;p_nbid=G62Q50IHMTQwOTA5MzE5OS40Mjc5MzQ6MToxNToxNDIuMTA0LjI0MC4xOTQ&amp;p_docref=</t>
+  </si>
+  <si>
+    <t>http://libsysdigi.library.uiuc.edu/OCA/Books2010-04/discardedsonorha/discardedsonorha01roch/</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=yr9UAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=njp.32101064907049</t>
+  </si>
+  <si>
+    <t>http://find.galegroup.com.ezproxy.library.uvic.ca/ecco/infomark.do?contentSet=ECCOArticles&amp;docType=ECCOArticles&amp;bookId=0948000801&amp;type=getFullCitation&amp;tabID=T001&amp;prodId=ECCO&amp;docLevel=TEXT_GRAPHICS&amp;version=1.0&amp;source=library&amp;userGroupName=uvictoria</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CCPEXWU476339179</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=-q0BAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://find.galegroup.com.ezproxy.library.uvic.ca/ecco/infomark.do?contentSet=ECCOArticles&amp;docType=ECCOArticles&amp;bookId=1524500101&amp;type=getFullCitation&amp;tabID=T001&amp;prodId=ECCO&amp;docLevel=TEXT_GRAPHICS&amp;version=1.0&amp;source=library&amp;userGroupName=uvictoria</t>
+  </si>
+  <si>
+    <t>http://infoweb.newsbank.com.ezproxy.library.uvic.ca/iw-search/we/Evans?p_action=doc&amp;p_theme=eai&amp;p_topdoc=1&amp;p_docnum=1&amp;p_sort=YMD_date:D&amp;p_product=SHAW&amp;p_text_direct-0=u433=(%201263%20)|u433ad=(%201263%20)&amp;p_nbid=I6FR5DWUMTQwOTA5NDE3MC45OTI0Mzk6MToxNToxNDIuMTA0LjI0MC4xOTQ&amp;p_docref=</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CDDSFWM285653368</t>
+  </si>
+  <si>
+    <t>http://libsysdigi.library.uiuc.edu/OCA/Books2010-04/bridalofdunamore/</t>
+  </si>
+  <si>
+    <t>none T_T</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc1.b4104603</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLCGGON913764745</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=G9pUAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=JoMqAAAAMAAJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3058,23 +3028,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3202,7 +3172,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3444,8 +3414,50 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3502,10 +3514,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="283">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3626,6 +3639,27 @@
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3746,6 +3780,27 @@
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7275,113 +7330,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7507,6 +7456,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7844,10 +7899,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G177" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I133" sqref="I133"/>
+      <selection pane="bottomRight" activeCell="J190" sqref="J190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8045,13 +8100,13 @@
         <v>523</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>527</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>529</v>
@@ -11473,11 +11528,11 @@
       <c r="M28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N28" s="27" t="s">
+      <c r="N28" s="30" t="s">
         <v>669</v>
       </c>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
       <c r="Q28" s="27"/>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
@@ -11542,11 +11597,11 @@
       <c r="M29" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N29" s="27" t="s">
+      <c r="N29" s="30" t="s">
         <v>669</v>
       </c>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
       <c r="Q29" s="27" t="s">
         <v>667</v>
       </c>
@@ -11727,11 +11782,11 @@
       <c r="M30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N30" s="27" t="s">
+      <c r="N30" s="30" t="s">
         <v>669</v>
       </c>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
       <c r="Q30" s="27" t="s">
         <v>674</v>
       </c>
@@ -12014,11 +12069,11 @@
       <c r="M31" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N31" s="27" t="s">
+      <c r="N31" s="30" t="s">
         <v>669</v>
       </c>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
       <c r="Q31" s="27" t="s">
         <v>675</v>
       </c>
@@ -12166,11 +12221,11 @@
       <c r="M32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N32" s="27" t="s">
+      <c r="N32" s="32" t="s">
         <v>676</v>
       </c>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
       <c r="Q32" s="27"/>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -12375,11 +12430,11 @@
       <c r="M33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N33" s="27" t="s">
+      <c r="N33" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
       <c r="Q33" s="27"/>
       <c r="R33" s="27"/>
       <c r="S33" s="27"/>
@@ -12468,11 +12523,11 @@
       <c r="M34" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N34" s="27" t="s">
+      <c r="N34" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
       <c r="Q34" s="27"/>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -12708,11 +12763,11 @@
       <c r="M35" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="27" t="s">
+      <c r="N35" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
       <c r="Q35" s="27" t="s">
         <v>677</v>
       </c>
@@ -12815,11 +12870,11 @@
       <c r="M36" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N36" s="27" t="s">
+      <c r="N36" s="32" t="s">
         <v>678</v>
       </c>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
       <c r="Q36" s="27" t="s">
         <v>679</v>
       </c>
@@ -12953,11 +13008,11 @@
       <c r="M37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N37" s="27" t="s">
+      <c r="N37" s="32" t="s">
         <v>680</v>
       </c>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
       <c r="Q37" s="27" t="s">
         <v>681</v>
       </c>
@@ -13095,11 +13150,11 @@
       <c r="M38" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N38" s="27" t="s">
+      <c r="N38" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
       <c r="Q38" s="27" t="s">
         <v>682</v>
       </c>
@@ -13196,11 +13251,11 @@
       <c r="M39" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N39" s="27" t="s">
+      <c r="N39" s="32" t="s">
         <v>684</v>
       </c>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
       <c r="Q39" s="27" t="s">
         <v>685</v>
       </c>
@@ -13353,13 +13408,13 @@
       <c r="M40" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N40" s="27" t="s">
+      <c r="N40" s="32" t="s">
+        <v>842</v>
+      </c>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="27" t="s">
         <v>843</v>
-      </c>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27" t="s">
-        <v>844</v>
       </c>
       <c r="R40" s="27"/>
       <c r="S40" s="27"/>
@@ -13413,11 +13468,11 @@
       <c r="M41" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N41" s="27" t="s">
+      <c r="N41" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
       <c r="Q41" s="27" t="s">
         <v>705</v>
       </c>
@@ -13543,11 +13598,11 @@
       <c r="M42" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N42" s="27" t="s">
+      <c r="N42" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
       <c r="Q42" s="27" t="s">
         <v>708</v>
       </c>
@@ -13663,7 +13718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:170" ht="16">
+    <row r="43" spans="1:170">
       <c r="B43" s="3" t="s">
         <v>306</v>
       </c>
@@ -13694,11 +13749,11 @@
       <c r="M43" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N43" s="30" t="s">
+      <c r="N43" s="32" t="s">
         <v>716</v>
       </c>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
       <c r="Q43" s="27" t="s">
         <v>711</v>
       </c>
@@ -13808,7 +13863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:170" ht="16">
+    <row r="44" spans="1:170">
       <c r="B44" s="3" t="s">
         <v>304</v>
       </c>
@@ -13841,13 +13896,13 @@
       <c r="M44" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N44" s="30" t="s">
+      <c r="N44" s="32" t="s">
         <v>717</v>
       </c>
-      <c r="O44" s="30" t="s">
+      <c r="O44" s="32" t="s">
         <v>718</v>
       </c>
-      <c r="P44" s="30" t="s">
+      <c r="P44" s="32" t="s">
         <v>718</v>
       </c>
       <c r="Q44" s="27" t="s">
@@ -13992,11 +14047,11 @@
       <c r="M45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N45" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
       <c r="Q45" s="27" t="s">
         <v>723</v>
       </c>
@@ -14090,11 +14145,11 @@
       <c r="M46" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N46" s="27" t="s">
+      <c r="N46" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
       <c r="S46" s="27"/>
@@ -14204,7 +14259,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:170" ht="16">
+    <row r="47" spans="1:170">
       <c r="B47" s="3" t="s">
         <v>298</v>
       </c>
@@ -14235,11 +14290,11 @@
       <c r="M47" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N47" s="30" t="s">
+      <c r="N47" s="32" t="s">
         <v>724</v>
       </c>
-      <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
+      <c r="O47" s="32"/>
+      <c r="P47" s="32"/>
       <c r="Q47" s="27" t="s">
         <v>725</v>
       </c>
@@ -14337,11 +14392,11 @@
       <c r="M48" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N48" s="27" t="s">
+      <c r="N48" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
       <c r="Q48" s="27" t="s">
         <v>726</v>
       </c>
@@ -14525,11 +14580,11 @@
       <c r="M49" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N49" s="27" t="s">
+      <c r="N49" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O49" s="27"/>
-      <c r="P49" s="27"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
       <c r="Q49" s="27" t="s">
         <v>729</v>
       </c>
@@ -14628,7 +14683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:170" ht="16">
+    <row r="50" spans="2:170">
       <c r="B50" s="3" t="s">
         <v>290</v>
       </c>
@@ -14659,11 +14714,11 @@
       <c r="M50" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N50" s="30" t="s">
+      <c r="N50" s="32" t="s">
         <v>730</v>
       </c>
-      <c r="O50" s="27"/>
-      <c r="P50" s="27"/>
+      <c r="O50" s="32"/>
+      <c r="P50" s="32"/>
       <c r="Q50" s="27" t="s">
         <v>731</v>
       </c>
@@ -14805,7 +14860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:170" ht="16">
+    <row r="51" spans="2:170">
       <c r="B51" s="3" t="s">
         <v>290</v>
       </c>
@@ -14836,13 +14891,13 @@
       <c r="M51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N51" s="30" t="s">
+      <c r="N51" s="32" t="s">
         <v>734</v>
       </c>
-      <c r="O51" s="30" t="s">
+      <c r="O51" s="32" t="s">
         <v>735</v>
       </c>
-      <c r="P51" s="27"/>
+      <c r="P51" s="32"/>
       <c r="Q51" s="27" t="s">
         <v>736</v>
       </c>
@@ -14929,7 +14984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:170" ht="16">
+    <row r="52" spans="2:170">
       <c r="B52" s="3" t="s">
         <v>290</v>
       </c>
@@ -14960,13 +15015,13 @@
       <c r="M52" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N52" s="30" t="s">
+      <c r="N52" s="32" t="s">
         <v>740</v>
       </c>
-      <c r="O52" s="30" t="s">
+      <c r="O52" s="32" t="s">
         <v>741</v>
       </c>
-      <c r="P52" s="30" t="s">
+      <c r="P52" s="32" t="s">
         <v>742</v>
       </c>
       <c r="Q52" s="27" t="s">
@@ -15070,11 +15125,11 @@
       <c r="M53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N53" s="27" t="s">
+      <c r="N53" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O53" s="27"/>
-      <c r="P53" s="27"/>
+      <c r="O53" s="32"/>
+      <c r="P53" s="32"/>
       <c r="Q53" s="27"/>
       <c r="R53" s="27"/>
       <c r="S53" s="27"/>
@@ -15175,11 +15230,11 @@
       <c r="M54" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N54" s="27" t="s">
+      <c r="N54" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O54" s="27"/>
-      <c r="P54" s="27"/>
+      <c r="O54" s="32"/>
+      <c r="P54" s="32"/>
       <c r="Q54" s="27" t="s">
         <v>745</v>
       </c>
@@ -15303,11 +15358,11 @@
       <c r="M55" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N55" s="27" t="s">
+      <c r="N55" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O55" s="27"/>
-      <c r="P55" s="27"/>
+      <c r="O55" s="32"/>
+      <c r="P55" s="32"/>
       <c r="Q55" s="27" t="s">
         <v>746</v>
       </c>
@@ -15439,11 +15494,11 @@
       <c r="M56" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="27" t="s">
+      <c r="N56" s="32" t="s">
         <v>747</v>
       </c>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="32"/>
       <c r="Q56" s="27" t="s">
         <v>748</v>
       </c>
@@ -15549,11 +15604,11 @@
       <c r="M57" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N57" s="27" t="s">
+      <c r="N57" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O57" s="27"/>
-      <c r="P57" s="27"/>
+      <c r="O57" s="32"/>
+      <c r="P57" s="32"/>
       <c r="Q57" s="27"/>
       <c r="R57" s="27"/>
       <c r="S57" s="27"/>
@@ -15656,7 +15711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:170" ht="16">
+    <row r="58" spans="2:170">
       <c r="B58" s="3" t="s">
         <v>282</v>
       </c>
@@ -15689,11 +15744,11 @@
       <c r="M58" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N58" s="30" t="s">
+      <c r="N58" s="32" t="s">
         <v>750</v>
       </c>
-      <c r="O58" s="27"/>
-      <c r="P58" s="27"/>
+      <c r="O58" s="32"/>
+      <c r="P58" s="32"/>
       <c r="Q58" s="27"/>
       <c r="R58" s="27"/>
       <c r="S58" s="27"/>
@@ -15818,11 +15873,11 @@
       <c r="M59" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N59" s="27" t="s">
+      <c r="N59" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O59" s="27"/>
-      <c r="P59" s="27"/>
+      <c r="O59" s="32"/>
+      <c r="P59" s="32"/>
       <c r="Q59" s="27" t="s">
         <v>751</v>
       </c>
@@ -15876,7 +15931,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="2:170" ht="16">
+    <row r="60" spans="2:170">
       <c r="B60" s="3" t="s">
         <v>279</v>
       </c>
@@ -15907,11 +15962,11 @@
       <c r="M60" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N60" s="30" t="s">
+      <c r="N60" s="32" t="s">
         <v>753</v>
       </c>
-      <c r="O60" s="27"/>
-      <c r="P60" s="27"/>
+      <c r="O60" s="32"/>
+      <c r="P60" s="32"/>
       <c r="Q60" s="27" t="s">
         <v>754</v>
       </c>
@@ -16037,7 +16092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:170" ht="16">
+    <row r="61" spans="2:170">
       <c r="B61" s="3" t="s">
         <v>276</v>
       </c>
@@ -16068,11 +16123,11 @@
       <c r="M61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N61" s="30" t="s">
+      <c r="N61" s="32" t="s">
         <v>755</v>
       </c>
-      <c r="O61" s="27"/>
-      <c r="P61" s="27"/>
+      <c r="O61" s="32"/>
+      <c r="P61" s="32"/>
       <c r="Q61" s="27" t="s">
         <v>756</v>
       </c>
@@ -16174,7 +16229,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="2:170" ht="16">
+    <row r="62" spans="2:170">
       <c r="B62" s="3" t="s">
         <v>276</v>
       </c>
@@ -16205,11 +16260,11 @@
       <c r="M62" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N62" s="30" t="s">
+      <c r="N62" s="32" t="s">
         <v>757</v>
       </c>
-      <c r="O62" s="27"/>
-      <c r="P62" s="27"/>
+      <c r="O62" s="32"/>
+      <c r="P62" s="32"/>
       <c r="Q62" s="27" t="s">
         <v>758</v>
       </c>
@@ -16323,7 +16378,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="2:170" ht="16">
+    <row r="63" spans="2:170">
       <c r="B63" s="3" t="s">
         <v>274</v>
       </c>
@@ -16356,11 +16411,11 @@
       <c r="M63" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N63" s="30" t="s">
+      <c r="N63" s="32" t="s">
         <v>759</v>
       </c>
-      <c r="O63" s="27"/>
-      <c r="P63" s="27"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
       <c r="Q63" s="27"/>
       <c r="R63" s="27"/>
       <c r="S63" s="27"/>
@@ -16539,11 +16594,11 @@
       <c r="M64" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="27" t="s">
+      <c r="N64" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O64" s="27"/>
-      <c r="P64" s="27"/>
+      <c r="O64" s="32"/>
+      <c r="P64" s="32"/>
       <c r="Q64" s="27" t="s">
         <v>760</v>
       </c>
@@ -16594,7 +16649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:170" ht="16">
+    <row r="65" spans="2:170">
       <c r="B65" s="3" t="s">
         <v>270</v>
       </c>
@@ -16625,11 +16680,11 @@
       <c r="M65" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N65" s="30" t="s">
+      <c r="N65" s="32" t="s">
         <v>761</v>
       </c>
-      <c r="O65" s="27"/>
-      <c r="P65" s="27"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
       <c r="Q65" s="27" t="s">
         <v>762</v>
       </c>
@@ -16834,11 +16889,11 @@
       <c r="M66" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N66" s="27" t="s">
+      <c r="N66" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O66" s="27"/>
-      <c r="P66" s="27"/>
+      <c r="O66" s="32"/>
+      <c r="P66" s="32"/>
       <c r="Q66" s="27" t="s">
         <v>766</v>
       </c>
@@ -16966,7 +17021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:170" ht="16">
+    <row r="67" spans="2:170">
       <c r="B67" s="3" t="s">
         <v>267</v>
       </c>
@@ -16997,11 +17052,11 @@
       <c r="M67" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N67" s="30" t="s">
+      <c r="N67" s="32" t="s">
         <v>768</v>
       </c>
-      <c r="O67" s="27"/>
-      <c r="P67" s="27"/>
+      <c r="O67" s="32"/>
+      <c r="P67" s="32"/>
       <c r="Q67" s="27" t="s">
         <v>769</v>
       </c>
@@ -17112,7 +17167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:170" ht="16">
+    <row r="68" spans="2:170">
       <c r="B68" s="3" t="s">
         <v>267</v>
       </c>
@@ -17145,11 +17200,11 @@
       <c r="M68" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N68" s="30" t="s">
+      <c r="N68" s="32" t="s">
         <v>771</v>
       </c>
-      <c r="O68" s="27"/>
-      <c r="P68" s="27"/>
+      <c r="O68" s="32"/>
+      <c r="P68" s="32"/>
       <c r="Q68" s="27" t="s">
         <v>772</v>
       </c>
@@ -17203,7 +17258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:170" ht="16">
+    <row r="69" spans="2:170">
       <c r="B69" s="3" t="s">
         <v>264</v>
       </c>
@@ -17236,16 +17291,16 @@
       <c r="M69" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N69" s="31" t="s">
+      <c r="N69" s="32" t="s">
+        <v>963</v>
+      </c>
+      <c r="O69" s="32"/>
+      <c r="P69" s="32"/>
+      <c r="Q69" s="27" t="s">
         <v>773</v>
       </c>
-      <c r="O69" s="27"/>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="27" t="s">
+      <c r="R69" s="27" t="s">
         <v>774</v>
-      </c>
-      <c r="R69" s="27" t="s">
-        <v>775</v>
       </c>
       <c r="S69" s="27"/>
       <c r="T69" s="27"/>
@@ -17356,16 +17411,16 @@
       <c r="M70" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N70" s="27" t="s">
+      <c r="N70" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O70" s="27"/>
-      <c r="P70" s="27"/>
+      <c r="O70" s="32"/>
+      <c r="P70" s="32"/>
       <c r="Q70" s="27" t="s">
+        <v>775</v>
+      </c>
+      <c r="R70" s="27" t="s">
         <v>776</v>
-      </c>
-      <c r="R70" s="27" t="s">
-        <v>777</v>
       </c>
       <c r="S70" s="27"/>
       <c r="T70" s="27"/>
@@ -17473,7 +17528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:170" ht="16">
+    <row r="71" spans="2:170">
       <c r="B71" s="3" t="s">
         <v>258</v>
       </c>
@@ -17506,13 +17561,13 @@
       <c r="M71" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N71" s="30" t="s">
+      <c r="N71" s="32" t="s">
+        <v>777</v>
+      </c>
+      <c r="O71" s="32"/>
+      <c r="P71" s="32"/>
+      <c r="Q71" s="27" t="s">
         <v>778</v>
-      </c>
-      <c r="O71" s="27"/>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="27" t="s">
-        <v>779</v>
       </c>
       <c r="R71" s="27"/>
       <c r="S71" s="27"/>
@@ -17711,18 +17766,18 @@
       <c r="M72" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N72" s="27" t="s">
+      <c r="N72" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O72" s="27"/>
-      <c r="P72" s="27"/>
+      <c r="O72" s="32"/>
+      <c r="P72" s="32"/>
       <c r="Q72" s="27"/>
       <c r="R72" s="27"/>
       <c r="S72" s="27"/>
       <c r="T72" s="27"/>
       <c r="U72" s="27"/>
       <c r="V72" s="27" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AA72" s="19">
         <v>1</v>
@@ -17866,7 +17921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:170" ht="16">
+    <row r="73" spans="2:170">
       <c r="B73" s="3" t="s">
         <v>258</v>
       </c>
@@ -17899,19 +17954,19 @@
       <c r="M73" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N73" s="30" t="s">
+      <c r="N73" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="O73" s="32"/>
+      <c r="P73" s="32"/>
+      <c r="Q73" s="27" t="s">
         <v>781</v>
       </c>
-      <c r="O73" s="27"/>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="27" t="s">
+      <c r="R73" s="27" t="s">
         <v>782</v>
       </c>
-      <c r="R73" s="27" t="s">
+      <c r="S73" s="27" t="s">
         <v>783</v>
-      </c>
-      <c r="S73" s="27" t="s">
-        <v>784</v>
       </c>
       <c r="T73" s="27"/>
       <c r="U73" s="27"/>
@@ -17970,13 +18025,13 @@
       <c r="M74" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N74" s="27" t="s">
+      <c r="N74" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O74" s="27"/>
-      <c r="P74" s="27"/>
+      <c r="O74" s="32"/>
+      <c r="P74" s="32"/>
       <c r="Q74" s="27" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="R74" s="27"/>
       <c r="S74" s="27"/>
@@ -18070,16 +18125,16 @@
       <c r="M75" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N75" s="27" t="s">
+      <c r="N75" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O75" s="27"/>
-      <c r="P75" s="27"/>
+      <c r="O75" s="32"/>
+      <c r="P75" s="32"/>
       <c r="Q75" s="27" t="s">
+        <v>785</v>
+      </c>
+      <c r="R75" s="27" t="s">
         <v>786</v>
-      </c>
-      <c r="R75" s="27" t="s">
-        <v>787</v>
       </c>
       <c r="S75" s="27"/>
       <c r="T75" s="27"/>
@@ -18262,13 +18317,13 @@
       <c r="M76" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N76" s="27" t="s">
+      <c r="N76" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O76" s="27"/>
-      <c r="P76" s="27"/>
+      <c r="O76" s="32"/>
+      <c r="P76" s="32"/>
       <c r="Q76" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="R76" s="27"/>
       <c r="S76" s="27"/>
@@ -18474,18 +18529,18 @@
       <c r="M77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N77" s="27" t="s">
+      <c r="N77" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O77" s="27"/>
-      <c r="P77" s="27"/>
+      <c r="O77" s="32"/>
+      <c r="P77" s="32"/>
       <c r="Q77" s="27"/>
       <c r="R77" s="27"/>
       <c r="S77" s="27"/>
       <c r="T77" s="27"/>
       <c r="U77" s="27"/>
       <c r="V77" s="27" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="AA77" s="19">
         <v>1</v>
@@ -18644,7 +18699,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="2:170" ht="16">
+    <row r="78" spans="2:170">
       <c r="B78" s="3" t="s">
         <v>251</v>
       </c>
@@ -18675,13 +18730,13 @@
       <c r="M78" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N78" s="30" t="s">
+      <c r="N78" s="32" t="s">
+        <v>789</v>
+      </c>
+      <c r="O78" s="32"/>
+      <c r="P78" s="32"/>
+      <c r="Q78" s="27" t="s">
         <v>790</v>
-      </c>
-      <c r="O78" s="27"/>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="27" t="s">
-        <v>791</v>
       </c>
       <c r="R78" s="27"/>
       <c r="S78" s="27"/>
@@ -18770,7 +18825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:170" ht="16">
+    <row r="79" spans="2:170">
       <c r="B79" s="3" t="s">
         <v>249</v>
       </c>
@@ -18803,13 +18858,13 @@
       <c r="M79" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N79" s="30" t="s">
+      <c r="N79" s="32" t="s">
+        <v>791</v>
+      </c>
+      <c r="O79" s="32"/>
+      <c r="P79" s="32"/>
+      <c r="Q79" s="27" t="s">
         <v>792</v>
-      </c>
-      <c r="O79" s="27"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="27" t="s">
-        <v>793</v>
       </c>
       <c r="R79" s="27"/>
       <c r="S79" s="27"/>
@@ -18946,13 +19001,13 @@
       <c r="M80" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N80" s="27" t="s">
+      <c r="N80" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O80" s="27"/>
-      <c r="P80" s="27"/>
+      <c r="O80" s="32"/>
+      <c r="P80" s="32"/>
       <c r="Q80" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="R80" s="27"/>
       <c r="S80" s="27"/>
@@ -19041,16 +19096,16 @@
       <c r="M81" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N81" s="27" t="s">
+      <c r="N81" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O81" s="27"/>
-      <c r="P81" s="27"/>
+      <c r="O81" s="32"/>
+      <c r="P81" s="32"/>
       <c r="Q81" s="27" t="s">
+        <v>794</v>
+      </c>
+      <c r="R81" s="27" t="s">
         <v>795</v>
-      </c>
-      <c r="R81" s="27" t="s">
-        <v>796</v>
       </c>
       <c r="S81" s="27"/>
       <c r="T81" s="27"/>
@@ -19188,18 +19243,18 @@
       <c r="M82" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N82" s="27" t="s">
+      <c r="N82" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O82" s="27"/>
-      <c r="P82" s="27"/>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
       <c r="Q82" s="27"/>
       <c r="R82" s="27"/>
       <c r="S82" s="27"/>
       <c r="T82" s="27"/>
       <c r="U82" s="27"/>
       <c r="V82" s="27" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="AO82" s="21">
         <v>1</v>
@@ -19256,7 +19311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:170" ht="16">
+    <row r="83" spans="1:170">
       <c r="B83" s="3" t="s">
         <v>240</v>
       </c>
@@ -19289,16 +19344,16 @@
       <c r="M83" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N83" s="30" t="s">
+      <c r="N83" s="32" t="s">
+        <v>797</v>
+      </c>
+      <c r="O83" s="32"/>
+      <c r="P83" s="32"/>
+      <c r="Q83" s="27" t="s">
         <v>798</v>
       </c>
-      <c r="O83" s="27"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="27" t="s">
+      <c r="R83" s="27" t="s">
         <v>799</v>
-      </c>
-      <c r="R83" s="27" t="s">
-        <v>800</v>
       </c>
       <c r="S83" s="27"/>
       <c r="T83" s="27"/>
@@ -19397,7 +19452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:170" ht="16">
+    <row r="84" spans="1:170">
       <c r="B84" s="3" t="s">
         <v>240</v>
       </c>
@@ -19428,13 +19483,13 @@
       <c r="M84" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N84" s="30" t="s">
+      <c r="N84" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="O84" s="32"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="27" t="s">
         <v>801</v>
-      </c>
-      <c r="O84" s="27"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27" t="s">
-        <v>802</v>
       </c>
       <c r="R84" s="27"/>
       <c r="S84" s="27"/>
@@ -19598,7 +19653,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:170" ht="16">
+    <row r="85" spans="1:170">
       <c r="B85" s="3" t="s">
         <v>240</v>
       </c>
@@ -19631,16 +19686,16 @@
       <c r="M85" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N85" s="30" t="s">
+      <c r="N85" s="32" t="s">
+        <v>802</v>
+      </c>
+      <c r="O85" s="32"/>
+      <c r="P85" s="32"/>
+      <c r="Q85" s="27" t="s">
         <v>803</v>
       </c>
-      <c r="O85" s="27"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="27" t="s">
+      <c r="R85" s="27" t="s">
         <v>804</v>
-      </c>
-      <c r="R85" s="27" t="s">
-        <v>805</v>
       </c>
       <c r="S85" s="27"/>
       <c r="T85" s="27"/>
@@ -19716,18 +19771,18 @@
       <c r="M86" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N86" s="27" t="s">
+      <c r="N86" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O86" s="27"/>
-      <c r="P86" s="27"/>
+      <c r="O86" s="32"/>
+      <c r="P86" s="32"/>
       <c r="Q86" s="27"/>
       <c r="R86" s="27"/>
       <c r="S86" s="27"/>
       <c r="T86" s="27"/>
       <c r="U86" s="27"/>
       <c r="V86" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="AA86" s="19">
         <v>1</v>
@@ -19886,13 +19941,13 @@
       <c r="M87" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N87" s="27" t="s">
+      <c r="N87" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O87" s="27"/>
-      <c r="P87" s="27"/>
+      <c r="O87" s="32"/>
+      <c r="P87" s="32"/>
       <c r="Q87" s="27" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="R87" s="27"/>
       <c r="S87" s="27"/>
@@ -20076,18 +20131,18 @@
       <c r="M88" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N88" s="27" t="s">
+      <c r="N88" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
+      <c r="O88" s="32"/>
+      <c r="P88" s="32"/>
       <c r="Q88" s="27"/>
       <c r="R88" s="27"/>
       <c r="S88" s="27"/>
       <c r="T88" s="27"/>
       <c r="U88" s="27"/>
       <c r="V88" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="AA88" s="19">
         <v>1</v>
@@ -20198,7 +20253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:170" ht="16">
+    <row r="89" spans="1:170">
       <c r="B89" s="3" t="s">
         <v>233</v>
       </c>
@@ -20231,16 +20286,16 @@
       <c r="M89" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N89" s="30" t="s">
+      <c r="N89" s="32" t="s">
+        <v>808</v>
+      </c>
+      <c r="O89" s="32"/>
+      <c r="P89" s="32"/>
+      <c r="Q89" s="27" t="s">
         <v>809</v>
       </c>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="27" t="s">
+      <c r="R89" s="27" t="s">
         <v>810</v>
-      </c>
-      <c r="R89" s="27" t="s">
-        <v>811</v>
       </c>
       <c r="S89" s="27"/>
       <c r="T89" s="27"/>
@@ -20379,13 +20434,13 @@
       <c r="M90" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N90" s="27" t="s">
+      <c r="N90" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O90" s="27"/>
-      <c r="P90" s="27"/>
+      <c r="O90" s="32"/>
+      <c r="P90" s="32"/>
       <c r="Q90" s="27" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="R90" s="27"/>
       <c r="S90" s="27"/>
@@ -20443,7 +20498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:170" ht="16">
+    <row r="91" spans="1:170">
       <c r="B91" s="3" t="s">
         <v>233</v>
       </c>
@@ -20476,15 +20531,15 @@
       <c r="M91" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N91" s="30" t="s">
+      <c r="N91" s="32" t="s">
+        <v>812</v>
+      </c>
+      <c r="O91" s="32" t="s">
         <v>813</v>
       </c>
-      <c r="O91" s="30" t="s">
+      <c r="P91" s="32"/>
+      <c r="Q91" s="27" t="s">
         <v>814</v>
-      </c>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="27" t="s">
-        <v>815</v>
       </c>
       <c r="R91" s="27"/>
       <c r="S91" s="27"/>
@@ -20611,7 +20666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:170" ht="16">
+    <row r="92" spans="1:170">
       <c r="B92" s="3" t="s">
         <v>231</v>
       </c>
@@ -20642,13 +20697,13 @@
       <c r="M92" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N92" s="30" t="s">
+      <c r="N92" s="32" t="s">
+        <v>815</v>
+      </c>
+      <c r="O92" s="32"/>
+      <c r="P92" s="32"/>
+      <c r="Q92" s="27" t="s">
         <v>816</v>
-      </c>
-      <c r="O92" s="27"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="27" t="s">
-        <v>817</v>
       </c>
       <c r="R92" s="27"/>
       <c r="S92" s="27"/>
@@ -20715,7 +20770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:170" ht="16">
+    <row r="93" spans="1:170">
       <c r="A93" s="3" t="s">
         <v>229</v>
       </c>
@@ -20751,17 +20806,17 @@
       <c r="M93" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N93" s="30" t="s">
+      <c r="N93" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="O93" s="32" t="s">
         <v>818</v>
       </c>
-      <c r="O93" s="30" t="s">
+      <c r="P93" s="32" t="s">
         <v>819</v>
       </c>
-      <c r="P93" s="30" t="s">
+      <c r="Q93" s="27" t="s">
         <v>820</v>
-      </c>
-      <c r="Q93" s="27" t="s">
-        <v>821</v>
       </c>
       <c r="R93" s="27"/>
       <c r="S93" s="27"/>
@@ -20922,18 +20977,18 @@
       <c r="M94" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N94" s="27" t="s">
+      <c r="N94" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O94" s="27"/>
-      <c r="P94" s="27"/>
+      <c r="O94" s="32"/>
+      <c r="P94" s="32"/>
       <c r="Q94" s="27"/>
       <c r="R94" s="27"/>
       <c r="S94" s="27"/>
       <c r="T94" s="27"/>
       <c r="U94" s="27"/>
       <c r="V94" s="27" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="AA94" s="19">
         <v>1</v>
@@ -21017,13 +21072,13 @@
       <c r="M95" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N95" s="27" t="s">
+      <c r="N95" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O95" s="27"/>
-      <c r="P95" s="27"/>
+      <c r="O95" s="32"/>
+      <c r="P95" s="32"/>
       <c r="Q95" s="27" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="R95" s="27"/>
       <c r="S95" s="27"/>
@@ -21069,7 +21124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:170" ht="16">
+    <row r="96" spans="1:170">
       <c r="B96" s="3" t="s">
         <v>221</v>
       </c>
@@ -21102,13 +21157,13 @@
       <c r="M96" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N96" s="30" t="s">
+      <c r="N96" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="O96" s="32"/>
+      <c r="P96" s="32"/>
+      <c r="Q96" s="27" t="s">
         <v>824</v>
-      </c>
-      <c r="O96" s="27"/>
-      <c r="P96" s="27"/>
-      <c r="Q96" s="27" t="s">
-        <v>825</v>
       </c>
       <c r="R96" s="27"/>
       <c r="S96" s="27"/>
@@ -21247,7 +21302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:170" ht="16">
+    <row r="97" spans="1:170">
       <c r="B97" s="3" t="s">
         <v>209</v>
       </c>
@@ -21280,13 +21335,13 @@
       <c r="M97" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N97" s="30" t="s">
+      <c r="N97" s="32" t="s">
+        <v>825</v>
+      </c>
+      <c r="O97" s="32"/>
+      <c r="P97" s="32"/>
+      <c r="Q97" s="27" t="s">
         <v>826</v>
-      </c>
-      <c r="O97" s="27"/>
-      <c r="P97" s="27"/>
-      <c r="Q97" s="27" t="s">
-        <v>827</v>
       </c>
       <c r="R97" s="27"/>
       <c r="S97" s="27"/>
@@ -21323,7 +21378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:170" ht="16">
+    <row r="98" spans="1:170">
       <c r="B98" s="3" t="s">
         <v>209</v>
       </c>
@@ -21356,19 +21411,19 @@
       <c r="M98" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N98" s="30" t="s">
+      <c r="N98" s="32" t="s">
+        <v>827</v>
+      </c>
+      <c r="O98" s="32"/>
+      <c r="P98" s="32"/>
+      <c r="Q98" s="27" t="s">
         <v>828</v>
       </c>
-      <c r="O98" s="27"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="27" t="s">
+      <c r="R98" s="27" t="s">
         <v>829</v>
       </c>
-      <c r="R98" s="27" t="s">
+      <c r="S98" s="27" t="s">
         <v>830</v>
-      </c>
-      <c r="S98" s="27" t="s">
-        <v>831</v>
       </c>
       <c r="T98" s="27"/>
       <c r="U98" s="27"/>
@@ -21535,7 +21590,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:170" ht="16">
+    <row r="99" spans="1:170">
       <c r="B99" s="3" t="s">
         <v>209</v>
       </c>
@@ -21568,13 +21623,13 @@
       <c r="M99" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N99" s="30" t="s">
+      <c r="N99" s="32" t="s">
+        <v>831</v>
+      </c>
+      <c r="O99" s="32"/>
+      <c r="P99" s="32"/>
+      <c r="Q99" s="27" t="s">
         <v>832</v>
-      </c>
-      <c r="O99" s="27"/>
-      <c r="P99" s="27"/>
-      <c r="Q99" s="27" t="s">
-        <v>833</v>
       </c>
       <c r="R99" s="27"/>
       <c r="S99" s="27"/>
@@ -21635,7 +21690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:170" ht="16">
+    <row r="100" spans="1:170">
       <c r="B100" s="3" t="s">
         <v>209</v>
       </c>
@@ -21668,21 +21723,21 @@
       <c r="M100" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N100" s="30" t="s">
+      <c r="N100" s="32" t="s">
+        <v>833</v>
+      </c>
+      <c r="O100" s="32" t="s">
         <v>834</v>
       </c>
-      <c r="O100" s="30" t="s">
+      <c r="P100" s="32"/>
+      <c r="Q100" s="27" t="s">
         <v>835</v>
       </c>
-      <c r="P100" s="27"/>
-      <c r="Q100" s="27" t="s">
+      <c r="R100" s="27" t="s">
         <v>836</v>
       </c>
-      <c r="R100" s="27" t="s">
+      <c r="S100" s="27" t="s">
         <v>837</v>
-      </c>
-      <c r="S100" s="27" t="s">
-        <v>838</v>
       </c>
       <c r="T100" s="27"/>
       <c r="U100" s="27"/>
@@ -21912,7 +21967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:170" ht="16">
+    <row r="101" spans="1:170">
       <c r="B101" s="3" t="s">
         <v>209</v>
       </c>
@@ -21945,19 +22000,19 @@
       <c r="M101" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N101" s="30" t="s">
+      <c r="N101" s="32" t="s">
+        <v>838</v>
+      </c>
+      <c r="O101" s="32"/>
+      <c r="P101" s="32"/>
+      <c r="Q101" s="27" t="s">
         <v>839</v>
       </c>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="27" t="s">
+      <c r="R101" s="27" t="s">
         <v>840</v>
       </c>
-      <c r="R101" s="27" t="s">
+      <c r="S101" s="27" t="s">
         <v>841</v>
-      </c>
-      <c r="S101" s="27" t="s">
-        <v>842</v>
       </c>
       <c r="T101" s="27"/>
       <c r="U101" s="27"/>
@@ -22121,18 +22176,18 @@
       <c r="M102" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N102" s="27" t="s">
+      <c r="N102" s="32" t="s">
+        <v>844</v>
+      </c>
+      <c r="O102" s="32" t="s">
         <v>845</v>
       </c>
-      <c r="O102" s="27" t="s">
+      <c r="P102" s="32"/>
+      <c r="Q102" s="27" t="s">
         <v>846</v>
       </c>
-      <c r="P102" s="27"/>
-      <c r="Q102" s="27" t="s">
+      <c r="R102" s="27" t="s">
         <v>847</v>
-      </c>
-      <c r="R102" s="27" t="s">
-        <v>848</v>
       </c>
       <c r="S102" s="27"/>
       <c r="T102" s="27"/>
@@ -22247,11 +22302,11 @@
       <c r="M103" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N103" s="27" t="s">
-        <v>849</v>
-      </c>
-      <c r="O103" s="27"/>
-      <c r="P103" s="27"/>
+      <c r="N103" s="32" t="s">
+        <v>848</v>
+      </c>
+      <c r="O103" s="32"/>
+      <c r="P103" s="32"/>
       <c r="Q103" s="27"/>
       <c r="R103" s="27"/>
       <c r="S103" s="27"/>
@@ -22333,13 +22388,13 @@
       <c r="M104" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N104" s="27" t="s">
+      <c r="N104" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O104" s="27"/>
-      <c r="P104" s="27"/>
+      <c r="O104" s="32"/>
+      <c r="P104" s="32"/>
       <c r="Q104" s="27" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="R104" s="27"/>
       <c r="S104" s="27"/>
@@ -22364,7 +22419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:170" ht="16">
+    <row r="105" spans="1:170">
       <c r="B105" s="3" t="s">
         <v>206</v>
       </c>
@@ -22397,18 +22452,18 @@
       <c r="M105" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N105" s="30" t="s">
+      <c r="N105" s="32" t="s">
+        <v>850</v>
+      </c>
+      <c r="O105" s="32" t="s">
         <v>851</v>
       </c>
-      <c r="O105" s="30" t="s">
+      <c r="P105" s="32"/>
+      <c r="Q105" s="27" t="s">
         <v>852</v>
       </c>
-      <c r="P105" s="27"/>
-      <c r="Q105" s="27" t="s">
+      <c r="R105" s="27" t="s">
         <v>853</v>
-      </c>
-      <c r="R105" s="27" t="s">
-        <v>854</v>
       </c>
       <c r="S105" s="27"/>
       <c r="T105" s="27"/>
@@ -22516,11 +22571,11 @@
       <c r="M106" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N106" s="27" t="s">
+      <c r="N106" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O106" s="27"/>
-      <c r="P106" s="27"/>
+      <c r="O106" s="32"/>
+      <c r="P106" s="32"/>
       <c r="Q106" s="27"/>
       <c r="R106" s="27"/>
       <c r="S106" s="27"/>
@@ -22597,11 +22652,11 @@
       <c r="M107" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N107" s="27" t="s">
+      <c r="N107" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O107" s="27"/>
-      <c r="P107" s="27"/>
+      <c r="O107" s="32"/>
+      <c r="P107" s="32"/>
       <c r="Q107" s="27"/>
       <c r="R107" s="27"/>
       <c r="S107" s="27"/>
@@ -22674,7 +22729,7 @@
       </c>
       <c r="FH107" s="23"/>
     </row>
-    <row r="108" spans="1:170" ht="16">
+    <row r="108" spans="1:170">
       <c r="B108" s="3" t="s">
         <v>196</v>
       </c>
@@ -22707,19 +22762,19 @@
       <c r="M108" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N108" s="30" t="s">
+      <c r="N108" s="32" t="s">
+        <v>854</v>
+      </c>
+      <c r="O108" s="32"/>
+      <c r="P108" s="32"/>
+      <c r="Q108" s="27" t="s">
         <v>855</v>
       </c>
-      <c r="O108" s="27"/>
-      <c r="P108" s="27"/>
-      <c r="Q108" s="27" t="s">
+      <c r="R108" s="27" t="s">
         <v>856</v>
       </c>
-      <c r="R108" s="27" t="s">
+      <c r="S108" s="27" t="s">
         <v>857</v>
-      </c>
-      <c r="S108" s="27" t="s">
-        <v>858</v>
       </c>
       <c r="T108" s="27"/>
       <c r="U108" s="27"/>
@@ -22888,13 +22943,13 @@
       <c r="M109" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N109" s="27" t="s">
+      <c r="N109" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O109" s="27"/>
-      <c r="P109" s="27"/>
+      <c r="O109" s="32"/>
+      <c r="P109" s="32"/>
       <c r="Q109" s="27" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="R109" s="27"/>
       <c r="S109" s="27"/>
@@ -23084,13 +23139,13 @@
       <c r="M110" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N110" s="27" t="s">
+      <c r="N110" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O110" s="27"/>
-      <c r="P110" s="27"/>
+      <c r="O110" s="32"/>
+      <c r="P110" s="32"/>
       <c r="Q110" s="27" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="R110" s="27"/>
       <c r="S110" s="27"/>
@@ -23265,7 +23320,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:170" ht="16">
+    <row r="111" spans="1:170">
       <c r="B111" s="3" t="s">
         <v>196</v>
       </c>
@@ -23296,16 +23351,16 @@
       <c r="M111" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N111" s="30" t="s">
+      <c r="N111" s="32" t="s">
+        <v>860</v>
+      </c>
+      <c r="O111" s="32"/>
+      <c r="P111" s="32"/>
+      <c r="Q111" s="27" t="s">
+        <v>862</v>
+      </c>
+      <c r="R111" s="27" t="s">
         <v>861</v>
-      </c>
-      <c r="O111" s="27"/>
-      <c r="P111" s="27"/>
-      <c r="Q111" s="27" t="s">
-        <v>863</v>
-      </c>
-      <c r="R111" s="27" t="s">
-        <v>862</v>
       </c>
       <c r="S111" s="27"/>
       <c r="T111" s="27"/>
@@ -23345,7 +23400,7 @@
       </c>
       <c r="FH111" s="23"/>
     </row>
-    <row r="112" spans="1:170" ht="16">
+    <row r="112" spans="1:170">
       <c r="B112" s="3" t="s">
         <v>196</v>
       </c>
@@ -23378,13 +23433,13 @@
       <c r="M112" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N112" s="30" t="s">
+      <c r="N112" s="32" t="s">
+        <v>863</v>
+      </c>
+      <c r="O112" s="32"/>
+      <c r="P112" s="32"/>
+      <c r="Q112" s="27" t="s">
         <v>864</v>
-      </c>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
-      <c r="Q112" s="27" t="s">
-        <v>865</v>
       </c>
       <c r="R112" s="27"/>
       <c r="S112" s="27"/>
@@ -23511,11 +23566,11 @@
       <c r="M113" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N113" s="27" t="s">
+      <c r="N113" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O113" s="27"/>
-      <c r="P113" s="27"/>
+      <c r="O113" s="32"/>
+      <c r="P113" s="32"/>
       <c r="Q113" s="27"/>
       <c r="R113" s="27"/>
       <c r="S113" s="27"/>
@@ -23669,13 +23724,13 @@
       <c r="M114" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N114" s="27" t="s">
+      <c r="N114" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O114" s="27"/>
-      <c r="P114" s="27"/>
+      <c r="O114" s="32"/>
+      <c r="P114" s="32"/>
       <c r="Q114" s="27" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="R114" s="27"/>
       <c r="S114" s="27"/>
@@ -23769,13 +23824,13 @@
       <c r="M115" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N115" s="27" t="s">
+      <c r="N115" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O115" s="27"/>
-      <c r="P115" s="27"/>
+      <c r="O115" s="32"/>
+      <c r="P115" s="32"/>
       <c r="Q115" s="27" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="R115" s="27"/>
       <c r="S115" s="27"/>
@@ -23917,13 +23972,13 @@
       <c r="M116" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N116" s="27" t="s">
+      <c r="N116" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O116" s="27"/>
-      <c r="P116" s="27"/>
+      <c r="O116" s="32"/>
+      <c r="P116" s="32"/>
       <c r="Q116" s="27" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="R116" s="27"/>
       <c r="S116" s="27"/>
@@ -23997,11 +24052,11 @@
       <c r="M117" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N117" s="27" t="s">
+      <c r="N117" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O117" s="27"/>
-      <c r="P117" s="27"/>
+      <c r="O117" s="32"/>
+      <c r="P117" s="32"/>
       <c r="Q117" s="27"/>
       <c r="R117" s="27"/>
       <c r="S117" s="27"/>
@@ -24101,7 +24156,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="118" spans="2:170" ht="16">
+    <row r="118" spans="2:170">
       <c r="B118" s="3" t="s">
         <v>186</v>
       </c>
@@ -24134,11 +24189,11 @@
       <c r="M118" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N118" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="O118" s="27"/>
-      <c r="P118" s="27"/>
+      <c r="N118" s="32" t="s">
+        <v>868</v>
+      </c>
+      <c r="O118" s="32"/>
+      <c r="P118" s="32"/>
       <c r="Q118" s="27"/>
       <c r="R118" s="27"/>
       <c r="S118" s="27"/>
@@ -24247,16 +24302,16 @@
       <c r="M119" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N119" s="27" t="s">
+      <c r="N119" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O119" s="27"/>
-      <c r="P119" s="27"/>
+      <c r="O119" s="32"/>
+      <c r="P119" s="32"/>
       <c r="Q119" s="27" t="s">
+        <v>869</v>
+      </c>
+      <c r="R119" s="27" t="s">
         <v>870</v>
-      </c>
-      <c r="R119" s="27" t="s">
-        <v>871</v>
       </c>
       <c r="S119" s="27"/>
       <c r="T119" s="27"/>
@@ -24374,13 +24429,13 @@
       <c r="M120" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N120" s="27" t="s">
+      <c r="N120" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O120" s="27"/>
-      <c r="P120" s="27"/>
+      <c r="O120" s="32"/>
+      <c r="P120" s="32"/>
       <c r="Q120" s="27" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="R120" s="27"/>
       <c r="S120" s="27"/>
@@ -24618,7 +24673,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="121" spans="2:170" ht="16">
+    <row r="121" spans="2:170">
       <c r="B121" s="3" t="s">
         <v>181</v>
       </c>
@@ -24649,24 +24704,24 @@
       <c r="M121" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N121" s="30" t="s">
+      <c r="N121" s="32" t="s">
+        <v>872</v>
+      </c>
+      <c r="O121" s="32" t="s">
         <v>873</v>
       </c>
-      <c r="O121" s="30" t="s">
+      <c r="P121" s="32"/>
+      <c r="Q121" s="27" t="s">
         <v>874</v>
       </c>
-      <c r="P121" s="27"/>
-      <c r="Q121" s="27" t="s">
+      <c r="R121" s="27" t="s">
         <v>875</v>
       </c>
-      <c r="R121" s="27" t="s">
+      <c r="S121" s="27" t="s">
         <v>876</v>
       </c>
-      <c r="S121" s="27" t="s">
+      <c r="T121" s="27" t="s">
         <v>877</v>
-      </c>
-      <c r="T121" s="27" t="s">
-        <v>878</v>
       </c>
       <c r="U121" s="27"/>
       <c r="V121" s="27" t="s">
@@ -24787,7 +24842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="2:170" ht="16">
+    <row r="122" spans="2:170">
       <c r="B122" s="3" t="s">
         <v>179</v>
       </c>
@@ -24820,24 +24875,24 @@
       <c r="M122" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N122" s="30" t="s">
+      <c r="N122" s="32" t="s">
+        <v>878</v>
+      </c>
+      <c r="O122" s="32" t="s">
         <v>879</v>
       </c>
-      <c r="O122" s="30" t="s">
+      <c r="P122" s="32"/>
+      <c r="Q122" s="27" t="s">
         <v>880</v>
       </c>
-      <c r="P122" s="27"/>
-      <c r="Q122" s="27" t="s">
+      <c r="R122" s="27" t="s">
         <v>881</v>
       </c>
-      <c r="R122" s="27" t="s">
+      <c r="S122" s="27" t="s">
         <v>882</v>
       </c>
-      <c r="S122" s="27" t="s">
+      <c r="T122" s="27" t="s">
         <v>883</v>
-      </c>
-      <c r="T122" s="27" t="s">
-        <v>884</v>
       </c>
       <c r="U122" s="27"/>
       <c r="V122" s="27" t="s">
@@ -24908,11 +24963,11 @@
       <c r="M123" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N123" s="27" t="s">
+      <c r="N123" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O123" s="27"/>
-      <c r="P123" s="27"/>
+      <c r="O123" s="32"/>
+      <c r="P123" s="32"/>
       <c r="Q123" s="27"/>
       <c r="R123" s="27"/>
       <c r="S123" s="27"/>
@@ -25061,11 +25116,11 @@
       <c r="M124" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N124" s="27" t="s">
+      <c r="N124" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O124" s="27"/>
-      <c r="P124" s="27"/>
+      <c r="O124" s="32"/>
+      <c r="P124" s="32"/>
       <c r="Q124" s="27"/>
       <c r="R124" s="27"/>
       <c r="S124" s="27"/>
@@ -25193,11 +25248,11 @@
       <c r="M125" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N125" s="27" t="s">
+      <c r="N125" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O125" s="27"/>
-      <c r="P125" s="27"/>
+      <c r="O125" s="32"/>
+      <c r="P125" s="32"/>
       <c r="Q125" s="27"/>
       <c r="R125" s="27"/>
       <c r="S125" s="27"/>
@@ -25258,11 +25313,11 @@
       <c r="M126" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N126" s="27" t="s">
-        <v>885</v>
-      </c>
-      <c r="O126" s="27"/>
-      <c r="P126" s="27"/>
+      <c r="N126" s="32" t="s">
+        <v>884</v>
+      </c>
+      <c r="O126" s="32"/>
+      <c r="P126" s="32"/>
       <c r="Q126" s="27"/>
       <c r="R126" s="27"/>
       <c r="S126" s="27"/>
@@ -25382,13 +25437,13 @@
         <v>327</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="J127" s="27" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="K127" s="27" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="L127" s="27" t="s">
         <v>532</v>
@@ -25396,11 +25451,11 @@
       <c r="M127" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N127" s="27" t="s">
+      <c r="N127" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O127" s="27"/>
-      <c r="P127" s="27"/>
+      <c r="O127" s="32"/>
+      <c r="P127" s="32"/>
       <c r="Q127" s="27"/>
       <c r="R127" s="27"/>
       <c r="S127" s="27"/>
@@ -25484,10 +25539,10 @@
         <v>327</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="J128" s="27" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="K128" s="27"/>
       <c r="L128" s="27" t="s">
@@ -25496,11 +25551,11 @@
       <c r="M128" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N128" s="27" t="s">
+      <c r="N128" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O128" s="27"/>
-      <c r="P128" s="27"/>
+      <c r="O128" s="32"/>
+      <c r="P128" s="32"/>
       <c r="Q128" s="27"/>
       <c r="R128" s="27"/>
       <c r="S128" s="27"/>
@@ -25677,13 +25732,13 @@
         <v>327</v>
       </c>
       <c r="I129" s="27" t="s">
+        <v>945</v>
+      </c>
+      <c r="J129" s="27" t="s">
+        <v>946</v>
+      </c>
+      <c r="K129" s="27" t="s">
         <v>948</v>
-      </c>
-      <c r="J129" s="27" t="s">
-        <v>949</v>
-      </c>
-      <c r="K129" s="27" t="s">
-        <v>951</v>
       </c>
       <c r="L129" s="27" t="s">
         <v>530</v>
@@ -25691,13 +25746,13 @@
       <c r="M129" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N129" s="27" t="s">
+      <c r="N129" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O129" s="27"/>
-      <c r="P129" s="27"/>
+      <c r="O129" s="32"/>
+      <c r="P129" s="32"/>
       <c r="Q129" s="27" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="R129" s="27"/>
       <c r="S129" s="27"/>
@@ -25827,7 +25882,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="2:170" ht="16">
+    <row r="130" spans="2:170">
       <c r="B130" s="3" t="s">
         <v>165</v>
       </c>
@@ -25850,13 +25905,13 @@
         <v>327</v>
       </c>
       <c r="I130" s="27" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="J130" s="27" t="s">
         <v>327</v>
       </c>
       <c r="K130" s="27" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="L130" s="27" t="s">
         <v>533</v>
@@ -25864,13 +25919,13 @@
       <c r="M130" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N130" s="30" t="s">
+      <c r="N130" s="32" t="s">
+        <v>886</v>
+      </c>
+      <c r="O130" s="32"/>
+      <c r="P130" s="32"/>
+      <c r="Q130" s="27" t="s">
         <v>887</v>
-      </c>
-      <c r="O130" s="27"/>
-      <c r="P130" s="27"/>
-      <c r="Q130" s="27" t="s">
-        <v>888</v>
       </c>
       <c r="R130" s="27"/>
       <c r="S130" s="27"/>
@@ -26125,13 +26180,13 @@
         <v>327</v>
       </c>
       <c r="I131" s="27" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="J131" s="27" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="K131" s="27" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="L131" s="27" t="s">
         <v>531</v>
@@ -26139,13 +26194,13 @@
       <c r="M131" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N131" s="27" t="s">
+      <c r="N131" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O131" s="27"/>
-      <c r="P131" s="27"/>
+      <c r="O131" s="32"/>
+      <c r="P131" s="32"/>
       <c r="Q131" s="27" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="R131" s="27"/>
       <c r="S131" s="27"/>
@@ -26314,7 +26369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:170" ht="16">
+    <row r="132" spans="2:170">
       <c r="B132" s="3" t="s">
         <v>161</v>
       </c>
@@ -26331,16 +26386,16 @@
         <v>131</v>
       </c>
       <c r="G132" s="27" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="H132" s="27" t="s">
         <v>327</v>
       </c>
       <c r="I132" s="27" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="J132" s="27" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="K132" s="27"/>
       <c r="L132" s="27" t="s">
@@ -26349,16 +26404,16 @@
       <c r="M132" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N132" s="30" t="s">
+      <c r="N132" s="32" t="s">
+        <v>889</v>
+      </c>
+      <c r="O132" s="32"/>
+      <c r="P132" s="32"/>
+      <c r="Q132" s="27" t="s">
         <v>890</v>
       </c>
-      <c r="O132" s="27"/>
-      <c r="P132" s="27"/>
-      <c r="Q132" s="27" t="s">
+      <c r="R132" s="27" t="s">
         <v>891</v>
-      </c>
-      <c r="R132" s="27" t="s">
-        <v>892</v>
       </c>
       <c r="S132" s="27"/>
       <c r="T132" s="27"/>
@@ -26394,7 +26449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:170" ht="16">
+    <row r="133" spans="2:170">
       <c r="B133" s="3" t="s">
         <v>159</v>
       </c>
@@ -26417,13 +26472,13 @@
         <v>347</v>
       </c>
       <c r="I133" s="27" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="J133" s="27" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="K133" s="27" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="L133" s="27" t="s">
         <v>530</v>
@@ -26431,21 +26486,21 @@
       <c r="M133" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N133" s="30" t="s">
+      <c r="N133" s="32" t="s">
+        <v>892</v>
+      </c>
+      <c r="O133" s="32" t="s">
         <v>893</v>
       </c>
-      <c r="O133" s="27" t="s">
+      <c r="P133" s="32"/>
+      <c r="Q133" s="27" t="s">
         <v>894</v>
       </c>
-      <c r="P133" s="27"/>
-      <c r="Q133" s="27" t="s">
+      <c r="R133" s="27" t="s">
         <v>895</v>
       </c>
-      <c r="R133" s="27" t="s">
+      <c r="S133" s="27" t="s">
         <v>896</v>
-      </c>
-      <c r="S133" s="27" t="s">
-        <v>897</v>
       </c>
       <c r="T133" s="27"/>
       <c r="U133" s="27"/>
@@ -26498,7 +26553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:170" ht="16">
+    <row r="134" spans="2:170">
       <c r="B134" s="3" t="s">
         <v>150</v>
       </c>
@@ -26521,10 +26576,10 @@
         <v>327</v>
       </c>
       <c r="I134" s="27" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="J134" s="27" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="K134" s="27"/>
       <c r="L134" s="27" t="s">
@@ -26533,15 +26588,15 @@
       <c r="M134" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N134" s="30" t="s">
+      <c r="N134" s="32" t="s">
+        <v>897</v>
+      </c>
+      <c r="O134" s="32" t="s">
         <v>898</v>
       </c>
-      <c r="O134" s="30" t="s">
+      <c r="P134" s="32"/>
+      <c r="Q134" s="27" t="s">
         <v>899</v>
-      </c>
-      <c r="P134" s="27"/>
-      <c r="Q134" s="27" t="s">
-        <v>900</v>
       </c>
       <c r="R134" s="27"/>
       <c r="S134" s="27"/>
@@ -26629,7 +26684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:170" ht="16">
+    <row r="135" spans="2:170">
       <c r="B135" s="3" t="s">
         <v>150</v>
       </c>
@@ -26652,13 +26707,13 @@
         <v>620</v>
       </c>
       <c r="I135" s="27" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="J135" s="27" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="K135" s="27" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="L135" s="27" t="s">
         <v>533</v>
@@ -26666,13 +26721,13 @@
       <c r="M135" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N135" s="30" t="s">
+      <c r="N135" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="O135" s="32"/>
+      <c r="P135" s="32"/>
+      <c r="Q135" s="27" t="s">
         <v>901</v>
-      </c>
-      <c r="O135" s="27"/>
-      <c r="P135" s="27"/>
-      <c r="Q135" s="27" t="s">
-        <v>902</v>
       </c>
       <c r="R135" s="27"/>
       <c r="S135" s="27"/>
@@ -26754,7 +26809,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="2:170" ht="16">
+    <row r="136" spans="2:170">
       <c r="B136" s="3" t="s">
         <v>150</v>
       </c>
@@ -26777,10 +26832,10 @@
         <v>327</v>
       </c>
       <c r="I136" s="27" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="J136" s="27" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="K136" s="27"/>
       <c r="L136" s="27" t="s">
@@ -26789,21 +26844,21 @@
       <c r="M136" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N136" s="30" t="s">
+      <c r="N136" s="32" t="s">
+        <v>902</v>
+      </c>
+      <c r="O136" s="32" t="s">
         <v>903</v>
       </c>
-      <c r="O136" s="30" t="s">
+      <c r="P136" s="32"/>
+      <c r="Q136" s="27" t="s">
         <v>904</v>
       </c>
-      <c r="P136" s="27"/>
-      <c r="Q136" s="27" t="s">
+      <c r="R136" s="27" t="s">
         <v>905</v>
       </c>
-      <c r="R136" s="27" t="s">
+      <c r="S136" s="27" t="s">
         <v>906</v>
-      </c>
-      <c r="S136" s="27" t="s">
-        <v>907</v>
       </c>
       <c r="T136" s="27"/>
       <c r="U136" s="27"/>
@@ -26979,7 +27034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="137" spans="2:170" ht="16">
+    <row r="137" spans="2:170">
       <c r="B137" s="3" t="s">
         <v>150</v>
       </c>
@@ -27006,23 +27061,23 @@
       <c r="M137" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N137" s="30" t="s">
+      <c r="N137" s="32" t="s">
+        <v>907</v>
+      </c>
+      <c r="O137" s="32" t="s">
         <v>908</v>
       </c>
-      <c r="O137" s="30" t="s">
+      <c r="P137" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="P137" s="30" t="s">
+      <c r="Q137" s="27" t="s">
         <v>910</v>
       </c>
-      <c r="Q137" s="27" t="s">
+      <c r="R137" s="27" t="s">
         <v>911</v>
       </c>
-      <c r="R137" s="27" t="s">
+      <c r="S137" s="27" t="s">
         <v>912</v>
-      </c>
-      <c r="S137" s="27" t="s">
-        <v>913</v>
       </c>
       <c r="T137" s="27"/>
       <c r="U137" s="27"/>
@@ -27183,7 +27238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:170" ht="16">
+    <row r="138" spans="2:170">
       <c r="B138" s="3" t="s">
         <v>150</v>
       </c>
@@ -27210,17 +27265,17 @@
       <c r="M138" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N138" s="30" t="s">
+      <c r="N138" s="32" t="s">
+        <v>913</v>
+      </c>
+      <c r="O138" s="32" t="s">
         <v>914</v>
       </c>
-      <c r="O138" s="30" t="s">
+      <c r="P138" s="32" t="s">
         <v>915</v>
       </c>
-      <c r="P138" s="30" t="s">
+      <c r="Q138" s="27" t="s">
         <v>916</v>
-      </c>
-      <c r="Q138" s="27" t="s">
-        <v>917</v>
       </c>
       <c r="R138" s="27"/>
       <c r="S138" s="27"/>
@@ -27383,7 +27438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:170" ht="16">
+    <row r="139" spans="2:170">
       <c r="B139" s="3" t="s">
         <v>150</v>
       </c>
@@ -27410,17 +27465,17 @@
       <c r="M139" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N139" s="30" t="s">
+      <c r="N139" s="32" t="s">
+        <v>917</v>
+      </c>
+      <c r="O139" s="32" t="s">
         <v>918</v>
       </c>
-      <c r="O139" s="30" t="s">
+      <c r="P139" s="32" t="s">
         <v>919</v>
       </c>
-      <c r="P139" s="30" t="s">
+      <c r="Q139" s="27" t="s">
         <v>920</v>
-      </c>
-      <c r="Q139" s="27" t="s">
-        <v>921</v>
       </c>
       <c r="R139" s="27"/>
       <c r="S139" s="27"/>
@@ -27610,13 +27665,13 @@
       <c r="M140" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N140" s="27" t="s">
+      <c r="N140" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O140" s="27"/>
-      <c r="P140" s="27"/>
+      <c r="O140" s="32"/>
+      <c r="P140" s="32"/>
       <c r="Q140" s="27" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="R140" s="27"/>
       <c r="S140" s="27"/>
@@ -27761,11 +27816,11 @@
       <c r="M141" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N141" s="27" t="s">
+      <c r="N141" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O141" s="27"/>
-      <c r="P141" s="27"/>
+      <c r="O141" s="32"/>
+      <c r="P141" s="32"/>
       <c r="Q141" s="27"/>
       <c r="R141" s="27"/>
       <c r="S141" s="27"/>
@@ -27844,7 +27899,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="142" spans="2:170" ht="16">
+    <row r="142" spans="2:170">
       <c r="B142" s="3" t="s">
         <v>144</v>
       </c>
@@ -27871,17 +27926,17 @@
       <c r="M142" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N142" s="30" t="s">
+      <c r="N142" s="32" t="s">
+        <v>922</v>
+      </c>
+      <c r="O142" s="32" t="s">
         <v>923</v>
       </c>
-      <c r="O142" s="30" t="s">
+      <c r="P142" s="32" t="s">
         <v>924</v>
       </c>
-      <c r="P142" s="30" t="s">
+      <c r="Q142" s="27" t="s">
         <v>925</v>
-      </c>
-      <c r="Q142" s="27" t="s">
-        <v>926</v>
       </c>
       <c r="R142" s="27"/>
       <c r="S142" s="27"/>
@@ -27897,7 +27952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:170" ht="16">
+    <row r="143" spans="2:170">
       <c r="B143" s="3" t="s">
         <v>144</v>
       </c>
@@ -27924,15 +27979,15 @@
       <c r="M143" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N143" s="31" t="s">
-        <v>927</v>
-      </c>
-      <c r="O143" s="31" t="s">
-        <v>928</v>
-      </c>
-      <c r="P143" s="27"/>
+      <c r="N143" s="32" t="s">
+        <v>964</v>
+      </c>
+      <c r="O143" s="32" t="s">
+        <v>965</v>
+      </c>
+      <c r="P143" s="32"/>
       <c r="Q143" s="27" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="R143" s="27"/>
       <c r="S143" s="27"/>
@@ -27987,7 +28042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="144" spans="2:170" ht="16">
+    <row r="144" spans="2:170">
       <c r="B144" s="3" t="s">
         <v>144</v>
       </c>
@@ -28014,21 +28069,21 @@
       <c r="M144" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N144" s="30" t="s">
+      <c r="N144" s="32" t="s">
+        <v>927</v>
+      </c>
+      <c r="O144" s="32" t="s">
+        <v>928</v>
+      </c>
+      <c r="P144" s="32"/>
+      <c r="Q144" s="27" t="s">
+        <v>929</v>
+      </c>
+      <c r="R144" s="27" t="s">
         <v>930</v>
       </c>
-      <c r="O144" s="30" t="s">
+      <c r="S144" s="27" t="s">
         <v>931</v>
-      </c>
-      <c r="P144" s="27"/>
-      <c r="Q144" s="27" t="s">
-        <v>932</v>
-      </c>
-      <c r="R144" s="27" t="s">
-        <v>933</v>
-      </c>
-      <c r="S144" s="27" t="s">
-        <v>934</v>
       </c>
       <c r="T144" s="27"/>
       <c r="U144" s="27"/>
@@ -28105,11 +28160,11 @@
       <c r="M145" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N145" s="27" t="s">
+      <c r="N145" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O145" s="27"/>
-      <c r="P145" s="27"/>
+      <c r="O145" s="32"/>
+      <c r="P145" s="32"/>
       <c r="Q145" s="27"/>
       <c r="R145" s="27"/>
       <c r="S145" s="27"/>
@@ -28230,11 +28285,11 @@
       <c r="M146" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N146" s="27" t="s">
+      <c r="N146" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O146" s="27"/>
-      <c r="P146" s="27"/>
+      <c r="O146" s="32"/>
+      <c r="P146" s="32"/>
       <c r="Q146" s="27"/>
       <c r="R146" s="27"/>
       <c r="S146" s="27"/>
@@ -28358,19 +28413,19 @@
       <c r="M147" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N147" s="27" t="s">
+      <c r="N147" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O147" s="27"/>
-      <c r="P147" s="27"/>
+      <c r="O147" s="32"/>
+      <c r="P147" s="32"/>
       <c r="Q147" s="27" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="R147" s="27" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="S147" s="27" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="T147" s="27"/>
       <c r="U147" s="27"/>
@@ -28459,18 +28514,20 @@
       <c r="M148" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N148" s="27" t="s">
+      <c r="N148" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="O148" s="27"/>
-      <c r="P148" s="27"/>
-      <c r="Q148" s="27"/>
+      <c r="O148" s="32"/>
+      <c r="P148" s="32"/>
+      <c r="Q148" s="27" t="s">
+        <v>980</v>
+      </c>
       <c r="R148" s="27"/>
       <c r="S148" s="27"/>
       <c r="T148" s="27"/>
       <c r="U148" s="27"/>
       <c r="V148" s="27" t="s">
-        <v>669</v>
+        <v>20</v>
       </c>
       <c r="AA148" s="19">
         <v>2</v>
@@ -28521,7 +28578,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="149" spans="2:170" ht="16">
+    <row r="149" spans="2:170">
       <c r="B149" s="3" t="s">
         <v>127</v>
       </c>
@@ -28548,13 +28605,13 @@
       <c r="M149" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N149" s="30" t="s">
-        <v>938</v>
-      </c>
-      <c r="O149" s="27"/>
-      <c r="P149" s="27"/>
+      <c r="N149" s="32" t="s">
+        <v>935</v>
+      </c>
+      <c r="O149" s="32"/>
+      <c r="P149" s="32"/>
       <c r="Q149" s="27" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="R149" s="27"/>
       <c r="S149" s="27"/>
@@ -28615,7 +28672,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="150" spans="2:170" ht="16">
+    <row r="150" spans="2:170">
       <c r="B150" s="3" t="s">
         <v>127</v>
       </c>
@@ -28642,25 +28699,25 @@
       <c r="M150" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N150" s="30" t="s">
+      <c r="N150" s="32" t="s">
+        <v>937</v>
+      </c>
+      <c r="O150" s="32"/>
+      <c r="P150" s="32"/>
+      <c r="Q150" s="27" t="s">
+        <v>938</v>
+      </c>
+      <c r="R150" s="27" t="s">
+        <v>939</v>
+      </c>
+      <c r="S150" s="27" t="s">
         <v>940</v>
       </c>
-      <c r="O150" s="27"/>
-      <c r="P150" s="27"/>
-      <c r="Q150" s="27" t="s">
+      <c r="T150" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="R150" s="27" t="s">
+      <c r="U150" s="27" t="s">
         <v>942</v>
-      </c>
-      <c r="S150" s="27" t="s">
-        <v>943</v>
-      </c>
-      <c r="T150" s="27" t="s">
-        <v>944</v>
-      </c>
-      <c r="U150" s="27" t="s">
-        <v>945</v>
       </c>
       <c r="V150" s="27" t="s">
         <v>669</v>
@@ -28852,13 +28909,13 @@
       <c r="M151" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N151" s="27" t="s">
+      <c r="N151" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O151" s="27"/>
-      <c r="P151" s="27"/>
+      <c r="O151" s="31"/>
+      <c r="P151" s="31"/>
       <c r="Q151" s="27" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="R151" s="27"/>
       <c r="S151" s="27"/>
@@ -29000,15 +29057,23 @@
       <c r="M152" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N152" s="27"/>
-      <c r="O152" s="27"/>
-      <c r="P152" s="27"/>
-      <c r="Q152" s="27"/>
-      <c r="R152" s="27"/>
+      <c r="N152" s="31" t="s">
+        <v>669</v>
+      </c>
+      <c r="O152" s="31"/>
+      <c r="P152" s="31"/>
+      <c r="Q152" s="27" t="s">
+        <v>966</v>
+      </c>
+      <c r="R152" s="27" t="s">
+        <v>967</v>
+      </c>
       <c r="S152" s="27"/>
       <c r="T152" s="27"/>
       <c r="U152" s="27"/>
-      <c r="V152" s="27"/>
+      <c r="V152" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="AA152" s="19">
         <v>1</v>
       </c>
@@ -29121,15 +29186,25 @@
       <c r="M153" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N153" s="27"/>
-      <c r="O153" s="27"/>
-      <c r="P153" s="27"/>
-      <c r="Q153" s="27"/>
-      <c r="R153" s="27"/>
-      <c r="S153" s="27"/>
+      <c r="N153" s="31" t="s">
+        <v>968</v>
+      </c>
+      <c r="O153" s="31"/>
+      <c r="P153" s="31"/>
+      <c r="Q153" s="27" t="s">
+        <v>969</v>
+      </c>
+      <c r="R153" s="27" t="s">
+        <v>970</v>
+      </c>
+      <c r="S153" s="27" t="s">
+        <v>971</v>
+      </c>
       <c r="T153" s="27"/>
       <c r="U153" s="27"/>
-      <c r="V153" s="27"/>
+      <c r="V153" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="AA153" s="19">
         <v>2</v>
       </c>
@@ -29245,15 +29320,25 @@
       <c r="M154" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N154" s="27"/>
-      <c r="O154" s="27"/>
-      <c r="P154" s="27"/>
-      <c r="Q154" s="27"/>
-      <c r="R154" s="27"/>
-      <c r="S154" s="27"/>
+      <c r="N154" s="31" t="s">
+        <v>972</v>
+      </c>
+      <c r="O154" s="31"/>
+      <c r="P154" s="31"/>
+      <c r="Q154" s="27" t="s">
+        <v>973</v>
+      </c>
+      <c r="R154" s="27" t="s">
+        <v>974</v>
+      </c>
+      <c r="S154" s="27" t="s">
+        <v>975</v>
+      </c>
       <c r="T154" s="27"/>
       <c r="U154" s="27"/>
-      <c r="V154" s="27"/>
+      <c r="V154" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="CN154" s="21">
         <v>1</v>
       </c>
@@ -29300,12 +29385,20 @@
       <c r="M155" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N155" s="27"/>
-      <c r="O155" s="27"/>
-      <c r="P155" s="27"/>
-      <c r="Q155" s="27"/>
-      <c r="R155" s="27"/>
-      <c r="S155" s="27"/>
+      <c r="N155" s="31" t="s">
+        <v>976</v>
+      </c>
+      <c r="O155" s="31"/>
+      <c r="P155" s="31"/>
+      <c r="Q155" s="27" t="s">
+        <v>977</v>
+      </c>
+      <c r="R155" s="27" t="s">
+        <v>978</v>
+      </c>
+      <c r="S155" s="27" t="s">
+        <v>979</v>
+      </c>
       <c r="T155" s="27"/>
       <c r="U155" s="27"/>
       <c r="V155" s="27"/>
@@ -29496,15 +29589,19 @@
       <c r="M156" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N156" s="27"/>
-      <c r="O156" s="27"/>
-      <c r="P156" s="27"/>
+      <c r="N156" s="31" t="s">
+        <v>669</v>
+      </c>
+      <c r="O156" s="31"/>
+      <c r="P156" s="31"/>
       <c r="Q156" s="27"/>
       <c r="R156" s="27"/>
       <c r="S156" s="27"/>
       <c r="T156" s="27"/>
       <c r="U156" s="27"/>
-      <c r="V156" s="27"/>
+      <c r="V156" s="27" t="s">
+        <v>981</v>
+      </c>
       <c r="AA156" s="19">
         <v>1</v>
       </c>
@@ -29626,15 +29723,25 @@
       <c r="M157" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N157" s="27"/>
-      <c r="O157" s="27"/>
-      <c r="P157" s="27"/>
-      <c r="Q157" s="27"/>
-      <c r="R157" s="27"/>
+      <c r="N157" s="31" t="s">
+        <v>984</v>
+      </c>
+      <c r="O157" s="31" t="s">
+        <v>985</v>
+      </c>
+      <c r="P157" s="31"/>
+      <c r="Q157" s="27" t="s">
+        <v>982</v>
+      </c>
+      <c r="R157" s="27" t="s">
+        <v>983</v>
+      </c>
       <c r="S157" s="27"/>
       <c r="T157" s="27"/>
       <c r="U157" s="27"/>
-      <c r="V157" s="27"/>
+      <c r="V157" s="27" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="158" spans="2:170">
       <c r="B158" s="3" t="s">
@@ -29663,9 +29770,9 @@
       <c r="M158" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N158" s="27"/>
-      <c r="O158" s="27"/>
-      <c r="P158" s="27"/>
+      <c r="N158" s="31"/>
+      <c r="O158" s="31"/>
+      <c r="P158" s="31"/>
       <c r="Q158" s="27"/>
       <c r="R158" s="27"/>
       <c r="S158" s="27"/>
@@ -29718,9 +29825,9 @@
       <c r="M159" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N159" s="27"/>
-      <c r="O159" s="27"/>
-      <c r="P159" s="27"/>
+      <c r="N159" s="31"/>
+      <c r="O159" s="31"/>
+      <c r="P159" s="31"/>
       <c r="Q159" s="27"/>
       <c r="R159" s="27"/>
       <c r="S159" s="27"/>
@@ -35188,8 +35295,9 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
☂ add full text 156 thru 175
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="0" windowWidth="23760" windowHeight="11800" tabRatio="500"/>
+    <workbookView xWindow="15240" yWindow="0" windowWidth="18260" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1020">
   <si>
     <t>f</t>
   </si>
@@ -2982,13 +2982,175 @@
   </si>
   <si>
     <t>books.google.com/books?id=JoMqAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=mT9WAAAAcAAJ</t>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=cZk_AAAAYAAJ</t>
+    </r>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=dul1.ark:/13960/t5q822n9w;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nnc1.0114584662;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=awdhz0l-q78C</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=dul1.ark:/13960/t76t18804;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nnc1.0022556613;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nnc1.0022556605;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CHEHTNA026449004</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=YuUyAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=2Zc3AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLWRLFF586538693</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=QxMnAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=t78NAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433075746978;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CFFKGFY892350853</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=sC8qAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Jh8GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://literature.proquest.com.ezproxy.library.uvic.ca/searchFulltext.do?id=Z000043531&amp;divLevel=0&amp;area=Prose&amp;DurUrl=Yes&amp;forward=textsFT&amp;queryType=findWork</t>
+  </si>
+  <si>
+    <t>http://www.jstor.org.ezproxy.library.uvic.ca/stable/4173295?seq=1</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=mS3QAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=inu.32000006720579;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CPMSYQJ800210126</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CFIFQJK867042992</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CKLFLVL071564054</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CHMZWKX989260613</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=w6cBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CZPGGIO251408764</t>
+  </si>
+  <si>
+    <t>none ;;</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CUFAGFA118634200</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLHIOMG185603352</t>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=zmIzAQAAMAAJ</t>
+    </r>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=inu.30000091678395;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CKIXTNH657247573</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3045,6 +3207,19 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3457,7 +3632,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3517,6 +3692,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="283">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7330,6 +7507,112 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -7456,112 +7739,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -7899,10 +8076,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="N163" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J190" sqref="J190"/>
+      <selection pane="bottomRight" activeCell="U184" sqref="U184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -29770,7 +29947,9 @@
       <c r="M158" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N158" s="31"/>
+      <c r="N158" s="31" t="s">
+        <v>669</v>
+      </c>
       <c r="O158" s="31"/>
       <c r="P158" s="31"/>
       <c r="Q158" s="27"/>
@@ -29778,7 +29957,9 @@
       <c r="S158" s="27"/>
       <c r="T158" s="27"/>
       <c r="U158" s="27"/>
-      <c r="V158" s="27"/>
+      <c r="V158" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="BG158" s="3">
         <v>1</v>
       </c>
@@ -29798,7 +29979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="2:170">
+    <row r="159" spans="2:170" ht="16">
       <c r="B159" s="3" t="s">
         <v>120</v>
       </c>
@@ -29825,7 +30006,9 @@
       <c r="M159" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N159" s="31"/>
+      <c r="N159" s="33" t="s">
+        <v>986</v>
+      </c>
       <c r="O159" s="31"/>
       <c r="P159" s="31"/>
       <c r="Q159" s="27"/>
@@ -29833,7 +30016,9 @@
       <c r="S159" s="27"/>
       <c r="T159" s="27"/>
       <c r="U159" s="27"/>
-      <c r="V159" s="27"/>
+      <c r="V159" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AF159" s="3">
         <v>1</v>
       </c>
@@ -29868,7 +30053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:170">
+    <row r="160" spans="2:170" ht="16">
       <c r="B160" s="3" t="s">
         <v>110</v>
       </c>
@@ -29895,15 +30080,23 @@
       <c r="M160" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N160" s="27"/>
+      <c r="N160" s="34" t="s">
+        <v>987</v>
+      </c>
       <c r="O160" s="27"/>
       <c r="P160" s="27"/>
-      <c r="Q160" s="27"/>
-      <c r="R160" s="27"/>
+      <c r="Q160" s="27" t="s">
+        <v>988</v>
+      </c>
+      <c r="R160" s="27" t="s">
+        <v>989</v>
+      </c>
       <c r="S160" s="27"/>
       <c r="T160" s="27"/>
       <c r="U160" s="27"/>
-      <c r="V160" s="27"/>
+      <c r="V160" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA160" s="19">
         <v>1</v>
       </c>
@@ -29944,7 +30137,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="161" spans="1:170">
+    <row r="161" spans="1:170" ht="16">
       <c r="B161" s="3" t="s">
         <v>110</v>
       </c>
@@ -29971,15 +30164,27 @@
       <c r="M161" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N161" s="27"/>
+      <c r="N161" s="33" t="s">
+        <v>990</v>
+      </c>
       <c r="O161" s="27"/>
       <c r="P161" s="27"/>
-      <c r="Q161" s="27"/>
-      <c r="R161" s="27"/>
-      <c r="S161" s="27"/>
-      <c r="T161" s="27"/>
+      <c r="Q161" s="27" t="s">
+        <v>991</v>
+      </c>
+      <c r="R161" s="27" t="s">
+        <v>992</v>
+      </c>
+      <c r="S161" s="27" t="s">
+        <v>993</v>
+      </c>
+      <c r="T161" s="27" t="s">
+        <v>994</v>
+      </c>
       <c r="U161" s="27"/>
-      <c r="V161" s="27"/>
+      <c r="V161" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA161" s="19">
         <v>1</v>
       </c>
@@ -30029,7 +30234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:170">
+    <row r="162" spans="1:170" ht="16">
       <c r="B162" s="3" t="s">
         <v>110</v>
       </c>
@@ -30056,15 +30261,23 @@
       <c r="M162" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N162" s="27"/>
-      <c r="O162" s="27"/>
+      <c r="N162" s="33" t="s">
+        <v>995</v>
+      </c>
+      <c r="O162" s="33" t="s">
+        <v>996</v>
+      </c>
       <c r="P162" s="27"/>
-      <c r="Q162" s="27"/>
+      <c r="Q162" s="27" t="s">
+        <v>997</v>
+      </c>
       <c r="R162" s="27"/>
       <c r="S162" s="27"/>
       <c r="T162" s="27"/>
       <c r="U162" s="27"/>
-      <c r="V162" s="27"/>
+      <c r="V162" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AO162" s="21">
         <v>1</v>
       </c>
@@ -30105,7 +30318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:170">
+    <row r="163" spans="1:170" ht="16">
       <c r="B163" s="3" t="s">
         <v>110</v>
       </c>
@@ -30132,15 +30345,25 @@
       <c r="M163" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N163" s="27"/>
-      <c r="O163" s="27"/>
+      <c r="N163" s="33" t="s">
+        <v>998</v>
+      </c>
+      <c r="O163" s="33" t="s">
+        <v>999</v>
+      </c>
       <c r="P163" s="27"/>
-      <c r="Q163" s="27"/>
-      <c r="R163" s="27"/>
+      <c r="Q163" s="27" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R163" s="27" t="s">
+        <v>1001</v>
+      </c>
       <c r="S163" s="27"/>
       <c r="T163" s="27"/>
       <c r="U163" s="27"/>
-      <c r="V163" s="27"/>
+      <c r="V163" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA163" s="19">
         <v>1</v>
       </c>
@@ -30260,7 +30483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:170">
+    <row r="164" spans="1:170" ht="16">
       <c r="B164" s="3" t="s">
         <v>110</v>
       </c>
@@ -30287,15 +30510,23 @@
       <c r="M164" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N164" s="27"/>
-      <c r="O164" s="27"/>
+      <c r="N164" s="33" t="s">
+        <v>1002</v>
+      </c>
+      <c r="O164" s="33" t="s">
+        <v>1003</v>
+      </c>
       <c r="P164" s="27"/>
-      <c r="Q164" s="27"/>
+      <c r="Q164" s="27" t="s">
+        <v>1004</v>
+      </c>
       <c r="R164" s="27"/>
       <c r="S164" s="27"/>
       <c r="T164" s="27"/>
       <c r="U164" s="27"/>
-      <c r="V164" s="27"/>
+      <c r="V164" s="27" t="s">
+        <v>668</v>
+      </c>
       <c r="AG164" s="19">
         <v>1</v>
       </c>
@@ -30348,15 +30579,21 @@
       <c r="M165" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N165" s="27"/>
+      <c r="N165" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O165" s="27"/>
       <c r="P165" s="27"/>
-      <c r="Q165" s="27"/>
+      <c r="Q165" s="27" t="s">
+        <v>1005</v>
+      </c>
       <c r="R165" s="27"/>
       <c r="S165" s="27"/>
       <c r="T165" s="27"/>
       <c r="U165" s="27"/>
-      <c r="V165" s="27"/>
+      <c r="V165" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="BR165" s="3">
         <v>1</v>
       </c>
@@ -30379,7 +30616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:170">
+    <row r="166" spans="1:170" ht="16">
       <c r="B166" s="3" t="s">
         <v>110</v>
       </c>
@@ -30406,15 +30643,23 @@
       <c r="M166" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N166" s="27"/>
+      <c r="N166" s="33" t="s">
+        <v>1006</v>
+      </c>
       <c r="O166" s="27"/>
       <c r="P166" s="27"/>
-      <c r="Q166" s="27"/>
-      <c r="R166" s="27"/>
+      <c r="Q166" s="27" t="s">
+        <v>1007</v>
+      </c>
+      <c r="R166" s="27" t="s">
+        <v>1008</v>
+      </c>
       <c r="S166" s="27"/>
       <c r="T166" s="27"/>
       <c r="U166" s="27"/>
-      <c r="V166" s="27"/>
+      <c r="V166" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AG166" s="19">
         <v>1</v>
       </c>
@@ -30506,7 +30751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:170">
+    <row r="167" spans="1:170" ht="16">
       <c r="B167" s="3" t="s">
         <v>107</v>
       </c>
@@ -30533,7 +30778,9 @@
       <c r="M167" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N167" s="27"/>
+      <c r="N167" s="33" t="s">
+        <v>669</v>
+      </c>
       <c r="O167" s="27"/>
       <c r="P167" s="27"/>
       <c r="Q167" s="27"/>
@@ -30541,7 +30788,9 @@
       <c r="S167" s="27"/>
       <c r="T167" s="27"/>
       <c r="U167" s="27"/>
-      <c r="V167" s="27"/>
+      <c r="V167" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA167" s="19">
         <v>1</v>
       </c>
@@ -30648,15 +30897,21 @@
       <c r="M168" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N168" s="27"/>
+      <c r="N168" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O168" s="27"/>
       <c r="P168" s="27"/>
-      <c r="Q168" s="27"/>
+      <c r="Q168" s="27" t="s">
+        <v>1009</v>
+      </c>
       <c r="R168" s="27"/>
       <c r="S168" s="27"/>
       <c r="T168" s="27"/>
       <c r="U168" s="27"/>
-      <c r="V168" s="27"/>
+      <c r="V168" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AN168" s="21">
         <v>1</v>
       </c>
@@ -30751,15 +31006,21 @@
       <c r="M169" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N169" s="27"/>
+      <c r="N169" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O169" s="27"/>
       <c r="P169" s="27"/>
-      <c r="Q169" s="27"/>
+      <c r="Q169" s="27" t="s">
+        <v>1010</v>
+      </c>
       <c r="R169" s="27"/>
       <c r="S169" s="27"/>
       <c r="T169" s="27"/>
       <c r="U169" s="27"/>
-      <c r="V169" s="27"/>
+      <c r="V169" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA169" s="19">
         <v>1</v>
       </c>
@@ -30905,15 +31166,21 @@
       <c r="M170" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N170" s="27"/>
+      <c r="N170" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O170" s="27"/>
       <c r="P170" s="27"/>
-      <c r="Q170" s="27"/>
+      <c r="Q170" s="27" t="s">
+        <v>1011</v>
+      </c>
       <c r="R170" s="27"/>
       <c r="S170" s="27"/>
       <c r="T170" s="27"/>
       <c r="U170" s="27"/>
-      <c r="V170" s="27"/>
+      <c r="V170" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="BT170" s="3">
         <v>1</v>
       </c>
@@ -30951,7 +31218,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="171" spans="1:170">
+    <row r="171" spans="1:170" ht="16">
       <c r="B171" s="3" t="s">
         <v>98</v>
       </c>
@@ -30978,15 +31245,21 @@
       <c r="M171" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N171" s="27"/>
+      <c r="N171" s="33" t="s">
+        <v>1012</v>
+      </c>
       <c r="O171" s="27"/>
       <c r="P171" s="27"/>
-      <c r="Q171" s="27"/>
+      <c r="Q171" s="27" t="s">
+        <v>1013</v>
+      </c>
       <c r="R171" s="27"/>
       <c r="S171" s="27"/>
       <c r="T171" s="27"/>
       <c r="U171" s="27"/>
-      <c r="V171" s="27"/>
+      <c r="V171" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AO171" s="21">
         <v>1</v>
       </c>
@@ -31085,7 +31358,9 @@
       <c r="M172" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N172" s="27"/>
+      <c r="N172" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O172" s="27"/>
       <c r="P172" s="27"/>
       <c r="Q172" s="27"/>
@@ -31093,7 +31368,9 @@
       <c r="S172" s="27"/>
       <c r="T172" s="27"/>
       <c r="U172" s="27"/>
-      <c r="V172" s="27"/>
+      <c r="V172" s="27" t="s">
+        <v>1014</v>
+      </c>
       <c r="W172" s="19">
         <v>1</v>
       </c>
@@ -31215,15 +31492,21 @@
       <c r="M173" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N173" s="27"/>
+      <c r="N173" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O173" s="27"/>
       <c r="P173" s="27"/>
-      <c r="Q173" s="27"/>
+      <c r="Q173" s="27" t="s">
+        <v>1015</v>
+      </c>
       <c r="R173" s="27"/>
       <c r="S173" s="27"/>
       <c r="T173" s="27"/>
       <c r="U173" s="27"/>
-      <c r="V173" s="27"/>
+      <c r="V173" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA173" s="19">
         <v>2</v>
       </c>
@@ -31337,7 +31620,9 @@
       <c r="M174" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N174" s="27"/>
+      <c r="N174" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O174" s="27"/>
       <c r="P174" s="27"/>
       <c r="Q174" s="27"/>
@@ -31345,7 +31630,9 @@
       <c r="S174" s="27"/>
       <c r="T174" s="27"/>
       <c r="U174" s="27"/>
-      <c r="V174" s="27"/>
+      <c r="V174" s="27" t="s">
+        <v>788</v>
+      </c>
       <c r="AL174" s="3">
         <v>1</v>
       </c>
@@ -31419,15 +31706,21 @@
       <c r="M175" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N175" s="27"/>
+      <c r="N175" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O175" s="27"/>
       <c r="P175" s="27"/>
-      <c r="Q175" s="27"/>
+      <c r="Q175" s="27" t="s">
+        <v>1016</v>
+      </c>
       <c r="R175" s="27"/>
       <c r="S175" s="27"/>
       <c r="T175" s="27"/>
       <c r="U175" s="27"/>
-      <c r="V175" s="27"/>
+      <c r="V175" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AF175" s="3">
         <v>1</v>
       </c>
@@ -31585,7 +31878,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="176" spans="1:170">
+    <row r="176" spans="1:170" ht="16">
       <c r="B176" s="3" t="s">
         <v>92</v>
       </c>
@@ -31612,15 +31905,23 @@
       <c r="M176" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N176" s="27"/>
+      <c r="N176" s="34" t="s">
+        <v>1017</v>
+      </c>
       <c r="O176" s="27"/>
       <c r="P176" s="27"/>
-      <c r="Q176" s="27"/>
-      <c r="R176" s="27"/>
+      <c r="Q176" s="27" t="s">
+        <v>1018</v>
+      </c>
+      <c r="R176" s="27" t="s">
+        <v>1019</v>
+      </c>
       <c r="S176" s="27"/>
       <c r="T176" s="27"/>
       <c r="U176" s="27"/>
-      <c r="V176" s="27"/>
+      <c r="V176" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AG176" s="19">
         <v>1</v>
       </c>
@@ -35297,7 +35598,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
☂ add full text 176 thru 185
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3333" uniqueCount="1045">
   <si>
     <t>f</t>
   </si>
@@ -3144,6 +3144,141 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CKIXTNH657247573</t>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=jyZMAAAAcAAJ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=4cvvngEACAAJ</t>
+    </r>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074910815;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=FcVEAAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=7Sg9AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=8KJbAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=ja8BAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Zh3roAEACAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t20c5kz2k;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CCLTHOV056916653</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=3OWZnQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7COXIKFC696504248</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=GicGAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=-hVwnQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7COBGUZG834856741</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=cRM7nQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CSVAAKT234546193</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=tSVonQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLPVLAB134971334</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=8DorSwAACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=dwP0mAEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CNEETSP119910357</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=rF5EMwEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=LfACoQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWBFGQB568546723</t>
   </si>
 </sst>
 </file>
@@ -7507,113 +7642,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7739,6 +7768,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -8076,10 +8211,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="N163" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="N171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U184" sqref="U184"/>
+      <selection pane="bottomRight" activeCell="N187" sqref="N187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -31983,7 +32118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:170">
+    <row r="177" spans="1:170" ht="16">
       <c r="B177" s="3" t="s">
         <v>92</v>
       </c>
@@ -32010,15 +32145,23 @@
       <c r="M177" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N177" s="27"/>
-      <c r="O177" s="27"/>
+      <c r="N177" s="34" t="s">
+        <v>1020</v>
+      </c>
+      <c r="O177" s="34" t="s">
+        <v>1021</v>
+      </c>
       <c r="P177" s="27"/>
-      <c r="Q177" s="27"/>
+      <c r="Q177" s="27" t="s">
+        <v>1022</v>
+      </c>
       <c r="R177" s="27"/>
       <c r="S177" s="27"/>
       <c r="T177" s="27"/>
       <c r="U177" s="27"/>
-      <c r="V177" s="27"/>
+      <c r="V177" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AX177" s="3">
         <v>1</v>
       </c>
@@ -32050,7 +32193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:170">
+    <row r="178" spans="1:170" ht="16">
       <c r="A178" s="3" t="s">
         <v>89</v>
       </c>
@@ -32080,15 +32223,23 @@
       <c r="M178" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N178" s="27"/>
-      <c r="O178" s="27"/>
-      <c r="P178" s="27"/>
+      <c r="N178" s="33" t="s">
+        <v>1023</v>
+      </c>
+      <c r="O178" s="33" t="s">
+        <v>1024</v>
+      </c>
+      <c r="P178" s="33" t="s">
+        <v>1025</v>
+      </c>
       <c r="Q178" s="27"/>
       <c r="R178" s="27"/>
       <c r="S178" s="27"/>
       <c r="T178" s="27"/>
       <c r="U178" s="27"/>
-      <c r="V178" s="27"/>
+      <c r="V178" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AE178" s="21">
         <v>1</v>
       </c>
@@ -32226,7 +32377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:170">
+    <row r="179" spans="1:170" ht="16">
       <c r="B179" s="3" t="s">
         <v>73</v>
       </c>
@@ -32253,15 +32404,25 @@
       <c r="M179" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N179" s="27"/>
-      <c r="O179" s="27"/>
+      <c r="N179" s="33" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O179" s="33" t="s">
+        <v>1027</v>
+      </c>
       <c r="P179" s="27"/>
-      <c r="Q179" s="27"/>
-      <c r="R179" s="27"/>
+      <c r="Q179" s="27" t="s">
+        <v>1028</v>
+      </c>
+      <c r="R179" s="27" t="s">
+        <v>1029</v>
+      </c>
       <c r="S179" s="27"/>
       <c r="T179" s="27"/>
       <c r="U179" s="27"/>
-      <c r="V179" s="27"/>
+      <c r="V179" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA179" s="19">
         <v>1</v>
       </c>
@@ -32341,7 +32502,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:170">
+    <row r="180" spans="1:170" ht="16">
       <c r="B180" s="3" t="s">
         <v>73</v>
       </c>
@@ -32368,15 +32529,21 @@
       <c r="M180" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N180" s="27"/>
+      <c r="N180" s="33" t="s">
+        <v>1030</v>
+      </c>
       <c r="O180" s="27"/>
       <c r="P180" s="27"/>
-      <c r="Q180" s="27"/>
+      <c r="Q180" s="27" t="s">
+        <v>1031</v>
+      </c>
       <c r="R180" s="27"/>
       <c r="S180" s="27"/>
       <c r="T180" s="27"/>
       <c r="U180" s="27"/>
-      <c r="V180" s="27"/>
+      <c r="V180" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA180" s="19">
         <v>1</v>
       </c>
@@ -32420,7 +32587,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="181" spans="1:170">
+    <row r="181" spans="1:170" ht="16">
       <c r="B181" s="3" t="s">
         <v>73</v>
       </c>
@@ -32447,15 +32614,23 @@
       <c r="M181" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N181" s="27"/>
-      <c r="O181" s="27"/>
+      <c r="N181" s="33" t="s">
+        <v>1032</v>
+      </c>
+      <c r="O181" s="33" t="s">
+        <v>1033</v>
+      </c>
       <c r="P181" s="27"/>
-      <c r="Q181" s="27"/>
+      <c r="Q181" s="27" t="s">
+        <v>1034</v>
+      </c>
       <c r="R181" s="27"/>
       <c r="S181" s="27"/>
       <c r="T181" s="27"/>
       <c r="U181" s="27"/>
-      <c r="V181" s="27"/>
+      <c r="V181" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AF181" s="3">
         <v>1</v>
       </c>
@@ -32586,7 +32761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="182" spans="1:170">
+    <row r="182" spans="1:170" ht="16">
       <c r="B182" s="3" t="s">
         <v>73</v>
       </c>
@@ -32613,15 +32788,21 @@
       <c r="M182" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N182" s="27"/>
+      <c r="N182" s="33" t="s">
+        <v>1035</v>
+      </c>
       <c r="O182" s="27"/>
       <c r="P182" s="27"/>
-      <c r="Q182" s="27"/>
+      <c r="Q182" s="27" t="s">
+        <v>1036</v>
+      </c>
       <c r="R182" s="27"/>
       <c r="S182" s="27"/>
       <c r="T182" s="27"/>
       <c r="U182" s="27"/>
-      <c r="V182" s="27"/>
+      <c r="V182" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="BG182" s="3">
         <v>1</v>
       </c>
@@ -32686,7 +32867,9 @@
       <c r="M183" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N183" s="27"/>
+      <c r="N183" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O183" s="27"/>
       <c r="P183" s="27"/>
       <c r="Q183" s="27"/>
@@ -32694,7 +32877,9 @@
       <c r="S183" s="27"/>
       <c r="T183" s="27"/>
       <c r="U183" s="27"/>
-      <c r="V183" s="27"/>
+      <c r="V183" s="27" t="s">
+        <v>796</v>
+      </c>
       <c r="AE183" s="21">
         <v>1</v>
       </c>
@@ -32765,7 +32950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:170">
+    <row r="184" spans="1:170" ht="16">
       <c r="B184" s="3" t="s">
         <v>73</v>
       </c>
@@ -32792,15 +32977,21 @@
       <c r="M184" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N184" s="27"/>
+      <c r="N184" s="33" t="s">
+        <v>1037</v>
+      </c>
       <c r="O184" s="27"/>
       <c r="P184" s="27"/>
-      <c r="Q184" s="27"/>
+      <c r="Q184" s="27" t="s">
+        <v>1038</v>
+      </c>
       <c r="R184" s="27"/>
       <c r="S184" s="27"/>
       <c r="T184" s="27"/>
       <c r="U184" s="27"/>
-      <c r="V184" s="27"/>
+      <c r="V184" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AT184" s="3">
         <v>2</v>
       </c>
@@ -32880,7 +33071,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="185" spans="1:170">
+    <row r="185" spans="1:170" ht="16">
       <c r="B185" s="3" t="s">
         <v>73</v>
       </c>
@@ -32907,15 +33098,23 @@
       <c r="M185" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N185" s="27"/>
-      <c r="O185" s="27"/>
+      <c r="N185" s="33" t="s">
+        <v>1039</v>
+      </c>
+      <c r="O185" s="33" t="s">
+        <v>1040</v>
+      </c>
       <c r="P185" s="27"/>
-      <c r="Q185" s="27"/>
+      <c r="Q185" s="27" t="s">
+        <v>1041</v>
+      </c>
       <c r="R185" s="27"/>
       <c r="S185" s="27"/>
       <c r="T185" s="27"/>
       <c r="U185" s="27"/>
-      <c r="V185" s="27"/>
+      <c r="V185" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA185" s="19">
         <v>1</v>
       </c>
@@ -32959,7 +33158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:170">
+    <row r="186" spans="1:170" ht="16">
       <c r="B186" s="3" t="s">
         <v>73</v>
       </c>
@@ -32986,15 +33185,23 @@
       <c r="M186" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N186" s="27"/>
-      <c r="O186" s="27"/>
+      <c r="N186" s="33" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O186" s="33" t="s">
+        <v>1043</v>
+      </c>
       <c r="P186" s="27"/>
-      <c r="Q186" s="27"/>
+      <c r="Q186" s="27" t="s">
+        <v>1044</v>
+      </c>
       <c r="R186" s="27"/>
       <c r="S186" s="27"/>
       <c r="T186" s="27"/>
       <c r="U186" s="27"/>
-      <c r="V186" s="27"/>
+      <c r="V186" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AH186" s="19">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
☂ add full text 186 thru 200
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="0" windowWidth="18260" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="15400" yWindow="0" windowWidth="18100" windowHeight="13140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3333" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="1078">
   <si>
     <t>f</t>
   </si>
@@ -3279,6 +3279,105 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CWBFGQB568546723</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=JB4GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=zJKfSwAACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;currPage=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;source=&amp;search_within_results=&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGTTPND642362568</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=loc.ark:/13960/t5bc55t6p;view=1up;seq=7</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=2zP3MgEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=MgbSNAEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=dj4_ywAACAAJ</t>
+  </si>
+  <si>
+    <t>none;__;</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=f6oBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=1171974477</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=IWpWMwEACAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t8w95tz11;view=1up;seq=5</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CORFLVR319334513</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=9997543475</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=0Wo1AAAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=h7QnAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGMTBEB719188860</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=DPhaAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=WR4GAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=1775410706</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CSJUNWH905874220</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=mh75VL-AI-EC</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Y34GqAAACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=fAR9nQEACAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CGVFRYF005579418</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uc1.31175035208993;view=1up;seq=1</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=n0HQAAAAMAAJ</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=inu.30000011865858;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://babel.hathitrust.org/cgi/pt?id=uiuo.ark:/13960/t10p1qp5d;view=1up;seq=9</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLHFUCQ661127745</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=Tm4tMwEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=tHScbwAACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=0979587115</t>
   </si>
 </sst>
 </file>
@@ -3482,8 +3581,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="283">
+  <cellStyleXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3830,7 +3931,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="283">
+  <cellStyles count="285">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3972,6 +4073,7 @@
     <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4113,6 +4215,7 @@
     <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8211,10 +8314,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="N171" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="N183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N187" sqref="N187"/>
+      <selection pane="bottomRight" activeCell="S203" sqref="S203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33296,7 +33399,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="187" spans="1:170">
+    <row r="187" spans="1:170" ht="16">
       <c r="B187" s="3" t="s">
         <v>70</v>
       </c>
@@ -33323,15 +33426,23 @@
       <c r="M187" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N187" s="27"/>
-      <c r="O187" s="27"/>
+      <c r="N187" s="33" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O187" s="33" t="s">
+        <v>1046</v>
+      </c>
       <c r="P187" s="27"/>
-      <c r="Q187" s="27"/>
+      <c r="Q187" s="27" t="s">
+        <v>1047</v>
+      </c>
       <c r="R187" s="27"/>
       <c r="S187" s="27"/>
       <c r="T187" s="27"/>
       <c r="U187" s="27"/>
-      <c r="V187" s="27"/>
+      <c r="V187" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AM187" s="21">
         <v>1</v>
       </c>
@@ -33441,15 +33552,21 @@
       <c r="M188" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N188" s="27"/>
+      <c r="N188" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O188" s="27"/>
       <c r="P188" s="27"/>
-      <c r="Q188" s="27"/>
+      <c r="Q188" s="27" t="s">
+        <v>1048</v>
+      </c>
       <c r="R188" s="27"/>
       <c r="S188" s="27"/>
       <c r="T188" s="27"/>
       <c r="U188" s="27"/>
-      <c r="V188" s="27"/>
+      <c r="V188" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA188" s="19">
         <v>1</v>
       </c>
@@ -33565,7 +33682,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="189" spans="1:170">
+    <row r="189" spans="1:170" ht="16">
       <c r="B189" s="2" t="s">
         <v>65</v>
       </c>
@@ -33592,15 +33709,23 @@
       <c r="M189" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N189" s="27"/>
-      <c r="O189" s="27"/>
-      <c r="P189" s="27"/>
+      <c r="N189" s="33" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O189" s="33" t="s">
+        <v>1050</v>
+      </c>
+      <c r="P189" s="33" t="s">
+        <v>1051</v>
+      </c>
       <c r="Q189" s="27"/>
       <c r="R189" s="27"/>
       <c r="S189" s="27"/>
       <c r="T189" s="27"/>
       <c r="U189" s="27"/>
-      <c r="V189" s="27"/>
+      <c r="V189" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA189" s="19">
         <v>1</v>
       </c>
@@ -33695,7 +33820,9 @@
       <c r="M190" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N190" s="27"/>
+      <c r="N190" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O190" s="27"/>
       <c r="P190" s="27"/>
       <c r="Q190" s="27"/>
@@ -33703,7 +33830,9 @@
       <c r="S190" s="27"/>
       <c r="T190" s="27"/>
       <c r="U190" s="27"/>
-      <c r="V190" s="27"/>
+      <c r="V190" s="27" t="s">
+        <v>1052</v>
+      </c>
       <c r="BG190" s="3">
         <v>1</v>
       </c>
@@ -33765,7 +33894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:170">
+    <row r="191" spans="1:170" ht="16">
       <c r="B191" s="3" t="s">
         <v>57</v>
       </c>
@@ -33792,15 +33921,27 @@
       <c r="M191" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N191" s="27"/>
-      <c r="O191" s="27"/>
-      <c r="P191" s="27"/>
-      <c r="Q191" s="27"/>
-      <c r="R191" s="27"/>
+      <c r="N191" s="33" t="s">
+        <v>1053</v>
+      </c>
+      <c r="O191" s="33" t="s">
+        <v>1054</v>
+      </c>
+      <c r="P191" s="33" t="s">
+        <v>1055</v>
+      </c>
+      <c r="Q191" s="27" t="s">
+        <v>1056</v>
+      </c>
+      <c r="R191" s="27" t="s">
+        <v>1057</v>
+      </c>
       <c r="S191" s="27"/>
       <c r="T191" s="27"/>
       <c r="U191" s="27"/>
-      <c r="V191" s="27"/>
+      <c r="V191" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA191" s="19">
         <v>2</v>
       </c>
@@ -33889,7 +34030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:170">
+    <row r="192" spans="1:170" ht="16">
       <c r="B192" s="3" t="s">
         <v>57</v>
       </c>
@@ -33916,7 +34057,9 @@
       <c r="M192" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N192" s="27"/>
+      <c r="N192" s="33" t="s">
+        <v>1058</v>
+      </c>
       <c r="O192" s="27"/>
       <c r="P192" s="27"/>
       <c r="Q192" s="27"/>
@@ -33924,7 +34067,9 @@
       <c r="S192" s="27"/>
       <c r="T192" s="27"/>
       <c r="U192" s="27"/>
-      <c r="V192" s="27"/>
+      <c r="V192" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AT192" s="3">
         <v>1</v>
       </c>
@@ -34037,7 +34182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:170">
+    <row r="193" spans="2:170" ht="16">
       <c r="B193" s="3" t="s">
         <v>57</v>
       </c>
@@ -34064,15 +34209,23 @@
       <c r="M193" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N193" s="27"/>
-      <c r="O193" s="27"/>
+      <c r="N193" s="33" t="s">
+        <v>1059</v>
+      </c>
+      <c r="O193" s="33" t="s">
+        <v>1060</v>
+      </c>
       <c r="P193" s="27"/>
-      <c r="Q193" s="27"/>
+      <c r="Q193" s="27" t="s">
+        <v>1061</v>
+      </c>
       <c r="R193" s="27"/>
       <c r="S193" s="27"/>
       <c r="T193" s="27"/>
       <c r="U193" s="27"/>
-      <c r="V193" s="27"/>
+      <c r="V193" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA193" s="19">
         <v>1</v>
       </c>
@@ -34147,7 +34300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="2:170">
+    <row r="194" spans="2:170" ht="16">
       <c r="B194" s="3" t="s">
         <v>55</v>
       </c>
@@ -34174,15 +34327,25 @@
       <c r="M194" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N194" s="27"/>
-      <c r="O194" s="27"/>
-      <c r="P194" s="27"/>
-      <c r="Q194" s="27"/>
+      <c r="N194" s="33" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O194" s="33" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P194" s="33" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Q194" s="27" t="s">
+        <v>1065</v>
+      </c>
       <c r="R194" s="27"/>
       <c r="S194" s="27"/>
       <c r="T194" s="27"/>
       <c r="U194" s="27"/>
-      <c r="V194" s="27"/>
+      <c r="V194" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AH194" s="19">
         <v>1</v>
       </c>
@@ -34304,7 +34467,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="195" spans="2:170">
+    <row r="195" spans="2:170" ht="16">
       <c r="B195" s="3" t="s">
         <v>52</v>
       </c>
@@ -34331,15 +34494,25 @@
       <c r="M195" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N195" s="27"/>
-      <c r="O195" s="27"/>
-      <c r="P195" s="27"/>
-      <c r="Q195" s="27"/>
+      <c r="N195" s="33" t="s">
+        <v>1066</v>
+      </c>
+      <c r="O195" s="33" t="s">
+        <v>1067</v>
+      </c>
+      <c r="P195" s="33" t="s">
+        <v>1068</v>
+      </c>
+      <c r="Q195" s="27" t="s">
+        <v>1069</v>
+      </c>
       <c r="R195" s="27"/>
       <c r="S195" s="27"/>
       <c r="T195" s="27"/>
       <c r="U195" s="27"/>
-      <c r="V195" s="27"/>
+      <c r="V195" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA195" s="19">
         <v>2</v>
       </c>
@@ -34419,15 +34592,21 @@
       <c r="M196" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N196" s="27"/>
+      <c r="N196" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O196" s="27"/>
       <c r="P196" s="27"/>
-      <c r="Q196" s="27"/>
+      <c r="Q196" s="27" t="s">
+        <v>1070</v>
+      </c>
       <c r="R196" s="27"/>
       <c r="S196" s="27"/>
       <c r="T196" s="27"/>
       <c r="U196" s="27"/>
-      <c r="V196" s="27"/>
+      <c r="V196" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="BB196" s="21">
         <v>1</v>
       </c>
@@ -34486,7 +34665,9 @@
       <c r="M197" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N197" s="27"/>
+      <c r="N197" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O197" s="27"/>
       <c r="P197" s="27"/>
       <c r="Q197" s="27"/>
@@ -34494,7 +34675,9 @@
       <c r="S197" s="27"/>
       <c r="T197" s="27"/>
       <c r="U197" s="27"/>
-      <c r="V197" s="27"/>
+      <c r="V197" s="27" t="s">
+        <v>981</v>
+      </c>
       <c r="BY197" s="21">
         <v>1</v>
       </c>
@@ -34505,7 +34688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:170">
+    <row r="198" spans="2:170" ht="16">
       <c r="B198" s="3" t="s">
         <v>48</v>
       </c>
@@ -34532,15 +34715,25 @@
       <c r="M198" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N198" s="27"/>
+      <c r="N198" s="33" t="s">
+        <v>1071</v>
+      </c>
       <c r="O198" s="27"/>
       <c r="P198" s="27"/>
-      <c r="Q198" s="27"/>
-      <c r="R198" s="27"/>
-      <c r="S198" s="27"/>
+      <c r="Q198" s="27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="R198" s="27" t="s">
+        <v>1073</v>
+      </c>
+      <c r="S198" s="27" t="s">
+        <v>1074</v>
+      </c>
       <c r="T198" s="27"/>
       <c r="U198" s="27"/>
-      <c r="V198" s="27"/>
+      <c r="V198" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AO198" s="21">
         <v>1</v>
       </c>
@@ -34572,7 +34765,9 @@
       <c r="M199" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N199" s="27"/>
+      <c r="N199" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O199" s="27"/>
       <c r="P199" s="27"/>
       <c r="Q199" s="27"/>
@@ -34580,7 +34775,9 @@
       <c r="S199" s="27"/>
       <c r="T199" s="27"/>
       <c r="U199" s="27"/>
-      <c r="V199" s="27"/>
+      <c r="V199" s="27" t="s">
+        <v>788</v>
+      </c>
       <c r="AM199" s="21">
         <v>1</v>
       </c>
@@ -34594,7 +34791,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="200" spans="2:170">
+    <row r="200" spans="2:170" ht="16">
       <c r="B200" s="3" t="s">
         <v>34</v>
       </c>
@@ -34621,15 +34818,23 @@
       <c r="M200" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N200" s="27"/>
-      <c r="O200" s="27"/>
-      <c r="P200" s="27"/>
+      <c r="N200" s="33" t="s">
+        <v>1075</v>
+      </c>
+      <c r="O200" s="33" t="s">
+        <v>1076</v>
+      </c>
+      <c r="P200" s="33" t="s">
+        <v>1077</v>
+      </c>
       <c r="Q200" s="27"/>
       <c r="R200" s="27"/>
       <c r="S200" s="27"/>
       <c r="T200" s="27"/>
       <c r="U200" s="27"/>
-      <c r="V200" s="27"/>
+      <c r="V200" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA200" s="19">
         <v>1</v>
       </c>
@@ -34775,7 +34980,9 @@
       <c r="M201" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N201" s="27"/>
+      <c r="N201" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O201" s="27"/>
       <c r="P201" s="27"/>
       <c r="Q201" s="27"/>
@@ -34783,7 +34990,9 @@
       <c r="S201" s="27"/>
       <c r="T201" s="27"/>
       <c r="U201" s="27"/>
-      <c r="V201" s="27"/>
+      <c r="V201" s="27" t="s">
+        <v>749</v>
+      </c>
       <c r="AA201" s="19">
         <v>1</v>
       </c>
@@ -35805,6 +36014,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
☂ add full text 201 thru 208 {fin}
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3413" uniqueCount="1092">
   <si>
     <t>f</t>
   </si>
@@ -3378,6 +3378,138 @@
   </si>
   <si>
     <t>books.google.com/books?isbn=0979587115</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=6sjdGwAACAAJ</t>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=4-A4AQAAMAAJ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?id=7_U7nQEACAAJ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.google.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF006621"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s?isbn=1170760066</t>
+    </r>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CSVPCUC341647438</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLNCNJI956080038</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=P8TGoAEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=1165106442</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=nqcBAAAAQAAJ</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJQGMCA030701507</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=3628137101</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=ixTeoAEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=3628489881</t>
+  </si>
+  <si>
+    <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJKKYMN411610255</t>
   </si>
 </sst>
 </file>
@@ -8314,10 +8446,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="N183" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="N187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S203" sqref="S203"/>
+      <selection pane="bottomRight" activeCell="R210" sqref="R210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -35090,7 +35222,9 @@
       <c r="M202" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N202" s="27"/>
+      <c r="N202" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O202" s="27"/>
       <c r="P202" s="27"/>
       <c r="Q202" s="27"/>
@@ -35098,7 +35232,9 @@
       <c r="S202" s="27"/>
       <c r="T202" s="27"/>
       <c r="U202" s="27"/>
-      <c r="V202" s="27"/>
+      <c r="V202" s="27" t="s">
+        <v>807</v>
+      </c>
       <c r="AA202" s="19">
         <v>1</v>
       </c>
@@ -35166,7 +35302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:170">
+    <row r="203" spans="2:170" ht="16">
       <c r="B203" s="3" t="s">
         <v>34</v>
       </c>
@@ -35193,15 +35329,21 @@
       <c r="M203" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N203" s="27"/>
-      <c r="O203" s="27"/>
+      <c r="N203" s="33" t="s">
+        <v>1078</v>
+      </c>
+      <c r="O203" s="33" t="s">
+        <v>1077</v>
+      </c>
       <c r="P203" s="27"/>
       <c r="Q203" s="27"/>
       <c r="R203" s="27"/>
       <c r="S203" s="27"/>
       <c r="T203" s="27"/>
       <c r="U203" s="27"/>
-      <c r="V203" s="27"/>
+      <c r="V203" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AA203" s="19">
         <v>1</v>
       </c>
@@ -35245,7 +35387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="2:170">
+    <row r="204" spans="2:170" ht="16">
       <c r="B204" s="3" t="s">
         <v>29</v>
       </c>
@@ -35272,15 +35414,23 @@
       <c r="M204" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N204" s="27"/>
-      <c r="O204" s="27"/>
-      <c r="P204" s="27"/>
+      <c r="N204" s="34" t="s">
+        <v>1079</v>
+      </c>
+      <c r="O204" s="34" t="s">
+        <v>1080</v>
+      </c>
+      <c r="P204" s="34" t="s">
+        <v>1081</v>
+      </c>
       <c r="Q204" s="27"/>
       <c r="R204" s="27"/>
       <c r="S204" s="27"/>
       <c r="T204" s="27"/>
       <c r="U204" s="27"/>
-      <c r="V204" s="27"/>
+      <c r="V204" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AL204" s="3">
         <v>1</v>
       </c>
@@ -35347,15 +35497,21 @@
       <c r="M205" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N205" s="27"/>
+      <c r="N205" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O205" s="27"/>
       <c r="P205" s="27"/>
-      <c r="Q205" s="27"/>
+      <c r="Q205" s="27" t="s">
+        <v>1082</v>
+      </c>
       <c r="R205" s="27"/>
       <c r="S205" s="27"/>
       <c r="T205" s="27"/>
       <c r="U205" s="27"/>
-      <c r="V205" s="27"/>
+      <c r="V205" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="AF205" s="3">
         <v>1</v>
       </c>
@@ -35510,15 +35666,21 @@
       <c r="M206" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N206" s="27"/>
+      <c r="N206" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O206" s="27"/>
       <c r="P206" s="27"/>
-      <c r="Q206" s="27"/>
+      <c r="Q206" s="27" t="s">
+        <v>1083</v>
+      </c>
       <c r="R206" s="27"/>
       <c r="S206" s="27"/>
       <c r="T206" s="27"/>
       <c r="U206" s="27"/>
-      <c r="V206" s="27"/>
+      <c r="V206" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AM206" s="21">
         <v>1</v>
       </c>
@@ -35568,7 +35730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="2:170">
+    <row r="207" spans="2:170" ht="16">
       <c r="B207" s="3" t="s">
         <v>16</v>
       </c>
@@ -35595,15 +35757,25 @@
       <c r="M207" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N207" s="27"/>
-      <c r="O207" s="27"/>
-      <c r="P207" s="27"/>
-      <c r="Q207" s="27"/>
+      <c r="N207" s="33" t="s">
+        <v>1084</v>
+      </c>
+      <c r="O207" s="33" t="s">
+        <v>1085</v>
+      </c>
+      <c r="P207" s="33" t="s">
+        <v>1086</v>
+      </c>
+      <c r="Q207" s="27" t="s">
+        <v>1087</v>
+      </c>
       <c r="R207" s="27"/>
       <c r="S207" s="27"/>
       <c r="T207" s="27"/>
       <c r="U207" s="27"/>
-      <c r="V207" s="27"/>
+      <c r="V207" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AE207" s="21">
         <v>1</v>
       </c>
@@ -35730,7 +35902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="2:170">
+    <row r="208" spans="2:170" ht="16">
       <c r="B208" s="3" t="s">
         <v>16</v>
       </c>
@@ -35757,15 +35929,25 @@
       <c r="M208" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N208" s="27"/>
-      <c r="O208" s="27"/>
-      <c r="P208" s="27"/>
-      <c r="Q208" s="27"/>
+      <c r="N208" s="33" t="s">
+        <v>1088</v>
+      </c>
+      <c r="O208" s="33" t="s">
+        <v>1089</v>
+      </c>
+      <c r="P208" s="33" t="s">
+        <v>1090</v>
+      </c>
+      <c r="Q208" s="27" t="s">
+        <v>1091</v>
+      </c>
       <c r="R208" s="27"/>
       <c r="S208" s="27"/>
       <c r="T208" s="27"/>
       <c r="U208" s="27"/>
-      <c r="V208" s="27"/>
+      <c r="V208" s="27" t="s">
+        <v>599</v>
+      </c>
       <c r="AA208" s="19">
         <v>1</v>
       </c>
@@ -35974,7 +36156,9 @@
       <c r="M209" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N209" s="27"/>
+      <c r="N209" s="27" t="s">
+        <v>669</v>
+      </c>
       <c r="O209" s="27"/>
       <c r="P209" s="27"/>
       <c r="Q209" s="27"/>
@@ -35982,7 +36166,9 @@
       <c r="S209" s="27"/>
       <c r="T209" s="27"/>
       <c r="U209" s="27"/>
-      <c r="V209" s="27"/>
+      <c r="V209" s="27" t="s">
+        <v>664</v>
+      </c>
       <c r="AT209" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
settings to 138 ✿
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="0" windowWidth="18100" windowHeight="13140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3413" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3427" uniqueCount="1095">
   <si>
     <t>f</t>
   </si>
@@ -2987,39 +2987,6 @@
     <t>books.google.com/books?id=mT9WAAAAcAAJ</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=cZk_AAAAYAAJ</t>
-    </r>
-  </si>
-  <si>
     <t>http://babel.hathitrust.org/cgi/pt?id=dul1.ark:/13960/t5q822n9w;view=1up;seq=5</t>
   </si>
   <si>
@@ -3107,111 +3074,12 @@
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CLHIOMG185603352</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=zmIzAQAAMAAJ</t>
-    </r>
-  </si>
-  <si>
     <t>http://babel.hathitrust.org/cgi/pt?id=inu.30000091678395;view=1up;seq=7</t>
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CKIXTNH657247573</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=jyZMAAAAcAAJ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=4cvvngEACAAJ</t>
-    </r>
-  </si>
-  <si>
     <t>http://babel.hathitrust.org/cgi/pt?id=nyp.33433074910815;view=1up;seq=7</t>
   </si>
   <si>
@@ -3383,105 +3251,6 @@
     <t>books.google.com/books?id=6sjdGwAACAAJ</t>
   </si>
   <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=4-A4AQAAMAAJ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?id=7_U7nQEACAAJ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.google.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>book</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s?isbn=1170760066</t>
-    </r>
-  </si>
-  <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CSVPCUC341647438</t>
   </si>
   <si>
@@ -3510,13 +3279,43 @@
   </si>
   <si>
     <t>http://gdc.galegroup.com.ezproxy.library.uvic.ca/gdc/ncco/MonographsDetailsPage/MonographsDetailsWindow?failOverType=&amp;query=&amp;prodId=NCCO&amp;windowstate=normal&amp;contentModules=&amp;display-query=&amp;mode=view&amp;displayGroupName=DVI-Monographs&amp;dviSelectedPage=1&amp;limiter=&amp;u=uvictoria&amp;currPage=&amp;source=&amp;disableHighlighting=false&amp;displayGroups=&amp;sortBy=&amp;search_within_results=&amp;p=NCCO&amp;action=e&amp;catId=&amp;activityType=&amp;scanId=&amp;documentId=GALE%7CJKKYMN411610255</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=cZk_AAAAYAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=zmIzAQAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=jyZMAAAAcAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=4cvvngEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=4-A4AQAAMAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?id=7_U7nQEACAAJ</t>
+  </si>
+  <si>
+    <t>books.google.com/books?isbn=1170760066</t>
+  </si>
+  <si>
+    <t>Switzerland/France, Italy</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>French</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3567,25 +3366,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4000,7 +3781,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4059,9 +3840,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="285">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7877,6 +7655,112 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -8003,112 +7887,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -8446,10 +8224,10 @@
   <dimension ref="A1:FN209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="N187" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R210" sqref="R210"/>
+      <selection pane="bottomRight" activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12768,11 +12546,11 @@
       <c r="M32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N32" s="32" t="s">
+      <c r="N32" s="31" t="s">
         <v>676</v>
       </c>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
       <c r="Q32" s="27"/>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -12977,11 +12755,11 @@
       <c r="M33" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N33" s="32" t="s">
+      <c r="N33" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
       <c r="Q33" s="27"/>
       <c r="R33" s="27"/>
       <c r="S33" s="27"/>
@@ -13070,11 +12848,11 @@
       <c r="M34" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N34" s="32" t="s">
+      <c r="N34" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
       <c r="Q34" s="27"/>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -13310,11 +13088,11 @@
       <c r="M35" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="32" t="s">
+      <c r="N35" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
       <c r="Q35" s="27" t="s">
         <v>677</v>
       </c>
@@ -13417,11 +13195,11 @@
       <c r="M36" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N36" s="32" t="s">
+      <c r="N36" s="31" t="s">
         <v>678</v>
       </c>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
       <c r="Q36" s="27" t="s">
         <v>679</v>
       </c>
@@ -13555,11 +13333,11 @@
       <c r="M37" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N37" s="32" t="s">
+      <c r="N37" s="31" t="s">
         <v>680</v>
       </c>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
       <c r="Q37" s="27" t="s">
         <v>681</v>
       </c>
@@ -13697,11 +13475,11 @@
       <c r="M38" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N38" s="32" t="s">
+      <c r="N38" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
       <c r="Q38" s="27" t="s">
         <v>682</v>
       </c>
@@ -13798,11 +13576,11 @@
       <c r="M39" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N39" s="32" t="s">
+      <c r="N39" s="31" t="s">
         <v>684</v>
       </c>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
       <c r="Q39" s="27" t="s">
         <v>685</v>
       </c>
@@ -13955,11 +13733,11 @@
       <c r="M40" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N40" s="32" t="s">
+      <c r="N40" s="31" t="s">
         <v>842</v>
       </c>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
       <c r="Q40" s="27" t="s">
         <v>843</v>
       </c>
@@ -14015,11 +13793,11 @@
       <c r="M41" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N41" s="32" t="s">
+      <c r="N41" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
       <c r="Q41" s="27" t="s">
         <v>705</v>
       </c>
@@ -14145,11 +13923,11 @@
       <c r="M42" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N42" s="32" t="s">
+      <c r="N42" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
       <c r="Q42" s="27" t="s">
         <v>708</v>
       </c>
@@ -14296,11 +14074,11 @@
       <c r="M43" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N43" s="32" t="s">
+      <c r="N43" s="31" t="s">
         <v>716</v>
       </c>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
       <c r="Q43" s="27" t="s">
         <v>711</v>
       </c>
@@ -14443,13 +14221,13 @@
       <c r="M44" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N44" s="32" t="s">
+      <c r="N44" s="31" t="s">
         <v>717</v>
       </c>
-      <c r="O44" s="32" t="s">
+      <c r="O44" s="31" t="s">
         <v>718</v>
       </c>
-      <c r="P44" s="32" t="s">
+      <c r="P44" s="31" t="s">
         <v>718</v>
       </c>
       <c r="Q44" s="27" t="s">
@@ -14594,11 +14372,11 @@
       <c r="M45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N45" s="32" t="s">
+      <c r="N45" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
       <c r="Q45" s="27" t="s">
         <v>723</v>
       </c>
@@ -14692,11 +14470,11 @@
       <c r="M46" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N46" s="32" t="s">
+      <c r="N46" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
       <c r="S46" s="27"/>
@@ -14837,11 +14615,11 @@
       <c r="M47" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N47" s="32" t="s">
+      <c r="N47" s="31" t="s">
         <v>724</v>
       </c>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
       <c r="Q47" s="27" t="s">
         <v>725</v>
       </c>
@@ -14939,11 +14717,11 @@
       <c r="M48" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="N48" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
       <c r="Q48" s="27" t="s">
         <v>726</v>
       </c>
@@ -15127,11 +14905,11 @@
       <c r="M49" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N49" s="32" t="s">
+      <c r="N49" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
       <c r="Q49" s="27" t="s">
         <v>729</v>
       </c>
@@ -15261,11 +15039,11 @@
       <c r="M50" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N50" s="32" t="s">
+      <c r="N50" s="31" t="s">
         <v>730</v>
       </c>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
       <c r="Q50" s="27" t="s">
         <v>731</v>
       </c>
@@ -15438,13 +15216,13 @@
       <c r="M51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N51" s="32" t="s">
+      <c r="N51" s="31" t="s">
         <v>734</v>
       </c>
-      <c r="O51" s="32" t="s">
+      <c r="O51" s="31" t="s">
         <v>735</v>
       </c>
-      <c r="P51" s="32"/>
+      <c r="P51" s="31"/>
       <c r="Q51" s="27" t="s">
         <v>736</v>
       </c>
@@ -15562,13 +15340,13 @@
       <c r="M52" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N52" s="32" t="s">
+      <c r="N52" s="31" t="s">
         <v>740</v>
       </c>
-      <c r="O52" s="32" t="s">
+      <c r="O52" s="31" t="s">
         <v>741</v>
       </c>
-      <c r="P52" s="32" t="s">
+      <c r="P52" s="31" t="s">
         <v>742</v>
       </c>
       <c r="Q52" s="27" t="s">
@@ -15672,11 +15450,11 @@
       <c r="M53" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N53" s="32" t="s">
+      <c r="N53" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="31"/>
       <c r="Q53" s="27"/>
       <c r="R53" s="27"/>
       <c r="S53" s="27"/>
@@ -15777,11 +15555,11 @@
       <c r="M54" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N54" s="32" t="s">
+      <c r="N54" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="31"/>
       <c r="Q54" s="27" t="s">
         <v>745</v>
       </c>
@@ -15905,11 +15683,11 @@
       <c r="M55" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N55" s="32" t="s">
+      <c r="N55" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
       <c r="Q55" s="27" t="s">
         <v>746</v>
       </c>
@@ -16041,11 +15819,11 @@
       <c r="M56" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="32" t="s">
+      <c r="N56" s="31" t="s">
         <v>747</v>
       </c>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32"/>
+      <c r="O56" s="31"/>
+      <c r="P56" s="31"/>
       <c r="Q56" s="27" t="s">
         <v>748</v>
       </c>
@@ -16151,11 +15929,11 @@
       <c r="M57" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N57" s="32" t="s">
+      <c r="N57" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
+      <c r="O57" s="31"/>
+      <c r="P57" s="31"/>
       <c r="Q57" s="27"/>
       <c r="R57" s="27"/>
       <c r="S57" s="27"/>
@@ -16291,11 +16069,11 @@
       <c r="M58" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N58" s="32" t="s">
+      <c r="N58" s="31" t="s">
         <v>750</v>
       </c>
-      <c r="O58" s="32"/>
-      <c r="P58" s="32"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
       <c r="Q58" s="27"/>
       <c r="R58" s="27"/>
       <c r="S58" s="27"/>
@@ -16420,11 +16198,11 @@
       <c r="M59" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N59" s="32" t="s">
+      <c r="N59" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O59" s="32"/>
-      <c r="P59" s="32"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
       <c r="Q59" s="27" t="s">
         <v>751</v>
       </c>
@@ -16509,11 +16287,11 @@
       <c r="M60" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N60" s="32" t="s">
+      <c r="N60" s="31" t="s">
         <v>753</v>
       </c>
-      <c r="O60" s="32"/>
-      <c r="P60" s="32"/>
+      <c r="O60" s="31"/>
+      <c r="P60" s="31"/>
       <c r="Q60" s="27" t="s">
         <v>754</v>
       </c>
@@ -16670,11 +16448,11 @@
       <c r="M61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N61" s="32" t="s">
+      <c r="N61" s="31" t="s">
         <v>755</v>
       </c>
-      <c r="O61" s="32"/>
-      <c r="P61" s="32"/>
+      <c r="O61" s="31"/>
+      <c r="P61" s="31"/>
       <c r="Q61" s="27" t="s">
         <v>756</v>
       </c>
@@ -16807,11 +16585,11 @@
       <c r="M62" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N62" s="32" t="s">
+      <c r="N62" s="31" t="s">
         <v>757</v>
       </c>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
+      <c r="O62" s="31"/>
+      <c r="P62" s="31"/>
       <c r="Q62" s="27" t="s">
         <v>758</v>
       </c>
@@ -16958,11 +16736,11 @@
       <c r="M63" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N63" s="32" t="s">
+      <c r="N63" s="31" t="s">
         <v>759</v>
       </c>
-      <c r="O63" s="32"/>
-      <c r="P63" s="32"/>
+      <c r="O63" s="31"/>
+      <c r="P63" s="31"/>
       <c r="Q63" s="27"/>
       <c r="R63" s="27"/>
       <c r="S63" s="27"/>
@@ -17141,11 +16919,11 @@
       <c r="M64" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="32" t="s">
+      <c r="N64" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O64" s="32"/>
-      <c r="P64" s="32"/>
+      <c r="O64" s="31"/>
+      <c r="P64" s="31"/>
       <c r="Q64" s="27" t="s">
         <v>760</v>
       </c>
@@ -17227,11 +17005,11 @@
       <c r="M65" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N65" s="32" t="s">
+      <c r="N65" s="31" t="s">
         <v>761</v>
       </c>
-      <c r="O65" s="32"/>
-      <c r="P65" s="32"/>
+      <c r="O65" s="31"/>
+      <c r="P65" s="31"/>
       <c r="Q65" s="27" t="s">
         <v>762</v>
       </c>
@@ -17436,11 +17214,11 @@
       <c r="M66" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N66" s="32" t="s">
+      <c r="N66" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O66" s="32"/>
-      <c r="P66" s="32"/>
+      <c r="O66" s="31"/>
+      <c r="P66" s="31"/>
       <c r="Q66" s="27" t="s">
         <v>766</v>
       </c>
@@ -17599,11 +17377,11 @@
       <c r="M67" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N67" s="32" t="s">
+      <c r="N67" s="31" t="s">
         <v>768</v>
       </c>
-      <c r="O67" s="32"/>
-      <c r="P67" s="32"/>
+      <c r="O67" s="31"/>
+      <c r="P67" s="31"/>
       <c r="Q67" s="27" t="s">
         <v>769</v>
       </c>
@@ -17747,11 +17525,11 @@
       <c r="M68" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N68" s="32" t="s">
+      <c r="N68" s="31" t="s">
         <v>771</v>
       </c>
-      <c r="O68" s="32"/>
-      <c r="P68" s="32"/>
+      <c r="O68" s="31"/>
+      <c r="P68" s="31"/>
       <c r="Q68" s="27" t="s">
         <v>772</v>
       </c>
@@ -17838,11 +17616,11 @@
       <c r="M69" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N69" s="32" t="s">
+      <c r="N69" s="31" t="s">
         <v>963</v>
       </c>
-      <c r="O69" s="32"/>
-      <c r="P69" s="32"/>
+      <c r="O69" s="31"/>
+      <c r="P69" s="31"/>
       <c r="Q69" s="27" t="s">
         <v>773</v>
       </c>
@@ -17958,11 +17736,11 @@
       <c r="M70" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N70" s="32" t="s">
+      <c r="N70" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O70" s="32"/>
-      <c r="P70" s="32"/>
+      <c r="O70" s="31"/>
+      <c r="P70" s="31"/>
       <c r="Q70" s="27" t="s">
         <v>775</v>
       </c>
@@ -18108,11 +17886,11 @@
       <c r="M71" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N71" s="32" t="s">
+      <c r="N71" s="31" t="s">
         <v>777</v>
       </c>
-      <c r="O71" s="32"/>
-      <c r="P71" s="32"/>
+      <c r="O71" s="31"/>
+      <c r="P71" s="31"/>
       <c r="Q71" s="27" t="s">
         <v>778</v>
       </c>
@@ -18313,11 +18091,11 @@
       <c r="M72" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N72" s="32" t="s">
+      <c r="N72" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O72" s="32"/>
-      <c r="P72" s="32"/>
+      <c r="O72" s="31"/>
+      <c r="P72" s="31"/>
       <c r="Q72" s="27"/>
       <c r="R72" s="27"/>
       <c r="S72" s="27"/>
@@ -18501,11 +18279,11 @@
       <c r="M73" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N73" s="32" t="s">
+      <c r="N73" s="31" t="s">
         <v>780</v>
       </c>
-      <c r="O73" s="32"/>
-      <c r="P73" s="32"/>
+      <c r="O73" s="31"/>
+      <c r="P73" s="31"/>
       <c r="Q73" s="27" t="s">
         <v>781</v>
       </c>
@@ -18572,11 +18350,11 @@
       <c r="M74" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N74" s="32" t="s">
+      <c r="N74" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O74" s="32"/>
-      <c r="P74" s="32"/>
+      <c r="O74" s="31"/>
+      <c r="P74" s="31"/>
       <c r="Q74" s="27" t="s">
         <v>784</v>
       </c>
@@ -18672,11 +18450,11 @@
       <c r="M75" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N75" s="32" t="s">
+      <c r="N75" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O75" s="32"/>
-      <c r="P75" s="32"/>
+      <c r="O75" s="31"/>
+      <c r="P75" s="31"/>
       <c r="Q75" s="27" t="s">
         <v>785</v>
       </c>
@@ -18864,11 +18642,11 @@
       <c r="M76" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N76" s="32" t="s">
+      <c r="N76" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O76" s="32"/>
-      <c r="P76" s="32"/>
+      <c r="O76" s="31"/>
+      <c r="P76" s="31"/>
       <c r="Q76" s="27" t="s">
         <v>787</v>
       </c>
@@ -19076,11 +18854,11 @@
       <c r="M77" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N77" s="32" t="s">
+      <c r="N77" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O77" s="32"/>
-      <c r="P77" s="32"/>
+      <c r="O77" s="31"/>
+      <c r="P77" s="31"/>
       <c r="Q77" s="27"/>
       <c r="R77" s="27"/>
       <c r="S77" s="27"/>
@@ -19277,11 +19055,11 @@
       <c r="M78" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N78" s="32" t="s">
+      <c r="N78" s="31" t="s">
         <v>789</v>
       </c>
-      <c r="O78" s="32"/>
-      <c r="P78" s="32"/>
+      <c r="O78" s="31"/>
+      <c r="P78" s="31"/>
       <c r="Q78" s="27" t="s">
         <v>790</v>
       </c>
@@ -19405,11 +19183,11 @@
       <c r="M79" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N79" s="32" t="s">
+      <c r="N79" s="31" t="s">
         <v>791</v>
       </c>
-      <c r="O79" s="32"/>
-      <c r="P79" s="32"/>
+      <c r="O79" s="31"/>
+      <c r="P79" s="31"/>
       <c r="Q79" s="27" t="s">
         <v>792</v>
       </c>
@@ -19548,11 +19326,11 @@
       <c r="M80" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N80" s="32" t="s">
+      <c r="N80" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O80" s="32"/>
-      <c r="P80" s="32"/>
+      <c r="O80" s="31"/>
+      <c r="P80" s="31"/>
       <c r="Q80" s="27" t="s">
         <v>793</v>
       </c>
@@ -19643,11 +19421,11 @@
       <c r="M81" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N81" s="32" t="s">
+      <c r="N81" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O81" s="32"/>
-      <c r="P81" s="32"/>
+      <c r="O81" s="31"/>
+      <c r="P81" s="31"/>
       <c r="Q81" s="27" t="s">
         <v>794</v>
       </c>
@@ -19790,11 +19568,11 @@
       <c r="M82" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N82" s="32" t="s">
+      <c r="N82" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O82" s="32"/>
-      <c r="P82" s="32"/>
+      <c r="O82" s="31"/>
+      <c r="P82" s="31"/>
       <c r="Q82" s="27"/>
       <c r="R82" s="27"/>
       <c r="S82" s="27"/>
@@ -19891,11 +19669,11 @@
       <c r="M83" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N83" s="32" t="s">
+      <c r="N83" s="31" t="s">
         <v>797</v>
       </c>
-      <c r="O83" s="32"/>
-      <c r="P83" s="32"/>
+      <c r="O83" s="31"/>
+      <c r="P83" s="31"/>
       <c r="Q83" s="27" t="s">
         <v>798</v>
       </c>
@@ -20030,11 +19808,11 @@
       <c r="M84" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N84" s="32" t="s">
+      <c r="N84" s="31" t="s">
         <v>800</v>
       </c>
-      <c r="O84" s="32"/>
-      <c r="P84" s="32"/>
+      <c r="O84" s="31"/>
+      <c r="P84" s="31"/>
       <c r="Q84" s="27" t="s">
         <v>801</v>
       </c>
@@ -20233,11 +20011,11 @@
       <c r="M85" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N85" s="32" t="s">
+      <c r="N85" s="31" t="s">
         <v>802</v>
       </c>
-      <c r="O85" s="32"/>
-      <c r="P85" s="32"/>
+      <c r="O85" s="31"/>
+      <c r="P85" s="31"/>
       <c r="Q85" s="27" t="s">
         <v>803</v>
       </c>
@@ -20318,11 +20096,11 @@
       <c r="M86" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N86" s="32" t="s">
+      <c r="N86" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O86" s="32"/>
-      <c r="P86" s="32"/>
+      <c r="O86" s="31"/>
+      <c r="P86" s="31"/>
       <c r="Q86" s="27"/>
       <c r="R86" s="27"/>
       <c r="S86" s="27"/>
@@ -20488,11 +20266,11 @@
       <c r="M87" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N87" s="32" t="s">
+      <c r="N87" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O87" s="32"/>
-      <c r="P87" s="32"/>
+      <c r="O87" s="31"/>
+      <c r="P87" s="31"/>
       <c r="Q87" s="27" t="s">
         <v>806</v>
       </c>
@@ -20678,11 +20456,11 @@
       <c r="M88" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N88" s="32" t="s">
+      <c r="N88" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O88" s="32"/>
-      <c r="P88" s="32"/>
+      <c r="O88" s="31"/>
+      <c r="P88" s="31"/>
       <c r="Q88" s="27"/>
       <c r="R88" s="27"/>
       <c r="S88" s="27"/>
@@ -20833,11 +20611,11 @@
       <c r="M89" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N89" s="32" t="s">
+      <c r="N89" s="31" t="s">
         <v>808</v>
       </c>
-      <c r="O89" s="32"/>
-      <c r="P89" s="32"/>
+      <c r="O89" s="31"/>
+      <c r="P89" s="31"/>
       <c r="Q89" s="27" t="s">
         <v>809</v>
       </c>
@@ -20981,11 +20759,11 @@
       <c r="M90" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N90" s="32" t="s">
+      <c r="N90" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O90" s="32"/>
-      <c r="P90" s="32"/>
+      <c r="O90" s="31"/>
+      <c r="P90" s="31"/>
       <c r="Q90" s="27" t="s">
         <v>811</v>
       </c>
@@ -21078,13 +20856,13 @@
       <c r="M91" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N91" s="32" t="s">
+      <c r="N91" s="31" t="s">
         <v>812</v>
       </c>
-      <c r="O91" s="32" t="s">
+      <c r="O91" s="31" t="s">
         <v>813</v>
       </c>
-      <c r="P91" s="32"/>
+      <c r="P91" s="31"/>
       <c r="Q91" s="27" t="s">
         <v>814</v>
       </c>
@@ -21244,11 +21022,11 @@
       <c r="M92" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N92" s="32" t="s">
+      <c r="N92" s="31" t="s">
         <v>815</v>
       </c>
-      <c r="O92" s="32"/>
-      <c r="P92" s="32"/>
+      <c r="O92" s="31"/>
+      <c r="P92" s="31"/>
       <c r="Q92" s="27" t="s">
         <v>816</v>
       </c>
@@ -21353,13 +21131,13 @@
       <c r="M93" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N93" s="32" t="s">
+      <c r="N93" s="31" t="s">
         <v>817</v>
       </c>
-      <c r="O93" s="32" t="s">
+      <c r="O93" s="31" t="s">
         <v>818</v>
       </c>
-      <c r="P93" s="32" t="s">
+      <c r="P93" s="31" t="s">
         <v>819</v>
       </c>
       <c r="Q93" s="27" t="s">
@@ -21524,11 +21302,11 @@
       <c r="M94" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N94" s="32" t="s">
+      <c r="N94" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O94" s="32"/>
-      <c r="P94" s="32"/>
+      <c r="O94" s="31"/>
+      <c r="P94" s="31"/>
       <c r="Q94" s="27"/>
       <c r="R94" s="27"/>
       <c r="S94" s="27"/>
@@ -21619,11 +21397,11 @@
       <c r="M95" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N95" s="32" t="s">
+      <c r="N95" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O95" s="32"/>
-      <c r="P95" s="32"/>
+      <c r="O95" s="31"/>
+      <c r="P95" s="31"/>
       <c r="Q95" s="27" t="s">
         <v>822</v>
       </c>
@@ -21704,11 +21482,11 @@
       <c r="M96" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N96" s="32" t="s">
+      <c r="N96" s="31" t="s">
         <v>823</v>
       </c>
-      <c r="O96" s="32"/>
-      <c r="P96" s="32"/>
+      <c r="O96" s="31"/>
+      <c r="P96" s="31"/>
       <c r="Q96" s="27" t="s">
         <v>824</v>
       </c>
@@ -21882,11 +21660,11 @@
       <c r="M97" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N97" s="32" t="s">
+      <c r="N97" s="31" t="s">
         <v>825</v>
       </c>
-      <c r="O97" s="32"/>
-      <c r="P97" s="32"/>
+      <c r="O97" s="31"/>
+      <c r="P97" s="31"/>
       <c r="Q97" s="27" t="s">
         <v>826</v>
       </c>
@@ -21958,11 +21736,11 @@
       <c r="M98" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N98" s="32" t="s">
+      <c r="N98" s="31" t="s">
         <v>827</v>
       </c>
-      <c r="O98" s="32"/>
-      <c r="P98" s="32"/>
+      <c r="O98" s="31"/>
+      <c r="P98" s="31"/>
       <c r="Q98" s="27" t="s">
         <v>828</v>
       </c>
@@ -22170,11 +21948,11 @@
       <c r="M99" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N99" s="32" t="s">
+      <c r="N99" s="31" t="s">
         <v>831</v>
       </c>
-      <c r="O99" s="32"/>
-      <c r="P99" s="32"/>
+      <c r="O99" s="31"/>
+      <c r="P99" s="31"/>
       <c r="Q99" s="27" t="s">
         <v>832</v>
       </c>
@@ -22270,13 +22048,13 @@
       <c r="M100" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N100" s="32" t="s">
+      <c r="N100" s="31" t="s">
         <v>833</v>
       </c>
-      <c r="O100" s="32" t="s">
+      <c r="O100" s="31" t="s">
         <v>834</v>
       </c>
-      <c r="P100" s="32"/>
+      <c r="P100" s="31"/>
       <c r="Q100" s="27" t="s">
         <v>835</v>
       </c>
@@ -22547,11 +22325,11 @@
       <c r="M101" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N101" s="32" t="s">
+      <c r="N101" s="31" t="s">
         <v>838</v>
       </c>
-      <c r="O101" s="32"/>
-      <c r="P101" s="32"/>
+      <c r="O101" s="31"/>
+      <c r="P101" s="31"/>
       <c r="Q101" s="27" t="s">
         <v>839</v>
       </c>
@@ -22723,13 +22501,13 @@
       <c r="M102" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N102" s="32" t="s">
+      <c r="N102" s="31" t="s">
         <v>844</v>
       </c>
-      <c r="O102" s="32" t="s">
+      <c r="O102" s="31" t="s">
         <v>845</v>
       </c>
-      <c r="P102" s="32"/>
+      <c r="P102" s="31"/>
       <c r="Q102" s="27" t="s">
         <v>846</v>
       </c>
@@ -22849,11 +22627,11 @@
       <c r="M103" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N103" s="32" t="s">
+      <c r="N103" s="31" t="s">
         <v>848</v>
       </c>
-      <c r="O103" s="32"/>
-      <c r="P103" s="32"/>
+      <c r="O103" s="31"/>
+      <c r="P103" s="31"/>
       <c r="Q103" s="27"/>
       <c r="R103" s="27"/>
       <c r="S103" s="27"/>
@@ -22935,11 +22713,11 @@
       <c r="M104" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N104" s="32" t="s">
+      <c r="N104" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O104" s="32"/>
-      <c r="P104" s="32"/>
+      <c r="O104" s="31"/>
+      <c r="P104" s="31"/>
       <c r="Q104" s="27" t="s">
         <v>849</v>
       </c>
@@ -22999,13 +22777,13 @@
       <c r="M105" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N105" s="32" t="s">
+      <c r="N105" s="31" t="s">
         <v>850</v>
       </c>
-      <c r="O105" s="32" t="s">
+      <c r="O105" s="31" t="s">
         <v>851</v>
       </c>
-      <c r="P105" s="32"/>
+      <c r="P105" s="31"/>
       <c r="Q105" s="27" t="s">
         <v>852</v>
       </c>
@@ -23118,11 +22896,11 @@
       <c r="M106" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N106" s="32" t="s">
+      <c r="N106" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O106" s="32"/>
-      <c r="P106" s="32"/>
+      <c r="O106" s="31"/>
+      <c r="P106" s="31"/>
       <c r="Q106" s="27"/>
       <c r="R106" s="27"/>
       <c r="S106" s="27"/>
@@ -23199,11 +22977,11 @@
       <c r="M107" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N107" s="32" t="s">
+      <c r="N107" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O107" s="32"/>
-      <c r="P107" s="32"/>
+      <c r="O107" s="31"/>
+      <c r="P107" s="31"/>
       <c r="Q107" s="27"/>
       <c r="R107" s="27"/>
       <c r="S107" s="27"/>
@@ -23309,11 +23087,11 @@
       <c r="M108" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N108" s="32" t="s">
+      <c r="N108" s="31" t="s">
         <v>854</v>
       </c>
-      <c r="O108" s="32"/>
-      <c r="P108" s="32"/>
+      <c r="O108" s="31"/>
+      <c r="P108" s="31"/>
       <c r="Q108" s="27" t="s">
         <v>855</v>
       </c>
@@ -23490,11 +23268,11 @@
       <c r="M109" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N109" s="32" t="s">
+      <c r="N109" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O109" s="32"/>
-      <c r="P109" s="32"/>
+      <c r="O109" s="31"/>
+      <c r="P109" s="31"/>
       <c r="Q109" s="27" t="s">
         <v>858</v>
       </c>
@@ -23686,11 +23464,11 @@
       <c r="M110" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N110" s="32" t="s">
+      <c r="N110" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O110" s="32"/>
-      <c r="P110" s="32"/>
+      <c r="O110" s="31"/>
+      <c r="P110" s="31"/>
       <c r="Q110" s="27" t="s">
         <v>859</v>
       </c>
@@ -23898,11 +23676,11 @@
       <c r="M111" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N111" s="32" t="s">
+      <c r="N111" s="31" t="s">
         <v>860</v>
       </c>
-      <c r="O111" s="32"/>
-      <c r="P111" s="32"/>
+      <c r="O111" s="31"/>
+      <c r="P111" s="31"/>
       <c r="Q111" s="27" t="s">
         <v>862</v>
       </c>
@@ -23980,11 +23758,11 @@
       <c r="M112" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N112" s="32" t="s">
+      <c r="N112" s="31" t="s">
         <v>863</v>
       </c>
-      <c r="O112" s="32"/>
-      <c r="P112" s="32"/>
+      <c r="O112" s="31"/>
+      <c r="P112" s="31"/>
       <c r="Q112" s="27" t="s">
         <v>864</v>
       </c>
@@ -24113,11 +23891,11 @@
       <c r="M113" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N113" s="32" t="s">
+      <c r="N113" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O113" s="32"/>
-      <c r="P113" s="32"/>
+      <c r="O113" s="31"/>
+      <c r="P113" s="31"/>
       <c r="Q113" s="27"/>
       <c r="R113" s="27"/>
       <c r="S113" s="27"/>
@@ -24271,11 +24049,11 @@
       <c r="M114" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N114" s="32" t="s">
+      <c r="N114" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O114" s="32"/>
-      <c r="P114" s="32"/>
+      <c r="O114" s="31"/>
+      <c r="P114" s="31"/>
       <c r="Q114" s="27" t="s">
         <v>865</v>
       </c>
@@ -24371,11 +24149,11 @@
       <c r="M115" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N115" s="32" t="s">
+      <c r="N115" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O115" s="32"/>
-      <c r="P115" s="32"/>
+      <c r="O115" s="31"/>
+      <c r="P115" s="31"/>
       <c r="Q115" s="27" t="s">
         <v>866</v>
       </c>
@@ -24519,11 +24297,11 @@
       <c r="M116" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N116" s="32" t="s">
+      <c r="N116" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O116" s="32"/>
-      <c r="P116" s="32"/>
+      <c r="O116" s="31"/>
+      <c r="P116" s="31"/>
       <c r="Q116" s="27" t="s">
         <v>867</v>
       </c>
@@ -24599,11 +24377,11 @@
       <c r="M117" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N117" s="32" t="s">
+      <c r="N117" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O117" s="32"/>
-      <c r="P117" s="32"/>
+      <c r="O117" s="31"/>
+      <c r="P117" s="31"/>
       <c r="Q117" s="27"/>
       <c r="R117" s="27"/>
       <c r="S117" s="27"/>
@@ -24736,11 +24514,11 @@
       <c r="M118" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N118" s="32" t="s">
+      <c r="N118" s="31" t="s">
         <v>868</v>
       </c>
-      <c r="O118" s="32"/>
-      <c r="P118" s="32"/>
+      <c r="O118" s="31"/>
+      <c r="P118" s="31"/>
       <c r="Q118" s="27"/>
       <c r="R118" s="27"/>
       <c r="S118" s="27"/>
@@ -24849,11 +24627,11 @@
       <c r="M119" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N119" s="32" t="s">
+      <c r="N119" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O119" s="32"/>
-      <c r="P119" s="32"/>
+      <c r="O119" s="31"/>
+      <c r="P119" s="31"/>
       <c r="Q119" s="27" t="s">
         <v>869</v>
       </c>
@@ -24976,11 +24754,11 @@
       <c r="M120" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N120" s="32" t="s">
+      <c r="N120" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O120" s="32"/>
-      <c r="P120" s="32"/>
+      <c r="O120" s="31"/>
+      <c r="P120" s="31"/>
       <c r="Q120" s="27" t="s">
         <v>871</v>
       </c>
@@ -25251,13 +25029,13 @@
       <c r="M121" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N121" s="32" t="s">
+      <c r="N121" s="31" t="s">
         <v>872</v>
       </c>
-      <c r="O121" s="32" t="s">
+      <c r="O121" s="31" t="s">
         <v>873</v>
       </c>
-      <c r="P121" s="32"/>
+      <c r="P121" s="31"/>
       <c r="Q121" s="27" t="s">
         <v>874</v>
       </c>
@@ -25422,13 +25200,13 @@
       <c r="M122" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N122" s="32" t="s">
+      <c r="N122" s="31" t="s">
         <v>878</v>
       </c>
-      <c r="O122" s="32" t="s">
+      <c r="O122" s="31" t="s">
         <v>879</v>
       </c>
-      <c r="P122" s="32"/>
+      <c r="P122" s="31"/>
       <c r="Q122" s="27" t="s">
         <v>880</v>
       </c>
@@ -25510,11 +25288,11 @@
       <c r="M123" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N123" s="32" t="s">
+      <c r="N123" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O123" s="32"/>
-      <c r="P123" s="32"/>
+      <c r="O123" s="31"/>
+      <c r="P123" s="31"/>
       <c r="Q123" s="27"/>
       <c r="R123" s="27"/>
       <c r="S123" s="27"/>
@@ -25663,11 +25441,11 @@
       <c r="M124" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N124" s="32" t="s">
+      <c r="N124" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O124" s="32"/>
-      <c r="P124" s="32"/>
+      <c r="O124" s="31"/>
+      <c r="P124" s="31"/>
       <c r="Q124" s="27"/>
       <c r="R124" s="27"/>
       <c r="S124" s="27"/>
@@ -25795,11 +25573,11 @@
       <c r="M125" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N125" s="32" t="s">
+      <c r="N125" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O125" s="32"/>
-      <c r="P125" s="32"/>
+      <c r="O125" s="31"/>
+      <c r="P125" s="31"/>
       <c r="Q125" s="27"/>
       <c r="R125" s="27"/>
       <c r="S125" s="27"/>
@@ -25860,11 +25638,11 @@
       <c r="M126" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N126" s="32" t="s">
+      <c r="N126" s="31" t="s">
         <v>884</v>
       </c>
-      <c r="O126" s="32"/>
-      <c r="P126" s="32"/>
+      <c r="O126" s="31"/>
+      <c r="P126" s="31"/>
       <c r="Q126" s="27"/>
       <c r="R126" s="27"/>
       <c r="S126" s="27"/>
@@ -25998,11 +25776,11 @@
       <c r="M127" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N127" s="32" t="s">
+      <c r="N127" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O127" s="32"/>
-      <c r="P127" s="32"/>
+      <c r="O127" s="31"/>
+      <c r="P127" s="31"/>
       <c r="Q127" s="27"/>
       <c r="R127" s="27"/>
       <c r="S127" s="27"/>
@@ -26098,11 +25876,11 @@
       <c r="M128" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N128" s="32" t="s">
+      <c r="N128" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O128" s="32"/>
-      <c r="P128" s="32"/>
+      <c r="O128" s="31"/>
+      <c r="P128" s="31"/>
       <c r="Q128" s="27"/>
       <c r="R128" s="27"/>
       <c r="S128" s="27"/>
@@ -26293,11 +26071,11 @@
       <c r="M129" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N129" s="32" t="s">
+      <c r="N129" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O129" s="32"/>
-      <c r="P129" s="32"/>
+      <c r="O129" s="31"/>
+      <c r="P129" s="31"/>
       <c r="Q129" s="27" t="s">
         <v>885</v>
       </c>
@@ -26466,11 +26244,11 @@
       <c r="M130" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N130" s="32" t="s">
+      <c r="N130" s="31" t="s">
         <v>886</v>
       </c>
-      <c r="O130" s="32"/>
-      <c r="P130" s="32"/>
+      <c r="O130" s="31"/>
+      <c r="P130" s="31"/>
       <c r="Q130" s="27" t="s">
         <v>887</v>
       </c>
@@ -26741,11 +26519,11 @@
       <c r="M131" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N131" s="32" t="s">
+      <c r="N131" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O131" s="32"/>
-      <c r="P131" s="32"/>
+      <c r="O131" s="31"/>
+      <c r="P131" s="31"/>
       <c r="Q131" s="27" t="s">
         <v>888</v>
       </c>
@@ -26951,11 +26729,11 @@
       <c r="M132" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N132" s="32" t="s">
+      <c r="N132" s="31" t="s">
         <v>889</v>
       </c>
-      <c r="O132" s="32"/>
-      <c r="P132" s="32"/>
+      <c r="O132" s="31"/>
+      <c r="P132" s="31"/>
       <c r="Q132" s="27" t="s">
         <v>890</v>
       </c>
@@ -27033,13 +26811,13 @@
       <c r="M133" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N133" s="32" t="s">
+      <c r="N133" s="31" t="s">
         <v>892</v>
       </c>
-      <c r="O133" s="32" t="s">
+      <c r="O133" s="31" t="s">
         <v>893</v>
       </c>
-      <c r="P133" s="32"/>
+      <c r="P133" s="31"/>
       <c r="Q133" s="27" t="s">
         <v>894</v>
       </c>
@@ -27135,13 +26913,13 @@
       <c r="M134" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N134" s="32" t="s">
+      <c r="N134" s="31" t="s">
         <v>897</v>
       </c>
-      <c r="O134" s="32" t="s">
+      <c r="O134" s="31" t="s">
         <v>898</v>
       </c>
-      <c r="P134" s="32"/>
+      <c r="P134" s="31"/>
       <c r="Q134" s="27" t="s">
         <v>899</v>
       </c>
@@ -27268,11 +27046,11 @@
       <c r="M135" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N135" s="32" t="s">
+      <c r="N135" s="31" t="s">
         <v>900</v>
       </c>
-      <c r="O135" s="32"/>
-      <c r="P135" s="32"/>
+      <c r="O135" s="31"/>
+      <c r="P135" s="31"/>
       <c r="Q135" s="27" t="s">
         <v>901</v>
       </c>
@@ -27391,13 +27169,13 @@
       <c r="M136" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N136" s="32" t="s">
+      <c r="N136" s="31" t="s">
         <v>902</v>
       </c>
-      <c r="O136" s="32" t="s">
+      <c r="O136" s="31" t="s">
         <v>903</v>
       </c>
-      <c r="P136" s="32"/>
+      <c r="P136" s="31"/>
       <c r="Q136" s="27" t="s">
         <v>904</v>
       </c>
@@ -27597,10 +27375,18 @@
       <c r="F137" s="18">
         <v>136</v>
       </c>
-      <c r="G137" s="27"/>
-      <c r="H137" s="27"/>
-      <c r="I137" s="27"/>
-      <c r="J137" s="27"/>
+      <c r="G137" s="27" t="s">
+        <v>1092</v>
+      </c>
+      <c r="H137" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I137" s="27" t="s">
+        <v>959</v>
+      </c>
+      <c r="J137" s="27" t="s">
+        <v>327</v>
+      </c>
       <c r="K137" s="27"/>
       <c r="L137" s="27" t="s">
         <v>533</v>
@@ -27608,13 +27394,13 @@
       <c r="M137" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N137" s="32" t="s">
+      <c r="N137" s="31" t="s">
         <v>907</v>
       </c>
-      <c r="O137" s="32" t="s">
+      <c r="O137" s="31" t="s">
         <v>908</v>
       </c>
-      <c r="P137" s="32" t="s">
+      <c r="P137" s="31" t="s">
         <v>909</v>
       </c>
       <c r="Q137" s="27" t="s">
@@ -27801,24 +27587,34 @@
       <c r="F138" s="18">
         <v>137</v>
       </c>
-      <c r="G138" s="27"/>
-      <c r="H138" s="27"/>
-      <c r="I138" s="27"/>
-      <c r="J138" s="27"/>
-      <c r="K138" s="27"/>
+      <c r="G138" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="H138" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I138" s="27" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J138" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="K138" s="27" t="s">
+        <v>1093</v>
+      </c>
       <c r="L138" s="27" t="s">
         <v>530</v>
       </c>
       <c r="M138" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N138" s="32" t="s">
+      <c r="N138" s="31" t="s">
         <v>913</v>
       </c>
-      <c r="O138" s="32" t="s">
+      <c r="O138" s="31" t="s">
         <v>914</v>
       </c>
-      <c r="P138" s="32" t="s">
+      <c r="P138" s="31" t="s">
         <v>915</v>
       </c>
       <c r="Q138" s="27" t="s">
@@ -28001,24 +27797,34 @@
       <c r="F139" s="18">
         <v>138</v>
       </c>
-      <c r="G139" s="27"/>
-      <c r="H139" s="27"/>
-      <c r="I139" s="27"/>
-      <c r="J139" s="27"/>
-      <c r="K139" s="27"/>
+      <c r="G139" s="27" t="s">
+        <v>560</v>
+      </c>
+      <c r="H139" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I139" s="27" t="s">
+        <v>959</v>
+      </c>
+      <c r="J139" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="K139" s="27" t="s">
+        <v>565</v>
+      </c>
       <c r="L139" s="27" t="s">
         <v>532</v>
       </c>
       <c r="M139" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N139" s="32" t="s">
+      <c r="N139" s="31" t="s">
         <v>917</v>
       </c>
-      <c r="O139" s="32" t="s">
+      <c r="O139" s="31" t="s">
         <v>918</v>
       </c>
-      <c r="P139" s="32" t="s">
+      <c r="P139" s="31" t="s">
         <v>919</v>
       </c>
       <c r="Q139" s="27" t="s">
@@ -28212,11 +28018,11 @@
       <c r="M140" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N140" s="32" t="s">
+      <c r="N140" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O140" s="32"/>
-      <c r="P140" s="32"/>
+      <c r="O140" s="31"/>
+      <c r="P140" s="31"/>
       <c r="Q140" s="27" t="s">
         <v>921</v>
       </c>
@@ -28363,11 +28169,11 @@
       <c r="M141" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N141" s="32" t="s">
+      <c r="N141" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O141" s="32"/>
-      <c r="P141" s="32"/>
+      <c r="O141" s="31"/>
+      <c r="P141" s="31"/>
       <c r="Q141" s="27"/>
       <c r="R141" s="27"/>
       <c r="S141" s="27"/>
@@ -28473,13 +28279,13 @@
       <c r="M142" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N142" s="32" t="s">
+      <c r="N142" s="31" t="s">
         <v>922</v>
       </c>
-      <c r="O142" s="32" t="s">
+      <c r="O142" s="31" t="s">
         <v>923</v>
       </c>
-      <c r="P142" s="32" t="s">
+      <c r="P142" s="31" t="s">
         <v>924</v>
       </c>
       <c r="Q142" s="27" t="s">
@@ -28526,13 +28332,13 @@
       <c r="M143" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N143" s="32" t="s">
+      <c r="N143" s="31" t="s">
         <v>964</v>
       </c>
-      <c r="O143" s="32" t="s">
+      <c r="O143" s="31" t="s">
         <v>965</v>
       </c>
-      <c r="P143" s="32"/>
+      <c r="P143" s="31"/>
       <c r="Q143" s="27" t="s">
         <v>926</v>
       </c>
@@ -28616,13 +28422,13 @@
       <c r="M144" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N144" s="32" t="s">
+      <c r="N144" s="31" t="s">
         <v>927</v>
       </c>
-      <c r="O144" s="32" t="s">
+      <c r="O144" s="31" t="s">
         <v>928</v>
       </c>
-      <c r="P144" s="32"/>
+      <c r="P144" s="31"/>
       <c r="Q144" s="27" t="s">
         <v>929</v>
       </c>
@@ -28707,11 +28513,11 @@
       <c r="M145" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N145" s="32" t="s">
+      <c r="N145" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O145" s="32"/>
-      <c r="P145" s="32"/>
+      <c r="O145" s="31"/>
+      <c r="P145" s="31"/>
       <c r="Q145" s="27"/>
       <c r="R145" s="27"/>
       <c r="S145" s="27"/>
@@ -28832,11 +28638,11 @@
       <c r="M146" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N146" s="32" t="s">
+      <c r="N146" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O146" s="32"/>
-      <c r="P146" s="32"/>
+      <c r="O146" s="31"/>
+      <c r="P146" s="31"/>
       <c r="Q146" s="27"/>
       <c r="R146" s="27"/>
       <c r="S146" s="27"/>
@@ -28960,11 +28766,11 @@
       <c r="M147" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N147" s="32" t="s">
+      <c r="N147" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O147" s="32"/>
-      <c r="P147" s="32"/>
+      <c r="O147" s="31"/>
+      <c r="P147" s="31"/>
       <c r="Q147" s="27" t="s">
         <v>932</v>
       </c>
@@ -29061,11 +28867,11 @@
       <c r="M148" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N148" s="32" t="s">
+      <c r="N148" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O148" s="32"/>
-      <c r="P148" s="32"/>
+      <c r="O148" s="31"/>
+      <c r="P148" s="31"/>
       <c r="Q148" s="27" t="s">
         <v>980</v>
       </c>
@@ -29152,11 +28958,11 @@
       <c r="M149" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N149" s="32" t="s">
+      <c r="N149" s="31" t="s">
         <v>935</v>
       </c>
-      <c r="O149" s="32"/>
-      <c r="P149" s="32"/>
+      <c r="O149" s="31"/>
+      <c r="P149" s="31"/>
       <c r="Q149" s="27" t="s">
         <v>936</v>
       </c>
@@ -29246,15 +29052,15 @@
       <c r="M150" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N150" s="32" t="s">
+      <c r="N150" s="31" t="s">
         <v>937</v>
       </c>
-      <c r="O150" s="32"/>
-      <c r="P150" s="32"/>
-      <c r="Q150" s="27" t="s">
+      <c r="O150" s="31"/>
+      <c r="P150" s="31"/>
+      <c r="Q150" s="31" t="s">
         <v>938</v>
       </c>
-      <c r="R150" s="27" t="s">
+      <c r="R150" s="31" t="s">
         <v>939</v>
       </c>
       <c r="S150" s="27" t="s">
@@ -29461,10 +29267,10 @@
       </c>
       <c r="O151" s="31"/>
       <c r="P151" s="31"/>
-      <c r="Q151" s="27" t="s">
+      <c r="Q151" s="31" t="s">
         <v>943</v>
       </c>
-      <c r="R151" s="27"/>
+      <c r="R151" s="31"/>
       <c r="S151" s="27"/>
       <c r="T151" s="27"/>
       <c r="U151" s="27"/>
@@ -29609,10 +29415,10 @@
       </c>
       <c r="O152" s="31"/>
       <c r="P152" s="31"/>
-      <c r="Q152" s="27" t="s">
+      <c r="Q152" s="31" t="s">
         <v>966</v>
       </c>
-      <c r="R152" s="27" t="s">
+      <c r="R152" s="31" t="s">
         <v>967</v>
       </c>
       <c r="S152" s="27"/>
@@ -29738,10 +29544,10 @@
       </c>
       <c r="O153" s="31"/>
       <c r="P153" s="31"/>
-      <c r="Q153" s="27" t="s">
+      <c r="Q153" s="31" t="s">
         <v>969</v>
       </c>
-      <c r="R153" s="27" t="s">
+      <c r="R153" s="31" t="s">
         <v>970</v>
       </c>
       <c r="S153" s="27" t="s">
@@ -29872,10 +29678,10 @@
       </c>
       <c r="O154" s="31"/>
       <c r="P154" s="31"/>
-      <c r="Q154" s="27" t="s">
+      <c r="Q154" s="31" t="s">
         <v>973</v>
       </c>
-      <c r="R154" s="27" t="s">
+      <c r="R154" s="31" t="s">
         <v>974</v>
       </c>
       <c r="S154" s="27" t="s">
@@ -29937,10 +29743,10 @@
       </c>
       <c r="O155" s="31"/>
       <c r="P155" s="31"/>
-      <c r="Q155" s="27" t="s">
+      <c r="Q155" s="31" t="s">
         <v>977</v>
       </c>
-      <c r="R155" s="27" t="s">
+      <c r="R155" s="31" t="s">
         <v>978</v>
       </c>
       <c r="S155" s="27" t="s">
@@ -30141,8 +29947,8 @@
       </c>
       <c r="O156" s="31"/>
       <c r="P156" s="31"/>
-      <c r="Q156" s="27"/>
-      <c r="R156" s="27"/>
+      <c r="Q156" s="31"/>
+      <c r="R156" s="31"/>
       <c r="S156" s="27"/>
       <c r="T156" s="27"/>
       <c r="U156" s="27"/>
@@ -30277,10 +30083,10 @@
         <v>985</v>
       </c>
       <c r="P157" s="31"/>
-      <c r="Q157" s="27" t="s">
+      <c r="Q157" s="31" t="s">
         <v>982</v>
       </c>
-      <c r="R157" s="27" t="s">
+      <c r="R157" s="31" t="s">
         <v>983</v>
       </c>
       <c r="S157" s="27"/>
@@ -30322,8 +30128,8 @@
       </c>
       <c r="O158" s="31"/>
       <c r="P158" s="31"/>
-      <c r="Q158" s="27"/>
-      <c r="R158" s="27"/>
+      <c r="Q158" s="31"/>
+      <c r="R158" s="31"/>
       <c r="S158" s="27"/>
       <c r="T158" s="27"/>
       <c r="U158" s="27"/>
@@ -30349,7 +30155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="2:170" ht="16">
+    <row r="159" spans="2:170">
       <c r="B159" s="3" t="s">
         <v>120</v>
       </c>
@@ -30376,13 +30182,13 @@
       <c r="M159" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N159" s="33" t="s">
+      <c r="N159" s="31" t="s">
         <v>986</v>
       </c>
       <c r="O159" s="31"/>
       <c r="P159" s="31"/>
-      <c r="Q159" s="27"/>
-      <c r="R159" s="27"/>
+      <c r="Q159" s="31"/>
+      <c r="R159" s="31"/>
       <c r="S159" s="27"/>
       <c r="T159" s="27"/>
       <c r="U159" s="27"/>
@@ -30423,7 +30229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:170" ht="16">
+    <row r="160" spans="2:170">
       <c r="B160" s="3" t="s">
         <v>110</v>
       </c>
@@ -30450,16 +30256,16 @@
       <c r="M160" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N160" s="34" t="s">
+      <c r="N160" s="31" t="s">
+        <v>1085</v>
+      </c>
+      <c r="O160" s="31"/>
+      <c r="P160" s="31"/>
+      <c r="Q160" s="31" t="s">
         <v>987</v>
       </c>
-      <c r="O160" s="27"/>
-      <c r="P160" s="27"/>
-      <c r="Q160" s="27" t="s">
+      <c r="R160" s="31" t="s">
         <v>988</v>
-      </c>
-      <c r="R160" s="27" t="s">
-        <v>989</v>
       </c>
       <c r="S160" s="27"/>
       <c r="T160" s="27"/>
@@ -30507,7 +30313,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="161" spans="1:170" ht="16">
+    <row r="161" spans="1:170">
       <c r="B161" s="3" t="s">
         <v>110</v>
       </c>
@@ -30534,22 +30340,22 @@
       <c r="M161" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N161" s="33" t="s">
+      <c r="N161" s="31" t="s">
+        <v>989</v>
+      </c>
+      <c r="O161" s="31"/>
+      <c r="P161" s="31"/>
+      <c r="Q161" s="31" t="s">
         <v>990</v>
       </c>
-      <c r="O161" s="27"/>
-      <c r="P161" s="27"/>
-      <c r="Q161" s="27" t="s">
+      <c r="R161" s="31" t="s">
         <v>991</v>
       </c>
-      <c r="R161" s="27" t="s">
+      <c r="S161" s="27" t="s">
         <v>992</v>
       </c>
-      <c r="S161" s="27" t="s">
+      <c r="T161" s="27" t="s">
         <v>993</v>
-      </c>
-      <c r="T161" s="27" t="s">
-        <v>994</v>
       </c>
       <c r="U161" s="27"/>
       <c r="V161" s="27" t="s">
@@ -30604,7 +30410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:170" ht="16">
+    <row r="162" spans="1:170">
       <c r="B162" s="3" t="s">
         <v>110</v>
       </c>
@@ -30631,17 +30437,17 @@
       <c r="M162" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N162" s="33" t="s">
+      <c r="N162" s="31" t="s">
+        <v>994</v>
+      </c>
+      <c r="O162" s="31" t="s">
         <v>995</v>
       </c>
-      <c r="O162" s="33" t="s">
+      <c r="P162" s="31"/>
+      <c r="Q162" s="31" t="s">
         <v>996</v>
       </c>
-      <c r="P162" s="27"/>
-      <c r="Q162" s="27" t="s">
-        <v>997</v>
-      </c>
-      <c r="R162" s="27"/>
+      <c r="R162" s="31"/>
       <c r="S162" s="27"/>
       <c r="T162" s="27"/>
       <c r="U162" s="27"/>
@@ -30688,7 +30494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:170" ht="16">
+    <row r="163" spans="1:170">
       <c r="B163" s="3" t="s">
         <v>110</v>
       </c>
@@ -30715,18 +30521,18 @@
       <c r="M163" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N163" s="33" t="s">
+      <c r="N163" s="31" t="s">
+        <v>997</v>
+      </c>
+      <c r="O163" s="31" t="s">
         <v>998</v>
       </c>
-      <c r="O163" s="33" t="s">
+      <c r="P163" s="31"/>
+      <c r="Q163" s="31" t="s">
         <v>999</v>
       </c>
-      <c r="P163" s="27"/>
-      <c r="Q163" s="27" t="s">
+      <c r="R163" s="31" t="s">
         <v>1000</v>
-      </c>
-      <c r="R163" s="27" t="s">
-        <v>1001</v>
       </c>
       <c r="S163" s="27"/>
       <c r="T163" s="27"/>
@@ -30853,7 +30659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:170" ht="16">
+    <row r="164" spans="1:170">
       <c r="B164" s="3" t="s">
         <v>110</v>
       </c>
@@ -30880,17 +30686,17 @@
       <c r="M164" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N164" s="33" t="s">
+      <c r="N164" s="31" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O164" s="31" t="s">
         <v>1002</v>
       </c>
-      <c r="O164" s="33" t="s">
+      <c r="P164" s="31"/>
+      <c r="Q164" s="31" t="s">
         <v>1003</v>
       </c>
-      <c r="P164" s="27"/>
-      <c r="Q164" s="27" t="s">
-        <v>1004</v>
-      </c>
-      <c r="R164" s="27"/>
+      <c r="R164" s="31"/>
       <c r="S164" s="27"/>
       <c r="T164" s="27"/>
       <c r="U164" s="27"/>
@@ -30949,15 +30755,15 @@
       <c r="M165" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N165" s="27" t="s">
+      <c r="N165" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O165" s="27"/>
-      <c r="P165" s="27"/>
-      <c r="Q165" s="27" t="s">
-        <v>1005</v>
-      </c>
-      <c r="R165" s="27"/>
+      <c r="O165" s="31"/>
+      <c r="P165" s="31"/>
+      <c r="Q165" s="31" t="s">
+        <v>1004</v>
+      </c>
+      <c r="R165" s="31"/>
       <c r="S165" s="27"/>
       <c r="T165" s="27"/>
       <c r="U165" s="27"/>
@@ -30986,7 +30792,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:170" ht="16">
+    <row r="166" spans="1:170">
       <c r="B166" s="3" t="s">
         <v>110</v>
       </c>
@@ -31013,16 +30819,16 @@
       <c r="M166" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N166" s="33" t="s">
+      <c r="N166" s="31" t="s">
+        <v>1005</v>
+      </c>
+      <c r="O166" s="31"/>
+      <c r="P166" s="31"/>
+      <c r="Q166" s="31" t="s">
         <v>1006</v>
       </c>
-      <c r="O166" s="27"/>
-      <c r="P166" s="27"/>
-      <c r="Q166" s="27" t="s">
+      <c r="R166" s="31" t="s">
         <v>1007</v>
-      </c>
-      <c r="R166" s="27" t="s">
-        <v>1008</v>
       </c>
       <c r="S166" s="27"/>
       <c r="T166" s="27"/>
@@ -31121,7 +30927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:170" ht="16">
+    <row r="167" spans="1:170">
       <c r="B167" s="3" t="s">
         <v>107</v>
       </c>
@@ -31148,13 +30954,13 @@
       <c r="M167" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N167" s="33" t="s">
+      <c r="N167" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O167" s="27"/>
-      <c r="P167" s="27"/>
-      <c r="Q167" s="27"/>
-      <c r="R167" s="27"/>
+      <c r="O167" s="31"/>
+      <c r="P167" s="31"/>
+      <c r="Q167" s="31"/>
+      <c r="R167" s="31"/>
       <c r="S167" s="27"/>
       <c r="T167" s="27"/>
       <c r="U167" s="27"/>
@@ -31267,15 +31073,15 @@
       <c r="M168" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N168" s="27" t="s">
+      <c r="N168" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O168" s="27"/>
-      <c r="P168" s="27"/>
-      <c r="Q168" s="27" t="s">
-        <v>1009</v>
-      </c>
-      <c r="R168" s="27"/>
+      <c r="O168" s="31"/>
+      <c r="P168" s="31"/>
+      <c r="Q168" s="31" t="s">
+        <v>1008</v>
+      </c>
+      <c r="R168" s="31"/>
       <c r="S168" s="27"/>
       <c r="T168" s="27"/>
       <c r="U168" s="27"/>
@@ -31376,15 +31182,15 @@
       <c r="M169" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N169" s="27" t="s">
+      <c r="N169" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O169" s="27"/>
-      <c r="P169" s="27"/>
-      <c r="Q169" s="27" t="s">
-        <v>1010</v>
-      </c>
-      <c r="R169" s="27"/>
+      <c r="O169" s="31"/>
+      <c r="P169" s="31"/>
+      <c r="Q169" s="31" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R169" s="31"/>
       <c r="S169" s="27"/>
       <c r="T169" s="27"/>
       <c r="U169" s="27"/>
@@ -31536,15 +31342,15 @@
       <c r="M170" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N170" s="27" t="s">
+      <c r="N170" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O170" s="27"/>
-      <c r="P170" s="27"/>
-      <c r="Q170" s="27" t="s">
-        <v>1011</v>
-      </c>
-      <c r="R170" s="27"/>
+      <c r="O170" s="31"/>
+      <c r="P170" s="31"/>
+      <c r="Q170" s="31" t="s">
+        <v>1010</v>
+      </c>
+      <c r="R170" s="31"/>
       <c r="S170" s="27"/>
       <c r="T170" s="27"/>
       <c r="U170" s="27"/>
@@ -31588,7 +31394,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="171" spans="1:170" ht="16">
+    <row r="171" spans="1:170">
       <c r="B171" s="3" t="s">
         <v>98</v>
       </c>
@@ -31615,15 +31421,15 @@
       <c r="M171" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N171" s="33" t="s">
+      <c r="N171" s="31" t="s">
+        <v>1011</v>
+      </c>
+      <c r="O171" s="31"/>
+      <c r="P171" s="31"/>
+      <c r="Q171" s="31" t="s">
         <v>1012</v>
       </c>
-      <c r="O171" s="27"/>
-      <c r="P171" s="27"/>
-      <c r="Q171" s="27" t="s">
-        <v>1013</v>
-      </c>
-      <c r="R171" s="27"/>
+      <c r="R171" s="31"/>
       <c r="S171" s="27"/>
       <c r="T171" s="27"/>
       <c r="U171" s="27"/>
@@ -31728,18 +31534,18 @@
       <c r="M172" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N172" s="27" t="s">
+      <c r="N172" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O172" s="27"/>
-      <c r="P172" s="27"/>
-      <c r="Q172" s="27"/>
-      <c r="R172" s="27"/>
+      <c r="O172" s="31"/>
+      <c r="P172" s="31"/>
+      <c r="Q172" s="31"/>
+      <c r="R172" s="31"/>
       <c r="S172" s="27"/>
       <c r="T172" s="27"/>
       <c r="U172" s="27"/>
       <c r="V172" s="27" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="W172" s="19">
         <v>1</v>
@@ -31862,15 +31668,15 @@
       <c r="M173" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N173" s="27" t="s">
+      <c r="N173" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O173" s="27"/>
-      <c r="P173" s="27"/>
-      <c r="Q173" s="27" t="s">
-        <v>1015</v>
-      </c>
-      <c r="R173" s="27"/>
+      <c r="O173" s="31"/>
+      <c r="P173" s="31"/>
+      <c r="Q173" s="31" t="s">
+        <v>1014</v>
+      </c>
+      <c r="R173" s="31"/>
       <c r="S173" s="27"/>
       <c r="T173" s="27"/>
       <c r="U173" s="27"/>
@@ -31990,13 +31796,13 @@
       <c r="M174" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N174" s="27" t="s">
+      <c r="N174" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O174" s="27"/>
-      <c r="P174" s="27"/>
-      <c r="Q174" s="27"/>
-      <c r="R174" s="27"/>
+      <c r="O174" s="31"/>
+      <c r="P174" s="31"/>
+      <c r="Q174" s="31"/>
+      <c r="R174" s="31"/>
       <c r="S174" s="27"/>
       <c r="T174" s="27"/>
       <c r="U174" s="27"/>
@@ -32076,15 +31882,15 @@
       <c r="M175" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N175" s="27" t="s">
+      <c r="N175" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O175" s="27"/>
-      <c r="P175" s="27"/>
-      <c r="Q175" s="27" t="s">
-        <v>1016</v>
-      </c>
-      <c r="R175" s="27"/>
+      <c r="O175" s="31"/>
+      <c r="P175" s="31"/>
+      <c r="Q175" s="31" t="s">
+        <v>1015</v>
+      </c>
+      <c r="R175" s="31"/>
       <c r="S175" s="27"/>
       <c r="T175" s="27"/>
       <c r="U175" s="27"/>
@@ -32248,7 +32054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="176" spans="1:170" ht="16">
+    <row r="176" spans="1:170">
       <c r="B176" s="3" t="s">
         <v>92</v>
       </c>
@@ -32275,16 +32081,16 @@
       <c r="M176" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N176" s="34" t="s">
+      <c r="N176" s="31" t="s">
+        <v>1086</v>
+      </c>
+      <c r="O176" s="31"/>
+      <c r="P176" s="31"/>
+      <c r="Q176" s="31" t="s">
+        <v>1016</v>
+      </c>
+      <c r="R176" s="31" t="s">
         <v>1017</v>
-      </c>
-      <c r="O176" s="27"/>
-      <c r="P176" s="27"/>
-      <c r="Q176" s="27" t="s">
-        <v>1018</v>
-      </c>
-      <c r="R176" s="27" t="s">
-        <v>1019</v>
       </c>
       <c r="S176" s="27"/>
       <c r="T176" s="27"/>
@@ -32353,7 +32159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:170" ht="16">
+    <row r="177" spans="1:170">
       <c r="B177" s="3" t="s">
         <v>92</v>
       </c>
@@ -32380,17 +32186,17 @@
       <c r="M177" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N177" s="34" t="s">
-        <v>1020</v>
-      </c>
-      <c r="O177" s="34" t="s">
-        <v>1021</v>
-      </c>
-      <c r="P177" s="27"/>
-      <c r="Q177" s="27" t="s">
-        <v>1022</v>
-      </c>
-      <c r="R177" s="27"/>
+      <c r="N177" s="31" t="s">
+        <v>1087</v>
+      </c>
+      <c r="O177" s="31" t="s">
+        <v>1088</v>
+      </c>
+      <c r="P177" s="31"/>
+      <c r="Q177" s="31" t="s">
+        <v>1018</v>
+      </c>
+      <c r="R177" s="31"/>
       <c r="S177" s="27"/>
       <c r="T177" s="27"/>
       <c r="U177" s="27"/>
@@ -32428,7 +32234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:170" ht="16">
+    <row r="178" spans="1:170">
       <c r="A178" s="3" t="s">
         <v>89</v>
       </c>
@@ -32458,17 +32264,17 @@
       <c r="M178" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N178" s="33" t="s">
-        <v>1023</v>
-      </c>
-      <c r="O178" s="33" t="s">
-        <v>1024</v>
-      </c>
-      <c r="P178" s="33" t="s">
-        <v>1025</v>
-      </c>
-      <c r="Q178" s="27"/>
-      <c r="R178" s="27"/>
+      <c r="N178" s="31" t="s">
+        <v>1019</v>
+      </c>
+      <c r="O178" s="31" t="s">
+        <v>1020</v>
+      </c>
+      <c r="P178" s="31" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q178" s="31"/>
+      <c r="R178" s="31"/>
       <c r="S178" s="27"/>
       <c r="T178" s="27"/>
       <c r="U178" s="27"/>
@@ -32612,7 +32418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:170" ht="16">
+    <row r="179" spans="1:170">
       <c r="B179" s="3" t="s">
         <v>73</v>
       </c>
@@ -32639,18 +32445,18 @@
       <c r="M179" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N179" s="33" t="s">
-        <v>1026</v>
-      </c>
-      <c r="O179" s="33" t="s">
-        <v>1027</v>
-      </c>
-      <c r="P179" s="27"/>
-      <c r="Q179" s="27" t="s">
-        <v>1028</v>
-      </c>
-      <c r="R179" s="27" t="s">
-        <v>1029</v>
+      <c r="N179" s="31" t="s">
+        <v>1022</v>
+      </c>
+      <c r="O179" s="31" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P179" s="31"/>
+      <c r="Q179" s="31" t="s">
+        <v>1024</v>
+      </c>
+      <c r="R179" s="31" t="s">
+        <v>1025</v>
       </c>
       <c r="S179" s="27"/>
       <c r="T179" s="27"/>
@@ -32737,7 +32543,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:170" ht="16">
+    <row r="180" spans="1:170">
       <c r="B180" s="3" t="s">
         <v>73</v>
       </c>
@@ -32764,15 +32570,15 @@
       <c r="M180" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N180" s="33" t="s">
-        <v>1030</v>
-      </c>
-      <c r="O180" s="27"/>
-      <c r="P180" s="27"/>
-      <c r="Q180" s="27" t="s">
-        <v>1031</v>
-      </c>
-      <c r="R180" s="27"/>
+      <c r="N180" s="31" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O180" s="31"/>
+      <c r="P180" s="31"/>
+      <c r="Q180" s="31" t="s">
+        <v>1027</v>
+      </c>
+      <c r="R180" s="31"/>
       <c r="S180" s="27"/>
       <c r="T180" s="27"/>
       <c r="U180" s="27"/>
@@ -32822,7 +32628,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="181" spans="1:170" ht="16">
+    <row r="181" spans="1:170">
       <c r="B181" s="3" t="s">
         <v>73</v>
       </c>
@@ -32849,17 +32655,17 @@
       <c r="M181" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N181" s="33" t="s">
-        <v>1032</v>
-      </c>
-      <c r="O181" s="33" t="s">
-        <v>1033</v>
-      </c>
-      <c r="P181" s="27"/>
-      <c r="Q181" s="27" t="s">
-        <v>1034</v>
-      </c>
-      <c r="R181" s="27"/>
+      <c r="N181" s="31" t="s">
+        <v>1028</v>
+      </c>
+      <c r="O181" s="31" t="s">
+        <v>1029</v>
+      </c>
+      <c r="P181" s="31"/>
+      <c r="Q181" s="31" t="s">
+        <v>1030</v>
+      </c>
+      <c r="R181" s="31"/>
       <c r="S181" s="27"/>
       <c r="T181" s="27"/>
       <c r="U181" s="27"/>
@@ -32996,7 +32802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="182" spans="1:170" ht="16">
+    <row r="182" spans="1:170">
       <c r="B182" s="3" t="s">
         <v>73</v>
       </c>
@@ -33023,15 +32829,15 @@
       <c r="M182" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N182" s="33" t="s">
-        <v>1035</v>
-      </c>
-      <c r="O182" s="27"/>
-      <c r="P182" s="27"/>
-      <c r="Q182" s="27" t="s">
-        <v>1036</v>
-      </c>
-      <c r="R182" s="27"/>
+      <c r="N182" s="31" t="s">
+        <v>1031</v>
+      </c>
+      <c r="O182" s="31"/>
+      <c r="P182" s="31"/>
+      <c r="Q182" s="31" t="s">
+        <v>1032</v>
+      </c>
+      <c r="R182" s="31"/>
       <c r="S182" s="27"/>
       <c r="T182" s="27"/>
       <c r="U182" s="27"/>
@@ -33102,13 +32908,13 @@
       <c r="M183" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N183" s="27" t="s">
+      <c r="N183" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O183" s="27"/>
-      <c r="P183" s="27"/>
-      <c r="Q183" s="27"/>
-      <c r="R183" s="27"/>
+      <c r="O183" s="31"/>
+      <c r="P183" s="31"/>
+      <c r="Q183" s="31"/>
+      <c r="R183" s="31"/>
       <c r="S183" s="27"/>
       <c r="T183" s="27"/>
       <c r="U183" s="27"/>
@@ -33185,7 +32991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:170" ht="16">
+    <row r="184" spans="1:170">
       <c r="B184" s="3" t="s">
         <v>73</v>
       </c>
@@ -33212,15 +33018,15 @@
       <c r="M184" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N184" s="33" t="s">
-        <v>1037</v>
-      </c>
-      <c r="O184" s="27"/>
-      <c r="P184" s="27"/>
-      <c r="Q184" s="27" t="s">
-        <v>1038</v>
-      </c>
-      <c r="R184" s="27"/>
+      <c r="N184" s="31" t="s">
+        <v>1033</v>
+      </c>
+      <c r="O184" s="31"/>
+      <c r="P184" s="31"/>
+      <c r="Q184" s="31" t="s">
+        <v>1034</v>
+      </c>
+      <c r="R184" s="31"/>
       <c r="S184" s="27"/>
       <c r="T184" s="27"/>
       <c r="U184" s="27"/>
@@ -33306,7 +33112,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="185" spans="1:170" ht="16">
+    <row r="185" spans="1:170">
       <c r="B185" s="3" t="s">
         <v>73</v>
       </c>
@@ -33333,17 +33139,17 @@
       <c r="M185" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N185" s="33" t="s">
-        <v>1039</v>
-      </c>
-      <c r="O185" s="33" t="s">
-        <v>1040</v>
-      </c>
-      <c r="P185" s="27"/>
-      <c r="Q185" s="27" t="s">
-        <v>1041</v>
-      </c>
-      <c r="R185" s="27"/>
+      <c r="N185" s="31" t="s">
+        <v>1035</v>
+      </c>
+      <c r="O185" s="31" t="s">
+        <v>1036</v>
+      </c>
+      <c r="P185" s="31"/>
+      <c r="Q185" s="31" t="s">
+        <v>1037</v>
+      </c>
+      <c r="R185" s="31"/>
       <c r="S185" s="27"/>
       <c r="T185" s="27"/>
       <c r="U185" s="27"/>
@@ -33393,7 +33199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:170" ht="16">
+    <row r="186" spans="1:170">
       <c r="B186" s="3" t="s">
         <v>73</v>
       </c>
@@ -33420,17 +33226,17 @@
       <c r="M186" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N186" s="33" t="s">
-        <v>1042</v>
-      </c>
-      <c r="O186" s="33" t="s">
-        <v>1043</v>
-      </c>
-      <c r="P186" s="27"/>
-      <c r="Q186" s="27" t="s">
-        <v>1044</v>
-      </c>
-      <c r="R186" s="27"/>
+      <c r="N186" s="31" t="s">
+        <v>1038</v>
+      </c>
+      <c r="O186" s="31" t="s">
+        <v>1039</v>
+      </c>
+      <c r="P186" s="31"/>
+      <c r="Q186" s="31" t="s">
+        <v>1040</v>
+      </c>
+      <c r="R186" s="31"/>
       <c r="S186" s="27"/>
       <c r="T186" s="27"/>
       <c r="U186" s="27"/>
@@ -33531,7 +33337,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="187" spans="1:170" ht="16">
+    <row r="187" spans="1:170">
       <c r="B187" s="3" t="s">
         <v>70</v>
       </c>
@@ -33558,17 +33364,17 @@
       <c r="M187" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N187" s="33" t="s">
-        <v>1045</v>
-      </c>
-      <c r="O187" s="33" t="s">
-        <v>1046</v>
-      </c>
-      <c r="P187" s="27"/>
-      <c r="Q187" s="27" t="s">
-        <v>1047</v>
-      </c>
-      <c r="R187" s="27"/>
+      <c r="N187" s="31" t="s">
+        <v>1041</v>
+      </c>
+      <c r="O187" s="31" t="s">
+        <v>1042</v>
+      </c>
+      <c r="P187" s="31"/>
+      <c r="Q187" s="31" t="s">
+        <v>1043</v>
+      </c>
+      <c r="R187" s="31"/>
       <c r="S187" s="27"/>
       <c r="T187" s="27"/>
       <c r="U187" s="27"/>
@@ -33684,15 +33490,15 @@
       <c r="M188" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N188" s="27" t="s">
+      <c r="N188" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O188" s="27"/>
-      <c r="P188" s="27"/>
-      <c r="Q188" s="27" t="s">
-        <v>1048</v>
-      </c>
-      <c r="R188" s="27"/>
+      <c r="O188" s="31"/>
+      <c r="P188" s="31"/>
+      <c r="Q188" s="31" t="s">
+        <v>1044</v>
+      </c>
+      <c r="R188" s="31"/>
       <c r="S188" s="27"/>
       <c r="T188" s="27"/>
       <c r="U188" s="27"/>
@@ -33814,7 +33620,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="189" spans="1:170" ht="16">
+    <row r="189" spans="1:170">
       <c r="B189" s="2" t="s">
         <v>65</v>
       </c>
@@ -33841,17 +33647,17 @@
       <c r="M189" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N189" s="33" t="s">
-        <v>1049</v>
-      </c>
-      <c r="O189" s="33" t="s">
-        <v>1050</v>
-      </c>
-      <c r="P189" s="33" t="s">
-        <v>1051</v>
-      </c>
-      <c r="Q189" s="27"/>
-      <c r="R189" s="27"/>
+      <c r="N189" s="31" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O189" s="31" t="s">
+        <v>1046</v>
+      </c>
+      <c r="P189" s="31" t="s">
+        <v>1047</v>
+      </c>
+      <c r="Q189" s="31"/>
+      <c r="R189" s="31"/>
       <c r="S189" s="27"/>
       <c r="T189" s="27"/>
       <c r="U189" s="27"/>
@@ -33952,18 +33758,18 @@
       <c r="M190" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N190" s="27" t="s">
+      <c r="N190" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O190" s="27"/>
-      <c r="P190" s="27"/>
-      <c r="Q190" s="27"/>
-      <c r="R190" s="27"/>
+      <c r="O190" s="31"/>
+      <c r="P190" s="31"/>
+      <c r="Q190" s="31"/>
+      <c r="R190" s="31"/>
       <c r="S190" s="27"/>
       <c r="T190" s="27"/>
       <c r="U190" s="27"/>
       <c r="V190" s="27" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="BG190" s="3">
         <v>1</v>
@@ -34026,7 +33832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:170" ht="16">
+    <row r="191" spans="1:170">
       <c r="B191" s="3" t="s">
         <v>57</v>
       </c>
@@ -34053,20 +33859,20 @@
       <c r="M191" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N191" s="33" t="s">
+      <c r="N191" s="31" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O191" s="31" t="s">
+        <v>1050</v>
+      </c>
+      <c r="P191" s="31" t="s">
+        <v>1051</v>
+      </c>
+      <c r="Q191" s="31" t="s">
+        <v>1052</v>
+      </c>
+      <c r="R191" s="31" t="s">
         <v>1053</v>
-      </c>
-      <c r="O191" s="33" t="s">
-        <v>1054</v>
-      </c>
-      <c r="P191" s="33" t="s">
-        <v>1055</v>
-      </c>
-      <c r="Q191" s="27" t="s">
-        <v>1056</v>
-      </c>
-      <c r="R191" s="27" t="s">
-        <v>1057</v>
       </c>
       <c r="S191" s="27"/>
       <c r="T191" s="27"/>
@@ -34162,7 +33968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:170" ht="16">
+    <row r="192" spans="1:170">
       <c r="B192" s="3" t="s">
         <v>57</v>
       </c>
@@ -34189,13 +33995,13 @@
       <c r="M192" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N192" s="33" t="s">
-        <v>1058</v>
-      </c>
-      <c r="O192" s="27"/>
-      <c r="P192" s="27"/>
-      <c r="Q192" s="27"/>
-      <c r="R192" s="27"/>
+      <c r="N192" s="31" t="s">
+        <v>1054</v>
+      </c>
+      <c r="O192" s="31"/>
+      <c r="P192" s="31"/>
+      <c r="Q192" s="31"/>
+      <c r="R192" s="31"/>
       <c r="S192" s="27"/>
       <c r="T192" s="27"/>
       <c r="U192" s="27"/>
@@ -34314,7 +34120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:170" ht="16">
+    <row r="193" spans="2:170">
       <c r="B193" s="3" t="s">
         <v>57</v>
       </c>
@@ -34341,17 +34147,17 @@
       <c r="M193" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N193" s="33" t="s">
-        <v>1059</v>
-      </c>
-      <c r="O193" s="33" t="s">
-        <v>1060</v>
-      </c>
-      <c r="P193" s="27"/>
-      <c r="Q193" s="27" t="s">
-        <v>1061</v>
-      </c>
-      <c r="R193" s="27"/>
+      <c r="N193" s="31" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O193" s="31" t="s">
+        <v>1056</v>
+      </c>
+      <c r="P193" s="31"/>
+      <c r="Q193" s="31" t="s">
+        <v>1057</v>
+      </c>
+      <c r="R193" s="31"/>
       <c r="S193" s="27"/>
       <c r="T193" s="27"/>
       <c r="U193" s="27"/>
@@ -34432,7 +34238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="2:170" ht="16">
+    <row r="194" spans="2:170">
       <c r="B194" s="3" t="s">
         <v>55</v>
       </c>
@@ -34459,19 +34265,19 @@
       <c r="M194" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N194" s="33" t="s">
-        <v>1062</v>
-      </c>
-      <c r="O194" s="33" t="s">
-        <v>1063</v>
-      </c>
-      <c r="P194" s="33" t="s">
-        <v>1064</v>
-      </c>
-      <c r="Q194" s="27" t="s">
-        <v>1065</v>
-      </c>
-      <c r="R194" s="27"/>
+      <c r="N194" s="31" t="s">
+        <v>1058</v>
+      </c>
+      <c r="O194" s="31" t="s">
+        <v>1059</v>
+      </c>
+      <c r="P194" s="31" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Q194" s="31" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R194" s="31"/>
       <c r="S194" s="27"/>
       <c r="T194" s="27"/>
       <c r="U194" s="27"/>
@@ -34599,7 +34405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="195" spans="2:170" ht="16">
+    <row r="195" spans="2:170">
       <c r="B195" s="3" t="s">
         <v>52</v>
       </c>
@@ -34626,19 +34432,19 @@
       <c r="M195" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N195" s="33" t="s">
-        <v>1066</v>
-      </c>
-      <c r="O195" s="33" t="s">
-        <v>1067</v>
-      </c>
-      <c r="P195" s="33" t="s">
-        <v>1068</v>
-      </c>
-      <c r="Q195" s="27" t="s">
-        <v>1069</v>
-      </c>
-      <c r="R195" s="27"/>
+      <c r="N195" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O195" s="31" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P195" s="31" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Q195" s="31" t="s">
+        <v>1065</v>
+      </c>
+      <c r="R195" s="31"/>
       <c r="S195" s="27"/>
       <c r="T195" s="27"/>
       <c r="U195" s="27"/>
@@ -34724,15 +34530,15 @@
       <c r="M196" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N196" s="27" t="s">
+      <c r="N196" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O196" s="27"/>
-      <c r="P196" s="27"/>
-      <c r="Q196" s="27" t="s">
-        <v>1070</v>
-      </c>
-      <c r="R196" s="27"/>
+      <c r="O196" s="31"/>
+      <c r="P196" s="31"/>
+      <c r="Q196" s="31" t="s">
+        <v>1066</v>
+      </c>
+      <c r="R196" s="31"/>
       <c r="S196" s="27"/>
       <c r="T196" s="27"/>
       <c r="U196" s="27"/>
@@ -34797,13 +34603,13 @@
       <c r="M197" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N197" s="27" t="s">
+      <c r="N197" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O197" s="27"/>
-      <c r="P197" s="27"/>
-      <c r="Q197" s="27"/>
-      <c r="R197" s="27"/>
+      <c r="O197" s="31"/>
+      <c r="P197" s="31"/>
+      <c r="Q197" s="31"/>
+      <c r="R197" s="31"/>
       <c r="S197" s="27"/>
       <c r="T197" s="27"/>
       <c r="U197" s="27"/>
@@ -34820,7 +34626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:170" ht="16">
+    <row r="198" spans="2:170">
       <c r="B198" s="3" t="s">
         <v>48</v>
       </c>
@@ -34847,19 +34653,19 @@
       <c r="M198" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N198" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="O198" s="27"/>
-      <c r="P198" s="27"/>
-      <c r="Q198" s="27" t="s">
-        <v>1072</v>
-      </c>
-      <c r="R198" s="27" t="s">
-        <v>1073</v>
+      <c r="N198" s="31" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O198" s="31"/>
+      <c r="P198" s="31"/>
+      <c r="Q198" s="31" t="s">
+        <v>1068</v>
+      </c>
+      <c r="R198" s="31" t="s">
+        <v>1069</v>
       </c>
       <c r="S198" s="27" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="T198" s="27"/>
       <c r="U198" s="27"/>
@@ -34897,13 +34703,13 @@
       <c r="M199" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N199" s="27" t="s">
+      <c r="N199" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O199" s="27"/>
-      <c r="P199" s="27"/>
-      <c r="Q199" s="27"/>
-      <c r="R199" s="27"/>
+      <c r="O199" s="31"/>
+      <c r="P199" s="31"/>
+      <c r="Q199" s="31"/>
+      <c r="R199" s="31"/>
       <c r="S199" s="27"/>
       <c r="T199" s="27"/>
       <c r="U199" s="27"/>
@@ -34923,7 +34729,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="200" spans="2:170" ht="16">
+    <row r="200" spans="2:170">
       <c r="B200" s="3" t="s">
         <v>34</v>
       </c>
@@ -34950,17 +34756,17 @@
       <c r="M200" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N200" s="33" t="s">
-        <v>1075</v>
-      </c>
-      <c r="O200" s="33" t="s">
-        <v>1076</v>
-      </c>
-      <c r="P200" s="33" t="s">
-        <v>1077</v>
-      </c>
-      <c r="Q200" s="27"/>
-      <c r="R200" s="27"/>
+      <c r="N200" s="31" t="s">
+        <v>1071</v>
+      </c>
+      <c r="O200" s="31" t="s">
+        <v>1072</v>
+      </c>
+      <c r="P200" s="31" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Q200" s="31"/>
+      <c r="R200" s="31"/>
       <c r="S200" s="27"/>
       <c r="T200" s="27"/>
       <c r="U200" s="27"/>
@@ -35112,13 +34918,13 @@
       <c r="M201" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N201" s="27" t="s">
+      <c r="N201" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O201" s="27"/>
-      <c r="P201" s="27"/>
-      <c r="Q201" s="27"/>
-      <c r="R201" s="27"/>
+      <c r="O201" s="31"/>
+      <c r="P201" s="31"/>
+      <c r="Q201" s="31"/>
+      <c r="R201" s="31"/>
       <c r="S201" s="27"/>
       <c r="T201" s="27"/>
       <c r="U201" s="27"/>
@@ -35222,13 +35028,13 @@
       <c r="M202" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N202" s="27" t="s">
+      <c r="N202" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O202" s="27"/>
-      <c r="P202" s="27"/>
-      <c r="Q202" s="27"/>
-      <c r="R202" s="27"/>
+      <c r="O202" s="31"/>
+      <c r="P202" s="31"/>
+      <c r="Q202" s="31"/>
+      <c r="R202" s="31"/>
       <c r="S202" s="27"/>
       <c r="T202" s="27"/>
       <c r="U202" s="27"/>
@@ -35302,7 +35108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:170" ht="16">
+    <row r="203" spans="2:170">
       <c r="B203" s="3" t="s">
         <v>34</v>
       </c>
@@ -35329,15 +35135,15 @@
       <c r="M203" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N203" s="33" t="s">
-        <v>1078</v>
-      </c>
-      <c r="O203" s="33" t="s">
-        <v>1077</v>
-      </c>
-      <c r="P203" s="27"/>
-      <c r="Q203" s="27"/>
-      <c r="R203" s="27"/>
+      <c r="N203" s="31" t="s">
+        <v>1074</v>
+      </c>
+      <c r="O203" s="31" t="s">
+        <v>1073</v>
+      </c>
+      <c r="P203" s="31"/>
+      <c r="Q203" s="31"/>
+      <c r="R203" s="31"/>
       <c r="S203" s="27"/>
       <c r="T203" s="27"/>
       <c r="U203" s="27"/>
@@ -35387,7 +35193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="2:170" ht="16">
+    <row r="204" spans="2:170">
       <c r="B204" s="3" t="s">
         <v>29</v>
       </c>
@@ -35414,17 +35220,17 @@
       <c r="M204" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N204" s="34" t="s">
-        <v>1079</v>
-      </c>
-      <c r="O204" s="34" t="s">
-        <v>1080</v>
-      </c>
-      <c r="P204" s="34" t="s">
-        <v>1081</v>
-      </c>
-      <c r="Q204" s="27"/>
-      <c r="R204" s="27"/>
+      <c r="N204" s="31" t="s">
+        <v>1089</v>
+      </c>
+      <c r="O204" s="31" t="s">
+        <v>1090</v>
+      </c>
+      <c r="P204" s="31" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Q204" s="31"/>
+      <c r="R204" s="31"/>
       <c r="S204" s="27"/>
       <c r="T204" s="27"/>
       <c r="U204" s="27"/>
@@ -35497,15 +35303,15 @@
       <c r="M205" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N205" s="27" t="s">
+      <c r="N205" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O205" s="27"/>
-      <c r="P205" s="27"/>
-      <c r="Q205" s="27" t="s">
-        <v>1082</v>
-      </c>
-      <c r="R205" s="27"/>
+      <c r="O205" s="31"/>
+      <c r="P205" s="31"/>
+      <c r="Q205" s="31" t="s">
+        <v>1075</v>
+      </c>
+      <c r="R205" s="31"/>
       <c r="S205" s="27"/>
       <c r="T205" s="27"/>
       <c r="U205" s="27"/>
@@ -35666,15 +35472,15 @@
       <c r="M206" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N206" s="27" t="s">
+      <c r="N206" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="O206" s="27"/>
-      <c r="P206" s="27"/>
-      <c r="Q206" s="27" t="s">
-        <v>1083</v>
-      </c>
-      <c r="R206" s="27"/>
+      <c r="O206" s="31"/>
+      <c r="P206" s="31"/>
+      <c r="Q206" s="31" t="s">
+        <v>1076</v>
+      </c>
+      <c r="R206" s="31"/>
       <c r="S206" s="27"/>
       <c r="T206" s="27"/>
       <c r="U206" s="27"/>
@@ -35730,7 +35536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="2:170" ht="16">
+    <row r="207" spans="2:170">
       <c r="B207" s="3" t="s">
         <v>16</v>
       </c>
@@ -35757,19 +35563,19 @@
       <c r="M207" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N207" s="33" t="s">
-        <v>1084</v>
-      </c>
-      <c r="O207" s="33" t="s">
-        <v>1085</v>
-      </c>
-      <c r="P207" s="33" t="s">
-        <v>1086</v>
-      </c>
-      <c r="Q207" s="27" t="s">
-        <v>1087</v>
-      </c>
-      <c r="R207" s="27"/>
+      <c r="N207" s="31" t="s">
+        <v>1077</v>
+      </c>
+      <c r="O207" s="31" t="s">
+        <v>1078</v>
+      </c>
+      <c r="P207" s="31" t="s">
+        <v>1079</v>
+      </c>
+      <c r="Q207" s="31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="R207" s="31"/>
       <c r="S207" s="27"/>
       <c r="T207" s="27"/>
       <c r="U207" s="27"/>
@@ -35902,7 +35708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="2:170" ht="16">
+    <row r="208" spans="2:170">
       <c r="B208" s="3" t="s">
         <v>16</v>
       </c>
@@ -35929,19 +35735,19 @@
       <c r="M208" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="N208" s="33" t="s">
-        <v>1088</v>
-      </c>
-      <c r="O208" s="33" t="s">
-        <v>1089</v>
-      </c>
-      <c r="P208" s="33" t="s">
-        <v>1090</v>
-      </c>
-      <c r="Q208" s="27" t="s">
-        <v>1091</v>
-      </c>
-      <c r="R208" s="27"/>
+      <c r="N208" s="31" t="s">
+        <v>1081</v>
+      </c>
+      <c r="O208" s="31" t="s">
+        <v>1082</v>
+      </c>
+      <c r="P208" s="31" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Q208" s="31" t="s">
+        <v>1084</v>
+      </c>
+      <c r="R208" s="31"/>
       <c r="S208" s="27"/>
       <c r="T208" s="27"/>
       <c r="U208" s="27"/>

</xml_diff>

<commit_message>
apparently I made changes to the spreadsheet?
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="23940" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4980" yWindow="0" windowWidth="23940" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3454" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="1090">
   <si>
     <t>f</t>
   </si>
@@ -3293,6 +3293,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>any digital</t>
   </si>
 </sst>
 </file>
@@ -3478,8 +3481,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3843,7 +3848,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="305">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3995,6 +4000,7 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4146,6 +4152,7 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -13040,11 +13047,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FN209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="Q135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D164" sqref="D164"/>
+      <selection pane="bottomRight" activeCell="S153" sqref="S153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40838,10 +40845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40969,7 +40976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>1086</v>
       </c>
@@ -40978,7 +40985,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>1087</v>
       </c>
@@ -40987,7 +40994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>669</v>
       </c>
@@ -40995,14 +41002,27 @@
         <f>B6+B9</f>
         <v>46</v>
       </c>
+      <c r="D19">
+        <f>B19/B20</f>
+        <v>0.22115384615384615</v>
+      </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>1088</v>
       </c>
       <c r="B20">
         <f>SUM(B16:B19)</f>
         <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B22">
+        <f>B16+B17+B18</f>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added gothic type for #1
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="12760" yWindow="0" windowWidth="15840" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="1126">
   <si>
     <t>f</t>
   </si>
@@ -3401,6 +3401,9 @@
   </si>
   <si>
     <t>Gothic Type</t>
+  </si>
+  <si>
+    <t>Gothic Rauberroman (elements of the monastic shocker)</t>
   </si>
 </sst>
 </file>
@@ -12693,6 +12696,112 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -12819,112 +12928,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -13262,10 +13265,10 @@
   <dimension ref="A1:GT209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
+      <selection pane="bottomRight" activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13296,7 +13299,7 @@
     <col min="28" max="28" width="4.5" style="19" customWidth="1"/>
     <col min="29" max="31" width="5.6640625" style="23" customWidth="1"/>
     <col min="32" max="37" width="4.83203125" style="23" customWidth="1"/>
-    <col min="38" max="38" width="19.6640625" style="44" customWidth="1"/>
+    <col min="38" max="38" width="48.1640625" style="44" customWidth="1"/>
     <col min="39" max="39" width="7.5" style="37" customWidth="1"/>
     <col min="40" max="40" width="4.5" style="23" customWidth="1"/>
     <col min="41" max="41" width="8.1640625" style="23" customWidth="1"/>
@@ -14151,7 +14154,9 @@
       <c r="AI2" s="27"/>
       <c r="AJ2" s="27"/>
       <c r="AK2" s="27"/>
-      <c r="AL2" s="43"/>
+      <c r="AL2" s="43" t="s">
+        <v>1125</v>
+      </c>
       <c r="AM2" s="36" t="s">
         <v>327</v>
       </c>

</xml_diff>

<commit_message>
Gothic type to 6
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="100" windowWidth="23080" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="11860" yWindow="0" windowWidth="18080" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -13,9 +13,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
-    <pivotCache cacheId="4" r:id="rId5"/>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="1131">
   <si>
     <t>f</t>
   </si>
@@ -3404,6 +3404,21 @@
   </si>
   <si>
     <t>Gothic Rauberroman (elements of the monastic shocker)</t>
+  </si>
+  <si>
+    <t>Pure of high Gothic (horror-terror modes)</t>
+  </si>
+  <si>
+    <t>Orientalized Gothic fantasy</t>
+  </si>
+  <si>
+    <t>Gothic chapbook</t>
+  </si>
+  <si>
+    <t>Gothified History (terror mode)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror mode)</t>
   </si>
 </sst>
 </file>
@@ -12604,7 +12619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField dataField="1" showAll="0"/>
@@ -12701,7 +12716,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -12827,112 +12948,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -13273,7 +13288,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF21" sqref="BF21"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14386,7 +14401,9 @@
       <c r="F3" s="18">
         <v>2</v>
       </c>
-      <c r="G3" s="43"/>
+      <c r="G3" s="43" t="s">
+        <v>1126</v>
+      </c>
       <c r="H3" s="36" t="s">
         <v>327</v>
       </c>
@@ -14455,7 +14472,9 @@
       <c r="F4" s="18">
         <v>3</v>
       </c>
-      <c r="G4" s="43"/>
+      <c r="G4" s="43" t="s">
+        <v>1127</v>
+      </c>
       <c r="H4" s="36" t="s">
         <v>375</v>
       </c>
@@ -14575,7 +14594,9 @@
       <c r="F5" s="18">
         <v>4</v>
       </c>
-      <c r="G5" s="43"/>
+      <c r="G5" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H5" s="36" t="s">
         <v>371</v>
       </c>
@@ -14698,7 +14719,9 @@
       <c r="F6" s="18">
         <v>5</v>
       </c>
-      <c r="G6" s="43"/>
+      <c r="G6" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H6" s="36" t="s">
         <v>348</v>
       </c>
@@ -14862,7 +14885,9 @@
       <c r="F7" s="18">
         <v>6</v>
       </c>
-      <c r="G7" s="43"/>
+      <c r="G7" s="43" t="s">
+        <v>1130</v>
+      </c>
       <c r="H7" s="36" t="s">
         <v>327</v>
       </c>

</xml_diff>

<commit_message>
gothic types to 30
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3520" uniqueCount="1139">
   <si>
     <t>f</t>
   </si>
@@ -3419,6 +3419,30 @@
   </si>
   <si>
     <t>Pure or high Gothic (terror mode)</t>
+  </si>
+  <si>
+    <t>(not indexed)</t>
+  </si>
+  <si>
+    <t>Gothified History</t>
+  </si>
+  <si>
+    <t>Sentimental Gothic</t>
+  </si>
+  <si>
+    <t>Philosophical Gothic (domestic elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (horror mode)</t>
+  </si>
+  <si>
+    <t>Gothified History (Wandering Jew legend)</t>
+  </si>
+  <si>
+    <t>Gothic chapbook (Shauerromantik elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (horror-terror modes)</t>
   </si>
 </sst>
 </file>
@@ -13288,7 +13312,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15037,7 +15061,9 @@
       <c r="F8" s="18">
         <v>7</v>
       </c>
-      <c r="G8" s="43"/>
+      <c r="G8" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H8" s="36" t="s">
         <v>348</v>
       </c>
@@ -15165,7 +15191,9 @@
       <c r="F9" s="18">
         <v>8</v>
       </c>
-      <c r="G9" s="43"/>
+      <c r="G9" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H9" s="36" t="s">
         <v>327</v>
       </c>
@@ -15255,7 +15283,9 @@
       <c r="F10" s="18">
         <v>9</v>
       </c>
-      <c r="G10" s="43"/>
+      <c r="G10" s="43" t="s">
+        <v>1132</v>
+      </c>
       <c r="H10" s="36" t="s">
         <v>557</v>
       </c>
@@ -15467,7 +15497,9 @@
       <c r="F11" s="18">
         <v>10</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="43" t="s">
+        <v>1130</v>
+      </c>
       <c r="H11" s="36" t="s">
         <v>327</v>
       </c>
@@ -15608,7 +15640,9 @@
       <c r="F12" s="18">
         <v>11</v>
       </c>
-      <c r="G12" s="43"/>
+      <c r="G12" s="43" t="s">
+        <v>1133</v>
+      </c>
       <c r="H12" s="36" t="s">
         <v>354</v>
       </c>
@@ -15743,7 +15777,9 @@
       <c r="F13" s="18">
         <v>12</v>
       </c>
-      <c r="G13" s="43"/>
+      <c r="G13" s="43" t="s">
+        <v>1134</v>
+      </c>
       <c r="H13" s="36" t="s">
         <v>348</v>
       </c>
@@ -15854,7 +15890,9 @@
       <c r="F14" s="18">
         <v>13</v>
       </c>
-      <c r="G14" s="43"/>
+      <c r="G14" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H14" s="36" t="s">
         <v>327</v>
       </c>
@@ -15954,7 +15992,9 @@
       <c r="F15" s="18">
         <v>14</v>
       </c>
-      <c r="G15" s="43"/>
+      <c r="G15" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H15" s="36" t="s">
         <v>348</v>
       </c>
@@ -16031,7 +16071,9 @@
       <c r="F16" s="18">
         <v>15</v>
       </c>
-      <c r="G16" s="43"/>
+      <c r="G16" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H16" s="36" t="s">
         <v>327</v>
       </c>
@@ -16123,7 +16165,9 @@
       <c r="F17" s="18">
         <v>16</v>
       </c>
-      <c r="G17" s="43"/>
+      <c r="G17" s="43" t="s">
+        <v>1130</v>
+      </c>
       <c r="H17" s="36" t="s">
         <v>558</v>
       </c>
@@ -16275,7 +16319,9 @@
       <c r="F18" s="18">
         <v>17</v>
       </c>
-      <c r="G18" s="43"/>
+      <c r="G18" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H18" s="36" t="s">
         <v>560</v>
       </c>
@@ -16361,7 +16407,9 @@
       <c r="F19" s="18">
         <v>18</v>
       </c>
-      <c r="G19" s="43"/>
+      <c r="G19" s="43" t="s">
+        <v>1135</v>
+      </c>
       <c r="H19" s="36" t="s">
         <v>327</v>
       </c>
@@ -16463,7 +16511,9 @@
       <c r="F20" s="18">
         <v>19</v>
       </c>
-      <c r="G20" s="43"/>
+      <c r="G20" s="43" t="s">
+        <v>1136</v>
+      </c>
       <c r="H20" s="36" t="s">
         <v>563</v>
       </c>
@@ -16579,7 +16629,9 @@
       <c r="F21" s="18">
         <v>20</v>
       </c>
-      <c r="G21" s="43"/>
+      <c r="G21" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H21" s="36" t="s">
         <v>560</v>
       </c>
@@ -16738,7 +16790,9 @@
       <c r="F22" s="18">
         <v>21</v>
       </c>
-      <c r="G22" s="43"/>
+      <c r="G22" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H22" s="36" t="s">
         <v>560</v>
       </c>
@@ -16838,7 +16892,9 @@
       <c r="F23" s="18">
         <v>22</v>
       </c>
-      <c r="G23" s="43"/>
+      <c r="G23" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H23" s="36" t="s">
         <v>560</v>
       </c>
@@ -16929,7 +16985,9 @@
       <c r="F24" s="18">
         <v>23</v>
       </c>
-      <c r="G24" s="43"/>
+      <c r="G24" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H24" s="36" t="s">
         <v>566</v>
       </c>
@@ -17028,7 +17086,9 @@
       <c r="F25" s="18">
         <v>24</v>
       </c>
-      <c r="G25" s="43"/>
+      <c r="G25" s="43" t="s">
+        <v>1131</v>
+      </c>
       <c r="H25" s="36" t="s">
         <v>566</v>
       </c>
@@ -17277,7 +17337,9 @@
       <c r="F26" s="18">
         <v>25</v>
       </c>
-      <c r="G26" s="43"/>
+      <c r="G26" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H26" s="36" t="s">
         <v>327</v>
       </c>
@@ -17383,7 +17445,9 @@
       <c r="F27" s="18">
         <v>26</v>
       </c>
-      <c r="G27" s="43"/>
+      <c r="G27" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H27" s="36" t="s">
         <v>327</v>
       </c>
@@ -17498,7 +17562,9 @@
       <c r="F28" s="18">
         <v>27</v>
       </c>
-      <c r="G28" s="43"/>
+      <c r="G28" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H28" s="36" t="s">
         <v>327</v>
       </c>
@@ -17581,7 +17647,9 @@
       <c r="F29" s="18">
         <v>28</v>
       </c>
-      <c r="G29" s="43"/>
+      <c r="G29" s="43" t="s">
+        <v>1130</v>
+      </c>
       <c r="H29" s="36" t="s">
         <v>572</v>
       </c>
@@ -17784,7 +17852,9 @@
       <c r="F30" s="18">
         <v>29</v>
       </c>
-      <c r="G30" s="43"/>
+      <c r="G30" s="43" t="s">
+        <v>1130</v>
+      </c>
       <c r="H30" s="36" t="s">
         <v>327</v>
       </c>
@@ -18085,7 +18155,9 @@
       <c r="F31" s="18">
         <v>30</v>
       </c>
-      <c r="G31" s="43"/>
+      <c r="G31" s="43" t="s">
+        <v>1138</v>
+      </c>
       <c r="H31" s="36" t="s">
         <v>327</v>
       </c>

</xml_diff>

<commit_message>
gothic types to 70
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="0" windowWidth="16460" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="15080" yWindow="0" windowWidth="13680" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -13,9 +13,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
-    <pivotCache cacheId="4" r:id="rId5"/>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="1165">
   <si>
     <t>f</t>
   </si>
@@ -3470,6 +3470,57 @@
   </si>
   <si>
     <t>Gothified history (sentimental and terror modes)</t>
+  </si>
+  <si>
+    <t>Gothic chapbook (based on THE MONK)</t>
+  </si>
+  <si>
+    <t>Contemporized Gothic (didactic and polemical elements)</t>
+  </si>
+  <si>
+    <t>Gothified history (didactic elements)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (various Richardsonian features)</t>
+  </si>
+  <si>
+    <t>Gothic Quest legend (elements of MELMOTH THE WANDERER)</t>
+  </si>
+  <si>
+    <t>Orientalized Gothic</t>
+  </si>
+  <si>
+    <t>Roman noir (horror-terror elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Vehmgericht or secret Fehmic tribunal)</t>
+  </si>
+  <si>
+    <t>Mixed Gothic (domestic fiction becoming Gothic)</t>
+  </si>
+  <si>
+    <t>Mixed Gothic (domestic fiction becoming Gothic in horror mode)</t>
+  </si>
+  <si>
+    <t>Sentimental fiction (Radcliffean terror elements)</t>
+  </si>
+  <si>
+    <t>Gothified history (Radcliffean imitation)</t>
+  </si>
+  <si>
+    <t>Gothified History (a witchcraft segment)</t>
+  </si>
+  <si>
+    <t>Doppleganger or Double Story (terror-horror modes)</t>
+  </si>
+  <si>
+    <t>Novel of Seduction and Radical Ideas (terror elements)</t>
+  </si>
+  <si>
+    <t>Gothified history (natural horror)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (no supernatural elements)</t>
   </si>
 </sst>
 </file>
@@ -12670,7 +12721,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField dataField="1" showAll="0"/>
@@ -12767,7 +12818,113 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -12893,112 +13050,6 @@
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -13336,10 +13387,10 @@
   <dimension ref="A1:GT209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20532,7 +20583,9 @@
       <c r="F46" s="18">
         <v>45</v>
       </c>
-      <c r="G46" s="43"/>
+      <c r="G46" s="43" t="s">
+        <v>1148</v>
+      </c>
       <c r="H46" s="36" t="s">
         <v>326</v>
       </c>
@@ -20693,7 +20746,9 @@
       <c r="F47" s="18">
         <v>46</v>
       </c>
-      <c r="G47" s="43"/>
+      <c r="G47" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H47" s="36" t="s">
         <v>326</v>
       </c>
@@ -20811,7 +20866,9 @@
       <c r="F48" s="18">
         <v>47</v>
       </c>
-      <c r="G48" s="43"/>
+      <c r="G48" s="43" t="s">
+        <v>1133</v>
+      </c>
       <c r="H48" s="36" t="s">
         <v>326</v>
       </c>
@@ -21013,7 +21070,9 @@
       <c r="F49" s="18">
         <v>48</v>
       </c>
-      <c r="G49" s="43"/>
+      <c r="G49" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H49" s="36" t="s">
         <v>585</v>
       </c>
@@ -21165,7 +21224,9 @@
       <c r="F50" s="18">
         <v>49</v>
       </c>
-      <c r="G50" s="43"/>
+      <c r="G50" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H50" s="36" t="s">
         <v>586</v>
       </c>
@@ -21358,7 +21419,9 @@
       <c r="F51" s="18">
         <v>50</v>
       </c>
-      <c r="G51" s="43"/>
+      <c r="G51" s="43" t="s">
+        <v>1150</v>
+      </c>
       <c r="H51" s="36" t="s">
         <v>587</v>
       </c>
@@ -21498,7 +21561,9 @@
       <c r="F52" s="18">
         <v>51</v>
       </c>
-      <c r="G52" s="43"/>
+      <c r="G52" s="43" t="s">
+        <v>1149</v>
+      </c>
       <c r="H52" s="36" t="s">
         <v>347</v>
       </c>
@@ -21622,7 +21687,9 @@
       <c r="F53" s="18">
         <v>52</v>
       </c>
-      <c r="G53" s="43"/>
+      <c r="G53" s="43" t="s">
+        <v>1151</v>
+      </c>
       <c r="H53" s="36" t="s">
         <v>347</v>
       </c>
@@ -21745,7 +21812,9 @@
       <c r="F54" s="18">
         <v>53</v>
       </c>
-      <c r="G54" s="43"/>
+      <c r="G54" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H54" s="36" t="s">
         <v>326</v>
       </c>
@@ -21887,7 +21956,9 @@
       <c r="F55" s="18">
         <v>54</v>
       </c>
-      <c r="G55" s="43"/>
+      <c r="G55" s="43" t="s">
+        <v>1153</v>
+      </c>
       <c r="H55" s="36" t="s">
         <v>559</v>
       </c>
@@ -22039,7 +22110,9 @@
       <c r="F56" s="18">
         <v>55</v>
       </c>
-      <c r="G56" s="43"/>
+      <c r="G56" s="43" t="s">
+        <v>1152</v>
+      </c>
       <c r="H56" s="36" t="s">
         <v>589</v>
       </c>
@@ -22167,7 +22240,9 @@
       <c r="F57" s="18">
         <v>56</v>
       </c>
-      <c r="G57" s="43"/>
+      <c r="G57" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H57" s="36" t="s">
         <v>590</v>
       </c>
@@ -22321,7 +22396,9 @@
       <c r="F58" s="18">
         <v>57</v>
       </c>
-      <c r="G58" s="43"/>
+      <c r="G58" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H58" s="36" t="s">
         <v>326</v>
       </c>
@@ -22468,7 +22545,9 @@
       <c r="F59" s="18">
         <v>58</v>
       </c>
-      <c r="G59" s="43"/>
+      <c r="G59" s="43" t="s">
+        <v>1154</v>
+      </c>
       <c r="H59" s="36" t="s">
         <v>326</v>
       </c>
@@ -22573,7 +22652,9 @@
       <c r="F60" s="18">
         <v>59</v>
       </c>
-      <c r="G60" s="43"/>
+      <c r="G60" s="43" t="s">
+        <v>1155</v>
+      </c>
       <c r="H60" s="36" t="s">
         <v>326</v>
       </c>
@@ -22750,7 +22831,9 @@
       <c r="F61" s="18">
         <v>60</v>
       </c>
-      <c r="G61" s="43"/>
+      <c r="G61" s="43" t="s">
+        <v>1156</v>
+      </c>
       <c r="H61" s="36" t="s">
         <v>557</v>
       </c>
@@ -22903,7 +22986,9 @@
       <c r="F62" s="18">
         <v>61</v>
       </c>
-      <c r="G62" s="43"/>
+      <c r="G62" s="43" t="s">
+        <v>1157</v>
+      </c>
       <c r="H62" s="36" t="s">
         <v>569</v>
       </c>
@@ -23068,7 +23153,9 @@
       <c r="F63" s="18">
         <v>62</v>
       </c>
-      <c r="G63" s="43"/>
+      <c r="G63" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H63" s="36" t="s">
         <v>347</v>
       </c>
@@ -23269,7 +23356,9 @@
       <c r="F64" s="18">
         <v>63</v>
       </c>
-      <c r="G64" s="43"/>
+      <c r="G64" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H64" s="36" t="s">
         <v>590</v>
       </c>
@@ -23371,7 +23460,9 @@
       <c r="F65" s="18">
         <v>64</v>
       </c>
-      <c r="G65" s="43"/>
+      <c r="G65" s="43" t="s">
+        <v>1158</v>
+      </c>
       <c r="H65" s="36" t="s">
         <v>347</v>
       </c>
@@ -23596,7 +23687,9 @@
       <c r="F66" s="18">
         <v>65</v>
       </c>
-      <c r="G66" s="43"/>
+      <c r="G66" s="43" t="s">
+        <v>1159</v>
+      </c>
       <c r="H66" s="36" t="s">
         <v>593</v>
       </c>
@@ -23775,7 +23868,9 @@
       <c r="F67" s="18">
         <v>66</v>
       </c>
-      <c r="G67" s="43"/>
+      <c r="G67" s="43" t="s">
+        <v>1161</v>
+      </c>
       <c r="H67" s="36" t="s">
         <v>590</v>
       </c>
@@ -23937,7 +24032,9 @@
       <c r="F68" s="18">
         <v>67</v>
       </c>
-      <c r="G68" s="43"/>
+      <c r="G68" s="43" t="s">
+        <v>1160</v>
+      </c>
       <c r="H68" s="36" t="s">
         <v>590</v>
       </c>
@@ -24044,7 +24141,9 @@
       <c r="F69" s="18">
         <v>68</v>
       </c>
-      <c r="G69" s="43"/>
+      <c r="G69" s="43" t="s">
+        <v>1162</v>
+      </c>
       <c r="H69" s="36" t="s">
         <v>370</v>
       </c>
@@ -24180,7 +24279,9 @@
       <c r="F70" s="18">
         <v>69</v>
       </c>
-      <c r="G70" s="43"/>
+      <c r="G70" s="43" t="s">
+        <v>1163</v>
+      </c>
       <c r="H70" s="36" t="s">
         <v>611</v>
       </c>
@@ -24346,7 +24447,9 @@
       <c r="F71" s="18">
         <v>70</v>
       </c>
-      <c r="G71" s="43"/>
+      <c r="G71" s="43" t="s">
+        <v>1164</v>
+      </c>
       <c r="H71" s="36" t="s">
         <v>353</v>
       </c>

</xml_diff>

<commit_message>
gothic types to 121
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1203">
   <si>
     <t>f</t>
   </si>
@@ -3521,6 +3521,120 @@
   </si>
   <si>
     <t>Pure or high Gothic (no supernatural elements)</t>
+  </si>
+  <si>
+    <t>Documentary Gothic (natural horror based on an actual incident)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (terror elements)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (monastic shocker in horror-terror modes; imitation of THE MONK)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic/Gothified history (horror-terror modes)</t>
+  </si>
+  <si>
+    <t>Sentimentalized and naturalized Gothic (Radcliffean methods and props)</t>
+  </si>
+  <si>
+    <t>Gothified history (naturalized terror)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Schauerromantik elements)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (more domestic than Gothic, a few terror elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (in the novel's maiden-centered episodes)</t>
+  </si>
+  <si>
+    <t>Gothic roman a clef (terror mode)</t>
+  </si>
+  <si>
+    <t>Orientalized Gothic/roman a clef</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (the supernatural acoustic)</t>
+  </si>
+  <si>
+    <t>Naturalized Gothic (domestic and sentimental elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (quest story, picaresque elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic</t>
+  </si>
+  <si>
+    <t>Gothified history (terror and sentimental elements)</t>
+  </si>
+  <si>
+    <t>Didactic and domestic novel (Gothic titling)</t>
+  </si>
+  <si>
+    <t>Gothified history (historical Gothic prototype, terror elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (horror, terror, and Schauerromantik modes, monastic shocker)</t>
+  </si>
+  <si>
+    <t>Rauberroman (terror mode)</t>
+  </si>
+  <si>
+    <t>Gothic chapbook (converted from Gothic drama)</t>
+  </si>
+  <si>
+    <t>Gothic anthology (terror, horror, and Schauerromantik modes represented with Germanic translations and imitations)</t>
+  </si>
+  <si>
+    <t>Political and polemical Gothic (satiric and philosophic elements, attack on Godwin and Jacobin novelists)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (several Gothic elements and characters)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (several touches of terror Gothicism)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror mode, revolutionary Irish politics)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (actually, a composite of Gothic types)</t>
+  </si>
+  <si>
+    <t>Gothified history (terror-horror modes)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (search for the father)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (domestic elements, genealogical entanglements)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (intermittent Gothic elements)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (intermitten Gothic effects)</t>
+  </si>
+  <si>
+    <t>Gothic bluebook (variable plagiarism from many Gothics)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (monastic shocker, excessive narual and supernatural horror)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror mode, in serialized form)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pure or high Gothics (a multiple Gothic containing elements of several subspecies of Gothic fiction) </t>
+  </si>
+  <si>
+    <t>Novel of domestic sadism (titular character is a prototypical Gothic villain)</t>
   </si>
 </sst>
 </file>
@@ -3774,7 +3888,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="314">
+  <cellStyleXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4089,6 +4203,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4178,7 +4296,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="314">
+  <cellStyles count="318">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4339,6 +4457,10 @@
     <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -13387,10 +13509,10 @@
   <dimension ref="A1:GT209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomRight" activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24670,7 +24792,9 @@
       <c r="F72" s="18">
         <v>71</v>
       </c>
-      <c r="G72" s="43"/>
+      <c r="G72" s="43" t="s">
+        <v>1166</v>
+      </c>
       <c r="H72" s="36" t="s">
         <v>326</v>
       </c>
@@ -24874,7 +24998,9 @@
       <c r="F73" s="18">
         <v>72</v>
       </c>
-      <c r="G73" s="43"/>
+      <c r="G73" s="43" t="s">
+        <v>1165</v>
+      </c>
       <c r="H73" s="36" t="s">
         <v>347</v>
       </c>
@@ -24964,7 +25090,9 @@
       <c r="F74" s="18">
         <v>73</v>
       </c>
-      <c r="G74" s="43"/>
+      <c r="G74" s="43" t="s">
+        <v>1167</v>
+      </c>
       <c r="H74" s="36" t="s">
         <v>326</v>
       </c>
@@ -25077,7 +25205,9 @@
       <c r="F75" s="18">
         <v>74</v>
       </c>
-      <c r="G75" s="43"/>
+      <c r="G75" s="43" t="s">
+        <v>1168</v>
+      </c>
       <c r="H75" s="36" t="s">
         <v>559</v>
       </c>
@@ -25285,7 +25415,9 @@
       <c r="F76" s="18">
         <v>75</v>
       </c>
-      <c r="G76" s="43"/>
+      <c r="G76" s="43" t="s">
+        <v>1169</v>
+      </c>
       <c r="H76" s="36" t="s">
         <v>621</v>
       </c>
@@ -25515,7 +25647,9 @@
       <c r="F77" s="18">
         <v>76</v>
       </c>
-      <c r="G77" s="43"/>
+      <c r="G77" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H77" s="36" t="s">
         <v>326</v>
       </c>
@@ -25732,7 +25866,9 @@
       <c r="F78" s="18">
         <v>77</v>
       </c>
-      <c r="G78" s="43"/>
+      <c r="G78" s="43" t="s">
+        <v>1170</v>
+      </c>
       <c r="H78" s="36" t="s">
         <v>326</v>
       </c>
@@ -25874,7 +26010,9 @@
       <c r="F79" s="18">
         <v>78</v>
       </c>
-      <c r="G79" s="43"/>
+      <c r="G79" s="43" t="s">
+        <v>1171</v>
+      </c>
       <c r="H79" s="36" t="s">
         <v>559</v>
       </c>
@@ -26035,7 +26173,9 @@
       <c r="F80" s="18">
         <v>79</v>
       </c>
-      <c r="G80" s="43"/>
+      <c r="G80" s="43" t="s">
+        <v>1172</v>
+      </c>
       <c r="H80" s="36" t="s">
         <v>326</v>
       </c>
@@ -26146,7 +26286,9 @@
       <c r="F81" s="18">
         <v>80</v>
       </c>
-      <c r="G81" s="43"/>
+      <c r="G81" s="43" t="s">
+        <v>1174</v>
+      </c>
       <c r="H81" s="36" t="s">
         <v>326</v>
       </c>
@@ -26307,7 +26449,9 @@
       <c r="F82" s="18">
         <v>81</v>
       </c>
-      <c r="G82" s="43"/>
+      <c r="G82" s="43" t="s">
+        <v>1173</v>
+      </c>
       <c r="H82" s="36" t="s">
         <v>326</v>
       </c>
@@ -26424,7 +26568,9 @@
       <c r="F83" s="18">
         <v>82</v>
       </c>
-      <c r="G83" s="43"/>
+      <c r="G83" s="44" t="s">
+        <v>1176</v>
+      </c>
       <c r="H83" s="36" t="s">
         <v>624</v>
       </c>
@@ -26581,7 +26727,9 @@
       <c r="F84" s="18">
         <v>83</v>
       </c>
-      <c r="G84" s="43"/>
+      <c r="G84" s="43" t="s">
+        <v>1175</v>
+      </c>
       <c r="H84" s="36" t="s">
         <v>626</v>
       </c>
@@ -26798,7 +26946,9 @@
       <c r="F85" s="18">
         <v>84</v>
       </c>
-      <c r="G85" s="43"/>
+      <c r="G85" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H85" s="36" t="s">
         <v>347</v>
       </c>
@@ -26901,7 +27051,9 @@
       <c r="F86" s="18">
         <v>85</v>
       </c>
-      <c r="G86" s="43"/>
+      <c r="G86" s="43" t="s">
+        <v>1179</v>
+      </c>
       <c r="H86" s="36" t="s">
         <v>326</v>
       </c>
@@ -27085,7 +27237,9 @@
       <c r="F87" s="18">
         <v>86</v>
       </c>
-      <c r="G87" s="43"/>
+      <c r="G87" s="43" t="s">
+        <v>1180</v>
+      </c>
       <c r="H87" s="36" t="s">
         <v>559</v>
       </c>
@@ -27291,7 +27445,9 @@
       <c r="F88" s="18">
         <v>87</v>
       </c>
-      <c r="G88" s="43"/>
+      <c r="G88" s="43" t="s">
+        <v>1177</v>
+      </c>
       <c r="H88" s="36" t="s">
         <v>581</v>
       </c>
@@ -27462,7 +27618,9 @@
       <c r="F89" s="18">
         <v>88</v>
       </c>
-      <c r="G89" s="43"/>
+      <c r="G89" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H89" s="36" t="s">
         <v>347</v>
       </c>
@@ -27628,7 +27786,9 @@
       <c r="F90" s="18">
         <v>89</v>
       </c>
-      <c r="G90" s="43"/>
+      <c r="G90" s="43" t="s">
+        <v>1178</v>
+      </c>
       <c r="H90" s="36" t="s">
         <v>580</v>
       </c>
@@ -27739,7 +27899,9 @@
       <c r="F91" s="18">
         <v>90</v>
       </c>
-      <c r="G91" s="43"/>
+      <c r="G91" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H91" s="36" t="s">
         <v>347</v>
       </c>
@@ -27923,7 +28085,9 @@
       <c r="F92" s="18">
         <v>91</v>
       </c>
-      <c r="G92" s="43"/>
+      <c r="G92" s="43" t="s">
+        <v>1172</v>
+      </c>
       <c r="H92" s="36" t="s">
         <v>631</v>
       </c>
@@ -28046,7 +28210,9 @@
       <c r="F93" s="18">
         <v>92</v>
       </c>
-      <c r="G93" s="43"/>
+      <c r="G93" s="43" t="s">
+        <v>1181</v>
+      </c>
       <c r="H93" s="36" t="s">
         <v>347</v>
       </c>
@@ -28235,7 +28401,9 @@
       <c r="F94" s="18">
         <v>93</v>
       </c>
-      <c r="G94" s="43"/>
+      <c r="G94" s="43" t="s">
+        <v>1135</v>
+      </c>
       <c r="H94" s="36" t="s">
         <v>326</v>
       </c>
@@ -28344,7 +28512,9 @@
       <c r="F95" s="18">
         <v>94</v>
       </c>
-      <c r="G95" s="43"/>
+      <c r="G95" s="43" t="s">
+        <v>1182</v>
+      </c>
       <c r="H95" s="36" t="s">
         <v>326</v>
       </c>
@@ -28445,7 +28615,9 @@
       <c r="F96" s="18">
         <v>95</v>
       </c>
-      <c r="G96" s="43"/>
+      <c r="G96" s="43" t="s">
+        <v>1183</v>
+      </c>
       <c r="H96" s="36" t="s">
         <v>347</v>
       </c>
@@ -28639,7 +28811,9 @@
       <c r="F97" s="18">
         <v>96</v>
       </c>
-      <c r="G97" s="43"/>
+      <c r="G97" s="43" t="s">
+        <v>1185</v>
+      </c>
       <c r="H97" s="36" t="s">
         <v>559</v>
       </c>
@@ -28731,7 +28905,9 @@
       <c r="F98" s="18">
         <v>97</v>
       </c>
-      <c r="G98" s="43"/>
+      <c r="G98" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H98" s="36" t="s">
         <v>326</v>
       </c>
@@ -28959,7 +29135,9 @@
       <c r="F99" s="18">
         <v>98</v>
       </c>
-      <c r="G99" s="43"/>
+      <c r="G99" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H99" s="36" t="s">
         <v>635</v>
       </c>
@@ -29075,7 +29253,9 @@
       <c r="F100" s="18">
         <v>99</v>
       </c>
-      <c r="G100" s="43"/>
+      <c r="G100" s="43" t="s">
+        <v>1184</v>
+      </c>
       <c r="H100" s="36" t="s">
         <v>569</v>
       </c>
@@ -29368,7 +29548,9 @@
       <c r="F101" s="18">
         <v>100</v>
       </c>
-      <c r="G101" s="43"/>
+      <c r="G101" s="43" t="s">
+        <v>1187</v>
+      </c>
       <c r="H101" s="36" t="s">
         <v>326</v>
       </c>
@@ -29560,7 +29742,9 @@
       <c r="F102" s="18">
         <v>101</v>
       </c>
-      <c r="G102" s="43"/>
+      <c r="G102" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H102" s="36" t="s">
         <v>326</v>
       </c>
@@ -29704,7 +29888,9 @@
       <c r="F103" s="18">
         <v>102</v>
       </c>
-      <c r="G103" s="43"/>
+      <c r="G103" s="43" t="s">
+        <v>1186</v>
+      </c>
       <c r="H103" s="36" t="s">
         <v>326</v>
       </c>
@@ -29804,7 +29990,9 @@
       <c r="F104" s="18">
         <v>103</v>
       </c>
-      <c r="G104" s="43"/>
+      <c r="G104" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H104" s="36" t="s">
         <v>642</v>
       </c>
@@ -29884,7 +30072,9 @@
       <c r="F105" s="18">
         <v>104</v>
       </c>
-      <c r="G105" s="43"/>
+      <c r="G105" s="43" t="s">
+        <v>1188</v>
+      </c>
       <c r="H105" s="36" t="s">
         <v>347</v>
       </c>
@@ -30019,7 +30209,9 @@
       <c r="F106" s="18">
         <v>105</v>
       </c>
-      <c r="G106" s="43"/>
+      <c r="G106" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H106" s="36" t="s">
         <v>644</v>
       </c>
@@ -30118,7 +30310,9 @@
       <c r="F107" s="18">
         <v>106</v>
       </c>
-      <c r="G107" s="43"/>
+      <c r="G107" s="43" t="s">
+        <v>1189</v>
+      </c>
       <c r="H107" s="36" t="s">
         <v>646</v>
       </c>
@@ -30242,7 +30436,9 @@
       <c r="F108" s="18">
         <v>107</v>
       </c>
-      <c r="G108" s="43"/>
+      <c r="G108" s="43" t="s">
+        <v>1193</v>
+      </c>
       <c r="H108" s="36" t="s">
         <v>326</v>
       </c>
@@ -30441,7 +30637,9 @@
       <c r="F109" s="18">
         <v>108</v>
       </c>
-      <c r="G109" s="43"/>
+      <c r="G109" s="43" t="s">
+        <v>1140</v>
+      </c>
       <c r="H109" s="36" t="s">
         <v>326</v>
       </c>
@@ -30651,7 +30849,9 @@
       <c r="F110" s="18">
         <v>109</v>
       </c>
-      <c r="G110" s="43"/>
+      <c r="G110" s="44" t="s">
+        <v>1192</v>
+      </c>
       <c r="H110" s="36" t="s">
         <v>645</v>
       </c>
@@ -30881,7 +31081,9 @@
       <c r="F111" s="18">
         <v>110</v>
       </c>
-      <c r="G111" s="43"/>
+      <c r="G111" s="43" t="s">
+        <v>1191</v>
+      </c>
       <c r="H111" s="36" t="s">
         <v>650</v>
       </c>
@@ -30977,7 +31179,9 @@
       <c r="F112" s="18">
         <v>111</v>
       </c>
-      <c r="G112" s="43"/>
+      <c r="G112" s="43" t="s">
+        <v>1190</v>
+      </c>
       <c r="H112" s="36" t="s">
         <v>651</v>
       </c>
@@ -31126,7 +31330,9 @@
       <c r="F113" s="18">
         <v>112</v>
       </c>
-      <c r="G113" s="43"/>
+      <c r="G113" s="43" t="s">
+        <v>1194</v>
+      </c>
       <c r="H113" s="36" t="s">
         <v>326</v>
       </c>
@@ -31300,7 +31506,9 @@
       <c r="F114" s="18">
         <v>113</v>
       </c>
-      <c r="G114" s="43"/>
+      <c r="G114" s="43" t="s">
+        <v>1195</v>
+      </c>
       <c r="H114" s="36" t="s">
         <v>692</v>
       </c>
@@ -31416,7 +31624,9 @@
       <c r="F115" s="18">
         <v>114</v>
       </c>
-      <c r="G115" s="43"/>
+      <c r="G115" s="43" t="s">
+        <v>1196</v>
+      </c>
       <c r="H115" s="36" t="s">
         <v>326</v>
       </c>
@@ -31580,7 +31790,9 @@
       <c r="F116" s="18">
         <v>115</v>
       </c>
-      <c r="G116" s="43"/>
+      <c r="G116" s="43" t="s">
+        <v>1197</v>
+      </c>
       <c r="H116" s="36" t="s">
         <v>326</v>
       </c>
@@ -31678,7 +31890,9 @@
       <c r="F117" s="18">
         <v>116</v>
       </c>
-      <c r="G117" s="43"/>
+      <c r="G117" s="43" t="s">
+        <v>1198</v>
+      </c>
       <c r="H117" s="36" t="s">
         <v>326</v>
       </c>
@@ -31829,7 +32043,9 @@
       <c r="F118" s="18">
         <v>117</v>
       </c>
-      <c r="G118" s="43"/>
+      <c r="G118" s="43" t="s">
+        <v>1199</v>
+      </c>
       <c r="H118" s="36" t="s">
         <v>559</v>
       </c>
@@ -31958,7 +32174,9 @@
       <c r="F119" s="18">
         <v>118</v>
       </c>
-      <c r="G119" s="43"/>
+      <c r="G119" s="43" t="s">
+        <v>1200</v>
+      </c>
       <c r="H119" s="36" t="s">
         <v>347</v>
       </c>
@@ -32103,7 +32321,9 @@
       <c r="F120" s="18">
         <v>119</v>
       </c>
-      <c r="G120" s="43"/>
+      <c r="G120" s="43" t="s">
+        <v>1201</v>
+      </c>
       <c r="H120" s="36" t="s">
         <v>569</v>
       </c>
@@ -32394,7 +32614,9 @@
       <c r="F121" s="18">
         <v>120</v>
       </c>
-      <c r="G121" s="43"/>
+      <c r="G121" s="43" t="s">
+        <v>1202</v>
+      </c>
       <c r="H121" s="36" t="s">
         <v>326</v>
       </c>
@@ -32579,7 +32801,9 @@
       <c r="F122" s="18">
         <v>121</v>
       </c>
-      <c r="G122" s="43"/>
+      <c r="G122" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H122" s="36" t="s">
         <v>694</v>
       </c>

</xml_diff>

<commit_message>
gothic types to 167
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="0" windowWidth="13680" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="16860" yWindow="0" windowWidth="11900" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1235">
   <si>
     <t>f</t>
   </si>
@@ -3635,6 +3635,102 @@
   </si>
   <si>
     <t>Novel of domestic sadism (titular character is a prototypical Gothic villain)</t>
+  </si>
+  <si>
+    <t>Grotto Gothic (horror mode, elements of Gothified history)</t>
+  </si>
+  <si>
+    <t>Tower Gothic (elements of Gothified history)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Germanic and Schauerromantik elements, sham translation)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror mode, explained supernatural)</t>
+  </si>
+  <si>
+    <t>Gothic parody (some serious motifs mixed with satire on the Gothic heroine)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (artificial terror, numerous elements of Gothic parody)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (elements of THE MONK, monster story, transformation motif)</t>
+  </si>
+  <si>
+    <t>Prototypical Vampire Tale (Gothic characterization and scenery)</t>
+  </si>
+  <si>
+    <t>Natural Gothic horror (uses incest motif)</t>
+  </si>
+  <si>
+    <t>Gothified history</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror and horror modes)</t>
+  </si>
+  <si>
+    <t>Gothified history (authentic supernatural elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (imitation of the "first" Mrs. Radcliffe)</t>
+  </si>
+  <si>
+    <t>Radcliffe, Mary Ann</t>
+  </si>
+  <si>
+    <t>Gothified history (subdued supernatural and domesticated Gothic)</t>
+  </si>
+  <si>
+    <t>Sentimental fiction (intermittent Gothic elements)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (has Gothic elements and bears a Gothic title)</t>
+  </si>
+  <si>
+    <t>Sentimentalized Gothic (uses the motif of the mysterious key)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (various Gothic elements)</t>
+  </si>
+  <si>
+    <t>Sentimentalized Gothic (numerous Radcliffean echoes and elements)</t>
+  </si>
+  <si>
+    <t>Sentimentalized Gothic (intermittent Radcliffean elements)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (numerous sentimental elements)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (various terror elements)</t>
+  </si>
+  <si>
+    <t>Semi-Domestic Gothic (Radcliffean scenery and elements)</t>
+  </si>
+  <si>
+    <t>Sentimental fiction (residual or secondary Gothic elements)</t>
+  </si>
+  <si>
+    <t>Rauberroman (Radcliffean and Shakespearean elements)</t>
+  </si>
+  <si>
+    <t>Fake Gothic (a sentimental and social novel under a Gothic title)</t>
+  </si>
+  <si>
+    <t>Philosophical Gothic (sometimes categorized as primitive science fiction)</t>
+  </si>
+  <si>
+    <t>Gothified history (uses the castle tyrant as its main character)</t>
+  </si>
+  <si>
+    <t>Apocalyptic Gothic (futuristic science fiction)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (recessive Gothic traits)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Schauerromantik features and characters)</t>
   </si>
 </sst>
 </file>
@@ -3888,7 +3984,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="318">
+  <cellStyleXfs count="322">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4207,6 +4303,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4296,7 +4396,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="318">
+  <cellStyles count="322">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4461,6 +4561,10 @@
     <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -13509,10 +13613,10 @@
   <dimension ref="A1:GT209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G123" sqref="G123"/>
+      <selection pane="bottomRight" activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -32907,7 +33011,9 @@
       <c r="F123" s="18">
         <v>122</v>
       </c>
-      <c r="G123" s="43"/>
+      <c r="G123" s="43" t="s">
+        <v>1203</v>
+      </c>
       <c r="H123" s="36" t="s">
         <v>347</v>
       </c>
@@ -33078,7 +33184,9 @@
       <c r="F124" s="18">
         <v>123</v>
       </c>
-      <c r="G124" s="43"/>
+      <c r="G124" s="43" t="s">
+        <v>1204</v>
+      </c>
       <c r="H124" s="36" t="s">
         <v>326</v>
       </c>
@@ -33226,7 +33334,9 @@
       <c r="F125" s="18">
         <v>124</v>
       </c>
-      <c r="G125" s="43"/>
+      <c r="G125" s="43" t="s">
+        <v>1207</v>
+      </c>
       <c r="H125" s="36" t="s">
         <v>326</v>
       </c>
@@ -33305,7 +33415,9 @@
       <c r="F126" s="18">
         <v>125</v>
       </c>
-      <c r="G126" s="43"/>
+      <c r="G126" s="43" t="s">
+        <v>1205</v>
+      </c>
       <c r="H126" s="36" t="s">
         <v>697</v>
       </c>
@@ -33455,7 +33567,9 @@
       <c r="F127" s="18">
         <v>126</v>
       </c>
-      <c r="G127" s="43"/>
+      <c r="G127" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H127" s="36" t="s">
         <v>347</v>
       </c>
@@ -33573,7 +33687,9 @@
       <c r="F128" s="18">
         <v>127</v>
       </c>
-      <c r="G128" s="43"/>
+      <c r="G128" s="43" t="s">
+        <v>1206</v>
+      </c>
       <c r="H128" s="36" t="s">
         <v>581</v>
       </c>
@@ -33782,7 +33898,9 @@
       <c r="F129" s="18">
         <v>128</v>
       </c>
-      <c r="G129" s="43"/>
+      <c r="G129" s="43" t="s">
+        <v>1208</v>
+      </c>
       <c r="H129" s="36" t="s">
         <v>347</v>
       </c>
@@ -33971,7 +34089,9 @@
       <c r="F130" s="18">
         <v>129</v>
       </c>
-      <c r="G130" s="43"/>
+      <c r="G130" s="43" t="s">
+        <v>1209</v>
+      </c>
       <c r="H130" s="36" t="s">
         <v>692</v>
       </c>
@@ -34262,7 +34382,9 @@
       <c r="F131" s="18">
         <v>130</v>
       </c>
-      <c r="G131" s="43"/>
+      <c r="G131" s="43" t="s">
+        <v>1211</v>
+      </c>
       <c r="H131" s="36" t="s">
         <v>326</v>
       </c>
@@ -34490,7 +34612,9 @@
       <c r="F132" s="18">
         <v>131</v>
       </c>
-      <c r="G132" s="43"/>
+      <c r="G132" s="43" t="s">
+        <v>1210</v>
+      </c>
       <c r="H132" s="36" t="s">
         <v>943</v>
       </c>
@@ -34586,7 +34710,9 @@
       <c r="F133" s="18">
         <v>132</v>
       </c>
-      <c r="G133" s="43"/>
+      <c r="G133" s="43" t="s">
+        <v>1212</v>
+      </c>
       <c r="H133" s="36" t="s">
         <v>692</v>
       </c>
@@ -34706,7 +34832,9 @@
       <c r="F134" s="18">
         <v>133</v>
       </c>
-      <c r="G134" s="43"/>
+      <c r="G134" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H134" s="36" t="s">
         <v>326</v>
       </c>
@@ -34853,7 +34981,9 @@
       <c r="F135" s="18">
         <v>134</v>
       </c>
-      <c r="G135" s="43"/>
+      <c r="G135" s="43" t="s">
+        <v>1214</v>
+      </c>
       <c r="H135" s="36" t="s">
         <v>347</v>
       </c>
@@ -34994,7 +35124,9 @@
       <c r="F136" s="18">
         <v>135</v>
       </c>
-      <c r="G136" s="43"/>
+      <c r="G136" s="43" t="s">
+        <v>1213</v>
+      </c>
       <c r="H136" s="36" t="s">
         <v>559</v>
       </c>
@@ -35235,7 +35367,9 @@
       <c r="F137" s="18">
         <v>136</v>
       </c>
-      <c r="G137" s="43"/>
+      <c r="G137" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H137" s="36" t="s">
         <v>1078</v>
       </c>
@@ -35463,7 +35597,9 @@
       <c r="F138" s="18">
         <v>137</v>
       </c>
-      <c r="G138" s="43"/>
+      <c r="G138" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H138" s="36" t="s">
         <v>370</v>
       </c>
@@ -35689,7 +35825,9 @@
       <c r="F139" s="18">
         <v>138</v>
       </c>
-      <c r="G139" s="43"/>
+      <c r="G139" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H139" s="36" t="s">
         <v>559</v>
       </c>
@@ -35901,7 +36039,7 @@
     </row>
     <row r="140" spans="2:202">
       <c r="B140" s="3" t="s">
-        <v>150</v>
+        <v>1216</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>0</v>
@@ -35915,7 +36053,9 @@
       <c r="F140" s="18">
         <v>139</v>
       </c>
-      <c r="G140" s="43"/>
+      <c r="G140" s="43" t="s">
+        <v>1215</v>
+      </c>
       <c r="H140" s="36"/>
       <c r="I140" s="27"/>
       <c r="J140" s="27"/>
@@ -36082,7 +36222,9 @@
       <c r="F141" s="18">
         <v>140</v>
       </c>
-      <c r="G141" s="43"/>
+      <c r="G141" s="43" t="s">
+        <v>1218</v>
+      </c>
       <c r="H141" s="36"/>
       <c r="I141" s="27"/>
       <c r="J141" s="27"/>
@@ -36208,7 +36350,9 @@
       <c r="F142" s="18">
         <v>141</v>
       </c>
-      <c r="G142" s="43"/>
+      <c r="G142" s="43" t="s">
+        <v>1217</v>
+      </c>
       <c r="H142" s="36"/>
       <c r="I142" s="27"/>
       <c r="J142" s="27"/>
@@ -36277,7 +36421,9 @@
       <c r="F143" s="18">
         <v>142</v>
       </c>
-      <c r="G143" s="43"/>
+      <c r="G143" s="43" t="s">
+        <v>1218</v>
+      </c>
       <c r="H143" s="36"/>
       <c r="I143" s="27"/>
       <c r="J143" s="27"/>
@@ -36383,7 +36529,9 @@
       <c r="F144" s="18">
         <v>143</v>
       </c>
-      <c r="G144" s="43"/>
+      <c r="G144" s="43" t="s">
+        <v>1218</v>
+      </c>
       <c r="H144" s="36"/>
       <c r="I144" s="27"/>
       <c r="J144" s="27"/>
@@ -36490,7 +36638,9 @@
       <c r="F145" s="18">
         <v>144</v>
       </c>
-      <c r="G145" s="43"/>
+      <c r="G145" s="43" t="s">
+        <v>1219</v>
+      </c>
       <c r="H145" s="36"/>
       <c r="I145" s="27"/>
       <c r="J145" s="27"/>
@@ -36631,7 +36781,9 @@
       <c r="F146" s="18">
         <v>145</v>
       </c>
-      <c r="G146" s="43"/>
+      <c r="G146" s="43" t="s">
+        <v>1220</v>
+      </c>
       <c r="H146" s="36"/>
       <c r="I146" s="27"/>
       <c r="J146" s="27"/>
@@ -36775,7 +36927,9 @@
       <c r="F147" s="18">
         <v>146</v>
       </c>
-      <c r="G147" s="43"/>
+      <c r="G147" s="43" t="s">
+        <v>1221</v>
+      </c>
       <c r="H147" s="36"/>
       <c r="I147" s="27"/>
       <c r="J147" s="27"/>
@@ -36892,7 +37046,9 @@
       <c r="F148" s="18">
         <v>147</v>
       </c>
-      <c r="G148" s="43"/>
+      <c r="G148" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H148" s="36"/>
       <c r="I148" s="27"/>
       <c r="J148" s="27"/>
@@ -36999,7 +37155,9 @@
       <c r="F149" s="18">
         <v>148</v>
       </c>
-      <c r="G149" s="43"/>
+      <c r="G149" s="43" t="s">
+        <v>1226</v>
+      </c>
       <c r="H149" s="36"/>
       <c r="I149" s="27"/>
       <c r="J149" s="27"/>
@@ -37109,7 +37267,9 @@
       <c r="F150" s="18">
         <v>149</v>
       </c>
-      <c r="G150" s="43"/>
+      <c r="G150" s="43" t="s">
+        <v>1223</v>
+      </c>
       <c r="H150" s="36"/>
       <c r="I150" s="27"/>
       <c r="J150" s="27"/>
@@ -37335,7 +37495,9 @@
       <c r="F151" s="18">
         <v>150</v>
       </c>
-      <c r="G151" s="43"/>
+      <c r="G151" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H151" s="36"/>
       <c r="I151" s="27"/>
       <c r="J151" s="27"/>
@@ -37499,7 +37661,9 @@
       <c r="F152" s="18">
         <v>151</v>
       </c>
-      <c r="G152" s="43"/>
+      <c r="G152" s="43" t="s">
+        <v>1227</v>
+      </c>
       <c r="H152" s="36"/>
       <c r="I152" s="27"/>
       <c r="J152" s="27"/>
@@ -37644,7 +37808,9 @@
       <c r="F153" s="18">
         <v>152</v>
       </c>
-      <c r="G153" s="43"/>
+      <c r="G153" s="43" t="s">
+        <v>1225</v>
+      </c>
       <c r="H153" s="36"/>
       <c r="I153" s="27"/>
       <c r="J153" s="27"/>
@@ -37794,7 +37960,9 @@
       <c r="F154" s="18">
         <v>153</v>
       </c>
-      <c r="G154" s="43"/>
+      <c r="G154" s="43" t="s">
+        <v>1222</v>
+      </c>
       <c r="H154" s="36"/>
       <c r="I154" s="27"/>
       <c r="J154" s="27"/>
@@ -37875,7 +38043,9 @@
       <c r="F155" s="18">
         <v>154</v>
       </c>
-      <c r="G155" s="43"/>
+      <c r="G155" s="43" t="s">
+        <v>1224</v>
+      </c>
       <c r="H155" s="36"/>
       <c r="I155" s="27"/>
       <c r="J155" s="27"/>
@@ -38097,7 +38267,9 @@
       <c r="F156" s="18">
         <v>155</v>
       </c>
-      <c r="G156" s="43"/>
+      <c r="G156" s="43" t="s">
+        <v>1228</v>
+      </c>
       <c r="H156" s="36"/>
       <c r="I156" s="27"/>
       <c r="J156" s="27"/>
@@ -38247,7 +38419,9 @@
       <c r="F157" s="18">
         <v>156</v>
       </c>
-      <c r="G157" s="43"/>
+      <c r="G157" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H157" s="36"/>
       <c r="I157" s="27"/>
       <c r="J157" s="27"/>
@@ -38310,7 +38484,9 @@
       <c r="F158" s="18">
         <v>157</v>
       </c>
-      <c r="G158" s="43"/>
+      <c r="G158" s="43" t="s">
+        <v>1229</v>
+      </c>
       <c r="H158" s="36"/>
       <c r="I158" s="27"/>
       <c r="J158" s="27"/>
@@ -38385,7 +38561,9 @@
       <c r="F159" s="18">
         <v>158</v>
       </c>
-      <c r="G159" s="43"/>
+      <c r="G159" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H159" s="36"/>
       <c r="I159" s="27"/>
       <c r="J159" s="27"/>
@@ -38475,7 +38653,9 @@
       <c r="F160" s="18">
         <v>159</v>
       </c>
-      <c r="G160" s="43"/>
+      <c r="G160" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H160" s="36"/>
       <c r="I160" s="27"/>
       <c r="J160" s="27"/>
@@ -38575,7 +38755,9 @@
       <c r="F161" s="18">
         <v>160</v>
       </c>
-      <c r="G161" s="43"/>
+      <c r="G161" s="43" t="s">
+        <v>1212</v>
+      </c>
       <c r="H161" s="36"/>
       <c r="I161" s="27"/>
       <c r="J161" s="27"/>
@@ -38688,7 +38870,9 @@
       <c r="F162" s="18">
         <v>161</v>
       </c>
-      <c r="G162" s="43"/>
+      <c r="G162" s="43" t="s">
+        <v>1230</v>
+      </c>
       <c r="H162" s="36"/>
       <c r="I162" s="27"/>
       <c r="J162" s="27"/>
@@ -38788,7 +38972,9 @@
       <c r="F163" s="18">
         <v>162</v>
       </c>
-      <c r="G163" s="43"/>
+      <c r="G163" s="43" t="s">
+        <v>1232</v>
+      </c>
       <c r="H163" s="36"/>
       <c r="I163" s="27"/>
       <c r="J163" s="27"/>
@@ -38969,7 +39155,9 @@
       <c r="F164" s="18">
         <v>163</v>
       </c>
-      <c r="G164" s="43"/>
+      <c r="G164" s="43" t="s">
+        <v>1233</v>
+      </c>
       <c r="H164" s="36"/>
       <c r="I164" s="27"/>
       <c r="J164" s="27"/>
@@ -39054,7 +39242,9 @@
       <c r="F165" s="18">
         <v>164</v>
       </c>
-      <c r="G165" s="43"/>
+      <c r="G165" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H165" s="36"/>
       <c r="I165" s="27"/>
       <c r="J165" s="27"/>
@@ -39134,7 +39324,9 @@
       <c r="F166" s="18">
         <v>165</v>
       </c>
-      <c r="G166" s="43"/>
+      <c r="G166" s="43" t="s">
+        <v>1231</v>
+      </c>
       <c r="H166" s="36"/>
       <c r="I166" s="27"/>
       <c r="J166" s="27"/>
@@ -39285,7 +39477,9 @@
       <c r="F167" s="18">
         <v>166</v>
       </c>
-      <c r="G167" s="43"/>
+      <c r="G167" s="43" t="s">
+        <v>1234</v>
+      </c>
       <c r="H167" s="36"/>
       <c r="I167" s="27"/>
       <c r="J167" s="27"/>
@@ -39420,7 +39614,9 @@
       <c r="F168" s="18">
         <v>167</v>
       </c>
-      <c r="G168" s="43"/>
+      <c r="G168" s="43" t="s">
+        <v>1234</v>
+      </c>
       <c r="H168" s="36"/>
       <c r="I168" s="27"/>
       <c r="J168" s="27"/>

</xml_diff>

<commit_message>
finished all 208 gothic types!
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="0" windowWidth="11900" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="0" windowWidth="24600" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="1262">
   <si>
     <t>f</t>
   </si>
@@ -3625,9 +3625,6 @@
     <t>Gothic bluebook (variable plagiarism from many Gothics)</t>
   </si>
   <si>
-    <t>Pure or high Gothic (monastic shocker, excessive narual and supernatural horror)</t>
-  </si>
-  <si>
     <t>Pure or high Gothic (terror mode, in serialized form)</t>
   </si>
   <si>
@@ -3731,6 +3728,90 @@
   </si>
   <si>
     <t>Pure or high Gothic (Schauerromantik features and characters)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (elements of THE MONK's loathsome descriptions)</t>
+  </si>
+  <si>
+    <t>Domestic Gothic (apparitional visitations)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (monastic shocker, excessive natural and supernatural horror)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror elements, Germanic elements and sublime topographies)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (horrific medievalism, situations from Walpole and Reeve)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Radcliffean imitation)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (terror elements)</t>
+  </si>
+  <si>
+    <t>Sentimentalized Gothic (various Radcliffean devices and effects)</t>
+  </si>
+  <si>
+    <t>Picaresque fiction (several heavily pre-Gothic episodes)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (imitation of THE ITALIAN, elements of the monastic shocker)</t>
+  </si>
+  <si>
+    <t>Sentimental Gothic (epistolary format, Radcliffean elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (monastic shocker elements)</t>
+  </si>
+  <si>
+    <t>Sentimental Gothic (numerous spectral components, especially in the subplots)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (natural terror)</t>
+  </si>
+  <si>
+    <t>Sentimental Gothic (no supernatural elements)</t>
+  </si>
+  <si>
+    <t>Gothified history (intermittent terror elements)</t>
+  </si>
+  <si>
+    <t>Orientalized Gothic (Gothic passions but minimal terror and horror)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (imitation of THE CASTLE OF OTRANTO)</t>
+  </si>
+  <si>
+    <t>Polemical fiction (numerous Gothic elements)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (strains of horror, terror, and Schauerromantik effects)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (first of the first Gothics and technical prototype)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (influence of THE CASTLE OF OTRANTO and Leland's LONGSWORD)</t>
+  </si>
+  <si>
+    <t>Domestic fiction (recessant Gothic traits)</t>
+  </si>
+  <si>
+    <t>Gothic chapbook (compressed Gothified history)</t>
+  </si>
+  <si>
+    <t>Gothic bluebook</t>
+  </si>
+  <si>
+    <t>Date from Frederick Frank</t>
+  </si>
+  <si>
+    <t>Domestic fiction (digressive Gothic tendencies)</t>
+  </si>
+  <si>
+    <t>Pure or high Gothic (Radcliffean elements)</t>
   </si>
 </sst>
 </file>
@@ -3984,7 +4065,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="322">
+  <cellStyleXfs count="327">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4307,6 +4388,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4396,7 +4482,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="322">
+  <cellStyles count="327">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4565,6 +4651,11 @@
     <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -13613,10 +13704,10 @@
   <dimension ref="A1:GT209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G145" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G169" sqref="G169"/>
+      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -32148,7 +32239,7 @@
         <v>117</v>
       </c>
       <c r="G118" s="43" t="s">
-        <v>1199</v>
+        <v>1236</v>
       </c>
       <c r="H118" s="36" t="s">
         <v>559</v>
@@ -32279,7 +32370,7 @@
         <v>118</v>
       </c>
       <c r="G119" s="43" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="H119" s="36" t="s">
         <v>347</v>
@@ -32426,7 +32517,7 @@
         <v>119</v>
       </c>
       <c r="G120" s="43" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="H120" s="36" t="s">
         <v>569</v>
@@ -32719,7 +32810,7 @@
         <v>120</v>
       </c>
       <c r="G121" s="43" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H121" s="36" t="s">
         <v>326</v>
@@ -33012,7 +33103,7 @@
         <v>122</v>
       </c>
       <c r="G123" s="43" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="H123" s="36" t="s">
         <v>347</v>
@@ -33185,7 +33276,7 @@
         <v>123</v>
       </c>
       <c r="G124" s="43" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="H124" s="36" t="s">
         <v>326</v>
@@ -33335,7 +33426,7 @@
         <v>124</v>
       </c>
       <c r="G125" s="43" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H125" s="36" t="s">
         <v>326</v>
@@ -33416,7 +33507,7 @@
         <v>125</v>
       </c>
       <c r="G126" s="43" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="H126" s="36" t="s">
         <v>697</v>
@@ -33688,7 +33779,7 @@
         <v>127</v>
       </c>
       <c r="G128" s="43" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H128" s="36" t="s">
         <v>581</v>
@@ -33899,7 +33990,7 @@
         <v>128</v>
       </c>
       <c r="G129" s="43" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H129" s="36" t="s">
         <v>347</v>
@@ -34090,7 +34181,7 @@
         <v>129</v>
       </c>
       <c r="G130" s="43" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="H130" s="36" t="s">
         <v>692</v>
@@ -34383,7 +34474,7 @@
         <v>130</v>
       </c>
       <c r="G131" s="43" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H131" s="36" t="s">
         <v>326</v>
@@ -34613,7 +34704,7 @@
         <v>131</v>
       </c>
       <c r="G132" s="43" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="H132" s="36" t="s">
         <v>943</v>
@@ -34711,7 +34802,7 @@
         <v>132</v>
       </c>
       <c r="G133" s="43" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H133" s="36" t="s">
         <v>692</v>
@@ -34982,7 +35073,7 @@
         <v>134</v>
       </c>
       <c r="G135" s="43" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H135" s="36" t="s">
         <v>347</v>
@@ -35125,7 +35216,7 @@
         <v>135</v>
       </c>
       <c r="G136" s="43" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="H136" s="36" t="s">
         <v>559</v>
@@ -36039,7 +36130,7 @@
     </row>
     <row r="140" spans="2:202">
       <c r="B140" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>0</v>
@@ -36054,7 +36145,7 @@
         <v>139</v>
       </c>
       <c r="G140" s="43" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="H140" s="36"/>
       <c r="I140" s="27"/>
@@ -36223,7 +36314,7 @@
         <v>140</v>
       </c>
       <c r="G141" s="43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H141" s="36"/>
       <c r="I141" s="27"/>
@@ -36351,7 +36442,7 @@
         <v>141</v>
       </c>
       <c r="G142" s="43" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="H142" s="36"/>
       <c r="I142" s="27"/>
@@ -36422,7 +36513,7 @@
         <v>142</v>
       </c>
       <c r="G143" s="43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H143" s="36"/>
       <c r="I143" s="27"/>
@@ -36530,7 +36621,7 @@
         <v>143</v>
       </c>
       <c r="G144" s="43" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H144" s="36"/>
       <c r="I144" s="27"/>
@@ -36639,7 +36730,7 @@
         <v>144</v>
       </c>
       <c r="G145" s="43" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H145" s="36"/>
       <c r="I145" s="27"/>
@@ -36782,7 +36873,7 @@
         <v>145</v>
       </c>
       <c r="G146" s="43" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H146" s="36"/>
       <c r="I146" s="27"/>
@@ -36928,7 +37019,7 @@
         <v>146</v>
       </c>
       <c r="G147" s="43" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H147" s="36"/>
       <c r="I147" s="27"/>
@@ -37156,7 +37247,7 @@
         <v>148</v>
       </c>
       <c r="G149" s="43" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="H149" s="36"/>
       <c r="I149" s="27"/>
@@ -37268,7 +37359,7 @@
         <v>149</v>
       </c>
       <c r="G150" s="43" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H150" s="36"/>
       <c r="I150" s="27"/>
@@ -37662,7 +37753,7 @@
         <v>151</v>
       </c>
       <c r="G152" s="43" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H152" s="36"/>
       <c r="I152" s="27"/>
@@ -37809,7 +37900,7 @@
         <v>152</v>
       </c>
       <c r="G153" s="43" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="H153" s="36"/>
       <c r="I153" s="27"/>
@@ -37961,7 +38052,7 @@
         <v>153</v>
       </c>
       <c r="G154" s="43" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="H154" s="36"/>
       <c r="I154" s="27"/>
@@ -38044,7 +38135,7 @@
         <v>154</v>
       </c>
       <c r="G155" s="43" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H155" s="36"/>
       <c r="I155" s="27"/>
@@ -38268,7 +38359,7 @@
         <v>155</v>
       </c>
       <c r="G156" s="43" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="H156" s="36"/>
       <c r="I156" s="27"/>
@@ -38485,7 +38576,7 @@
         <v>157</v>
       </c>
       <c r="G158" s="43" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="H158" s="36"/>
       <c r="I158" s="27"/>
@@ -38756,7 +38847,7 @@
         <v>160</v>
       </c>
       <c r="G161" s="43" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H161" s="36"/>
       <c r="I161" s="27"/>
@@ -38871,7 +38962,7 @@
         <v>161</v>
       </c>
       <c r="G162" s="43" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="H162" s="36"/>
       <c r="I162" s="27"/>
@@ -38973,7 +39064,7 @@
         <v>162</v>
       </c>
       <c r="G163" s="43" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="H163" s="36"/>
       <c r="I163" s="27"/>
@@ -39156,7 +39247,7 @@
         <v>163</v>
       </c>
       <c r="G164" s="43" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="H164" s="36"/>
       <c r="I164" s="27"/>
@@ -39325,7 +39416,7 @@
         <v>165</v>
       </c>
       <c r="G166" s="43" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="H166" s="36"/>
       <c r="I166" s="27"/>
@@ -39478,7 +39569,7 @@
         <v>166</v>
       </c>
       <c r="G167" s="43" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="H167" s="36"/>
       <c r="I167" s="27"/>
@@ -39615,7 +39706,7 @@
         <v>167</v>
       </c>
       <c r="G168" s="43" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="H168" s="36"/>
       <c r="I168" s="27"/>
@@ -39741,7 +39832,9 @@
       <c r="F169" s="18">
         <v>168</v>
       </c>
-      <c r="G169" s="43"/>
+      <c r="G169" s="43" t="s">
+        <v>1234</v>
+      </c>
       <c r="H169" s="36"/>
       <c r="I169" s="27"/>
       <c r="J169" s="27"/>
@@ -39917,7 +40010,9 @@
       <c r="F170" s="18">
         <v>169</v>
       </c>
-      <c r="G170" s="43"/>
+      <c r="G170" s="43" t="s">
+        <v>1235</v>
+      </c>
       <c r="H170" s="36"/>
       <c r="I170" s="27"/>
       <c r="J170" s="27"/>
@@ -40012,7 +40107,9 @@
       <c r="F171" s="18">
         <v>170</v>
       </c>
-      <c r="G171" s="43"/>
+      <c r="G171" s="43" t="s">
+        <v>1238</v>
+      </c>
       <c r="H171" s="36"/>
       <c r="I171" s="27"/>
       <c r="J171" s="27"/>
@@ -40141,7 +40238,9 @@
       <c r="F172" s="18">
         <v>171</v>
       </c>
-      <c r="G172" s="43"/>
+      <c r="G172" s="43" t="s">
+        <v>1237</v>
+      </c>
       <c r="H172" s="36"/>
       <c r="I172" s="27"/>
       <c r="J172" s="27"/>
@@ -40291,7 +40390,9 @@
       <c r="F173" s="18">
         <v>172</v>
       </c>
-      <c r="G173" s="43"/>
+      <c r="G173" s="43" t="s">
+        <v>1239</v>
+      </c>
       <c r="H173" s="36"/>
       <c r="I173" s="27"/>
       <c r="J173" s="27"/>
@@ -40435,7 +40536,9 @@
       <c r="F174" s="18">
         <v>173</v>
       </c>
-      <c r="G174" s="43"/>
+      <c r="G174" s="43" t="s">
+        <v>1240</v>
+      </c>
       <c r="H174" s="36"/>
       <c r="I174" s="27"/>
       <c r="J174" s="27"/>
@@ -40537,7 +40640,9 @@
       <c r="F175" s="18">
         <v>174</v>
       </c>
-      <c r="G175" s="43"/>
+      <c r="G175" s="43" t="s">
+        <v>1140</v>
+      </c>
       <c r="H175" s="36"/>
       <c r="I175" s="27"/>
       <c r="J175" s="27"/>
@@ -40752,7 +40857,9 @@
       <c r="F176" s="18">
         <v>175</v>
       </c>
-      <c r="G176" s="43"/>
+      <c r="G176" s="43" t="s">
+        <v>1241</v>
+      </c>
       <c r="H176" s="36"/>
       <c r="I176" s="27"/>
       <c r="J176" s="27"/>
@@ -40873,7 +40980,9 @@
       <c r="F177" s="18">
         <v>176</v>
       </c>
-      <c r="G177" s="43"/>
+      <c r="G177" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H177" s="36"/>
       <c r="I177" s="27"/>
       <c r="J177" s="27"/>
@@ -40967,7 +41076,9 @@
       <c r="F178" s="18">
         <v>177</v>
       </c>
-      <c r="G178" s="43"/>
+      <c r="G178" s="43" t="s">
+        <v>1242</v>
+      </c>
       <c r="H178" s="36"/>
       <c r="I178" s="27"/>
       <c r="J178" s="27"/>
@@ -41164,7 +41275,9 @@
       <c r="F179" s="18">
         <v>178</v>
       </c>
-      <c r="G179" s="43"/>
+      <c r="G179" s="43" t="s">
+        <v>1243</v>
+      </c>
       <c r="H179" s="36"/>
       <c r="I179" s="27"/>
       <c r="J179" s="27"/>
@@ -41305,7 +41418,9 @@
       <c r="F180" s="18">
         <v>179</v>
       </c>
-      <c r="G180" s="43"/>
+      <c r="G180" s="43" t="s">
+        <v>1250</v>
+      </c>
       <c r="H180" s="36"/>
       <c r="I180" s="27"/>
       <c r="J180" s="27"/>
@@ -41406,7 +41521,9 @@
       <c r="F181" s="18">
         <v>180</v>
       </c>
-      <c r="G181" s="43"/>
+      <c r="G181" s="43" t="s">
+        <v>1245</v>
+      </c>
       <c r="H181" s="36"/>
       <c r="I181" s="27"/>
       <c r="J181" s="27"/>
@@ -41596,7 +41713,9 @@
       <c r="F182" s="18">
         <v>181</v>
       </c>
-      <c r="G182" s="43"/>
+      <c r="G182" s="43" t="s">
+        <v>1246</v>
+      </c>
       <c r="H182" s="36"/>
       <c r="I182" s="27"/>
       <c r="J182" s="27"/>
@@ -41691,7 +41810,9 @@
       <c r="F183" s="18">
         <v>182</v>
       </c>
-      <c r="G183" s="43"/>
+      <c r="G183" s="43" t="s">
+        <v>1244</v>
+      </c>
       <c r="H183" s="36"/>
       <c r="I183" s="27"/>
       <c r="J183" s="27"/>
@@ -41817,7 +41938,9 @@
       <c r="F184" s="18">
         <v>183</v>
       </c>
-      <c r="G184" s="43"/>
+      <c r="G184" s="43" t="s">
+        <v>1248</v>
+      </c>
       <c r="H184" s="36"/>
       <c r="I184" s="27"/>
       <c r="J184" s="27"/>
@@ -41954,7 +42077,9 @@
       <c r="F185" s="18">
         <v>184</v>
       </c>
-      <c r="G185" s="43"/>
+      <c r="G185" s="43" t="s">
+        <v>1249</v>
+      </c>
       <c r="H185" s="36"/>
       <c r="I185" s="27"/>
       <c r="J185" s="27"/>
@@ -42057,7 +42182,9 @@
       <c r="F186" s="18">
         <v>185</v>
       </c>
-      <c r="G186" s="43"/>
+      <c r="G186" s="43" t="s">
+        <v>1247</v>
+      </c>
       <c r="H186" s="36"/>
       <c r="I186" s="27"/>
       <c r="J186" s="27"/>
@@ -42211,7 +42338,9 @@
       <c r="F187" s="18">
         <v>186</v>
       </c>
-      <c r="G187" s="43"/>
+      <c r="G187" s="43" t="s">
+        <v>1137</v>
+      </c>
       <c r="H187" s="36"/>
       <c r="I187" s="27"/>
       <c r="J187" s="27"/>
@@ -42353,7 +42482,9 @@
       <c r="F188" s="18">
         <v>187</v>
       </c>
-      <c r="G188" s="43"/>
+      <c r="G188" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H188" s="36"/>
       <c r="I188" s="27"/>
       <c r="J188" s="27"/>
@@ -42526,7 +42657,9 @@
       <c r="F189" s="18">
         <v>188</v>
       </c>
-      <c r="G189" s="43"/>
+      <c r="G189" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H189" s="36"/>
       <c r="I189" s="27"/>
       <c r="J189" s="27"/>
@@ -42653,7 +42786,9 @@
       <c r="F190" s="18">
         <v>189</v>
       </c>
-      <c r="G190" s="43"/>
+      <c r="G190" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H190" s="36"/>
       <c r="I190" s="27"/>
       <c r="J190" s="27"/>
@@ -42770,7 +42905,9 @@
       <c r="F191" s="18">
         <v>190</v>
       </c>
-      <c r="G191" s="43"/>
+      <c r="G191" s="43" t="s">
+        <v>1253</v>
+      </c>
       <c r="H191" s="36"/>
       <c r="I191" s="27"/>
       <c r="J191" s="27"/>
@@ -42922,7 +43059,9 @@
       <c r="F192" s="18">
         <v>191</v>
       </c>
-      <c r="G192" s="43"/>
+      <c r="G192" s="43" t="s">
+        <v>1251</v>
+      </c>
       <c r="H192" s="36"/>
       <c r="I192" s="27"/>
       <c r="J192" s="27"/>
@@ -43074,7 +43213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:202">
+    <row r="193" spans="1:202">
       <c r="B193" s="3" t="s">
         <v>57</v>
       </c>
@@ -43090,7 +43229,9 @@
       <c r="F193" s="18">
         <v>192</v>
       </c>
-      <c r="G193" s="43"/>
+      <c r="G193" s="43" t="s">
+        <v>1252</v>
+      </c>
       <c r="H193" s="36"/>
       <c r="I193" s="27"/>
       <c r="J193" s="27"/>
@@ -43208,7 +43349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="2:202">
+    <row r="194" spans="1:202">
       <c r="B194" s="3" t="s">
         <v>55</v>
       </c>
@@ -43224,7 +43365,9 @@
       <c r="F194" s="18">
         <v>193</v>
       </c>
-      <c r="G194" s="43"/>
+      <c r="G194" s="43" t="s">
+        <v>1254</v>
+      </c>
       <c r="H194" s="36"/>
       <c r="I194" s="27"/>
       <c r="J194" s="27"/>
@@ -43391,7 +43534,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="195" spans="2:202">
+    <row r="195" spans="1:202">
       <c r="B195" s="3" t="s">
         <v>52</v>
       </c>
@@ -43407,7 +43550,9 @@
       <c r="F195" s="18">
         <v>194</v>
       </c>
-      <c r="G195" s="43"/>
+      <c r="G195" s="43" t="s">
+        <v>1255</v>
+      </c>
       <c r="H195" s="36"/>
       <c r="I195" s="27"/>
       <c r="J195" s="27"/>
@@ -43505,7 +43650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:202">
+    <row r="196" spans="1:202">
       <c r="B196" s="3" t="s">
         <v>48</v>
       </c>
@@ -43521,7 +43666,9 @@
       <c r="F196" s="18">
         <v>195</v>
       </c>
-      <c r="G196" s="43"/>
+      <c r="G196" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H196" s="36"/>
       <c r="I196" s="27"/>
       <c r="J196" s="27"/>
@@ -43594,7 +43741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="2:202">
+    <row r="197" spans="1:202">
       <c r="B197" s="3" t="s">
         <v>48</v>
       </c>
@@ -43610,7 +43757,9 @@
       <c r="F197" s="18">
         <v>196</v>
       </c>
-      <c r="G197" s="43"/>
+      <c r="G197" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H197" s="36"/>
       <c r="I197" s="27"/>
       <c r="J197" s="27"/>
@@ -43660,7 +43809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:202">
+    <row r="198" spans="1:202">
       <c r="B198" s="3" t="s">
         <v>48</v>
       </c>
@@ -43676,7 +43825,9 @@
       <c r="F198" s="18">
         <v>197</v>
       </c>
-      <c r="G198" s="43"/>
+      <c r="G198" s="43" t="s">
+        <v>1256</v>
+      </c>
       <c r="H198" s="36"/>
       <c r="I198" s="27"/>
       <c r="J198" s="27"/>
@@ -43726,7 +43877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="2:202">
+    <row r="199" spans="1:202">
       <c r="B199" s="3" t="s">
         <v>34</v>
       </c>
@@ -43742,7 +43893,9 @@
       <c r="F199" s="18">
         <v>198</v>
       </c>
-      <c r="G199" s="43"/>
+      <c r="G199" s="43" t="s">
+        <v>1257</v>
+      </c>
       <c r="H199" s="36"/>
       <c r="I199" s="27"/>
       <c r="J199" s="27"/>
@@ -43795,7 +43948,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="200" spans="2:202">
+    <row r="200" spans="1:202">
       <c r="B200" s="3" t="s">
         <v>34</v>
       </c>
@@ -43811,7 +43964,9 @@
       <c r="F200" s="18">
         <v>199</v>
       </c>
-      <c r="G200" s="43"/>
+      <c r="G200" s="43" t="s">
+        <v>1128</v>
+      </c>
       <c r="H200" s="36"/>
       <c r="I200" s="27"/>
       <c r="J200" s="27"/>
@@ -43973,7 +44128,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="201" spans="2:202">
+    <row r="201" spans="1:202">
+      <c r="A201" s="3" t="s">
+        <v>1259</v>
+      </c>
       <c r="B201" s="3" t="s">
         <v>34</v>
       </c>
@@ -43983,13 +44141,15 @@
       <c r="D201" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E201" s="5" t="s">
-        <v>32</v>
+      <c r="E201" s="4">
+        <v>1820</v>
       </c>
       <c r="F201" s="18">
         <v>200</v>
       </c>
-      <c r="G201" s="43"/>
+      <c r="G201" s="43" t="s">
+        <v>1135</v>
+      </c>
       <c r="H201" s="36"/>
       <c r="I201" s="27"/>
       <c r="J201" s="27"/>
@@ -44099,7 +44259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="2:202">
+    <row r="202" spans="1:202">
       <c r="B202" s="3" t="s">
         <v>34</v>
       </c>
@@ -44115,7 +44275,9 @@
       <c r="F202" s="18">
         <v>201</v>
       </c>
-      <c r="G202" s="43"/>
+      <c r="G202" s="43" t="s">
+        <v>1258</v>
+      </c>
       <c r="H202" s="36"/>
       <c r="I202" s="27"/>
       <c r="J202" s="27"/>
@@ -44222,7 +44384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:202">
+    <row r="203" spans="1:202">
       <c r="B203" s="3" t="s">
         <v>34</v>
       </c>
@@ -44238,7 +44400,9 @@
       <c r="F203" s="18">
         <v>202</v>
       </c>
-      <c r="G203" s="43"/>
+      <c r="G203" s="43" t="s">
+        <v>1126</v>
+      </c>
       <c r="H203" s="36"/>
       <c r="I203" s="27"/>
       <c r="J203" s="27"/>
@@ -44323,7 +44487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="2:202">
+    <row r="204" spans="1:202">
       <c r="B204" s="3" t="s">
         <v>29</v>
       </c>
@@ -44339,7 +44503,9 @@
       <c r="F204" s="18">
         <v>203</v>
       </c>
-      <c r="G204" s="43"/>
+      <c r="G204" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H204" s="36"/>
       <c r="I204" s="27"/>
       <c r="J204" s="27"/>
@@ -44422,7 +44588,7 @@
       <c r="DY204" s="23"/>
       <c r="FJ204" s="23"/>
     </row>
-    <row r="205" spans="2:202">
+    <row r="205" spans="1:202">
       <c r="B205" s="3" t="s">
         <v>22</v>
       </c>
@@ -44438,7 +44604,9 @@
       <c r="F205" s="18">
         <v>204</v>
       </c>
-      <c r="G205" s="43"/>
+      <c r="G205" s="43" t="s">
+        <v>1129</v>
+      </c>
       <c r="H205" s="36"/>
       <c r="I205" s="27"/>
       <c r="J205" s="27"/>
@@ -44607,7 +44775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="2:202">
+    <row r="206" spans="1:202">
       <c r="B206" s="3" t="s">
         <v>22</v>
       </c>
@@ -44623,7 +44791,9 @@
       <c r="F206" s="18">
         <v>205</v>
       </c>
-      <c r="G206" s="43"/>
+      <c r="G206" s="43" t="s">
+        <v>1260</v>
+      </c>
       <c r="H206" s="36"/>
       <c r="I206" s="27"/>
       <c r="J206" s="27"/>
@@ -44714,7 +44884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="2:202">
+    <row r="207" spans="1:202">
       <c r="B207" s="3" t="s">
         <v>16</v>
       </c>
@@ -44730,7 +44900,9 @@
       <c r="F207" s="18">
         <v>206</v>
       </c>
-      <c r="G207" s="43"/>
+      <c r="G207" s="43" t="s">
+        <v>1133</v>
+      </c>
       <c r="H207" s="36"/>
       <c r="I207" s="27"/>
       <c r="J207" s="27"/>
@@ -44902,7 +45074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="2:202">
+    <row r="208" spans="1:202">
       <c r="B208" s="3" t="s">
         <v>16</v>
       </c>
@@ -44918,7 +45090,9 @@
       <c r="F208" s="18">
         <v>207</v>
       </c>
-      <c r="G208" s="43"/>
+      <c r="G208" s="43" t="s">
+        <v>1133</v>
+      </c>
       <c r="H208" s="36"/>
       <c r="I208" s="27"/>
       <c r="J208" s="27"/>
@@ -45161,7 +45335,9 @@
       <c r="F209" s="18">
         <v>208</v>
       </c>
-      <c r="G209" s="43"/>
+      <c r="G209" s="43" t="s">
+        <v>1261</v>
+      </c>
       <c r="H209" s="36"/>
       <c r="I209" s="27"/>
       <c r="J209" s="27"/>

</xml_diff>

<commit_message>
outline of a tentative argument!
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7340" yWindow="4700" windowWidth="20420" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -12,17 +12,14 @@
     <sheet name="ocr" sheetId="7" r:id="rId3"/>
     <sheet name="length" sheetId="6" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="2" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
-    <pivotCache cacheId="4" r:id="rId10"/>
-    <pivotCache cacheId="91" r:id="rId11"/>
+    <pivotCache cacheId="128" r:id="rId5"/>
+    <pivotCache cacheId="129" r:id="rId6"/>
+    <pivotCache cacheId="130" r:id="rId7"/>
+    <pivotCache cacheId="131" r:id="rId8"/>
+    <pivotCache cacheId="132" r:id="rId9"/>
+    <pivotCache cacheId="133" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -5172,7 +5169,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5231,7 +5227,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5286,7 +5281,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5348,7 +5342,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5408,7 +5401,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5470,7 +5462,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5623,19 +5614,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="murder"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18678,121 +18656,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="33">
-        <item x="5"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="23"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="20"/>
-        <item m="1" x="31"/>
-        <item m="1" x="27"/>
-        <item m="1" x="22"/>
-        <item m="1" x="21"/>
-        <item m="1" x="19"/>
-        <item m="1" x="24"/>
-        <item m="1" x="28"/>
-        <item m="1" x="30"/>
-        <item m="1" x="25"/>
-        <item m="1" x="18"/>
-        <item m="1" x="29"/>
-        <item m="1" x="17"/>
-        <item m="1" x="26"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="132" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E1:I32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -19317,8 +19181,122 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="133" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="33">
+        <item x="5"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="20"/>
+        <item m="1" x="31"/>
+        <item m="1" x="27"/>
+        <item m="1" x="22"/>
+        <item m="1" x="21"/>
+        <item m="1" x="19"/>
+        <item m="1" x="24"/>
+        <item m="1" x="28"/>
+        <item m="1" x="30"/>
+        <item m="1" x="25"/>
+        <item m="1" x="18"/>
+        <item m="1" x="29"/>
+        <item m="1" x="17"/>
+        <item m="1" x="26"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="131" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B137" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" countASubtotal="1">
@@ -19899,7 +19877,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="130" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField dataField="1" showAll="0"/>
@@ -19996,113 +19974,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="128" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -20228,6 +20100,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="129" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -20564,11 +20542,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GU209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B102" sqref="B102"/>
+      <selection pane="bottomRight" activeCell="S87" sqref="S87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52851,7 +52829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I137"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
gothic types to F53, for real this time
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4436,7 +4436,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="354">
+  <cellStyleXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4791,6 +4791,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4940,7 +4941,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="354">
+  <cellStyles count="355">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5141,6 +5142,7 @@
     <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -20902,7 +20904,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H60" sqref="H60"/>
+      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
gothic types to 105
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="14840" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="0" windowWidth="18020" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -14,12 +14,12 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId5"/>
-    <pivotCache cacheId="7" r:id="rId6"/>
-    <pivotCache cacheId="8" r:id="rId7"/>
-    <pivotCache cacheId="9" r:id="rId8"/>
-    <pivotCache cacheId="10" r:id="rId9"/>
-    <pivotCache cacheId="11" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId9"/>
+    <pivotCache cacheId="5" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -4490,7 +4490,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="360">
+  <cellStyleXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4851,6 +4851,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5000,7 +5001,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="360">
+  <cellStyles count="361">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5207,6 +5208,7 @@
     <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -19078,121 +19080,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="33">
-        <item x="5"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="23"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="20"/>
-        <item m="1" x="31"/>
-        <item m="1" x="27"/>
-        <item m="1" x="22"/>
-        <item m="1" x="21"/>
-        <item m="1" x="19"/>
-        <item m="1" x="24"/>
-        <item m="1" x="28"/>
-        <item m="1" x="30"/>
-        <item m="1" x="25"/>
-        <item m="1" x="18"/>
-        <item m="1" x="29"/>
-        <item m="1" x="17"/>
-        <item m="1" x="26"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E1:I32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -19717,8 +19605,122 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="33">
+        <item x="5"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="20"/>
+        <item m="1" x="31"/>
+        <item m="1" x="27"/>
+        <item m="1" x="22"/>
+        <item m="1" x="21"/>
+        <item m="1" x="19"/>
+        <item m="1" x="24"/>
+        <item m="1" x="28"/>
+        <item m="1" x="30"/>
+        <item m="1" x="25"/>
+        <item m="1" x="18"/>
+        <item m="1" x="29"/>
+        <item m="1" x="17"/>
+        <item m="1" x="26"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B137" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" countASubtotal="1">
@@ -20299,7 +20301,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField dataField="1" showAll="0"/>
@@ -20396,113 +20398,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -20628,6 +20524,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -20964,8 +20966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GV262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
@@ -56949,10 +56951,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58682,6 +58684,17 @@
         <v>208</v>
       </c>
     </row>
+    <row r="139" spans="1:2">
+      <c r="A139">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140">
+        <f>208-30</f>
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="E34:F51">
     <sortCondition descending="1" ref="F36"/>

</xml_diff>

<commit_message>
put together slides for SWPACA presentation!
</commit_message>
<xml_diff>
--- a/SPREADSHEET.xlsx
+++ b/SPREADSHEET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="0" windowWidth="18020" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="1640" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DATA" sheetId="2" r:id="rId1"/>
@@ -14,12 +14,12 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="302" r:id="rId5"/>
-    <pivotCache cacheId="303" r:id="rId6"/>
-    <pivotCache cacheId="304" r:id="rId7"/>
-    <pivotCache cacheId="305" r:id="rId8"/>
-    <pivotCache cacheId="306" r:id="rId9"/>
-    <pivotCache cacheId="307" r:id="rId10"/>
+    <pivotCache cacheId="308" r:id="rId5"/>
+    <pivotCache cacheId="309" r:id="rId6"/>
+    <pivotCache cacheId="310" r:id="rId7"/>
+    <pivotCache cacheId="311" r:id="rId8"/>
+    <pivotCache cacheId="312" r:id="rId9"/>
+    <pivotCache cacheId="313" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19101,121 +19101,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="307" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="33">
-        <item x="5"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="23"/>
-        <item m="1" x="15"/>
-        <item m="1" x="16"/>
-        <item m="1" x="20"/>
-        <item m="1" x="31"/>
-        <item m="1" x="27"/>
-        <item m="1" x="22"/>
-        <item m="1" x="21"/>
-        <item m="1" x="19"/>
-        <item m="1" x="24"/>
-        <item m="1" x="28"/>
-        <item m="1" x="30"/>
-        <item m="1" x="25"/>
-        <item m="1" x="18"/>
-        <item m="1" x="29"/>
-        <item m="1" x="17"/>
-        <item m="1" x="26"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="306" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="312" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E1:I32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -19740,8 +19626,122 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="313" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="E34:F51" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="33">
+        <item x="5"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="16"/>
+        <item m="1" x="20"/>
+        <item m="1" x="31"/>
+        <item m="1" x="27"/>
+        <item m="1" x="22"/>
+        <item m="1" x="21"/>
+        <item m="1" x="19"/>
+        <item m="1" x="24"/>
+        <item m="1" x="28"/>
+        <item m="1" x="30"/>
+        <item m="1" x="25"/>
+        <item m="1" x="18"/>
+        <item m="1" x="29"/>
+        <item m="1" x="17"/>
+        <item m="1" x="26"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Title" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="305" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="311" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B137" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" countASubtotal="1">
@@ -20322,7 +20322,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="304" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="310" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField dataField="1" showAll="0"/>
@@ -20419,113 +20419,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="303" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="2"/>
-        <item x="15"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="302" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="308" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -20651,6 +20545,112 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="309" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="2"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Author" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -20988,10 +20988,10 @@
   <dimension ref="A1:GV268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="BG188" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G73" sqref="G73"/>
+      <selection pane="bottomRight" activeCell="BW224" sqref="BW224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>